<commit_message>
KCOR ASMR computation upgraded
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -481,17 +481,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.1727</t>
+          <t>0.9919</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.020</t>
         </is>
       </c>
     </row>
@@ -504,17 +504,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9186</t>
+          <t>0.9509</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.707</t>
+          <t>0.732</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -527,17 +527,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7849</t>
+          <t>0.7677</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.700</t>
+          <t>0.684</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.862</t>
         </is>
       </c>
     </row>
@@ -550,17 +550,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8212</t>
+          <t>0.8327</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.758</t>
+          <t>0.768</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.903</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1888</t>
+          <t>1.0673</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0015</t>
+          <t>1.0057</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0737</t>
+          <t>1.0036</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>0.940</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -642,17 +642,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2292</t>
+          <t>1.1486</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.323</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -665,17 +665,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.3463</t>
+          <t>1.1557</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -688,17 +688,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.2006</t>
+          <t>1.1638</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.304</t>
         </is>
       </c>
     </row>
@@ -711,17 +711,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.8715</t>
+          <t>0.9308</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.064</t>
         </is>
       </c>
     </row>
@@ -734,17 +734,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.2357</t>
+          <t>1.1867</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.014</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.446</t>
+          <t>1.389</t>
         </is>
       </c>
     </row>
@@ -757,17 +757,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.2498</t>
+          <t>1.1811</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.519</t>
+          <t>1.436</t>
         </is>
       </c>
     </row>
@@ -780,17 +780,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.6555</t>
+          <t>0.6772</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.502</t>
+          <t>0.518</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>0.885</t>
         </is>
       </c>
     </row>
@@ -803,17 +803,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0604</t>
+          <t>1.3873</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.629</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.788</t>
+          <t>2.341</t>
         </is>
       </c>
     </row>
@@ -826,17 +826,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3.2430</t>
+          <t>2.5871</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.318</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>7.982</t>
+          <t>6.370</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.2718</t>
+          <t>0.4564</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -859,7 +859,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.718</t>
+          <t>4.564</t>
         </is>
       </c>
     </row>
@@ -872,17 +872,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.1148</t>
+          <t>0.2059</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.065</t>
+          <t>0.117</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.203</t>
+          <t>0.364</t>
         </is>
       </c>
     </row>
@@ -913,17 +913,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.3078</t>
+          <t>1.2238</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.198</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.250</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8870</t>
+          <t>0.8381</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.779</t>
+          <t>0.736</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.010</t>
+          <t>0.954</t>
         </is>
       </c>
     </row>
@@ -959,17 +959,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.7904</t>
+          <t>0.8553</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.738</t>
+          <t>0.798</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.847</t>
+          <t>0.916</t>
         </is>
       </c>
     </row>
@@ -982,17 +982,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9592</t>
+          <t>0.9577</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.912</t>
+          <t>0.910</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.008</t>
         </is>
       </c>
     </row>
@@ -1005,17 +1005,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.3569</t>
+          <t>1.2503</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.289</t>
+          <t>1.188</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.428</t>
+          <t>1.316</t>
         </is>
       </c>
     </row>
@@ -1028,17 +1028,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2348</t>
+          <t>1.2554</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.194</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3990</t>
+          <t>1.3348</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.327</t>
+          <t>1.266</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.475</t>
+          <t>1.408</t>
         </is>
       </c>
     </row>
@@ -1074,17 +1074,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.7457</t>
+          <t>1.5970</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.496</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.864</t>
+          <t>1.705</t>
         </is>
       </c>
     </row>
@@ -1097,17 +1097,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.6760</t>
+          <t>1.5021</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.535</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.830</t>
+          <t>1.640</t>
         </is>
       </c>
     </row>
@@ -1120,17 +1120,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.4945</t>
+          <t>1.3333</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.193</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.670</t>
+          <t>1.490</t>
         </is>
       </c>
     </row>
@@ -1143,17 +1143,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.6977</t>
+          <t>1.7816</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.412</t>
+          <t>1.481</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.042</t>
+          <t>2.143</t>
         </is>
       </c>
     </row>
@@ -1166,17 +1166,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8615</t>
+          <t>1.0074</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.838</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.211</t>
         </is>
       </c>
     </row>
@@ -1189,17 +1189,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.6615</t>
+          <t>1.7876</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.255</t>
+          <t>2.427</t>
         </is>
       </c>
     </row>
@@ -1212,17 +1212,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9527</t>
+          <t>0.8739</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.692</t>
+          <t>0.634</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.204</t>
         </is>
       </c>
     </row>
@@ -1235,17 +1235,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8508</t>
+          <t>1.1669</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.504</t>
+          <t>0.691</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.436</t>
+          <t>1.971</t>
         </is>
       </c>
     </row>
@@ -1258,17 +1258,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3.4836</t>
+          <t>1.9053</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.800</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>6.743</t>
+          <t>3.689</t>
         </is>
       </c>
     </row>
@@ -1281,17 +1281,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0.4243</t>
+          <t>0.7450</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.220</t>
+          <t>0.386</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.819</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -1304,17 +1304,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.4599</t>
+          <t>0.5804</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.233</t>
+          <t>0.294</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>1.146</t>
         </is>
       </c>
     </row>
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2216</t>
+          <t>1.2350</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.200</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.407</t>
+          <t>1.271</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1368,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.9655</t>
+          <t>0.8814</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.681</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.0071</t>
+          <t>1.1142</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>1.245</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1414,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.1680</t>
+          <t>1.1501</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.242</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1437,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1414</t>
+          <t>1.1714</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>1.265</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2330</t>
+          <t>1.2482</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.165</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.337</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.3030</t>
+          <t>1.3300</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.245</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.392</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.4202</t>
+          <t>1.3904</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.282</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.540</t>
+          <t>1.508</t>
         </is>
       </c>
     </row>
@@ -1529,17 +1529,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.2449</t>
+          <t>1.2998</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.169</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.384</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -1552,17 +1552,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.2448</t>
+          <t>1.1456</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.317</t>
         </is>
       </c>
     </row>
@@ -1575,17 +1575,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.9481</t>
+          <t>1.9141</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.585</t>
+          <t>1.557</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.394</t>
+          <t>2.353</t>
         </is>
       </c>
     </row>
@@ -1598,17 +1598,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.6972</t>
+          <t>0.8489</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.561</t>
+          <t>0.683</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>0.867</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -1621,17 +1621,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.3293</t>
+          <t>1.5134</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.948</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.864</t>
+          <t>2.123</t>
         </is>
       </c>
     </row>
@@ -1644,17 +1644,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.4535</t>
+          <t>1.2904</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.888</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2.112</t>
+          <t>1.876</t>
         </is>
       </c>
     </row>
@@ -1667,17 +1667,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8024</t>
+          <t>0.8411</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.394</t>
+          <t>0.413</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.633</t>
+          <t>1.712</t>
         </is>
       </c>
     </row>
@@ -1690,17 +1690,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.0742</t>
+          <t>0.7365</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.366</t>
+          <t>0.251</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3.156</t>
+          <t>2.165</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.5562</t>
+          <t>2.6726</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>25.562</t>
+          <t>26.726</t>
         </is>
       </c>
     </row>
@@ -1736,17 +1736,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>4.0048</t>
+          <t>2.8191</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.811</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>8.855</t>
+          <t>6.245</t>
         </is>
       </c>
     </row>
@@ -1823,17 +1823,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0712</t>
+          <t>1.0374</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.992</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -1846,17 +1846,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.5148</t>
+          <t>0.6639</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.356</t>
+          <t>0.457</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.745</t>
+          <t>0.964</t>
         </is>
       </c>
     </row>
@@ -1869,17 +1869,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.5158</t>
+          <t>1.3529</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.887</t>
+          <t>1.686</t>
         </is>
       </c>
     </row>
@@ -1892,17 +1892,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0495</t>
+          <t>1.0821</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>0.962</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -1915,17 +1915,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.3043</t>
+          <t>1.2875</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.144</t>
+          <t>1.129</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.487</t>
+          <t>1.468</t>
         </is>
       </c>
     </row>
@@ -1938,17 +1938,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.7888</t>
+          <t>0.8473</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>0.936</t>
         </is>
       </c>
     </row>
@@ -1961,17 +1961,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9066</t>
+          <t>0.9453</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.010</t>
+          <t>1.054</t>
         </is>
       </c>
     </row>
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2288</t>
+          <t>1.2491</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.096</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.400</t>
+          <t>1.424</t>
         </is>
       </c>
     </row>
@@ -2007,17 +2007,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9963</t>
+          <t>0.9681</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.868</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.112</t>
         </is>
       </c>
     </row>
@@ -2030,17 +2030,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1929</t>
+          <t>1.0766</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>0.899</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.427</t>
+          <t>1.289</t>
         </is>
       </c>
     </row>
@@ -2053,17 +2053,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.2211</t>
+          <t>0.8938</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>0.737</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.478</t>
+          <t>1.083</t>
         </is>
       </c>
     </row>
@@ -2076,17 +2076,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.6250</t>
+          <t>0.8520</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.493</t>
+          <t>0.671</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.792</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -2099,17 +2099,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.8821</t>
+          <t>0.8624</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.670</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.133</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -2122,17 +2122,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0620</t>
+          <t>1.0274</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.741</t>
+          <t>0.715</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.523</t>
+          <t>1.476</t>
         </is>
       </c>
     </row>
@@ -2145,17 +2145,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.6612</t>
+          <t>0.9029</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.414</t>
+          <t>0.564</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.446</t>
         </is>
       </c>
     </row>
@@ -2168,17 +2168,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>3.1001</t>
+          <t>2.3662</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.612</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5.963</t>
+          <t>4.560</t>
         </is>
       </c>
     </row>
@@ -2191,17 +2191,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.6026</t>
+          <t>0.6787</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.296</t>
+          <t>0.332</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.388</t>
         </is>
       </c>
     </row>
@@ -2214,17 +2214,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2.3779</t>
+          <t>1.7949</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>0.708</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>6.013</t>
+          <t>4.552</t>
         </is>
       </c>
     </row>
@@ -2255,17 +2255,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2476</t>
+          <t>1.0366</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.168</t>
+          <t>1.013</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>
@@ -2278,17 +2278,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.7420</t>
+          <t>0.7552</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.620</t>
+          <t>0.630</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.905</t>
         </is>
       </c>
     </row>
@@ -2301,17 +2301,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0909</t>
+          <t>0.9374</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.020</t>
         </is>
       </c>
     </row>
@@ -2324,17 +2324,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.1227</t>
+          <t>1.0844</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.151</t>
         </is>
       </c>
     </row>
@@ -2347,17 +2347,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.9911</t>
+          <t>1.0100</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.952</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -2370,17 +2370,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9945</t>
+          <t>0.9759</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>0.923</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.032</t>
         </is>
       </c>
     </row>
@@ -2393,17 +2393,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0404</t>
+          <t>0.9979</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.943</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>1.055</t>
         </is>
       </c>
     </row>
@@ -2416,17 +2416,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4872</t>
+          <t>1.3080</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.391</t>
+          <t>1.223</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.590</t>
+          <t>1.399</t>
         </is>
       </c>
     </row>
@@ -2439,17 +2439,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0326</t>
+          <t>1.0008</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.923</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.085</t>
         </is>
       </c>
     </row>
@@ -2462,17 +2462,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0073</t>
+          <t>1.0181</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.917</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.118</t>
+          <t>1.131</t>
         </is>
       </c>
     </row>
@@ -2485,17 +2485,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9644</t>
+          <t>0.9680</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.856</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.7775</t>
+          <t>0.8644</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.679</t>
+          <t>0.754</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -2531,17 +2531,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2.0621</t>
+          <t>1.8328</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.684</t>
+          <t>1.495</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.525</t>
+          <t>2.246</t>
         </is>
       </c>
     </row>
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.1418</t>
+          <t>1.0605</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>0.835</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.348</t>
         </is>
       </c>
     </row>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8731</t>
+          <t>1.0561</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.631</t>
+          <t>0.763</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.207</t>
+          <t>1.463</t>
         </is>
       </c>
     </row>
@@ -2600,17 +2600,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2.1000</t>
+          <t>1.5748</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.088</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3.036</t>
+          <t>2.280</t>
         </is>
       </c>
     </row>
@@ -2623,17 +2623,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.2194</t>
+          <t>1.0330</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.735</t>
+          <t>0.622</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.022</t>
+          <t>1.716</t>
         </is>
       </c>
     </row>
@@ -2646,17 +2646,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>4.1069</t>
+          <t>2.6985</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.285</t>
+          <t>1.499</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>7.381</t>
+          <t>4.857</t>
         </is>
       </c>
     </row>
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.1647</t>
+          <t>0.9993</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.300</t>
+          <t>1.045</t>
         </is>
       </c>
     </row>
@@ -2710,17 +2710,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.4414</t>
+          <t>1.1375</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.981</t>
+          <t>0.771</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2.118</t>
+          <t>1.677</t>
         </is>
       </c>
     </row>
@@ -2733,17 +2733,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.7197</t>
+          <t>0.6929</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.576</t>
+          <t>0.554</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.899</t>
+          <t>0.866</t>
         </is>
       </c>
     </row>
@@ -2756,17 +2756,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0697</t>
+          <t>1.0021</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.889</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -2779,17 +2779,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.7599</t>
+          <t>0.7844</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.666</t>
+          <t>0.687</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.866</t>
+          <t>0.895</t>
         </is>
       </c>
     </row>
@@ -2802,17 +2802,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2609</t>
+          <t>1.1517</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.391</t>
+          <t>1.271</t>
         </is>
       </c>
     </row>
@@ -2825,17 +2825,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.1476</t>
+          <t>1.0556</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -2848,17 +2848,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.2103</t>
+          <t>1.0471</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>0.916</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.197</t>
         </is>
       </c>
     </row>
@@ -2871,17 +2871,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.0364</t>
+          <t>1.0338</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.898</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.190</t>
         </is>
       </c>
     </row>
@@ -2894,17 +2894,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.8444</t>
+          <t>0.9456</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.702</t>
+          <t>0.785</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -2917,17 +2917,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.7898</t>
+          <t>1.0830</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.649</t>
+          <t>0.889</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>1.319</t>
         </is>
       </c>
     </row>
@@ -2940,17 +2940,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.2440</t>
+          <t>1.0146</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.798</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.291</t>
         </is>
       </c>
     </row>
@@ -2963,17 +2963,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2.3377</t>
+          <t>2.1253</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.758</t>
+          <t>1.596</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3.108</t>
+          <t>2.830</t>
         </is>
       </c>
     </row>
@@ -2986,17 +2986,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0751</t>
+          <t>1.0322</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.733</t>
+          <t>0.703</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.516</t>
         </is>
       </c>
     </row>
@@ -3009,17 +3009,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3204</t>
+          <t>1.1697</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.787</t>
+          <t>0.696</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2.214</t>
+          <t>1.966</t>
         </is>
       </c>
     </row>
@@ -3032,17 +3032,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.6774</t>
+          <t>0.6656</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.337</t>
+          <t>0.331</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.361</t>
+          <t>1.340</t>
         </is>
       </c>
     </row>
@@ -3055,17 +3055,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.0237</t>
+          <t>1.5221</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.992</t>
+          <t>0.743</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>4.128</t>
+          <t>3.117</t>
         </is>
       </c>
     </row>
@@ -3078,17 +3078,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.7271</t>
+          <t>1.5034</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>0.542</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4.774</t>
+          <t>4.166</t>
         </is>
       </c>
     </row>
@@ -3119,17 +3119,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.6866</t>
+          <t>1.5481</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.566</t>
+          <t>1.518</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.816</t>
+          <t>1.579</t>
         </is>
       </c>
     </row>
@@ -3142,17 +3142,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.4643</t>
+          <t>1.1995</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.274</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.683</t>
+          <t>1.380</t>
         </is>
       </c>
     </row>
@@ -3165,17 +3165,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.5004</t>
+          <t>1.3211</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.401</t>
+          <t>1.233</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.607</t>
+          <t>1.416</t>
         </is>
       </c>
     </row>
@@ -3188,17 +3188,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.6313</t>
+          <t>1.5049</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.553</t>
+          <t>1.433</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.713</t>
+          <t>1.581</t>
         </is>
       </c>
     </row>
@@ -3211,17 +3211,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.5421</t>
+          <t>1.4957</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.467</t>
+          <t>1.423</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.621</t>
+          <t>1.572</t>
         </is>
       </c>
     </row>
@@ -3234,17 +3234,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.6823</t>
+          <t>1.6091</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.532</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.767</t>
+          <t>1.691</t>
         </is>
       </c>
     </row>
@@ -3257,17 +3257,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.8626</t>
+          <t>1.6700</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.772</t>
+          <t>1.588</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.958</t>
+          <t>1.756</t>
         </is>
       </c>
     </row>
@@ -3280,17 +3280,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2.0618</t>
+          <t>1.7767</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.945</t>
+          <t>1.675</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>2.186</t>
+          <t>1.884</t>
         </is>
       </c>
     </row>
@@ -3303,17 +3303,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.6106</t>
+          <t>1.4631</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1.495</t>
+          <t>1.357</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.735</t>
+          <t>1.577</t>
         </is>
       </c>
     </row>
@@ -3326,17 +3326,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.4006</t>
+          <t>1.3359</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.209</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.476</t>
         </is>
       </c>
     </row>
@@ -3349,17 +3349,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.1474</t>
+          <t>1.1756</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.038</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.331</t>
         </is>
       </c>
     </row>
@@ -3372,17 +3372,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.3524</t>
+          <t>1.3730</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.160</t>
+          <t>1.177</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.602</t>
         </is>
       </c>
     </row>
@@ -3395,17 +3395,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2.0824</t>
+          <t>1.9356</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.680</t>
+          <t>1.560</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2.582</t>
+          <t>2.401</t>
         </is>
       </c>
     </row>
@@ -3418,17 +3418,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.2798</t>
+          <t>1.1657</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.653</t>
+          <t>1.507</t>
         </is>
       </c>
     </row>
@@ -3441,17 +3441,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0.8286</t>
+          <t>0.9280</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.592</t>
+          <t>0.661</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.302</t>
         </is>
       </c>
     </row>
@@ -3464,17 +3464,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2.5956</t>
+          <t>2.3353</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.510</t>
+          <t>1.356</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4.463</t>
+          <t>4.022</t>
         </is>
       </c>
     </row>
@@ -3487,17 +3487,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>3.0357</t>
+          <t>1.1689</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.714</t>
+          <t>0.659</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>5.376</t>
+          <t>2.075</t>
         </is>
       </c>
     </row>
@@ -3510,17 +3510,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2.8743</t>
+          <t>1.3889</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>0.769</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>5.176</t>
+          <t>2.507</t>
         </is>
       </c>
     </row>
@@ -3551,17 +3551,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.3519</t>
+          <t>1.4934</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.463</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.469</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -3574,17 +3574,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1.9734</t>
+          <t>1.5883</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1.658</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2.349</t>
+          <t>1.893</t>
         </is>
       </c>
     </row>
@@ -3597,17 +3597,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.3754</t>
+          <t>1.4092</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.304</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1.486</t>
+          <t>1.523</t>
         </is>
       </c>
     </row>
@@ -3620,17 +3620,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1.4530</t>
+          <t>1.3878</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1.532</t>
+          <t>1.464</t>
         </is>
       </c>
     </row>
@@ -3643,17 +3643,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1.5559</t>
+          <t>1.4810</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1.479</t>
+          <t>1.407</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1.637</t>
+          <t>1.559</t>
         </is>
       </c>
     </row>
@@ -3666,17 +3666,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.6915</t>
+          <t>1.6489</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.611</t>
+          <t>1.570</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.776</t>
+          <t>1.731</t>
         </is>
       </c>
     </row>
@@ -3689,17 +3689,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1.7903</t>
+          <t>1.6735</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1.704</t>
+          <t>1.592</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.881</t>
+          <t>1.759</t>
         </is>
       </c>
     </row>
@@ -3712,17 +3712,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1.3863</t>
+          <t>1.3583</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.301</t>
+          <t>1.274</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1.478</t>
+          <t>1.448</t>
         </is>
       </c>
     </row>
@@ -3735,17 +3735,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.5598</t>
+          <t>1.4619</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.350</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.688</t>
+          <t>1.583</t>
         </is>
       </c>
     </row>
@@ -3758,17 +3758,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>1.3905</t>
+          <t>1.3122</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.176</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1.550</t>
+          <t>1.464</t>
         </is>
       </c>
     </row>
@@ -3781,17 +3781,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1.1898</t>
+          <t>1.2145</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1.356</t>
+          <t>1.385</t>
         </is>
       </c>
     </row>
@@ -3804,17 +3804,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>1.7395</t>
+          <t>1.5885</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1.488</t>
+          <t>1.358</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>2.034</t>
+          <t>1.859</t>
         </is>
       </c>
     </row>
@@ -3827,17 +3827,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>1.0099</t>
+          <t>1.0561</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.783</t>
+          <t>0.819</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1.302</t>
+          <t>1.363</t>
         </is>
       </c>
     </row>
@@ -3850,17 +3850,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1.1209</t>
+          <t>1.0992</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1.492</t>
+          <t>1.465</t>
         </is>
       </c>
     </row>
@@ -3873,17 +3873,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0.9491</t>
+          <t>0.8787</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>0.635</t>
+          <t>0.587</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1.418</t>
+          <t>1.315</t>
         </is>
       </c>
     </row>
@@ -3896,17 +3896,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1.2360</t>
+          <t>1.4829</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.683</t>
+          <t>0.818</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2.238</t>
+          <t>2.690</t>
         </is>
       </c>
     </row>
@@ -3919,17 +3919,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2.4895</t>
+          <t>1.1316</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>1.404</t>
+          <t>0.637</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>4.414</t>
+          <t>2.011</t>
         </is>
       </c>
     </row>
@@ -3942,17 +3942,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0.6999</t>
+          <t>0.5147</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.341</t>
+          <t>0.250</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
KCOR dual output to console and file
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -7,8 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,17 +482,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.9919</t>
+          <t>1.4384</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>1.399</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.479</t>
         </is>
       </c>
     </row>
@@ -504,17 +505,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9509</t>
+          <t>1.0954</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.732</t>
+          <t>0.876</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -527,17 +528,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7677</t>
+          <t>1.0430</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>1.138</t>
         </is>
       </c>
     </row>
@@ -550,17 +551,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8327</t>
+          <t>1.0372</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.768</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>1.101</t>
         </is>
       </c>
     </row>
@@ -573,17 +574,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0673</t>
+          <t>1.2582</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>1.192</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.328</t>
         </is>
       </c>
     </row>
@@ -596,17 +597,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0057</t>
+          <t>1.6523</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>1.574</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.735</t>
         </is>
       </c>
     </row>
@@ -619,17 +620,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0036</t>
+          <t>1.7959</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>1.702</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.895</t>
         </is>
       </c>
     </row>
@@ -642,17 +643,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1486</t>
+          <t>1.7322</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>1.571</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.909</t>
         </is>
       </c>
     </row>
@@ -665,17 +666,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1557</t>
+          <t>1.6728</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.451</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.264</t>
+          <t>1.929</t>
         </is>
       </c>
     </row>
@@ -688,17 +689,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1638</t>
+          <t>1.8539</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.473</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.304</t>
+          <t>2.333</t>
         </is>
       </c>
     </row>
@@ -711,17 +712,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.9308</t>
+          <t>1.6915</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>1.276</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.064</t>
+          <t>2.242</t>
         </is>
       </c>
     </row>
@@ -734,17 +735,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.1867</t>
+          <t>1.9128</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.330</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.389</t>
+          <t>2.750</t>
         </is>
       </c>
     </row>
@@ -757,17 +758,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.1811</t>
+          <t>1.4165</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.855</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.436</t>
+          <t>2.347</t>
         </is>
       </c>
     </row>
@@ -780,17 +781,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.6772</t>
+          <t>2.2191</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.518</t>
+          <t>0.920</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.885</t>
+          <t>5.354</t>
         </is>
       </c>
     </row>
@@ -803,17 +804,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3873</t>
+          <t>0.5014</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.822</t>
+          <t>0.209</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2.341</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -826,17 +827,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.5871</t>
+          <t>1.2788</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>6.370</t>
+          <t>12.788</t>
         </is>
       </c>
     </row>
@@ -849,7 +850,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.4564</t>
+          <t>2.7232</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -859,7 +860,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4.564</t>
+          <t>27.232</t>
         </is>
       </c>
     </row>
@@ -872,17 +873,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.2059</t>
+          <t>5.1710</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.117</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.364</t>
+          <t>51.710</t>
         </is>
       </c>
     </row>
@@ -913,17 +914,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2238</t>
+          <t>1.7619</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.198</t>
+          <t>1.708</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.818</t>
         </is>
       </c>
     </row>
@@ -936,17 +937,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8381</t>
+          <t>0.9372</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.736</t>
+          <t>0.816</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>1.077</t>
         </is>
       </c>
     </row>
@@ -959,17 +960,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.8553</t>
+          <t>1.3136</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>1.226</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.916</t>
+          <t>1.408</t>
         </is>
       </c>
     </row>
@@ -982,17 +983,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9577</t>
+          <t>1.6230</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.910</t>
+          <t>1.544</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.706</t>
         </is>
       </c>
     </row>
@@ -1005,17 +1006,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.2503</t>
+          <t>2.0454</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.944</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>2.152</t>
         </is>
       </c>
     </row>
@@ -1028,17 +1029,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2554</t>
+          <t>1.9872</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.868</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>2.114</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1052,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3348</t>
+          <t>1.8347</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.266</t>
+          <t>1.682</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>2.001</t>
         </is>
       </c>
     </row>
@@ -1074,17 +1075,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5970</t>
+          <t>1.8089</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.496</t>
+          <t>1.599</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.705</t>
+          <t>2.046</t>
         </is>
       </c>
     </row>
@@ -1097,17 +1098,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.5021</t>
+          <t>1.6578</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>1.378</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.640</t>
+          <t>1.995</t>
         </is>
       </c>
     </row>
@@ -1120,17 +1121,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3333</t>
+          <t>1.8451</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.454</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>2.341</t>
         </is>
       </c>
     </row>
@@ -1143,17 +1144,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.7816</t>
+          <t>1.7436</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.143</t>
+          <t>2.387</t>
         </is>
       </c>
     </row>
@@ -1166,17 +1167,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0074</t>
+          <t>2.2821</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.838</t>
+          <t>1.530</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.211</t>
+          <t>3.405</t>
         </is>
       </c>
     </row>
@@ -1189,17 +1190,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.7876</t>
+          <t>1.1980</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>0.643</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.427</t>
+          <t>2.233</t>
         </is>
       </c>
     </row>
@@ -1212,17 +1213,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.8739</t>
+          <t>0.6066</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.634</t>
+          <t>0.404</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.204</t>
+          <t>0.910</t>
         </is>
       </c>
     </row>
@@ -1235,17 +1236,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.1669</t>
+          <t>0.7044</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.691</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.971</t>
+          <t>7.044</t>
         </is>
       </c>
     </row>
@@ -1258,17 +1259,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.9053</t>
+          <t>1.5904</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.652</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3.689</t>
+          <t>3.882</t>
         </is>
       </c>
     </row>
@@ -1281,17 +1282,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>0.7450</t>
+          <t>3.0805</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.386</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>30.805</t>
         </is>
       </c>
     </row>
@@ -1304,17 +1305,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.5804</t>
+          <t>3.3321</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.294</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>33.321</t>
         </is>
       </c>
     </row>
@@ -1345,17 +1346,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2350</t>
+          <t>1.2193</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.172</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.271</t>
+          <t>1.268</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1369,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.8814</t>
+          <t>0.8556</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.681</t>
+          <t>0.678</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1392,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.1142</t>
+          <t>1.2594</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>1.144</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.386</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1415,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.1501</t>
+          <t>1.5648</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.464</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.672</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1438,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1714</t>
+          <t>1.6257</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.525</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.733</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1461,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2482</t>
+          <t>1.2027</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.119</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.293</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1484,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.3300</t>
+          <t>1.0216</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.127</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1507,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.3904</t>
+          <t>1.0443</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.282</t>
+          <t>0.896</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.508</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -1529,17 +1530,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.2998</t>
+          <t>0.9910</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>0.788</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.247</t>
         </is>
       </c>
     </row>
@@ -1552,17 +1553,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1456</t>
+          <t>0.9953</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.380</t>
         </is>
       </c>
     </row>
@@ -1575,17 +1576,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.9141</t>
+          <t>1.0308</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.557</t>
+          <t>0.680</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.353</t>
+          <t>1.564</t>
         </is>
       </c>
     </row>
@@ -1598,17 +1599,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.8489</t>
+          <t>1.1931</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.683</t>
+          <t>0.699</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>2.035</t>
         </is>
       </c>
     </row>
@@ -1621,17 +1622,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.5134</t>
+          <t>0.8458</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>0.382</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2.123</t>
+          <t>1.874</t>
         </is>
       </c>
     </row>
@@ -1644,17 +1645,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.2904</t>
+          <t>0.2734</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.105</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.876</t>
+          <t>0.713</t>
         </is>
       </c>
     </row>
@@ -1667,17 +1668,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8411</t>
+          <t>0.9429</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.413</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.712</t>
+          <t>9.429</t>
         </is>
       </c>
     </row>
@@ -1690,17 +1691,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.7365</t>
+          <t>1.3978</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.251</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2.165</t>
+          <t>13.978</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1714,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.6726</t>
+          <t>1.1312</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1723,7 +1724,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>26.726</t>
+          <t>11.312</t>
         </is>
       </c>
     </row>
@@ -1736,17 +1737,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2.8191</t>
+          <t>0.6444</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>6.245</t>
+          <t>6.444</t>
         </is>
       </c>
     </row>
@@ -1763,6 +1764,1348 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dose_Combination</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>YearOfBirth</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>KCOR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CI_Lower</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CI_Upper</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1 vs 0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.9919</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1.020</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.9509</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.732</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.236</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1925</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.7677</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.684</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.862</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.8327</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.768</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.903</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1935</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.0673</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.985</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1.157</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.0057</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.938</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.079</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1945</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1.0036</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.940</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1.071</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.1486</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1.067</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1.236</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1955</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.1557</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1.056</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1.264</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1.1638</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1.039</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1.304</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1965</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.9308</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.815</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1.064</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1.1867</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1.014</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1.389</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1975</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1.1811</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.972</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1.436</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0.6772</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.518</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0.885</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1985</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1.3873</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.822</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2.341</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2.5871</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>1.051</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>6.370</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.4564</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>4.564</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.2059</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.117</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.364</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1.2238</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1.198</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0.8381</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.736</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0.954</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1925</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0.8553</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.798</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.916</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.9577</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.910</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1.008</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>1935</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1.2503</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>1.188</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1.316</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1.2554</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>1.194</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1.320</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>1945</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1.3348</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1.266</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>1.408</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1.5970</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>1.496</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1.705</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1955</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1.5021</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1.375</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1.640</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>1.3333</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1.193</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>1.490</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1965</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1.7816</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>1.481</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2.143</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>1.0074</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.838</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1.211</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1975</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1.7876</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>1.316</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2.427</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.8739</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.634</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>1.204</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1985</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1.1669</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.691</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>1.971</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>1.9053</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.984</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>3.689</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0.7450</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0.386</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>1.439</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.5804</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.294</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>1.146</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1.2350</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>1.200</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>1.271</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.8814</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0.681</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>1.141</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1925</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>1.1142</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.997</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>1.245</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>1.1501</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>1.065</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>1.242</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1935</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1.1714</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>1.085</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>1.265</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>1.2482</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>1.165</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>1.337</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1945</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>1.3300</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>1.245</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>1.421</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1.3904</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>1.282</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>1.508</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1955</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1.2998</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>1.169</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1.445</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1.1456</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.997</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>1.317</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1965</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1.9141</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1.557</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2.353</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>0.8489</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>0.683</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1.056</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1975</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1.5134</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1.079</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2.123</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1.2904</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.888</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1.876</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1985</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.8411</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0.413</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1.712</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>0.7365</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>0.251</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2.165</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2.6726</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>26.726</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2.8191</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>1.273</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>6.245</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
updated with new baseline sanity check
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -7,9 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_13" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -482,17 +481,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.4384</t>
+          <t>1.0516</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.479</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -505,17 +504,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0954</t>
+          <t>1.0592</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.370</t>
+          <t>1.376</t>
         </is>
       </c>
     </row>
@@ -528,17 +527,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0430</t>
+          <t>0.9682</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.863</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.087</t>
         </is>
       </c>
     </row>
@@ -551,17 +550,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0372</t>
+          <t>1.0076</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.092</t>
         </is>
       </c>
     </row>
@@ -574,17 +573,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2582</t>
+          <t>1.0673</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.328</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>
@@ -597,17 +596,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6523</t>
+          <t>1.0057</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.574</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.735</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
@@ -620,17 +619,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.7959</t>
+          <t>1.0036</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.702</t>
+          <t>0.940</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.895</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -643,17 +642,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.7322</t>
+          <t>1.1486</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.571</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.909</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -666,17 +665,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6728</t>
+          <t>1.1557</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.451</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.929</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -689,17 +688,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.8539</t>
+          <t>1.1638</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2.333</t>
+          <t>1.304</t>
         </is>
       </c>
     </row>
@@ -712,17 +711,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.6915</t>
+          <t>1.0280</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.276</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.242</t>
+          <t>1.175</t>
         </is>
       </c>
     </row>
@@ -735,17 +734,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.9128</t>
+          <t>1.1867</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.014</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.750</t>
+          <t>1.389</t>
         </is>
       </c>
     </row>
@@ -758,17 +757,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.4165</t>
+          <t>1.1811</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2.347</t>
+          <t>1.436</t>
         </is>
       </c>
     </row>
@@ -781,17 +780,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2.2191</t>
+          <t>1.0137</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.920</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5.354</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -804,17 +803,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.5014</t>
+          <t>1.3873</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.209</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>2.341</t>
         </is>
       </c>
     </row>
@@ -827,17 +826,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2788</t>
+          <t>2.5871</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12.788</t>
+          <t>6.370</t>
         </is>
       </c>
     </row>
@@ -850,7 +849,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2.7232</t>
+          <t>1.4870</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -860,7 +859,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>27.232</t>
+          <t>14.870</t>
         </is>
       </c>
     </row>
@@ -873,17 +872,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5.1710</t>
+          <t>1.5327</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.868</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>51.710</t>
+          <t>2.708</t>
         </is>
       </c>
     </row>
@@ -914,17 +913,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.7619</t>
+          <t>1.2579</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.708</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.818</t>
+          <t>1.285</t>
         </is>
       </c>
     </row>
@@ -937,17 +936,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9372</t>
+          <t>0.9691</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.104</t>
         </is>
       </c>
     </row>
@@ -960,17 +959,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.3136</t>
+          <t>1.0397</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>0.970</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -983,17 +982,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.6230</t>
+          <t>0.9884</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.544</t>
+          <t>0.939</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.706</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
@@ -1006,17 +1005,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2.0454</t>
+          <t>1.2503</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.944</t>
+          <t>1.188</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2.152</t>
+          <t>1.316</t>
         </is>
       </c>
     </row>
@@ -1029,17 +1028,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.9872</t>
+          <t>1.2554</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>1.194</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2.114</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -1052,17 +1051,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.8347</t>
+          <t>1.3348</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.682</t>
+          <t>1.266</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2.001</t>
+          <t>1.408</t>
         </is>
       </c>
     </row>
@@ -1075,17 +1074,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.8089</t>
+          <t>1.5970</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.599</t>
+          <t>1.496</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2.046</t>
+          <t>1.705</t>
         </is>
       </c>
     </row>
@@ -1098,17 +1097,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.6578</t>
+          <t>1.5021</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.995</t>
+          <t>1.640</t>
         </is>
       </c>
     </row>
@@ -1121,17 +1120,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.8451</t>
+          <t>1.3333</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.454</t>
+          <t>1.193</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2.341</t>
+          <t>1.490</t>
         </is>
       </c>
     </row>
@@ -1144,17 +1143,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.7436</t>
+          <t>1.7816</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.481</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.387</t>
+          <t>2.143</t>
         </is>
       </c>
     </row>
@@ -1167,17 +1166,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.2821</t>
+          <t>1.1135</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.530</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3.405</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -1190,17 +1189,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.1980</t>
+          <t>1.7876</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.233</t>
+          <t>2.427</t>
         </is>
       </c>
     </row>
@@ -1213,17 +1212,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.6066</t>
+          <t>0.9114</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.404</t>
+          <t>0.661</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.910</t>
+          <t>1.256</t>
         </is>
       </c>
     </row>
@@ -1236,17 +1235,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.7044</t>
+          <t>1.2977</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.768</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7.044</t>
+          <t>2.191</t>
         </is>
       </c>
     </row>
@@ -1259,17 +1258,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.5904</t>
+          <t>1.9053</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.652</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3.882</t>
+          <t>3.689</t>
         </is>
       </c>
     </row>
@@ -1282,17 +1281,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>3.0805</t>
+          <t>1.5577</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>30.805</t>
+          <t>3.009</t>
         </is>
       </c>
     </row>
@@ -1305,17 +1304,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3.3321</t>
+          <t>1.1682</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.592</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>33.321</t>
+          <t>2.307</t>
         </is>
       </c>
     </row>
@@ -1346,17 +1345,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2193</t>
+          <t>1.2435</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.172</t>
+          <t>1.208</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.268</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -1369,17 +1368,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.8556</t>
+          <t>0.9149</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.706</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.185</t>
         </is>
       </c>
     </row>
@@ -1392,17 +1391,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.2594</t>
+          <t>1.1142</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.144</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.386</t>
+          <t>1.245</t>
         </is>
       </c>
     </row>
@@ -1415,17 +1414,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.5648</t>
+          <t>1.1501</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.672</t>
+          <t>1.242</t>
         </is>
       </c>
     </row>
@@ -1438,17 +1437,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.6257</t>
+          <t>1.1714</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.733</t>
+          <t>1.265</t>
         </is>
       </c>
     </row>
@@ -1461,17 +1460,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2027</t>
+          <t>1.2482</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.165</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>1.337</t>
         </is>
       </c>
     </row>
@@ -1484,17 +1483,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0216</t>
+          <t>1.3300</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>1.245</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.127</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -1507,17 +1506,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.0443</t>
+          <t>1.3904</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.896</t>
+          <t>1.282</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.218</t>
+          <t>1.508</t>
         </is>
       </c>
     </row>
@@ -1530,17 +1529,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0.9910</t>
+          <t>1.2998</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>1.169</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -1553,17 +1552,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.9953</t>
+          <t>1.1456</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.718</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.380</t>
+          <t>1.317</t>
         </is>
       </c>
     </row>
@@ -1576,17 +1575,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0308</t>
+          <t>1.9141</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.680</t>
+          <t>1.557</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.564</t>
+          <t>2.353</t>
         </is>
       </c>
     </row>
@@ -1599,17 +1598,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.1931</t>
+          <t>1.1750</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.699</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2.035</t>
+          <t>1.461</t>
         </is>
       </c>
     </row>
@@ -1622,17 +1621,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>0.8458</t>
+          <t>1.5134</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.382</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.874</t>
+          <t>2.123</t>
         </is>
       </c>
     </row>
@@ -1645,17 +1644,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.2734</t>
+          <t>1.2904</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.105</t>
+          <t>0.888</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>1.876</t>
         </is>
       </c>
     </row>
@@ -1668,17 +1667,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.9429</t>
+          <t>1.0548</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.518</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>9.429</t>
+          <t>2.147</t>
         </is>
       </c>
     </row>
@@ -1691,17 +1690,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.3978</t>
+          <t>0.8226</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.280</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>13.978</t>
+          <t>2.418</t>
         </is>
       </c>
     </row>
@@ -1714,7 +1713,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.1312</t>
+          <t>2.6726</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1724,7 +1723,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>11.312</t>
+          <t>26.726</t>
         </is>
       </c>
     </row>
@@ -1737,17 +1736,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.6444</t>
+          <t>2.8191</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>6.444</t>
+          <t>6.245</t>
         </is>
       </c>
     </row>
@@ -1764,1348 +1763,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E61"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Dose_Combination</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>YearOfBirth</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>KCOR</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>CI_Lower</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CI_Upper</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1 vs 0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.9919</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0.964</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1.020</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1920</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.9509</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.732</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1.236</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1925</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.7677</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.684</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0.862</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1930</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.8327</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.768</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0.903</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1935</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.0673</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.985</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1.157</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.0057</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>0.938</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1.079</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1945</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1.0036</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>0.940</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.071</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1.1486</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.067</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1.236</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1955</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.1557</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1.056</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1.264</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1960</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1.1638</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1.039</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1.304</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1965</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0.9308</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.815</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1.064</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1970</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1.1867</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1.014</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1.389</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1975</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1.1811</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0.972</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>1.436</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1980</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0.6772</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0.518</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>0.885</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1985</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1.3873</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.822</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2.341</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2.5871</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1.051</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>6.370</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0.4564</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>4.564</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.2059</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.117</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0.364</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2 vs 0</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>1.2238</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>1.198</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>1.250</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>1920</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>0.8381</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0.736</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>0.954</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>1925</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0.8553</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0.798</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0.916</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>1930</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0.9577</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0.910</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1.008</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>1935</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>1.2503</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>1.188</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1.316</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>1.2554</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>1.194</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1.320</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>1945</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>1.3348</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>1.266</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>1.408</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>1.5970</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>1.496</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>1.705</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>1955</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>1.5021</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>1.375</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>1.640</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>1960</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>1.3333</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>1.193</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>1.490</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>1965</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>1.7816</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>1.481</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2.143</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>1970</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>1.0074</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>0.838</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>1.211</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>1975</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>1.7876</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>1.316</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>2.427</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>1980</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>0.8739</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>0.634</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>1.204</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>1985</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>1.1669</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>0.691</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>1.971</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1.9053</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>0.984</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>3.689</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr"/>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>0.7450</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>0.386</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>1.439</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr"/>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>0.5804</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>0.294</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>1.146</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr"/>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2 vs 1</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>ASMR (pooled)</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1.2350</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>1.200</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>1.271</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr"/>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>1920</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>0.8814</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>0.681</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>1.141</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>1925</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1.1142</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>0.997</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>1.245</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr"/>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>1930</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1.1501</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>1.065</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>1.242</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr"/>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>1935</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>1.1714</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>1.085</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>1.265</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr"/>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>1940</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>1.2482</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>1.165</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>1.337</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr"/>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>1945</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>1.3300</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>1.245</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>1.421</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr"/>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>1950</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>1.3904</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>1.282</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>1.508</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>1955</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>1.2998</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>1.169</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>1.445</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>1960</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>1.1456</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>0.997</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>1.317</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr"/>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>1965</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>1.9141</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>1.557</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>2.353</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr"/>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>1970</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>0.8489</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>0.683</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>1.056</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr"/>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>1975</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>1.5134</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>1.079</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2.123</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr"/>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>1980</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>1.2904</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>0.888</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>1.876</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr"/>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>1985</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>0.8411</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>0.413</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>1.712</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr"/>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>0.7365</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>0.251</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2.165</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr"/>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>1995</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>2.6726</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>0.000</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>26.726</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr"/>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>2.8191</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>1.273</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>6.245</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr"/>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3166,17 +1823,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0374</t>
+          <t>1.1194</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.992</t>
+          <t>1.071</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.170</t>
         </is>
       </c>
     </row>
@@ -3189,17 +1846,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6639</t>
+          <t>1.2078</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.457</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>1.755</t>
         </is>
       </c>
     </row>
@@ -3281,17 +1938,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8473</t>
+          <t>1.0636</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.767</t>
+          <t>0.963</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -3304,17 +1961,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9453</t>
+          <t>1.0217</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.916</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.054</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -3350,17 +2007,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9681</t>
+          <t>0.9831</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.856</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.129</t>
         </is>
       </c>
     </row>
@@ -3419,17 +2076,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.8520</t>
+          <t>1.2643</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.671</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.605</t>
         </is>
       </c>
     </row>
@@ -3442,17 +2099,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.8624</t>
+          <t>0.9690</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.670</t>
+          <t>0.753</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.247</t>
         </is>
       </c>
     </row>
@@ -3488,17 +2145,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9029</t>
+          <t>1.2508</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.564</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.446</t>
+          <t>2.003</t>
         </is>
       </c>
     </row>
@@ -3534,17 +2191,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.6787</t>
+          <t>1.2070</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.332</t>
+          <t>0.590</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.388</t>
+          <t>2.469</t>
         </is>
       </c>
     </row>
@@ -3598,17 +2255,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0366</t>
+          <t>1.0502</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.013</t>
+          <t>1.027</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -3621,17 +2278,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.7552</t>
+          <t>1.0324</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.630</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>1.237</t>
         </is>
       </c>
     </row>
@@ -3690,17 +2347,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.0100</t>
+          <t>1.0247</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.952</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.087</t>
         </is>
       </c>
     </row>
@@ -3713,17 +2370,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9759</t>
+          <t>0.9890</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>0.935</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.046</t>
         </is>
       </c>
     </row>
@@ -3828,17 +2485,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9680</t>
+          <t>1.0026</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.134</t>
         </is>
       </c>
     </row>
@@ -3851,17 +2508,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8644</t>
+          <t>1.0967</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.754</t>
+          <t>0.957</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>1.257</t>
         </is>
       </c>
     </row>
@@ -3920,17 +2577,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0561</t>
+          <t>1.1717</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.623</t>
         </is>
       </c>
     </row>
@@ -4030,17 +2687,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9993</t>
+          <t>1.0697</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>1.023</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>1.119</t>
         </is>
       </c>
     </row>
@@ -4076,17 +2733,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.6929</t>
+          <t>0.9878</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.554</t>
+          <t>0.790</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.866</t>
+          <t>1.235</t>
         </is>
       </c>
     </row>
@@ -4122,17 +2779,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.7844</t>
+          <t>1.0291</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>0.895</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -4237,17 +2894,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.9456</t>
+          <t>1.1008</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.785</t>
+          <t>0.914</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.325</t>
         </is>
       </c>
     </row>
@@ -4260,17 +2917,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0830</t>
+          <t>1.2781</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.319</t>
+          <t>1.556</t>
         </is>
       </c>
     </row>
@@ -4375,17 +3032,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.6656</t>
+          <t>0.8761</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.331</t>
+          <t>0.435</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.764</t>
         </is>
       </c>
     </row>
@@ -4462,7 +3119,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.5481</t>
+          <t>1.5487</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -4472,7 +3129,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.579</t>
+          <t>1.580</t>
         </is>
       </c>
     </row>
@@ -4784,17 +3441,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0.9280</t>
+          <t>1.0823</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.771</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.302</t>
+          <t>1.518</t>
         </is>
       </c>
     </row>
@@ -4894,12 +3551,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.4934</t>
+          <t>1.4941</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.464</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -5216,17 +3873,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0.8787</t>
+          <t>0.9237</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>0.587</t>
+          <t>0.617</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1.315</t>
+          <t>1.383</t>
         </is>
       </c>
     </row>
@@ -5285,17 +3942,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0.5147</t>
+          <t>0.7737</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.250</t>
+          <t>0.376</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.593</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
everything CMR should work i hope
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2021_24" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2022_06" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,17 +481,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.0516</t>
+          <t>0.6033</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>0.518</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>0.703</t>
         </is>
       </c>
     </row>
@@ -504,17 +504,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0592</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.376</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -527,17 +527,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9682</t>
+          <t>0.0361</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.863</t>
+          <t>0.032</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>0.041</t>
         </is>
       </c>
     </row>
@@ -550,17 +550,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0076</t>
+          <t>1.3283</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>1.226</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -573,17 +573,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0673</t>
+          <t>1.0358</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.122</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0057</t>
+          <t>1.0008</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -619,17 +619,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0036</t>
+          <t>1.0025</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>0.939</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.070</t>
         </is>
       </c>
     </row>
@@ -642,7 +642,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1486</t>
+          <t>1.1488</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -665,17 +665,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1557</t>
+          <t>1.1561</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.264</t>
+          <t>1.265</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1638</t>
+          <t>1.1642</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -698,7 +698,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.304</t>
+          <t>1.305</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.5871</t>
+          <t>2.5869</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -913,17 +913,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2579</t>
+          <t>0.7287</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>0.683</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.285</t>
+          <t>0.777</t>
         </is>
       </c>
     </row>
@@ -936,17 +936,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9691</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.851</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -959,17 +959,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0397</t>
+          <t>0.0402</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.038</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>0.043</t>
         </is>
       </c>
     </row>
@@ -982,17 +982,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9884</t>
+          <t>1.5212</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>1.447</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.040</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -1005,17 +1005,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.2503</t>
+          <t>1.2110</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.151</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.275</t>
         </is>
       </c>
     </row>
@@ -1028,17 +1028,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2554</t>
+          <t>1.2473</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.186</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.311</t>
         </is>
       </c>
     </row>
@@ -1051,17 +1051,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3348</t>
+          <t>1.3323</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.266</t>
+          <t>1.263</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>1.405</t>
         </is>
       </c>
     </row>
@@ -1074,17 +1074,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5970</t>
+          <t>1.5959</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.496</t>
+          <t>1.495</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.705</t>
+          <t>1.704</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.5021</t>
+          <t>1.5014</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1120,12 +1120,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3333</t>
+          <t>1.3326</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.192</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.7816</t>
+          <t>1.7815</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.7876</t>
+          <t>1.7875</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.9053</t>
+          <t>1.9052</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.1682</t>
+          <t>1.1681</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2435</t>
+          <t>1.0921</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1368,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.9149</t>
+          <t>0.9104</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>0.704</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.178</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.1142</t>
+          <t>1.1134</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.244</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1414,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.1501</t>
+          <t>1.1453</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.061</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1437,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1714</t>
+          <t>1.1692</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.083</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.262</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2482</t>
+          <t>1.2463</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.164</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.335</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.3300</t>
+          <t>1.3290</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.419</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.3904</t>
+          <t>1.3892</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.282</t>
+          <t>1.281</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.508</t>
+          <t>1.507</t>
         </is>
       </c>
     </row>
@@ -1529,17 +1529,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.2998</t>
+          <t>1.2987</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.168</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.444</t>
         </is>
       </c>
     </row>
@@ -1552,17 +1552,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1456</t>
+          <t>1.1447</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.315</t>
         </is>
       </c>
     </row>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.9141</t>
+          <t>1.9137</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.6726</t>
+          <t>1.7761</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>26.726</t>
+          <t>17.761</t>
         </is>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2.8191</t>
+          <t>2.8197</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>6.245</t>
+          <t>6.246</t>
         </is>
       </c>
     </row>
@@ -1823,17 +1823,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.1194</t>
+          <t>0.5400</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>0.492</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>0.592</t>
         </is>
       </c>
     </row>
@@ -1846,17 +1846,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2078</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.831</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.755</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1869,17 +1869,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.3529</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.686</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1892,17 +1892,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0821</t>
+          <t>0.4533</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.962</t>
+          <t>0.405</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.218</t>
+          <t>0.508</t>
         </is>
       </c>
     </row>
@@ -1915,17 +1915,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2875</t>
+          <t>1.3099</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.149</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.468</t>
+          <t>1.494</t>
         </is>
       </c>
     </row>
@@ -1938,17 +1938,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0636</t>
+          <t>1.0703</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.969</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.182</t>
         </is>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0217</t>
+          <t>1.0216</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2491</t>
+          <t>1.2475</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.424</t>
+          <t>1.422</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9831</t>
+          <t>0.9835</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0766</t>
+          <t>1.0765</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.737</t>
+          <t>0.738</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.3662</t>
+          <t>2.3661</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2255,17 +2255,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0502</t>
+          <t>0.4660</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>0.448</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>0.485</t>
         </is>
       </c>
     </row>
@@ -2278,17 +2278,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.0324</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -2301,17 +2301,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.9374</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -2324,17 +2324,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.0844</t>
+          <t>0.3859</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>0.367</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>0.405</t>
         </is>
       </c>
     </row>
@@ -2347,17 +2347,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.0247</t>
+          <t>1.0308</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.093</t>
         </is>
       </c>
     </row>
@@ -2370,17 +2370,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9890</t>
+          <t>0.9953</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.052</t>
         </is>
       </c>
     </row>
@@ -2393,17 +2393,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9979</t>
+          <t>0.9986</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.943</t>
+          <t>0.944</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.3080</t>
+          <t>1.3082</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0008</t>
+          <t>1.0007</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0181</t>
+          <t>1.0180</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2687,17 +2687,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0697</t>
+          <t>1.0791</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.183</t>
         </is>
       </c>
     </row>
@@ -2710,17 +2710,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.1375</t>
+          <t>1.0547</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.771</t>
+          <t>0.729</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.677</t>
+          <t>1.526</t>
         </is>
       </c>
     </row>
@@ -2733,17 +2733,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.9878</t>
+          <t>1.3579</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.790</t>
+          <t>1.093</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.687</t>
         </is>
       </c>
     </row>
@@ -2756,17 +2756,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0021</t>
+          <t>1.0630</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>0.943</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.130</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -2779,17 +2779,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0291</t>
+          <t>1.0236</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.902</t>
+          <t>0.897</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.168</t>
         </is>
       </c>
     </row>
@@ -2802,17 +2802,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.1517</t>
+          <t>1.1547</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.271</t>
+          <t>1.275</t>
         </is>
       </c>
     </row>
@@ -2825,17 +2825,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0556</t>
+          <t>1.0567</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.947</t>
+          <t>0.948</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.178</t>
         </is>
       </c>
     </row>
@@ -2848,17 +2848,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.0471</t>
+          <t>1.0486</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.916</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.0338</t>
+          <t>1.0342</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.191</t>
         </is>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.2781</t>
+          <t>1.2782</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2940,12 +2940,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.0146</t>
+          <t>1.0145</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>0.797</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0322</t>
+          <t>1.0323</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -3119,17 +3119,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.5487</t>
+          <t>0.7400</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.518</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>0.763</t>
         </is>
       </c>
     </row>
@@ -3142,17 +3142,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.1995</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.380</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -3165,17 +3165,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.3211</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.233</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.416</t>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -3188,17 +3188,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.5049</t>
+          <t>0.6205</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.433</t>
+          <t>0.598</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.581</t>
+          <t>0.644</t>
         </is>
       </c>
     </row>
@@ -3211,17 +3211,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.4957</t>
+          <t>1.5214</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.423</t>
+          <t>1.448</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.572</t>
+          <t>1.599</t>
         </is>
       </c>
     </row>
@@ -3234,17 +3234,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.6091</t>
+          <t>1.5961</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.532</t>
+          <t>1.519</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.691</t>
+          <t>1.677</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.6700</t>
+          <t>1.6702</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3280,7 +3280,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.7767</t>
+          <t>1.7763</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.4631</t>
+          <t>1.4627</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.3359</t>
+          <t>1.3358</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3382,7 +3382,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.601</t>
         </is>
       </c>
     </row>
@@ -3551,17 +3551,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.4941</t>
+          <t>1.5758</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.514</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.641</t>
         </is>
       </c>
     </row>
@@ -3574,17 +3574,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1.5883</t>
+          <t>1.0899</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1.893</t>
+          <t>1.262</t>
         </is>
       </c>
     </row>
@@ -3597,17 +3597,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.4092</t>
+          <t>1.5096</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1.304</t>
+          <t>1.402</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1.523</t>
+          <t>1.625</t>
         </is>
       </c>
     </row>
@@ -3620,17 +3620,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1.3878</t>
+          <t>1.6080</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.525</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.695</t>
         </is>
       </c>
     </row>
@@ -3643,17 +3643,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1.4810</t>
+          <t>1.4759</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1.407</t>
+          <t>1.403</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.553</t>
         </is>
       </c>
     </row>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.6489</t>
+          <t>1.6486</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3689,17 +3689,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1.6735</t>
+          <t>1.6725</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1.592</t>
+          <t>1.591</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.759</t>
+          <t>1.758</t>
         </is>
       </c>
     </row>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1.3583</t>
+          <t>1.3579</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -3735,7 +3735,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.4619</t>
+          <t>1.4617</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.583</t>
+          <t>1.582</t>
         </is>
       </c>
     </row>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>1.5885</t>
+          <t>1.5884</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">

</xml_diff>

<commit_message>
slope adjustments start on wek 0
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1031</t>
+          <t>1.1030</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.882</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.380</t>
+          <t>1.379</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.736</t>
+          <t>1.737</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.709</t>
+          <t>1.708</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -665,7 +665,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.928</t>
+          <t>1.929</t>
         </is>
       </c>
     </row>
@@ -683,12 +683,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.460</t>
+          <t>1.462</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.941</t>
+          <t>1.938</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.475</t>
+          <t>1.476</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.336</t>
+          <t>2.335</t>
         </is>
       </c>
     </row>
@@ -729,12 +729,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.393</t>
+          <t>1.394</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.521</t>
+          <t>2.520</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2.737</t>
+          <t>2.735</t>
         </is>
       </c>
     </row>
@@ -775,12 +775,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2.357</t>
+          <t>2.378</t>
         </is>
       </c>
     </row>
@@ -798,12 +798,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5.293</t>
+          <t>5.341</t>
         </is>
       </c>
     </row>
@@ -821,12 +821,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.553</t>
+          <t>0.535</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3.180</t>
+          <t>3.287</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2019</t>
+          <t>1.1976</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>12.019</t>
+          <t>11.976</t>
         </is>
       </c>
     </row>
@@ -862,7 +862,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2.5772</t>
+          <t>2.5819</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>25.772</t>
+          <t>25.819</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5.1270</t>
+          <t>5.1835</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>51.270</t>
+          <t>51.835</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.707</t>
+          <t>1.706</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.212</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.890</t>
+          <t>1.889</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2.004</t>
+          <t>2.005</t>
         </is>
       </c>
     </row>
@@ -1092,12 +1092,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.610</t>
+          <t>1.611</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.060</t>
+          <t>2.059</t>
         </is>
       </c>
     </row>
@@ -1115,12 +1115,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.370</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.985</t>
+          <t>1.986</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.460</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.347</t>
+          <t>2.345</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.279</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.396</t>
+          <t>2.394</t>
         </is>
       </c>
     </row>
@@ -1184,12 +1184,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.550</t>
+          <t>1.560</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3.450</t>
+          <t>3.428</t>
         </is>
       </c>
     </row>
@@ -1207,12 +1207,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.633</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.233</t>
+          <t>2.266</t>
         </is>
       </c>
     </row>
@@ -1230,12 +1230,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.609</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.372</t>
+          <t>1.373</t>
         </is>
       </c>
     </row>
@@ -1276,12 +1276,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.642</t>
+          <t>0.646</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3.824</t>
+          <t>3.796</t>
         </is>
       </c>
     </row>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3.7054</t>
+          <t>3.7972</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>37.054</t>
+          <t>37.972</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>4.1480</t>
+          <t>4.1937</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>41.480</t>
+          <t>41.937</t>
         </is>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.2216</t>
+          <t>1.2215</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.437</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>1.309</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.954</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.215</t>
+          <t>1.214</t>
         </is>
       </c>
     </row>
@@ -1570,12 +1570,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>0.720</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.380</t>
         </is>
       </c>
     </row>
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.614</t>
+          <t>0.615</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.443</t>
+          <t>1.441</t>
         </is>
       </c>
     </row>
@@ -1616,12 +1616,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.712</t>
+          <t>0.716</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2.072</t>
+          <t>2.062</t>
         </is>
       </c>
     </row>
@@ -1639,12 +1639,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.435</t>
+          <t>0.428</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2.136</t>
+          <t>2.172</t>
         </is>
       </c>
     </row>
@@ -1662,12 +1662,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.317</t>
+          <t>0.315</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2.160</t>
+          <t>2.178</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.1459</t>
+          <t>1.1741</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>11.459</t>
+          <t>11.741</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.7273</t>
+          <t>1.7561</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>17.273</t>
+          <t>17.561</t>
         </is>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.4377</t>
+          <t>1.4707</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>14.377</t>
+          <t>14.707</t>
         </is>
       </c>
     </row>
@@ -1875,12 +1875,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.388</t>
+          <t>1.385</t>
         </is>
       </c>
     </row>
@@ -1898,12 +1898,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.863</t>
+          <t>0.864</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>1.085</t>
         </is>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -2059,12 +2059,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.295</t>
         </is>
       </c>
     </row>
@@ -2082,12 +2082,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>0.906</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.186</t>
         </is>
       </c>
     </row>
@@ -2105,12 +2105,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.040</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.431</t>
         </is>
       </c>
     </row>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.935</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2151,12 +2151,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.775</t>
+          <t>0.773</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.327</t>
         </is>
       </c>
     </row>
@@ -2174,12 +2174,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.769</t>
+          <t>0.761</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.920</t>
+          <t>1.942</t>
         </is>
       </c>
     </row>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>6.619</t>
+          <t>6.620</t>
         </is>
       </c>
     </row>
@@ -2243,12 +2243,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.650</t>
+          <t>2.708</t>
         </is>
       </c>
     </row>
@@ -2307,12 +2307,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>0.858</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -2330,12 +2330,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.967</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.109</t>
         </is>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.201</t>
+          <t>1.202</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2468,12 +2468,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.415</t>
+          <t>1.414</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.690</t>
+          <t>1.691</t>
         </is>
       </c>
     </row>
@@ -2514,12 +2514,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.489</t>
+          <t>1.488</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.154</t>
+          <t>2.156</t>
         </is>
       </c>
     </row>
@@ -2537,12 +2537,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.919</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.331</t>
+          <t>1.333</t>
         </is>
       </c>
     </row>
@@ -2560,12 +2560,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.443</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.757</t>
+          <t>2.762</t>
         </is>
       </c>
     </row>
@@ -2606,12 +2606,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3.296</t>
+          <t>3.340</t>
         </is>
       </c>
     </row>
@@ -2629,12 +2629,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3.739</t>
+          <t>3.698</t>
         </is>
       </c>
     </row>
@@ -2652,12 +2652,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.799</t>
+          <t>0.793</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2.981</t>
+          <t>3.003</t>
         </is>
       </c>
     </row>
@@ -2739,12 +2739,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.706</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.184</t>
         </is>
       </c>
     </row>
@@ -2762,12 +2762,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.992</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.267</t>
+          <t>1.266</t>
         </is>
       </c>
     </row>
@@ -2877,12 +2877,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.291</t>
+          <t>1.290</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.518</t>
+          <t>1.519</t>
         </is>
       </c>
     </row>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.018</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2946,12 +2946,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.552</t>
+          <t>1.550</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2.345</t>
+          <t>2.349</t>
         </is>
       </c>
     </row>
@@ -2969,12 +2969,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>0.940</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.460</t>
+          <t>1.463</t>
         </is>
       </c>
     </row>
@@ -2992,12 +2992,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>1.235</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2.504</t>
+          <t>2.509</t>
         </is>
       </c>
     </row>
@@ -3015,12 +3015,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>0.912</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.931</t>
+          <t>1.935</t>
         </is>
       </c>
     </row>
@@ -3038,12 +3038,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.794</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3.609</t>
+          <t>3.673</t>
         </is>
       </c>
     </row>
@@ -3061,12 +3061,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.273</t>
+          <t>0.275</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2.359</t>
+          <t>2.343</t>
         </is>
       </c>
     </row>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.7762</t>
+          <t>1.8156</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>17.762</t>
+          <t>18.156</t>
         </is>
       </c>
     </row>
@@ -3107,12 +3107,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.253</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>6.246</t>
+          <t>6.345</t>
         </is>
       </c>
     </row>
@@ -3210,7 +3210,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -3228,12 +3228,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.832</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.761</t>
+          <t>1.764</t>
         </is>
       </c>
     </row>
@@ -3246,17 +3246,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.3710</t>
+          <t>1.3711</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.099</t>
+          <t>1.101</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.711</t>
+          <t>1.707</t>
         </is>
       </c>
     </row>
@@ -3274,12 +3274,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.952</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -3297,12 +3297,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.132</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.469</t>
         </is>
       </c>
     </row>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.965</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -3412,12 +3412,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.314</t>
+          <t>1.313</t>
         </is>
       </c>
     </row>
@@ -3435,12 +3435,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.749</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>1.098</t>
         </is>
       </c>
     </row>
@@ -3458,12 +3458,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.591</t>
+          <t>1.596</t>
         </is>
       </c>
     </row>
@@ -3481,12 +3481,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.787</t>
+          <t>0.788</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.303</t>
+          <t>1.302</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.454</t>
         </is>
       </c>
     </row>
@@ -3527,12 +3527,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.778</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.995</t>
+          <t>2.001</t>
         </is>
       </c>
     </row>
@@ -3550,12 +3550,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.218</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4.475</t>
+          <t>4.429</t>
         </is>
       </c>
     </row>
@@ -3573,12 +3573,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.583</t>
+          <t>0.580</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2.439</t>
+          <t>2.452</t>
         </is>
       </c>
     </row>
@@ -3596,12 +3596,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.677</t>
+          <t>0.686</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4.353</t>
+          <t>4.293</t>
         </is>
       </c>
     </row>
@@ -3660,12 +3660,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.847</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.218</t>
+          <t>1.216</t>
         </is>
       </c>
     </row>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.050</t>
         </is>
       </c>
     </row>
@@ -3706,12 +3706,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3757,7 +3757,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -3798,12 +3798,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>1.407</t>
         </is>
       </c>
     </row>
@@ -3844,7 +3844,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>0.924</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.242</t>
         </is>
       </c>
     </row>
@@ -3913,12 +3913,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.500</t>
+          <t>1.502</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.254</t>
+          <t>2.252</t>
         </is>
       </c>
     </row>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.375</t>
         </is>
       </c>
     </row>
@@ -3959,12 +3959,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.618</t>
+          <t>1.619</t>
         </is>
       </c>
     </row>
@@ -3982,12 +3982,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.323</t>
+          <t>2.316</t>
         </is>
       </c>
     </row>
@@ -4010,7 +4010,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.721</t>
+          <t>1.722</t>
         </is>
       </c>
     </row>
@@ -4028,12 +4028,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>1.438</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4.645</t>
+          <t>4.631</t>
         </is>
       </c>
     </row>
@@ -4092,12 +4092,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.791</t>
+          <t>0.790</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.726</t>
+          <t>1.729</t>
         </is>
       </c>
     </row>
@@ -4115,12 +4115,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.809</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.267</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -4138,12 +4138,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.898</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -4161,12 +4161,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.886</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -4276,12 +4276,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.904</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.308</t>
         </is>
       </c>
     </row>
@@ -4299,12 +4299,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.527</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -4322,12 +4322,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.794</t>
+          <t>0.792</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.286</t>
+          <t>1.290</t>
         </is>
       </c>
     </row>
@@ -4345,12 +4345,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.532</t>
+          <t>1.533</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2.716</t>
+          <t>2.713</t>
         </is>
       </c>
     </row>
@@ -4368,12 +4368,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.728</t>
+          <t>0.727</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.570</t>
+          <t>1.571</t>
         </is>
       </c>
     </row>
@@ -4391,12 +4391,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.697</t>
+          <t>0.694</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.968</t>
+          <t>1.976</t>
         </is>
       </c>
     </row>
@@ -4414,12 +4414,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.452</t>
+          <t>0.457</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.830</t>
+          <t>1.810</t>
         </is>
       </c>
     </row>
@@ -4437,12 +4437,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.755</t>
+          <t>0.752</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3.163</t>
+          <t>3.175</t>
         </is>
       </c>
     </row>
@@ -4460,12 +4460,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.543</t>
+          <t>0.550</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4.166</t>
+          <t>4.106</t>
         </is>
       </c>
     </row>
@@ -4524,12 +4524,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.435</t>
+          <t>1.433</t>
         </is>
       </c>
     </row>
@@ -4547,7 +4547,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.270</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>1.595</t>
         </is>
       </c>
     </row>
@@ -4736,7 +4736,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.345</t>
         </is>
       </c>
     </row>
@@ -4754,12 +4754,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.172</t>
+          <t>1.171</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1.594</t>
+          <t>1.595</t>
         </is>
       </c>
     </row>
@@ -4777,12 +4777,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.575</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2.425</t>
+          <t>2.426</t>
         </is>
       </c>
     </row>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.541</t>
+          <t>1.542</t>
         </is>
       </c>
     </row>
@@ -4828,7 +4828,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -4846,12 +4846,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.373</t>
+          <t>1.370</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>4.072</t>
+          <t>4.081</t>
         </is>
       </c>
     </row>
@@ -4869,12 +4869,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0.651</t>
+          <t>0.657</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2.049</t>
+          <t>2.029</t>
         </is>
       </c>
     </row>
@@ -4892,12 +4892,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.769</t>
+          <t>0.778</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2.506</t>
+          <t>2.478</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1.930</t>
+          <t>1.929</t>
         </is>
       </c>
     </row>
@@ -4979,12 +4979,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.303</t>
+          <t>1.304</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1.523</t>
+          <t>1.522</t>
         </is>
       </c>
     </row>
@@ -5122,7 +5122,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1.583</t>
+          <t>1.584</t>
         </is>
       </c>
     </row>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.462</t>
         </is>
       </c>
     </row>
@@ -5163,12 +5163,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1.403</t>
+          <t>1.405</t>
         </is>
       </c>
     </row>
@@ -5186,12 +5186,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.368</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1.874</t>
+          <t>1.876</t>
         </is>
       </c>
     </row>
@@ -5214,7 +5214,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.372</t>
         </is>
       </c>
     </row>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1.469</t>
+          <t>1.470</t>
         </is>
       </c>
     </row>
@@ -5255,12 +5255,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.621</t>
+          <t>0.619</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1.391</t>
+          <t>1.395</t>
         </is>
       </c>
     </row>
@@ -5278,12 +5278,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0.813</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>2.673</t>
+          <t>2.674</t>
         </is>
       </c>
     </row>
@@ -5301,12 +5301,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.627</t>
+          <t>0.635</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.981</t>
+          <t>1.957</t>
         </is>
       </c>
     </row>
@@ -5324,12 +5324,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.393</t>
+          <t>0.397</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1.665</t>
+          <t>1.646</t>
         </is>
       </c>
     </row>
@@ -5445,12 +5445,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.890</t>
+          <t>1.889</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2.975</t>
+          <t>2.977</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.045</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.625</t>
+          <t>1.626</t>
         </is>
       </c>
     </row>
@@ -5629,12 +5629,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.418</t>
+          <t>1.419</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.093</t>
+          <t>2.092</t>
         </is>
       </c>
     </row>
@@ -5652,12 +5652,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.789</t>
+          <t>0.787</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.285</t>
         </is>
       </c>
     </row>
@@ -5670,17 +5670,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2.7491</t>
+          <t>2.7492</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.828</t>
+          <t>1.841</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4.135</t>
+          <t>4.105</t>
         </is>
       </c>
     </row>
@@ -5698,12 +5698,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.875</t>
+          <t>1.902</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5.439</t>
+          <t>5.361</t>
         </is>
       </c>
     </row>
@@ -5721,12 +5721,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.916</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2.018</t>
+          <t>1.982</t>
         </is>
       </c>
     </row>
@@ -5739,17 +5739,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4.9978</t>
+          <t>4.9979</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.980</t>
+          <t>2.100</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12.617</t>
+          <t>11.893</t>
         </is>
       </c>
     </row>
@@ -5767,12 +5767,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.583</t>
+          <t>0.575</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.137</t>
+          <t>2.170</t>
         </is>
       </c>
     </row>
@@ -5790,12 +5790,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.438</t>
+          <t>0.448</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2.997</t>
+          <t>2.928</t>
         </is>
       </c>
     </row>
@@ -5818,7 +5818,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.996</t>
+          <t>2.998</t>
         </is>
       </c>
     </row>
@@ -5877,12 +5877,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.474</t>
+          <t>0.476</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.873</t>
+          <t>2.865</t>
         </is>
       </c>
     </row>
@@ -5900,12 +5900,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.754</t>
+          <t>0.757</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -5923,12 +5923,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.167</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.622</t>
+          <t>1.625</t>
         </is>
       </c>
     </row>
@@ -5946,12 +5946,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.301</t>
+          <t>1.299</t>
         </is>
       </c>
     </row>
@@ -5992,12 +5992,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.460</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.882</t>
+          <t>1.885</t>
         </is>
       </c>
     </row>
@@ -6015,12 +6015,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.404</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.892</t>
+          <t>1.894</t>
         </is>
       </c>
     </row>
@@ -6043,7 +6043,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.501</t>
+          <t>1.500</t>
         </is>
       </c>
     </row>
@@ -6061,12 +6061,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.372</t>
+          <t>1.374</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.270</t>
+          <t>2.267</t>
         </is>
       </c>
     </row>
@@ -6084,12 +6084,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.723</t>
+          <t>0.724</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.394</t>
+          <t>1.393</t>
         </is>
       </c>
     </row>
@@ -6107,12 +6107,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.764</t>
+          <t>1.777</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4.341</t>
+          <t>4.310</t>
         </is>
       </c>
     </row>
@@ -6130,12 +6130,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2.729</t>
+          <t>2.763</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>8.585</t>
+          <t>8.480</t>
         </is>
       </c>
     </row>
@@ -6153,12 +6153,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.382</t>
+          <t>0.380</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>1.602</t>
         </is>
       </c>
     </row>
@@ -6171,17 +6171,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5.4849</t>
+          <t>5.4851</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.999</t>
+          <t>2.114</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>15.052</t>
+          <t>14.231</t>
         </is>
       </c>
     </row>
@@ -6199,12 +6199,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.502</t>
+          <t>0.496</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.286</t>
+          <t>2.310</t>
         </is>
       </c>
     </row>
@@ -6222,12 +6222,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.521</t>
+          <t>0.515</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>6.486</t>
+          <t>6.550</t>
         </is>
       </c>
     </row>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2.6269</t>
+          <t>2.3717</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -6250,7 +6250,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>26.269</t>
+          <t>23.717</t>
         </is>
       </c>
     </row>
@@ -6309,12 +6309,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.293</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2.348</t>
+          <t>2.350</t>
         </is>
       </c>
     </row>
@@ -6332,12 +6332,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.904</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.153</t>
+          <t>1.152</t>
         </is>
       </c>
     </row>
@@ -6406,7 +6406,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.266</t>
         </is>
       </c>
     </row>
@@ -6498,7 +6498,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.302</t>
+          <t>2.301</t>
         </is>
       </c>
     </row>
@@ -6516,12 +6516,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>0.838</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.387</t>
         </is>
       </c>
     </row>
@@ -6539,12 +6539,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.937</t>
+          <t>1.950</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4.421</t>
+          <t>4.390</t>
         </is>
       </c>
     </row>
@@ -6562,12 +6562,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2.049</t>
+          <t>2.079</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>5.987</t>
+          <t>5.901</t>
         </is>
       </c>
     </row>
@@ -6585,12 +6585,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.749</t>
+          <t>0.763</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.705</t>
+          <t>1.675</t>
         </is>
       </c>
     </row>
@@ -6603,17 +6603,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>6.4106</t>
+          <t>6.4108</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.510</t>
+          <t>2.661</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>16.375</t>
+          <t>15.443</t>
         </is>
       </c>
     </row>
@@ -6631,12 +6631,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.638</t>
+          <t>0.630</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2.387</t>
+          <t>2.417</t>
         </is>
       </c>
     </row>
@@ -6654,12 +6654,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.532</t>
+          <t>0.544</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3.641</t>
+          <t>3.562</t>
         </is>
       </c>
     </row>
@@ -6677,12 +6677,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.492</t>
+          <t>0.493</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3.205</t>
+          <t>3.196</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.562</t>
+          <t>1.561</t>
         </is>
       </c>
     </row>
@@ -6764,7 +6764,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -6787,7 +6787,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.246</t>
         </is>
       </c>
     </row>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>1.087</t>
         </is>
       </c>
     </row>
@@ -6884,7 +6884,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.478</t>
+          <t>1.479</t>
         </is>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2.216</t>
+          <t>2.215</t>
         </is>
       </c>
     </row>
@@ -6948,12 +6948,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.774</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.254</t>
+          <t>1.259</t>
         </is>
       </c>
     </row>
@@ -6971,12 +6971,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.725</t>
+          <t>1.737</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>3.899</t>
+          <t>3.871</t>
         </is>
       </c>
     </row>
@@ -6994,12 +6994,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.785</t>
+          <t>1.811</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>5.200</t>
+          <t>5.125</t>
         </is>
       </c>
     </row>
@@ -7017,12 +7017,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.823</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.858</t>
+          <t>1.825</t>
         </is>
       </c>
     </row>
@@ -7035,17 +7035,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>8.4201</t>
+          <t>8.4202</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3.298</t>
+          <t>3.493</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>21.497</t>
+          <t>20.300</t>
         </is>
       </c>
     </row>
@@ -7063,12 +7063,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.620</t>
+          <t>0.612</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2.333</t>
+          <t>2.363</t>
         </is>
       </c>
     </row>
@@ -7086,12 +7086,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0.479</t>
+          <t>0.493</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3.598</t>
+          <t>3.493</t>
         </is>
       </c>
     </row>
@@ -7109,12 +7109,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.523</t>
+          <t>0.529</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>4.029</t>
+          <t>3.976</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new KCOR files generated with no min final KCOR value
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -816,17 +816,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3262</t>
+          <t>0.5117</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.535</t>
+          <t>0.206</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3.287</t>
+          <t>1.268</t>
         </is>
       </c>
     </row>
@@ -949,17 +949,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0551</t>
+          <t>0.8986</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.918</t>
+          <t>0.782</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.032</t>
         </is>
       </c>
     </row>
@@ -1225,17 +1225,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.9145</t>
+          <t>0.6229</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.609</t>
+          <t>0.415</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.373</t>
+          <t>0.935</t>
         </is>
       </c>
     </row>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.2776</t>
+          <t>0.7986</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>12.776</t>
+          <t>7.986</t>
         </is>
       </c>
     </row>
@@ -1381,17 +1381,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.0628</t>
+          <t>0.8146</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>0.645</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.343</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -1496,17 +1496,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.0533</t>
+          <t>1.0185</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.923</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -1542,17 +1542,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1564</t>
+          <t>0.9801</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.779</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>1.233</t>
         </is>
       </c>
     </row>
@@ -1588,17 +1588,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.9415</t>
+          <t>0.9337</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.615</t>
+          <t>0.610</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -1634,17 +1634,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9636</t>
+          <t>0.8419</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.428</t>
+          <t>0.374</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2.172</t>
+          <t>1.898</t>
         </is>
       </c>
     </row>
@@ -1657,17 +1657,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8278</t>
+          <t>0.2839</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.315</t>
+          <t>0.108</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>2.178</t>
+          <t>0.747</t>
         </is>
       </c>
     </row>
@@ -1870,17 +1870,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0670</t>
+          <t>0.9706</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.822</t>
+          <t>0.748</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.385</t>
+          <t>1.260</t>
         </is>
       </c>
     </row>
@@ -1893,17 +1893,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9682</t>
+          <t>0.7755</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.864</t>
+          <t>0.692</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>0.869</t>
         </is>
       </c>
     </row>
@@ -1916,17 +1916,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0019</t>
+          <t>0.8445</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.924</t>
+          <t>0.779</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>0.916</t>
         </is>
       </c>
     </row>
@@ -2077,17 +2077,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.0368</t>
+          <t>0.9388</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.906</t>
+          <t>0.821</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -2146,17 +2146,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0131</t>
+          <t>0.6768</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.773</t>
+          <t>0.517</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.327</t>
+          <t>0.887</t>
         </is>
       </c>
     </row>
@@ -2169,17 +2169,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2156</t>
+          <t>1.0291</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.761</t>
+          <t>0.644</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.942</t>
+          <t>1.644</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4736</t>
+          <t>0.7909</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>14.736</t>
+          <t>7.909</t>
         </is>
       </c>
     </row>
@@ -2238,17 +2238,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.5000</t>
+          <t>0.2015</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.831</t>
+          <t>0.112</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.708</t>
+          <t>0.364</t>
         </is>
       </c>
     </row>
@@ -2302,17 +2302,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.9756</t>
+          <t>0.8326</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.732</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>0.947</t>
         </is>
       </c>
     </row>
@@ -2325,17 +2325,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.0356</t>
+          <t>0.8584</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.967</t>
+          <t>0.802</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.109</t>
+          <t>0.919</t>
         </is>
       </c>
     </row>
@@ -2348,17 +2348,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.9868</t>
+          <t>0.9624</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.013</t>
         </is>
       </c>
     </row>
@@ -2532,17 +2532,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.1069</t>
+          <t>1.0084</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.214</t>
         </is>
       </c>
     </row>
@@ -2578,17 +2578,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.9376</t>
+          <t>0.8990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.680</t>
+          <t>0.652</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.292</t>
+          <t>1.239</t>
         </is>
       </c>
     </row>
@@ -2647,17 +2647,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.5437</t>
+          <t>0.7383</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.793</t>
+          <t>0.379</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>3.003</t>
+          <t>1.436</t>
         </is>
       </c>
     </row>
@@ -2670,17 +2670,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.1432</t>
+          <t>0.5681</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>0.579</t>
+          <t>0.288</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2.257</t>
+          <t>1.122</t>
         </is>
       </c>
     </row>
@@ -2734,17 +2734,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.9144</t>
+          <t>0.8578</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.184</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -2964,17 +2964,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.1727</t>
+          <t>0.8265</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.031</t>
         </is>
       </c>
     </row>
@@ -3056,17 +3056,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.8023</t>
+          <t>0.7184</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.275</t>
+          <t>0.246</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2.343</t>
+          <t>2.098</t>
         </is>
       </c>
     </row>
@@ -3223,17 +3223,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2104</t>
+          <t>0.6596</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.831</t>
+          <t>0.453</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.764</t>
+          <t>0.961</t>
         </is>
       </c>
     </row>
@@ -3315,17 +3315,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0664</t>
+          <t>0.8578</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.777</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.178</t>
+          <t>0.947</t>
         </is>
       </c>
     </row>
@@ -3338,17 +3338,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0196</t>
+          <t>0.9434</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.052</t>
         </is>
       </c>
     </row>
@@ -3453,17 +3453,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1.2532</t>
+          <t>0.8445</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>1.075</t>
         </is>
       </c>
     </row>
@@ -3476,17 +3476,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0130</t>
+          <t>0.9015</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.701</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.302</t>
+          <t>1.159</t>
         </is>
       </c>
     </row>
@@ -3522,17 +3522,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2460</t>
+          <t>0.8994</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.776</t>
+          <t>0.560</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2.001</t>
+          <t>1.444</t>
         </is>
       </c>
     </row>
@@ -3568,17 +3568,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1923</t>
+          <t>0.6704</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.580</t>
+          <t>0.326</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2.452</t>
+          <t>1.379</t>
         </is>
       </c>
     </row>
@@ -3655,17 +3655,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0150</t>
+          <t>0.7706</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.847</t>
+          <t>0.643</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>0.923</t>
         </is>
       </c>
     </row>
@@ -3724,17 +3724,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0303</t>
+          <t>1.0170</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.078</t>
         </is>
       </c>
     </row>
@@ -3747,17 +3747,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9947</t>
+          <t>0.9822</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -3862,17 +3862,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.9986</t>
+          <t>0.9641</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.090</t>
         </is>
       </c>
     </row>
@@ -3885,17 +3885,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.0828</t>
+          <t>0.8534</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>0.744</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -3954,17 +3954,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.1685</t>
+          <t>1.0533</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.760</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.619</t>
+          <t>1.460</t>
         </is>
       </c>
     </row>
@@ -4110,17 +4110,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0122</t>
+          <t>0.7044</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>0.564</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.264</t>
+          <t>0.880</t>
         </is>
       </c>
     </row>
@@ -4156,17 +4156,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.0098</t>
+          <t>0.7884</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.692</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>0.898</t>
         </is>
       </c>
     </row>
@@ -4271,17 +4271,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0872</t>
+          <t>0.9340</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.904</t>
+          <t>0.777</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>1.123</t>
         </is>
       </c>
     </row>
@@ -4294,17 +4294,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.2540</t>
+          <t>1.0625</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>0.874</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -4409,17 +4409,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.9092</t>
+          <t>0.6908</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.457</t>
+          <t>0.347</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.810</t>
+          <t>1.375</t>
         </is>
       </c>
     </row>
@@ -4818,17 +4818,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1.0863</t>
+          <t>0.9315</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.774</t>
+          <t>0.663</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.308</t>
         </is>
       </c>
     </row>
@@ -5250,17 +5250,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0.9296</t>
+          <t>0.8844</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.619</t>
+          <t>0.589</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1.395</t>
+          <t>1.327</t>
         </is>
       </c>
     </row>
@@ -5319,17 +5319,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>0.8087</t>
+          <t>0.5380</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.397</t>
+          <t>0.264</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1.646</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -5762,17 +5762,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.1167</t>
+          <t>0.5340</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.575</t>
+          <t>0.275</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.170</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -5785,17 +5785,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1454</t>
+          <t>0.8316</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.448</t>
+          <t>0.325</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2.928</t>
+          <t>2.126</t>
         </is>
       </c>
     </row>
@@ -5808,17 +5808,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1402</t>
+          <t>0.4408</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.434</t>
+          <t>0.168</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.998</t>
+          <t>1.159</t>
         </is>
       </c>
     </row>
@@ -5872,17 +5872,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1673</t>
+          <t>1.1495</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.476</t>
+          <t>0.468</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.865</t>
+          <t>2.821</t>
         </is>
       </c>
     </row>
@@ -5895,17 +5895,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9831</t>
+          <t>0.9550</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -6079,17 +6079,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0044</t>
+          <t>0.4953</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>0.357</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.393</t>
+          <t>0.687</t>
         </is>
       </c>
     </row>
@@ -6148,17 +6148,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.7803</t>
+          <t>0.5117</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.380</t>
+          <t>0.249</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -6194,17 +6194,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.0709</t>
+          <t>0.6231</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.496</t>
+          <t>0.289</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.310</t>
+          <t>1.344</t>
         </is>
       </c>
     </row>
@@ -6327,17 +6327,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0204</t>
+          <t>0.9561</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.904</t>
+          <t>0.847</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.152</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
@@ -6626,17 +6626,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.2341</t>
+          <t>0.5293</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.630</t>
+          <t>0.270</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2.417</t>
+          <t>1.037</t>
         </is>
       </c>
     </row>
@@ -6672,17 +6672,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.2554</t>
+          <t>0.3897</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.493</t>
+          <t>0.153</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3.196</t>
+          <t>0.992</t>
         </is>
       </c>
     </row>
@@ -6943,17 +6943,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.9869</t>
+          <t>0.9795</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.774</t>
+          <t>0.768</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.259</t>
+          <t>1.249</t>
         </is>
       </c>
     </row>
@@ -7058,17 +7058,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1.2023</t>
+          <t>0.5113</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.612</t>
+          <t>0.260</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2.363</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -7081,17 +7081,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.3127</t>
+          <t>0.6230</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>0.493</t>
+          <t>0.234</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3.493</t>
+          <t>1.658</t>
         </is>
       </c>
     </row>
@@ -7104,17 +7104,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1.4509</t>
+          <t>0.2063</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>0.529</t>
+          <t>0.075</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3.976</t>
+          <t>0.565</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
latest changes. to README and re-ran with 2004 and the bug fix on enrollment. Added CMRR analysis to KCOR_CMR_analysis
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.4176</t>
+          <t>1.3870</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.379</t>
+          <t>1.349</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.457</t>
+          <t>1.426</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0606</t>
+          <t>0.9562</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.882</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.036</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1182</t>
+          <t>1.1516</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.7242</t>
+          <t>1.6557</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.663</t>
+          <t>1.597</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.788</t>
+          <t>1.716</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5448</t>
+          <t>1.5213</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.425</t>
+          <t>1.397</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.674</t>
+          <t>1.657</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2.3480</t>
+          <t>1.7967</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.960</t>
+          <t>1.499</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.813</t>
+          <t>2.154</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.3816</t>
+          <t>1.2856</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.863</t>
+          <t>1.730</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1173</t>
+          <t>1.5204</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.594</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.101</t>
+          <t>2.851</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.8595</t>
+          <t>1.9119</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>18.595</t>
+          <t>19.119</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5.4405</t>
+          <t>6.6914</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>54.405</t>
+          <t>66.914</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5855</t>
+          <t>1.5504</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.501</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.602</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1952</t>
+          <t>1.1817</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.123</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>1.258</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.7055</t>
+          <t>1.6916</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.646</t>
+          <t>1.631</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.767</t>
+          <t>1.755</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6450</t>
+          <t>1.6920</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.600</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.727</t>
+          <t>1.789</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.5478</t>
+          <t>1.3836</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.247</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.536</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.8734</t>
+          <t>1.9049</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.553</t>
+          <t>1.563</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.260</t>
+          <t>2.321</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.4348</t>
+          <t>1.2708</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>0.908</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.999</t>
+          <t>1.778</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.5056</t>
+          <t>0.3440</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.338</t>
+          <t>0.229</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.517</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.9652</t>
+          <t>1.6347</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.793</t>
+          <t>0.668</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.868</t>
+          <t>4.002</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.5058</t>
+          <t>2.6556</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>35.058</t>
+          <t>26.556</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1175</t>
+          <t>1.1176</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.073</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.1269</t>
+          <t>1.2358</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.131</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.350</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5253</t>
+          <t>1.4689</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.457</t>
+          <t>1.403</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.597</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9540</t>
+          <t>1.0219</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.010</t>
+          <t>1.088</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0019</t>
+          <t>0.9095</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.797</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.7979</t>
+          <t>1.0602</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.617</t>
+          <t>0.813</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.382</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0385</t>
+          <t>0.9885</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.634</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.616</t>
+          <t>1.541</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4526</t>
+          <t>0.2263</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.216</t>
+          <t>0.108</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.474</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.8081</t>
+          <t>0.7738</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>8.081</t>
+          <t>7.738</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.6444</t>
+          <t>0.3969</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>6.444</t>
+          <t>3.969</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0481</t>
+          <t>1.0841</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9085</t>
+          <t>0.9338</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.819</t>
+          <t>0.844</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.033</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9832</t>
+          <t>1.0141</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.072</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0834</t>
+          <t>1.1232</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.072</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1867</t>
+          <t>1.2476</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.122</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.256</t>
+          <t>1.317</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1199</t>
+          <t>1.1305</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.221</t>
+          <t>1.228</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1573</t>
+          <t>1.0609</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.197</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.6337</t>
+          <t>0.6321</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.503</t>
+          <t>0.505</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>0.792</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>4.0864</t>
+          <t>3.5740</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.606</t>
+          <t>1.456</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>10.400</t>
+          <t>8.775</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.2420</t>
+          <t>0.6728</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.131</t>
+          <t>0.264</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.446</t>
+          <t>1.711</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.2052</t>
+          <t>1.1996</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.174</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8608</t>
+          <t>0.8674</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.810</t>
+          <t>0.816</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.922</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0770</t>
+          <t>1.0733</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.035</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.113</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3126</t>
+          <t>1.2762</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.266</t>
+          <t>1.230</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.361</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -1635,12 +1635,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.5214</t>
+          <t>1.5182</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.443</t>
+          <t>1.437</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3346</t>
+          <t>1.3526</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.467</t>
+          <t>1.501</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1710</t>
+          <t>1.2546</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>1.060</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.485</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8802</t>
+          <t>0.9778</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.663</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.334</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8986</t>
+          <t>0.9727</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.564</t>
+          <t>0.610</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.431</t>
+          <t>1.551</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.6286</t>
+          <t>1.4530</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.315</t>
+          <t>0.584</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>3.613</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1499</t>
+          <t>1.1066</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.075</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.183</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9476</t>
+          <t>0.9289</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.857</t>
+          <t>0.842</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.025</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0954</t>
+          <t>1.0584</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.004</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.116</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2115</t>
+          <t>1.1362</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.084</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>1.191</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2821</t>
+          <t>1.2169</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>1.141</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.367</t>
+          <t>1.298</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.1917</t>
+          <t>1.1965</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.064</t>
+          <t>1.063</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.347</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0118</t>
+          <t>1.1826</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.978</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.3891</t>
+          <t>1.5469</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>1.081</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.949</t>
+          <t>2.214</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.2199</t>
+          <t>0.2722</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.079</t>
+          <t>0.101</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.731</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2.5975</t>
+          <t>2.1597</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>0.614</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>5.979</t>
+          <t>7.598</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0060</t>
+          <t>1.0348</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.990</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2279</t>
+          <t>1.3341</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.485</t>
+          <t>1.627</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1207</t>
+          <t>1.1327</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.223</t>
+          <t>1.235</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8488</t>
+          <t>0.8772</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.789</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>0.944</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1640</t>
+          <t>1.2184</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.340</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0063</t>
+          <t>0.9983</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.877</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.7556</t>
+          <t>0.7500</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.634</t>
+          <t>0.631</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>0.891</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7770</t>
+          <t>0.7943</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.581</t>
+          <t>0.595</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.8070</t>
+          <t>0.6889</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.499</t>
+          <t>0.445</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.305</t>
+          <t>1.065</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.6251</t>
+          <t>2.6272</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.068</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.448</t>
+          <t>6.465</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0614</t>
+          <t>1.0725</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0377</t>
+          <t>1.0736</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.962</t>
+          <t>0.995</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.158</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0499</t>
+          <t>1.0693</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9910</t>
+          <t>0.9997</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.961</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2777</t>
+          <t>1.2589</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.196</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.325</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9771</t>
+          <t>0.9935</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.902</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.076</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0850</t>
+          <t>1.1055</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0763</t>
+          <t>1.0913</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.903</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.304</t>
+          <t>1.319</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.5720</t>
+          <t>1.6620</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.236</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.099</t>
+          <t>2.235</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.1330</t>
+          <t>4.2222</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2.312</t>
+          <t>2.364</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7.387</t>
+          <t>7.541</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0550</t>
+          <t>1.0364</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>0.991</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.103</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.8451</t>
+          <t>0.8047</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.697</t>
+          <t>0.658</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>0.984</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9369</t>
+          <t>0.9440</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.865</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.030</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1675</t>
+          <t>1.1396</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.059</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.257</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0977</t>
+          <t>1.0332</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.210</t>
+          <t>1.138</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9710</t>
+          <t>0.9952</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.871</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.4360</t>
+          <t>1.4739</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.722</t>
+          <t>1.764</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.3851</t>
+          <t>1.3740</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.892</t>
+          <t>1.873</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.9478</t>
+          <t>2.4128</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.175</t>
+          <t>1.512</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3.228</t>
+          <t>3.851</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.5744</t>
+          <t>1.6071</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.588</t>
+          <t>0.599</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4.218</t>
+          <t>4.311</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6330</t>
+          <t>1.6269</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.601</t>
+          <t>1.595</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.666</t>
+          <t>1.659</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.4932</t>
+          <t>1.4961</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.404</t>
+          <t>1.406</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.589</t>
+          <t>1.592</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.5585</t>
+          <t>1.5511</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.505</t>
+          <t>1.498</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.614</t>
+          <t>1.607</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.7256</t>
+          <t>1.7160</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.666</t>
+          <t>1.657</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.787</t>
+          <t>1.778</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7196</t>
+          <t>1.7316</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.642</t>
+          <t>1.653</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.801</t>
+          <t>1.814</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.3536</t>
+          <t>1.3366</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>1.236</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.7359</t>
+          <t>1.6958</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.534</t>
+          <t>1.498</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.965</t>
+          <t>1.919</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.3960</t>
+          <t>1.3538</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.102</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.709</t>
+          <t>1.663</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.6408</t>
+          <t>1.6497</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.132</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2.379</t>
+          <t>2.392</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>3.0065</t>
+          <t>2.8179</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.702</t>
+          <t>1.601</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5.312</t>
+          <t>4.961</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5386</t>
+          <t>1.5170</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.507</t>
+          <t>1.486</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.571</t>
+          <t>1.548</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.4390</t>
+          <t>1.3936</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.341</t>
+          <t>1.298</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.496</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.4844</t>
+          <t>1.4506</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.398</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.540</t>
+          <t>1.505</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.7413</t>
+          <t>1.7165</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.682</t>
+          <t>1.658</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.803</t>
+          <t>1.777</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.3459</t>
+          <t>1.3756</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.309</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.414</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3853</t>
+          <t>1.3454</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.274</t>
+          <t>1.237</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.507</t>
+          <t>1.463</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.5999</t>
+          <t>1.5340</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.400</t>
+          <t>1.342</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.828</t>
+          <t>1.753</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.2971</t>
+          <t>1.2405</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.982</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.637</t>
+          <t>1.567</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.0438</t>
+          <t>0.9926</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.698</t>
+          <t>0.660</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.562</t>
+          <t>1.493</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7274</t>
+          <t>0.6674</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.362</t>
+          <t>0.333</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.462</t>
+          <t>1.337</t>
         </is>
       </c>
     </row>
@@ -3393,17 +3393,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2862</t>
+          <t>1.2803</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.248</t>
+          <t>1.242</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -3416,17 +3416,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.6233</t>
+          <t>1.6084</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.484</t>
+          <t>1.470</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.776</t>
+          <t>1.760</t>
         </is>
       </c>
     </row>
@@ -3439,17 +3439,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1788</t>
+          <t>1.1660</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.123</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>1.224</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3462,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1810</t>
+          <t>1.1762</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.119</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.237</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.3745</t>
+          <t>1.3796</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.284</t>
+          <t>1.289</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.477</t>
         </is>
       </c>
     </row>
@@ -3508,17 +3508,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.3835</t>
+          <t>1.3576</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.166</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.611</t>
+          <t>1.581</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.2398</t>
+          <t>3.1916</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.366</t>
+          <t>2.328</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4.436</t>
+          <t>4.376</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3554,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.5696</t>
+          <t>1.5789</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.205</t>
+          <t>2.217</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3577,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.7912</t>
+          <t>0.6202</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.464</t>
+          <t>0.362</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.349</t>
+          <t>1.062</t>
         </is>
       </c>
     </row>
@@ -3600,17 +3600,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.4882</t>
+          <t>4.0061</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.185</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>40.061</t>
         </is>
       </c>
     </row>
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.4658</t>
+          <t>1.4554</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.387</t>
+          <t>1.377</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0285</t>
+          <t>1.0434</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.323</t>
+          <t>1.342</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2916</t>
+          <t>1.2819</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.159</t>
+          <t>1.151</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>1.427</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6304</t>
+          <t>1.6093</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.487</t>
+          <t>1.467</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.788</t>
+          <t>1.765</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4290</t>
+          <t>1.4526</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.298</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.599</t>
+          <t>1.626</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2178</t>
+          <t>1.1731</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>0.961</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.486</t>
+          <t>1.431</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5.1441</t>
+          <t>5.0675</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3.641</t>
+          <t>3.583</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>7.267</t>
+          <t>7.168</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.4641</t>
+          <t>1.4727</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.907</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.378</t>
+          <t>2.392</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.9588</t>
+          <t>1.5354</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.804</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3.728</t>
+          <t>2.932</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.4026</t>
+          <t>3.8004</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>44.026</t>
+          <t>38.004</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2666</t>
+          <t>1.2608</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.222</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.307</t>
+          <t>1.301</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0720</t>
+          <t>1.0473</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.935</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.172</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.2798</t>
+          <t>1.2647</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.201</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.347</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2532</t>
+          <t>1.2496</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.187</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.319</t>
+          <t>1.316</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0925</t>
+          <t>1.0942</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.019</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.175</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.4769</t>
+          <t>1.4547</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.263</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.727</t>
+          <t>1.701</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>3.6011</t>
+          <t>3.5269</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.622</t>
+          <t>2.565</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4.946</t>
+          <t>4.850</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.6684</t>
+          <t>1.6784</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.372</t>
+          <t>2.385</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.0533</t>
+          <t>0.8258</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.614</t>
+          <t>0.480</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.806</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -4096,17 +4096,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.3500</t>
+          <t>2.3521</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.137</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>23.521</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.2531</t>
+          <t>1.2465</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.221</t>
+          <t>1.214</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.286</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.3431</t>
+          <t>1.3231</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.223</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.452</t>
+          <t>1.431</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.1926</t>
+          <t>1.1708</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.148</t>
+          <t>1.126</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.217</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.1664</t>
+          <t>1.1573</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.112</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.3004</t>
+          <t>1.3080</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.230</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.390</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4101</t>
+          <t>1.3794</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.188</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.637</t>
+          <t>1.602</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2.9715</t>
+          <t>2.9288</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2.170</t>
+          <t>2.136</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4.070</t>
+          <t>4.017</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.7163</t>
+          <t>1.7269</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.209</t>
+          <t>1.217</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2.436</t>
+          <t>2.450</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8570</t>
+          <t>0.6454</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.496</t>
+          <t>0.372</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.480</t>
+          <t>1.119</t>
         </is>
       </c>
     </row>
@@ -4344,17 +4344,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.1796</t>
+          <t>1.7436</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.065</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.493</t>
+          <t>17.436</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to correct the 2000 cutoff. now the % vaxxed are accurate
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.6914</t>
+          <t>7.9660</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>66.914</t>
+          <t>79.660</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.6556</t>
+          <t>3.1674</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>26.556</t>
+          <t>31.674</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.3969</t>
+          <t>0.3976</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.969</t>
+          <t>3.976</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0841</t>
+          <t>1.0814</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.052</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>1.112</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.6728</t>
+          <t>0.4953</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.264</t>
+          <t>0.196</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.711</t>
+          <t>1.250</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1996</t>
+          <t>1.1986</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.173</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.225</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4530</t>
+          <t>1.1109</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.584</t>
+          <t>0.450</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3.613</t>
+          <t>2.740</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1066</t>
+          <t>1.1084</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.077</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2.1597</t>
+          <t>2.2428</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.614</t>
+          <t>0.638</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7.598</t>
+          <t>7.890</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0348</t>
+          <t>1.0350</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.6272</t>
+          <t>2.0390</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>0.830</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.465</t>
+          <t>5.010</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0725</t>
+          <t>1.0718</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.048</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.2222</t>
+          <t>1.6744</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2.364</t>
+          <t>1.140</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7.541</t>
+          <t>2.459</t>
         </is>
       </c>
     </row>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0364</t>
+          <t>1.0355</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.083</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.6071</t>
+          <t>0.8212</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.599</t>
+          <t>0.326</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4.311</t>
+          <t>2.067</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6269</t>
+          <t>1.6281</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.595</t>
+          <t>1.596</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.659</t>
+          <t>1.661</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2.8179</t>
+          <t>3.4111</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1.601</t>
+          <t>2.008</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4.961</t>
+          <t>5.795</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5170</t>
+          <t>1.5190</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.486</t>
+          <t>1.488</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.548</t>
+          <t>1.551</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.6674</t>
+          <t>2.0372</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.333</t>
+          <t>1.152</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>3.603</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.0061</t>
+          <t>4.1845</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>40.061</t>
+          <t>41.845</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.8004</t>
+          <t>4.9146</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>38.004</t>
+          <t>49.146</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2.3521</t>
+          <t>3.5630</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>23.521</t>
+          <t>35.630</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.7436</t>
+          <t>3.7594</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>17.436</t>
+          <t>37.594</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
check in before changing the  MASSIVE change in formula to subtract first.
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3870</t>
+          <t>1.5019</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.349</t>
+          <t>1.461</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.426</t>
+          <t>1.544</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9562</t>
+          <t>1.1943</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>1.102</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.294</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1516</t>
+          <t>1.2437</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.196</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.198</t>
+          <t>1.293</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6557</t>
+          <t>1.8376</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.597</t>
+          <t>1.773</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.716</t>
+          <t>1.905</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5213</t>
+          <t>1.5456</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.419</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.657</t>
+          <t>1.683</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.7967</t>
+          <t>1.5894</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.499</t>
+          <t>1.326</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.154</t>
+          <t>1.906</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2856</t>
+          <t>1.5770</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>1.173</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.730</t>
+          <t>2.120</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.5204</t>
+          <t>1.6376</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>0.876</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.851</t>
+          <t>3.062</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.9119</t>
+          <t>1.7281</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>19.119</t>
+          <t>17.281</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.9660</t>
+          <t>8.0955</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>79.660</t>
+          <t>80.955</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5504</t>
+          <t>1.6879</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.501</t>
+          <t>1.634</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.744</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1817</t>
+          <t>1.5732</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.478</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.258</t>
+          <t>1.675</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.6916</t>
+          <t>1.9558</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.631</t>
+          <t>1.886</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.755</t>
+          <t>2.029</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6920</t>
+          <t>1.8148</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.717</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.789</t>
+          <t>1.919</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3836</t>
+          <t>1.3536</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.536</t>
+          <t>1.502</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.9049</t>
+          <t>1.4626</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.563</t>
+          <t>1.199</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.321</t>
+          <t>1.784</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2708</t>
+          <t>1.3922</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.778</t>
+          <t>1.945</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.3440</t>
+          <t>0.6550</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.229</t>
+          <t>0.438</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.517</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.6347</t>
+          <t>2.0453</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.668</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.002</t>
+          <t>4.959</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.1674</t>
+          <t>3.2189</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>31.674</t>
+          <t>32.189</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1176</t>
+          <t>1.1229</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.073</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>1.170</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.2358</t>
+          <t>1.3173</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.131</t>
+          <t>1.206</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.350</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4689</t>
+          <t>1.5726</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.403</t>
+          <t>1.502</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.647</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0219</t>
+          <t>0.9876</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.928</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9095</t>
+          <t>0.8758</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.797</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0602</t>
+          <t>0.9202</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.813</t>
+          <t>0.705</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.200</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.9885</t>
+          <t>0.8828</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.634</t>
+          <t>0.567</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.541</t>
+          <t>1.374</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.2263</t>
+          <t>0.4000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.108</t>
+          <t>0.192</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.474</t>
+          <t>0.833</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.7738</t>
+          <t>1.0896</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>7.738</t>
+          <t>10.896</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0814</t>
+          <t>1.1929</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.160</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9338</t>
+          <t>0.9462</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.855</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0141</t>
+          <t>1.0840</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>1.025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.146</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1232</t>
+          <t>1.2713</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.213</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2476</t>
+          <t>1.3714</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.299</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.448</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1305</t>
+          <t>1.3244</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.438</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0609</t>
+          <t>1.2309</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.388</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.6321</t>
+          <t>0.8595</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.505</t>
+          <t>0.687</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.792</t>
+          <t>1.075</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.5740</t>
+          <t>3.9998</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.456</t>
+          <t>1.642</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>8.775</t>
+          <t>9.745</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.4953</t>
+          <t>1.0927</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.196</t>
+          <t>0.443</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>2.696</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1986</t>
+          <t>1.3704</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.341</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.225</t>
+          <t>1.400</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8674</t>
+          <t>1.0828</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>1.019</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.922</t>
+          <t>1.151</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0733</t>
+          <t>1.2331</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.189</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2762</t>
+          <t>1.4916</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.230</t>
+          <t>1.438</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.547</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.5182</t>
+          <t>1.6234</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.437</t>
+          <t>1.537</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>1.715</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3526</t>
+          <t>1.3924</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.255</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.501</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2546</t>
+          <t>1.4244</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.204</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.485</t>
+          <t>1.685</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9778</t>
+          <t>1.2366</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.683</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9727</t>
+          <t>1.0700</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.672</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.551</t>
+          <t>1.704</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1109</t>
+          <t>1.1812</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.450</t>
+          <t>0.479</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.740</t>
+          <t>2.914</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1084</t>
+          <t>1.1487</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.182</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9289</t>
+          <t>1.1443</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>1.037</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.262</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0584</t>
+          <t>1.1375</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.004</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.199</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1362</t>
+          <t>1.1733</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.229</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2169</t>
+          <t>1.1838</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.263</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.1965</t>
+          <t>1.0514</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.063</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.347</t>
+          <t>1.183</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1826</t>
+          <t>1.1572</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.5469</t>
+          <t>1.4386</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.081</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.214</t>
+          <t>2.052</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.2722</t>
+          <t>0.2675</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.101</t>
+          <t>0.100</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.731</t>
+          <t>0.713</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2.2428</t>
+          <t>1.0810</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.638</t>
+          <t>0.312</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7.890</t>
+          <t>3.739</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0350</t>
+          <t>1.0689</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>1.023</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.117</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.3341</t>
+          <t>1.2860</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.627</t>
+          <t>1.568</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1327</t>
+          <t>1.1245</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8772</t>
+          <t>0.9575</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>1.030</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2184</t>
+          <t>1.1957</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.087</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.315</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9983</t>
+          <t>0.9700</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>0.852</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.104</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.7500</t>
+          <t>0.9634</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.631</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>1.143</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7943</t>
+          <t>1.0706</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.595</t>
+          <t>0.803</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.427</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.6889</t>
+          <t>1.1050</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.445</t>
+          <t>0.719</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.699</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2.0390</t>
+          <t>1.7519</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.830</t>
+          <t>0.706</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5.010</t>
+          <t>4.345</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0718</t>
+          <t>1.0605</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.037</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0736</t>
+          <t>0.9535</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.995</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.158</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0693</t>
+          <t>1.0785</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.026</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9997</t>
+          <t>1.0149</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.040</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2589</t>
+          <t>1.1590</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.101</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.325</t>
+          <t>1.220</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9935</t>
+          <t>1.0527</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.918</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1055</t>
+          <t>1.1585</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>1.036</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.295</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0913</t>
+          <t>1.1282</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.319</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.6620</t>
+          <t>1.3582</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.235</t>
+          <t>1.832</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.6744</t>
+          <t>1.4233</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>0.968</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.459</t>
+          <t>2.093</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0355</t>
+          <t>0.9921</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.949</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.037</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.8047</t>
+          <t>0.7415</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.658</t>
+          <t>0.606</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.907</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9440</t>
+          <t>0.9591</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.865</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.046</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1396</t>
+          <t>1.0599</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0332</t>
+          <t>0.9693</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.068</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9952</t>
+          <t>1.0853</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.4739</t>
+          <t>1.2025</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.006</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.764</t>
+          <t>1.437</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.3740</t>
+          <t>1.0537</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>0.774</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.873</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2.4128</t>
+          <t>1.2292</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.512</t>
+          <t>0.773</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3.851</t>
+          <t>1.954</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8212</t>
+          <t>0.8124</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.326</t>
+          <t>0.320</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2.067</t>
+          <t>2.065</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6281</t>
+          <t>1.6880</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.596</t>
+          <t>1.655</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.661</t>
+          <t>1.722</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.4961</t>
+          <t>1.4012</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.317</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.592</t>
+          <t>1.490</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.5511</t>
+          <t>1.6389</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.498</t>
+          <t>1.582</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.607</t>
+          <t>1.697</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.7160</t>
+          <t>1.8140</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.657</t>
+          <t>1.751</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.778</t>
+          <t>1.879</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7316</t>
+          <t>1.7760</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.653</t>
+          <t>1.696</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.814</t>
+          <t>1.860</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.3366</t>
+          <t>1.4229</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.6958</t>
+          <t>1.6409</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.498</t>
+          <t>1.449</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.919</t>
+          <t>1.858</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.3538</t>
+          <t>1.1953</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>0.971</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.663</t>
+          <t>1.471</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.6497</t>
+          <t>1.4701</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.011</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2.392</t>
+          <t>2.139</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>3.4111</t>
+          <t>1.0949</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2.008</t>
+          <t>0.627</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>5.795</t>
+          <t>1.912</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5190</t>
+          <t>1.5917</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.488</t>
+          <t>1.559</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.551</t>
+          <t>1.625</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.3936</t>
+          <t>1.4695</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.369</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.496</t>
+          <t>1.577</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.4506</t>
+          <t>1.5195</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.464</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.505</t>
+          <t>1.577</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.7165</t>
+          <t>1.7873</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.658</t>
+          <t>1.726</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.777</t>
+          <t>1.851</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.3756</t>
+          <t>1.5324</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.458</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.610</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3454</t>
+          <t>1.3517</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.243</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.470</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.5340</t>
+          <t>1.4165</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.239</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.753</t>
+          <t>1.619</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.2405</t>
+          <t>1.0595</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.340</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.9926</t>
+          <t>1.0824</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.660</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.493</t>
+          <t>1.635</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2.0372</t>
+          <t>0.7693</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.152</t>
+          <t>0.424</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>3.603</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -3393,17 +3393,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2803</t>
+          <t>1.3201</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.281</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.361</t>
         </is>
       </c>
     </row>
@@ -3416,17 +3416,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.6084</t>
+          <t>1.4970</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.368</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.760</t>
+          <t>1.638</t>
         </is>
       </c>
     </row>
@@ -3439,17 +3439,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1660</t>
+          <t>1.2118</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.154</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3462,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1762</t>
+          <t>1.2986</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.235</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.3796</t>
+          <t>1.4239</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.289</t>
+          <t>1.330</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.477</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -3508,17 +3508,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.3576</t>
+          <t>1.5274</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.166</t>
+          <t>1.312</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.581</t>
+          <t>1.778</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.1916</t>
+          <t>2.0696</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.328</t>
+          <t>1.503</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4.376</t>
+          <t>2.849</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3554,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.5789</t>
+          <t>0.7346</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>0.516</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.217</t>
+          <t>1.045</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3577,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.6202</t>
+          <t>0.6613</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.362</t>
+          <t>0.386</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>1.133</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.1845</t>
+          <t>4.2108</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>41.845</t>
+          <t>42.108</t>
         </is>
       </c>
     </row>
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.4554</t>
+          <t>1.4465</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.377</t>
+          <t>1.369</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.528</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0434</t>
+          <t>1.1299</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.455</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2819</t>
+          <t>1.3817</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.241</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.427</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6093</t>
+          <t>1.5873</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.467</t>
+          <t>1.448</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.765</t>
+          <t>1.740</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4526</t>
+          <t>1.4909</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.626</t>
+          <t>1.669</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1731</t>
+          <t>1.3669</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.431</t>
+          <t>1.668</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5.0675</t>
+          <t>2.3933</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3.583</t>
+          <t>1.687</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>7.168</t>
+          <t>3.395</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.4727</t>
+          <t>0.4435</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>0.272</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.392</t>
+          <t>0.724</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.5354</t>
+          <t>0.9133</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.804</t>
+          <t>0.480</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.932</t>
+          <t>1.738</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.9146</t>
+          <t>3.8273</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>49.146</t>
+          <t>38.273</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2608</t>
+          <t>1.3020</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.222</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.301</t>
+          <t>1.344</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0473</t>
+          <t>1.0790</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.172</t>
+          <t>1.208</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.2647</t>
+          <t>1.2837</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.201</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.352</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2496</t>
+          <t>1.3089</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.243</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.378</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0942</t>
+          <t>1.3016</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.212</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.175</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.4547</t>
+          <t>1.5054</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.288</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.701</t>
+          <t>1.760</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>3.5269</t>
+          <t>2.1529</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.565</t>
+          <t>1.559</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4.850</t>
+          <t>2.973</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.6784</t>
+          <t>0.7758</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>0.539</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.385</t>
+          <t>1.116</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.8258</t>
+          <t>0.9312</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.480</t>
+          <t>0.541</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.604</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3.5630</t>
+          <t>5.0326</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>35.630</t>
+          <t>50.326</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.2465</t>
+          <t>1.2474</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.215</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.281</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.3231</t>
+          <t>1.3400</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.223</t>
+          <t>1.239</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.431</t>
+          <t>1.449</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.1708</t>
+          <t>1.1606</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.126</t>
+          <t>1.117</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.1573</t>
+          <t>1.2272</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.179</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.3080</t>
+          <t>1.3146</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.230</t>
+          <t>1.237</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.390</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.3794</t>
+          <t>1.4505</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.250</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.684</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2.9288</t>
+          <t>1.8937</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2.136</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>4.017</t>
+          <t>2.608</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.7269</t>
+          <t>0.8047</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>0.560</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2.450</t>
+          <t>1.156</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.6454</t>
+          <t>0.8414</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.372</t>
+          <t>0.485</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.461</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>3.7594</t>
+          <t>4.9744</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>37.594</t>
+          <t>49.744</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new Czech slope normalization is awesome.
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.5019</t>
+          <t>1.3906</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.352</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.544</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1943</t>
+          <t>0.9549</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>0.881</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.035</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2437</t>
+          <t>1.1517</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.8376</t>
+          <t>1.6773</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.773</t>
+          <t>1.618</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.905</t>
+          <t>1.739</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5456</t>
+          <t>1.5238</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.419</t>
+          <t>1.399</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.683</t>
+          <t>1.659</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.5770</t>
+          <t>1.5195</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.130</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.120</t>
+          <t>2.043</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6376</t>
+          <t>1.6303</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.872</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.062</t>
+          <t>3.048</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8.0955</t>
+          <t>7.9660</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>80.955</t>
+          <t>79.660</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.6879</t>
+          <t>1.5633</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.634</t>
+          <t>1.513</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.744</t>
+          <t>1.615</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.5732</t>
+          <t>1.2579</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.478</t>
+          <t>1.182</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.675</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.9558</t>
+          <t>1.8112</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.886</t>
+          <t>1.746</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2.029</t>
+          <t>1.879</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.8148</t>
+          <t>1.6564</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.717</t>
+          <t>1.567</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.919</t>
+          <t>1.751</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3536</t>
+          <t>1.3345</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.202</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3922</t>
+          <t>1.3414</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.945</t>
+          <t>1.875</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6550</t>
+          <t>0.6520</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.438</t>
+          <t>0.436</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.2189</t>
+          <t>3.1674</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>32.189</t>
+          <t>31.674</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1929</t>
+          <t>1.0948</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.160</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.126</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9462</t>
+          <t>0.9336</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.844</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.033</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0840</t>
+          <t>1.0134</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2713</t>
+          <t>1.1255</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.074</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.3714</t>
+          <t>1.2537</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.187</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.3244</t>
+          <t>1.2049</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.308</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2309</t>
+          <t>1.1353</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.388</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8595</t>
+          <t>0.8069</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.645</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.009</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.0927</t>
+          <t>0.9435</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.443</t>
+          <t>0.383</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.696</t>
+          <t>2.327</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3704</t>
+          <t>1.2577</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.341</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.400</t>
+          <t>1.285</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0828</t>
+          <t>1.0684</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.005</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2331</t>
+          <t>1.1528</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.112</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.4916</t>
+          <t>1.3206</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.6234</t>
+          <t>1.4842</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.537</t>
+          <t>1.405</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.568</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3924</t>
+          <t>1.2668</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.255</t>
+          <t>1.142</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.405</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.4244</t>
+          <t>1.3137</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.204</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.685</t>
+          <t>1.554</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2366</t>
+          <t>1.1608</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.683</t>
+          <t>1.580</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1812</t>
+          <t>1.0200</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.479</t>
+          <t>0.414</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.914</t>
+          <t>2.516</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0689</t>
+          <t>1.0464</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.094</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9575</t>
+          <t>0.9128</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9634</t>
+          <t>0.8771</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.739</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0706</t>
+          <t>0.9461</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.710</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.427</t>
+          <t>1.261</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1050</t>
+          <t>0.9657</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>0.628</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.699</t>
+          <t>1.484</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0605</t>
+          <t>1.0382</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.062</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0149</t>
+          <t>0.9674</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>0.930</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1585</t>
+          <t>1.0548</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>0.944</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.295</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.1282</t>
+          <t>0.9969</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.3582</t>
+          <t>1.1870</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>0.881</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.832</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6880</t>
+          <t>1.6525</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>1.620</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.722</t>
+          <t>1.686</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.8140</t>
+          <t>1.7291</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.751</t>
+          <t>1.669</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.879</t>
+          <t>1.791</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.6409</t>
+          <t>1.4940</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.320</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.858</t>
+          <t>1.691</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1953</t>
+          <t>1.0562</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.859</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.299</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.4701</t>
+          <t>1.2848</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2.139</t>
+          <t>1.868</t>
         </is>
       </c>
     </row>
@@ -3393,17 +3393,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3201</t>
+          <t>1.2823</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.361</t>
+          <t>1.322</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3462,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2986</t>
+          <t>1.2202</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.283</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4239</t>
+          <t>1.4155</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.322</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.515</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.0696</t>
+          <t>1.8479</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.503</t>
+          <t>1.342</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.849</t>
+          <t>2.544</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3554,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7346</t>
+          <t>0.6339</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.516</t>
+          <t>0.446</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>0.901</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3577,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.6613</t>
+          <t>0.5545</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.386</t>
+          <t>0.324</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.133</t>
+          <t>0.950</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.2108</t>
+          <t>3.9484</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>42.108</t>
+          <t>39.484</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
NEW SLOPE METHOD WORKED
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3906</t>
+          <t>1.3509</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.314</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.389</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9549</t>
+          <t>1.1593</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>1.070</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.257</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1517</t>
+          <t>1.0564</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.198</t>
+          <t>1.099</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6773</t>
+          <t>1.5362</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.618</t>
+          <t>1.482</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.739</t>
+          <t>1.592</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5238</t>
+          <t>1.5418</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.416</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.659</t>
+          <t>1.679</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5894</t>
+          <t>1.9595</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.633</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.906</t>
+          <t>2.351</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.5195</t>
+          <t>0.8338</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.130</t>
+          <t>0.623</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.043</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6303</t>
+          <t>3.8202</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>2.035</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.048</t>
+          <t>7.171</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.7281</t>
+          <t>0.6522</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>17.281</t>
+          <t>6.522</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.9660</t>
+          <t>15.6989</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>79.660</t>
+          <t>156.989</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5633</t>
+          <t>1.3126</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.513</t>
+          <t>1.271</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.615</t>
+          <t>1.356</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.2579</t>
+          <t>0.8255</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.339</t>
+          <t>0.878</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.8112</t>
+          <t>1.6200</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.746</t>
+          <t>1.562</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.879</t>
+          <t>1.680</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6564</t>
+          <t>1.5608</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.476</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.751</t>
+          <t>1.650</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3345</t>
+          <t>0.7137</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>0.644</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>0.791</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.4626</t>
+          <t>2.0646</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.691</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.784</t>
+          <t>2.521</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3414</t>
+          <t>1.8872</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>1.348</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.875</t>
+          <t>2.642</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6520</t>
+          <t>1.5912</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.436</t>
+          <t>1.061</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>2.386</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.0453</t>
+          <t>0.3335</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.139</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.959</t>
+          <t>0.799</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.1674</t>
+          <t>6.2421</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>31.674</t>
+          <t>62.421</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1229</t>
+          <t>0.9772</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.018</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3173</t>
+          <t>0.7121</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>0.652</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>0.778</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5726</t>
+          <t>1.5334</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>1.465</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.647</t>
+          <t>1.606</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9876</t>
+          <t>1.0160</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.928</t>
+          <t>0.954</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.8758</t>
+          <t>0.4629</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.767</t>
+          <t>0.406</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.528</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9202</t>
+          <t>1.0537</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.376</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8828</t>
+          <t>2.2634</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.567</t>
+          <t>1.457</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>3.516</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4000</t>
+          <t>0.4165</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.192</t>
+          <t>0.199</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.873</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.0896</t>
+          <t>0.4971</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10.896</t>
+          <t>4.971</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0948</t>
+          <t>1.0220</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>0.994</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.126</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9336</t>
+          <t>1.6093</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>1.453</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.782</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0134</t>
+          <t>0.7304</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>0.691</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>0.772</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1255</t>
+          <t>1.2363</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.180</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.296</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2537</t>
+          <t>1.1702</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.235</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2049</t>
+          <t>0.7018</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>0.647</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>0.762</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1353</t>
+          <t>0.9530</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>0.845</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8069</t>
+          <t>0.5019</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.645</t>
+          <t>0.403</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>0.625</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.9998</t>
+          <t>1.2168</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.642</t>
+          <t>0.499</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>9.745</t>
+          <t>2.966</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.9435</t>
+          <t>6.6490</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.383</t>
+          <t>2.673</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.327</t>
+          <t>16.540</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.2577</t>
+          <t>1.1487</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.285</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0684</t>
+          <t>1.1116</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.1528</t>
+          <t>0.8410</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>0.872</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3206</t>
+          <t>1.2780</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.370</t>
+          <t>1.326</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4842</t>
+          <t>1.5048</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.425</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.568</t>
+          <t>1.590</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2668</t>
+          <t>1.5611</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.406</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.733</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3137</t>
+          <t>1.1042</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.554</t>
+          <t>1.306</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.1608</t>
+          <t>2.1261</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>1.561</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>2.896</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.0700</t>
+          <t>0.4298</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.672</t>
+          <t>0.271</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.704</t>
+          <t>0.682</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0200</t>
+          <t>2.0936</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.414</t>
+          <t>0.850</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.516</t>
+          <t>5.159</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1487</t>
+          <t>1.1240</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.1443</t>
+          <t>0.6907</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>0.626</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>0.763</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1375</t>
+          <t>1.1515</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.214</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1733</t>
+          <t>1.0337</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.229</t>
+          <t>1.083</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.1838</t>
+          <t>1.2860</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.206</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.263</t>
+          <t>1.372</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0514</t>
+          <t>2.2246</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>1.977</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.183</t>
+          <t>2.504</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1572</t>
+          <t>1.1587</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.400</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.4386</t>
+          <t>4.2360</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>2.973</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.052</t>
+          <t>6.035</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.2675</t>
+          <t>0.3532</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.100</t>
+          <t>0.133</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>0.940</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0810</t>
+          <t>0.3149</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.312</t>
+          <t>0.090</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.739</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0464</t>
+          <t>1.1220</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.074</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.172</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2860</t>
+          <t>0.8176</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>0.674</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.568</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1245</t>
+          <t>1.2319</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.129</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.344</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9128</t>
+          <t>0.8681</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.934</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1957</t>
+          <t>1.4653</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.331</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.315</t>
+          <t>1.613</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9700</t>
+          <t>1.7452</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.852</t>
+          <t>1.529</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>1.992</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8771</t>
+          <t>1.9465</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.739</t>
+          <t>1.635</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>2.318</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9461</t>
+          <t>2.0873</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.710</t>
+          <t>1.557</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>2.798</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9657</t>
+          <t>1.3405</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.628</t>
+          <t>0.869</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.484</t>
+          <t>2.068</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.7519</t>
+          <t>3.1262</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>1.270</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.345</t>
+          <t>7.696</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0382</t>
+          <t>1.0198</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9535</t>
+          <t>0.8228</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.763</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.887</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0785</t>
+          <t>0.9352</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>0.897</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>0.975</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9674</t>
+          <t>1.0959</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>1.054</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1590</t>
+          <t>1.0842</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.030</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0527</t>
+          <t>0.9069</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.838</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0548</t>
+          <t>1.1798</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.319</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9969</t>
+          <t>1.0963</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.908</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.323</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1870</t>
+          <t>3.6832</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>2.715</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>4.997</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4233</t>
+          <t>4.2188</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>2.879</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.093</t>
+          <t>6.182</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9921</t>
+          <t>0.9089</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.870</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>0.950</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.7415</t>
+          <t>1.0064</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.828</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>1.224</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9591</t>
+          <t>0.7592</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.695</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>0.829</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0599</t>
+          <t>1.2623</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>1.174</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.358</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9693</t>
+          <t>0.7399</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.671</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>0.816</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0853</t>
+          <t>0.5197</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.454</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>0.595</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.2025</t>
+          <t>0.6061</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>0.505</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.437</t>
+          <t>0.727</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.0537</t>
+          <t>0.5252</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.774</t>
+          <t>0.384</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>0.719</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.2292</t>
+          <t>2.7476</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.773</t>
+          <t>1.714</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.954</t>
+          <t>4.404</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8124</t>
+          <t>1.3495</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.320</t>
+          <t>0.532</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2.065</t>
+          <t>3.420</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6525</t>
+          <t>1.6293</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.620</t>
+          <t>1.597</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.686</t>
+          <t>1.662</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.4012</t>
+          <t>1.4330</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.347</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.6389</t>
+          <t>1.4447</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.582</t>
+          <t>1.395</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.697</t>
+          <t>1.496</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.7291</t>
+          <t>1.8425</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.779</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.791</t>
+          <t>1.908</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7760</t>
+          <t>1.7557</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.696</t>
+          <t>1.676</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.860</t>
+          <t>1.839</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4229</t>
+          <t>1.5044</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.392</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.626</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.4940</t>
+          <t>1.4376</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.270</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.691</t>
+          <t>1.627</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0562</t>
+          <t>1.0735</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.318</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2848</t>
+          <t>0.9452</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.654</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>1.366</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0949</t>
+          <t>0.8850</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.627</t>
+          <t>0.518</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.912</t>
+          <t>1.513</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5917</t>
+          <t>1.5977</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.565</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.625</t>
+          <t>1.631</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.4695</t>
+          <t>1.7415</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.623</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.869</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.5195</t>
+          <t>1.5448</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.489</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.603</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.7873</t>
+          <t>1.6813</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.726</t>
+          <t>1.624</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.851</t>
+          <t>1.741</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.5324</t>
+          <t>1.6193</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.541</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.610</t>
+          <t>1.701</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3517</t>
+          <t>1.6588</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.526</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.804</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.4165</t>
+          <t>1.2186</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.066</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.619</t>
+          <t>1.393</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0595</t>
+          <t>0.9792</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.0824</t>
+          <t>0.2566</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.170</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>0.388</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7693</t>
+          <t>0.2098</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.424</t>
+          <t>0.117</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>0.376</t>
         </is>
       </c>
     </row>
@@ -3393,17 +3393,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2823</t>
+          <t>1.1551</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.121</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.322</t>
+          <t>1.190</t>
         </is>
       </c>
     </row>
@@ -3416,17 +3416,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.4970</t>
+          <t>1.8015</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.368</t>
+          <t>1.646</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.638</t>
+          <t>1.971</t>
         </is>
       </c>
     </row>
@@ -3439,17 +3439,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2118</t>
+          <t>0.8489</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.154</t>
+          <t>0.809</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>0.891</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3462,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2202</t>
+          <t>1.2149</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.156</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4155</t>
+          <t>1.2039</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.322</t>
+          <t>1.125</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.515</t>
+          <t>1.288</t>
         </is>
       </c>
     </row>
@@ -3508,17 +3508,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5274</t>
+          <t>1.5648</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.344</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.778</t>
+          <t>1.821</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.8479</t>
+          <t>2.3385</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.696</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.544</t>
+          <t>3.225</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3554,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.6339</t>
+          <t>1.4439</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.446</t>
+          <t>1.012</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>2.060</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3577,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.5545</t>
+          <t>0.7234</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.324</t>
+          <t>0.423</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>1.238</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.9484</t>
+          <t>9.5750</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>39.484</t>
+          <t>95.750</t>
         </is>
       </c>
     </row>
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.4465</t>
+          <t>1.1034</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.044</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.528</t>
+          <t>1.166</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1299</t>
+          <t>2.6423</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>2.064</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>3.382</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3817</t>
+          <t>0.8357</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>0.931</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.5873</t>
+          <t>1.4639</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>1.335</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.740</t>
+          <t>1.605</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4909</t>
+          <t>1.0665</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.194</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3669</t>
+          <t>0.6444</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>0.527</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.668</t>
+          <t>0.788</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2.3933</t>
+          <t>0.9549</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.687</t>
+          <t>0.670</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3.395</t>
+          <t>1.360</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.4435</t>
+          <t>0.4320</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.272</t>
+          <t>0.263</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>0.709</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9133</t>
+          <t>0.2292</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.480</t>
+          <t>0.119</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.738</t>
+          <t>0.441</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.8273</t>
+          <t>4.1025</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>38.273</t>
+          <t>41.025</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.3020</t>
+          <t>1.1947</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.158</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.233</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0790</t>
+          <t>1.2090</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>1.080</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>1.354</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.2837</t>
+          <t>1.0871</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.144</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.3089</t>
+          <t>1.1065</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.165</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3016</t>
+          <t>1.2195</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.136</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.309</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.5054</t>
+          <t>1.9446</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.664</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.760</t>
+          <t>2.272</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.1529</t>
+          <t>2.6442</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.911</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.973</t>
+          <t>3.658</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.7758</t>
+          <t>1.7315</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.539</t>
+          <t>1.200</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>2.498</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9312</t>
+          <t>0.3904</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.541</t>
+          <t>0.226</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>0.674</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>5.0326</t>
+          <t>4.1678</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>50.326</t>
+          <t>41.678</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.2474</t>
+          <t>1.0765</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.215</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.105</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.3400</t>
+          <t>1.7862</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.651</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.932</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.1606</t>
+          <t>0.8624</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>0.830</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>0.896</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2272</t>
+          <t>1.0631</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.021</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.107</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.3146</t>
+          <t>1.0367</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.102</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4505</t>
+          <t>1.4325</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.234</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.684</t>
+          <t>1.663</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.8937</t>
+          <t>2.4178</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>1.752</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2.608</t>
+          <t>3.336</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.8047</t>
+          <t>1.8669</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.560</t>
+          <t>1.296</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>2.689</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8414</t>
+          <t>0.6681</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.485</t>
+          <t>0.384</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.161</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>4.9744</t>
+          <t>7.1111</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>49.744</t>
+          <t>71.111</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
code updated to new version and new normalization. added cohorts to booster so all 6 there. Logs are the logs from the successful run before removing old code
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3509</t>
+          <t>1.3906</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.314</t>
+          <t>1.352</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.389</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1593</t>
+          <t>0.9549</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.070</t>
+          <t>0.881</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.257</t>
+          <t>1.035</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0564</t>
+          <t>1.1517</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.099</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.5362</t>
+          <t>1.6773</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.482</t>
+          <t>1.618</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.592</t>
+          <t>1.739</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5418</t>
+          <t>1.5238</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.416</t>
+          <t>1.399</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.679</t>
+          <t>1.659</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.9595</t>
+          <t>1.5894</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.633</t>
+          <t>1.326</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.351</t>
+          <t>1.906</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8338</t>
+          <t>1.5195</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.623</t>
+          <t>1.130</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>2.043</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3.8202</t>
+          <t>1.6303</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.035</t>
+          <t>0.872</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7.171</t>
+          <t>3.048</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.6522</t>
+          <t>1.7281</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6.522</t>
+          <t>17.281</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>15.6989</t>
+          <t>7.9660</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>156.989</t>
+          <t>79.660</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3126</t>
+          <t>1.5633</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.271</t>
+          <t>1.513</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.356</t>
+          <t>1.615</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8255</t>
+          <t>1.2579</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.776</t>
+          <t>1.182</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.6200</t>
+          <t>1.8112</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.562</t>
+          <t>1.746</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.680</t>
+          <t>1.879</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.5608</t>
+          <t>1.6564</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.476</t>
+          <t>1.567</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.650</t>
+          <t>1.751</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.7137</t>
+          <t>1.3345</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.644</t>
+          <t>1.202</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.791</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2.0646</t>
+          <t>1.4626</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.691</t>
+          <t>1.199</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.521</t>
+          <t>1.784</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.8872</t>
+          <t>1.3414</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.348</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2.642</t>
+          <t>1.875</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.5912</t>
+          <t>0.6520</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>0.436</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.386</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.3335</t>
+          <t>2.0453</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.139</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.799</t>
+          <t>4.959</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>6.2421</t>
+          <t>3.1674</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>62.421</t>
+          <t>31.674</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9772</t>
+          <t>1.1229</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.018</t>
+          <t>1.170</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.7121</t>
+          <t>1.3173</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.652</t>
+          <t>1.206</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.778</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5334</t>
+          <t>1.5726</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.465</t>
+          <t>1.502</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.606</t>
+          <t>1.647</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0160</t>
+          <t>0.9876</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.928</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.4629</t>
+          <t>0.8758</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.406</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.528</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0537</t>
+          <t>0.9202</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.807</t>
+          <t>0.705</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.376</t>
+          <t>1.200</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.2634</t>
+          <t>0.8828</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.457</t>
+          <t>0.567</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3.516</t>
+          <t>1.374</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4165</t>
+          <t>0.4000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.199</t>
+          <t>0.192</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.873</t>
+          <t>0.833</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.4971</t>
+          <t>1.0896</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4.971</t>
+          <t>10.896</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0220</t>
+          <t>1.0948</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.994</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.126</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.6093</t>
+          <t>0.9336</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>0.844</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.782</t>
+          <t>1.033</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.7304</t>
+          <t>1.0134</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.691</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.772</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2363</t>
+          <t>1.1255</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.074</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.296</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1702</t>
+          <t>1.2537</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.187</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.7018</t>
+          <t>1.2049</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.647</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.762</t>
+          <t>1.308</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9530</t>
+          <t>1.1353</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.845</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.5019</t>
+          <t>0.8069</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.403</t>
+          <t>0.645</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>1.009</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.2168</t>
+          <t>3.9998</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.499</t>
+          <t>1.642</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2.966</t>
+          <t>9.745</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.6490</t>
+          <t>0.9435</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.673</t>
+          <t>0.383</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>16.540</t>
+          <t>2.327</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1487</t>
+          <t>1.2577</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.285</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1116</t>
+          <t>1.0684</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.005</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8410</t>
+          <t>1.1528</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>1.112</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2780</t>
+          <t>1.3206</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.5048</t>
+          <t>1.4842</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.425</t>
+          <t>1.405</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.590</t>
+          <t>1.568</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.5611</t>
+          <t>1.2668</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.142</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.733</t>
+          <t>1.405</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1042</t>
+          <t>1.3137</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.306</t>
+          <t>1.554</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2.1261</t>
+          <t>1.1608</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.561</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.896</t>
+          <t>1.580</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.4298</t>
+          <t>1.0700</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.271</t>
+          <t>0.672</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.682</t>
+          <t>1.704</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.0936</t>
+          <t>1.0200</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.414</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5.159</t>
+          <t>2.516</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1240</t>
+          <t>1.1487</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.182</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.6907</t>
+          <t>1.1443</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.626</t>
+          <t>1.037</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>1.262</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1515</t>
+          <t>1.1375</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.199</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0337</t>
+          <t>1.1733</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.229</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2860</t>
+          <t>1.1838</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.372</t>
+          <t>1.263</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2.2246</t>
+          <t>1.0514</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.977</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.504</t>
+          <t>1.183</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1587</t>
+          <t>1.1572</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.400</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4.2360</t>
+          <t>1.4386</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.973</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>6.035</t>
+          <t>2.052</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.3532</t>
+          <t>0.2675</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.133</t>
+          <t>0.100</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>0.713</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.3149</t>
+          <t>1.0810</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.090</t>
+          <t>0.312</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>3.739</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1220</t>
+          <t>1.0464</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.172</t>
+          <t>1.094</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8176</t>
+          <t>1.2860</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.674</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>1.568</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2319</t>
+          <t>1.1245</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8681</t>
+          <t>0.9128</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.807</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4653</t>
+          <t>1.1957</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.331</t>
+          <t>1.087</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.613</t>
+          <t>1.315</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.7452</t>
+          <t>0.9700</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.529</t>
+          <t>0.852</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.992</t>
+          <t>1.104</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.9465</t>
+          <t>0.8771</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>0.739</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.318</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2.0873</t>
+          <t>0.9461</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.557</t>
+          <t>0.710</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.798</t>
+          <t>1.261</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3405</t>
+          <t>0.9657</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.869</t>
+          <t>0.628</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2.068</t>
+          <t>1.484</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.1262</t>
+          <t>1.7519</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>0.706</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>7.696</t>
+          <t>4.345</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0198</t>
+          <t>1.0382</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.062</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8228</t>
+          <t>0.9535</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.9352</t>
+          <t>1.0785</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.975</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0959</t>
+          <t>0.9674</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.054</t>
+          <t>0.930</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0842</t>
+          <t>1.1590</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.101</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.220</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9069</t>
+          <t>1.0527</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.838</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1798</t>
+          <t>1.0548</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>0.944</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.319</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0963</t>
+          <t>0.9969</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.323</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>3.6832</t>
+          <t>1.1870</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2.715</t>
+          <t>0.881</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.997</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.2188</t>
+          <t>1.4233</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2.879</t>
+          <t>0.968</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>6.182</t>
+          <t>2.093</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9089</t>
+          <t>0.9921</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>0.949</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>1.037</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0064</t>
+          <t>0.7415</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.828</t>
+          <t>0.606</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>0.907</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.7592</t>
+          <t>0.9591</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.695</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.829</t>
+          <t>1.046</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2623</t>
+          <t>1.0599</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>0.985</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.358</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.7399</t>
+          <t>0.9693</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.671</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>1.068</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.5197</t>
+          <t>1.0853</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.454</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.595</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.6061</t>
+          <t>1.2025</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.505</t>
+          <t>1.006</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.727</t>
+          <t>1.437</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.5252</t>
+          <t>1.0537</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.384</t>
+          <t>0.774</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2.7476</t>
+          <t>1.2292</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.714</t>
+          <t>0.773</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4.404</t>
+          <t>1.954</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.3495</t>
+          <t>0.8124</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.532</t>
+          <t>0.320</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.420</t>
+          <t>2.065</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6293</t>
+          <t>1.6525</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.597</t>
+          <t>1.620</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.662</t>
+          <t>1.686</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.4330</t>
+          <t>1.4012</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.347</t>
+          <t>1.317</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.490</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.4447</t>
+          <t>1.6389</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.395</t>
+          <t>1.582</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.496</t>
+          <t>1.697</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.8425</t>
+          <t>1.7291</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.779</t>
+          <t>1.669</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.908</t>
+          <t>1.791</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7557</t>
+          <t>1.7760</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.676</t>
+          <t>1.696</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.839</t>
+          <t>1.860</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.5044</t>
+          <t>1.4229</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.392</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.626</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.4376</t>
+          <t>1.4940</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>1.320</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.627</t>
+          <t>1.691</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0735</t>
+          <t>1.0562</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.859</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.318</t>
+          <t>1.299</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.9452</t>
+          <t>1.2848</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.654</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.366</t>
+          <t>1.868</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.8850</t>
+          <t>1.0949</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.518</t>
+          <t>0.627</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.513</t>
+          <t>1.912</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5977</t>
+          <t>1.5917</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.565</t>
+          <t>1.559</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.631</t>
+          <t>1.625</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.7415</t>
+          <t>1.4695</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.623</t>
+          <t>1.369</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.869</t>
+          <t>1.577</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.5448</t>
+          <t>1.5195</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.489</t>
+          <t>1.464</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.603</t>
+          <t>1.577</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.6813</t>
+          <t>1.7873</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.624</t>
+          <t>1.726</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.741</t>
+          <t>1.851</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.6193</t>
+          <t>1.5324</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.541</t>
+          <t>1.458</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.701</t>
+          <t>1.610</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.6588</t>
+          <t>1.3517</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.526</t>
+          <t>1.243</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.804</t>
+          <t>1.470</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.2186</t>
+          <t>1.4165</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.239</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.393</t>
+          <t>1.619</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.9792</t>
+          <t>1.0595</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.776</t>
+          <t>0.837</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.236</t>
+          <t>1.340</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.2566</t>
+          <t>1.0824</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.170</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.388</t>
+          <t>1.635</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.2098</t>
+          <t>0.7693</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.117</t>
+          <t>0.424</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.376</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -3393,17 +3393,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1551</t>
+          <t>1.2823</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.322</t>
         </is>
       </c>
     </row>
@@ -3416,17 +3416,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.8015</t>
+          <t>1.4970</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.646</t>
+          <t>1.368</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.971</t>
+          <t>1.638</t>
         </is>
       </c>
     </row>
@@ -3439,17 +3439,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8489</t>
+          <t>1.2118</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.809</t>
+          <t>1.154</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3462,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2149</t>
+          <t>1.2202</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.283</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3485,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2039</t>
+          <t>1.4155</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>1.322</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.515</t>
         </is>
       </c>
     </row>
@@ -3508,17 +3508,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5648</t>
+          <t>1.5274</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.312</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.821</t>
+          <t>1.778</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3531,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.3385</t>
+          <t>1.8479</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.696</t>
+          <t>1.342</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3.225</t>
+          <t>2.544</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3554,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.4439</t>
+          <t>0.6339</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>0.446</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.060</t>
+          <t>0.901</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3577,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.7234</t>
+          <t>0.5545</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.423</t>
+          <t>0.324</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>0.950</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9.5750</t>
+          <t>3.9484</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>95.750</t>
+          <t>39.484</t>
         </is>
       </c>
     </row>
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1034</t>
+          <t>1.4465</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.369</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.166</t>
+          <t>1.528</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2.6423</t>
+          <t>1.1299</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2.064</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3.382</t>
+          <t>1.455</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8357</t>
+          <t>1.3817</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>1.241</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>1.538</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.4639</t>
+          <t>1.5873</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.335</t>
+          <t>1.448</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.605</t>
+          <t>1.740</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0665</t>
+          <t>1.4909</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.669</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.6444</t>
+          <t>1.3669</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.527</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>1.668</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9549</t>
+          <t>2.3933</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.670</t>
+          <t>1.687</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.360</t>
+          <t>3.395</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.4320</t>
+          <t>0.4435</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.263</t>
+          <t>0.272</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.709</t>
+          <t>0.724</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.2292</t>
+          <t>0.9133</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.119</t>
+          <t>0.480</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.441</t>
+          <t>1.738</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4.1025</t>
+          <t>3.8273</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>41.025</t>
+          <t>38.273</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1947</t>
+          <t>1.3020</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.158</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.233</t>
+          <t>1.344</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.2090</t>
+          <t>1.0790</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.354</t>
+          <t>1.208</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0871</t>
+          <t>1.2837</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.144</t>
+          <t>1.352</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1065</t>
+          <t>1.3089</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.243</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.378</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2195</t>
+          <t>1.3016</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.212</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.9446</t>
+          <t>1.5054</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.664</t>
+          <t>1.288</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2.272</t>
+          <t>1.760</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.6442</t>
+          <t>2.1529</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.911</t>
+          <t>1.559</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3.658</t>
+          <t>2.973</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.7315</t>
+          <t>0.7758</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>0.539</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.498</t>
+          <t>1.116</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.3904</t>
+          <t>0.9312</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.226</t>
+          <t>0.541</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.674</t>
+          <t>1.604</t>
         </is>
       </c>
     </row>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>4.1678</t>
+          <t>5.0326</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>41.678</t>
+          <t>50.326</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.0765</t>
+          <t>1.2474</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.215</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.105</t>
+          <t>1.281</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.7862</t>
+          <t>1.3400</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.651</t>
+          <t>1.239</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.932</t>
+          <t>1.449</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>0.8624</t>
+          <t>1.1606</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.830</t>
+          <t>1.117</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>0.896</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0631</t>
+          <t>1.2272</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.179</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.0367</t>
+          <t>1.3146</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>1.237</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4325</t>
+          <t>1.4505</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.234</t>
+          <t>1.250</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.663</t>
+          <t>1.684</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2.4178</t>
+          <t>1.8937</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.752</t>
+          <t>1.375</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3.336</t>
+          <t>2.608</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.8669</t>
+          <t>0.8047</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.296</t>
+          <t>0.560</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2.689</t>
+          <t>1.156</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.6681</t>
+          <t>0.8414</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.384</t>
+          <t>0.485</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.461</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>7.1111</t>
+          <t>4.9744</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>71.111</t>
+          <t>49.744</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
KCOR should be nearly clean now
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3906</t>
+          <t>1.5012</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.459</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9549</t>
+          <t>1.1943</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>1.102</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.294</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1517</t>
+          <t>1.2437</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.196</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.198</t>
+          <t>1.293</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6773</t>
+          <t>1.8376</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.618</t>
+          <t>1.773</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.739</t>
+          <t>1.905</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5238</t>
+          <t>1.5456</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.419</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.659</t>
+          <t>1.683</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.5195</t>
+          <t>1.5770</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.130</t>
+          <t>1.173</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.043</t>
+          <t>2.120</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6303</t>
+          <t>1.6376</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>0.876</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.048</t>
+          <t>3.062</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.9660</t>
+          <t>8.0955</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>79.660</t>
+          <t>80.955</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5633</t>
+          <t>1.6843</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.513</t>
+          <t>1.629</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.615</t>
+          <t>1.741</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.2579</t>
+          <t>1.5732</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.478</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.339</t>
+          <t>1.675</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.8112</t>
+          <t>1.9558</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.746</t>
+          <t>1.886</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.879</t>
+          <t>2.029</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6564</t>
+          <t>1.8148</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.717</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.751</t>
+          <t>1.919</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3345</t>
+          <t>1.3536</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.502</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3414</t>
+          <t>1.3922</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.875</t>
+          <t>1.945</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6520</t>
+          <t>0.6550</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.436</t>
+          <t>0.438</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.1674</t>
+          <t>3.2189</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>31.674</t>
+          <t>32.189</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1229</t>
+          <t>1.1203</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>1.075</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.168</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0948</t>
+          <t>1.1956</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.126</t>
+          <t>1.231</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9336</t>
+          <t>0.9462</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.855</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0134</t>
+          <t>1.0840</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>1.025</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.146</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1255</t>
+          <t>1.2713</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.213</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2537</t>
+          <t>1.3714</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.299</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.448</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2049</t>
+          <t>1.3244</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>1.438</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1353</t>
+          <t>1.2309</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.388</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8069</t>
+          <t>0.8595</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.645</t>
+          <t>0.687</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.075</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.9435</t>
+          <t>1.0927</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.383</t>
+          <t>0.443</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.327</t>
+          <t>2.696</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.2577</t>
+          <t>1.3673</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.336</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.285</t>
+          <t>1.399</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0684</t>
+          <t>1.0828</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.019</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.151</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.1528</t>
+          <t>1.2331</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.189</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3206</t>
+          <t>1.4916</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.438</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.370</t>
+          <t>1.547</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4842</t>
+          <t>1.6234</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.537</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.568</t>
+          <t>1.715</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2668</t>
+          <t>1.3924</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.255</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3137</t>
+          <t>1.4244</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>1.204</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.554</t>
+          <t>1.685</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.1608</t>
+          <t>1.2366</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.683</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.0200</t>
+          <t>1.1812</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.414</t>
+          <t>0.479</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.516</t>
+          <t>2.914</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1487</t>
+          <t>1.1436</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.180</t>
         </is>
       </c>
     </row>
@@ -2030,7 +2030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0464</t>
+          <t>1.0673</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.021</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9128</t>
+          <t>0.9575</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>1.030</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8771</t>
+          <t>0.9634</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.739</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.143</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9461</t>
+          <t>1.0706</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.710</t>
+          <t>0.803</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.427</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9657</t>
+          <t>1.1050</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.628</t>
+          <t>0.719</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.484</t>
+          <t>1.699</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0382</t>
+          <t>1.0599</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.036</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9674</t>
+          <t>1.0149</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0548</t>
+          <t>1.1585</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>1.036</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.295</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9969</t>
+          <t>1.1282</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1870</t>
+          <t>1.3582</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.832</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9921</t>
+          <t>0.9931</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6525</t>
+          <t>1.6883</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.620</t>
+          <t>1.655</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.686</t>
+          <t>1.722</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.7291</t>
+          <t>1.8140</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.751</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.791</t>
+          <t>1.879</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.4940</t>
+          <t>1.6409</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.449</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.691</t>
+          <t>1.858</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0562</t>
+          <t>1.1953</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.971</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.471</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.2848</t>
+          <t>1.4701</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>1.011</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>2.139</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3071,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>3 vs 2</t>
+          <t>3 vs 1</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5917</t>
+          <t>1.5819</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.515</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.625</t>
+          <t>1.652</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.4695</t>
+          <t>1.0896</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>0.895</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.326</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.5195</t>
+          <t>1.4574</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.340</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.585</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.7873</t>
+          <t>1.8944</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.726</t>
+          <t>1.764</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.851</t>
+          <t>2.034</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.5324</t>
+          <t>1.4853</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.351</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.610</t>
+          <t>1.633</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3517</t>
+          <t>1.4670</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.285</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.675</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.4165</t>
+          <t>1.7033</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.413</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.619</t>
+          <t>2.053</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0595</t>
+          <t>1.1164</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.536</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.0824</t>
+          <t>1.3305</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.794</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>2.228</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7693</t>
+          <t>0.6250</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.424</t>
+          <t>0.226</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.726</t>
         </is>
       </c>
     </row>
@@ -3315,6 +3315,254 @@
       <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>3 vs 2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>1.5929</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>1.560</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>1.626</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>1.4695</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>1.369</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>1.577</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>1.5195</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>1.464</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>1.577</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>1.7873</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>1.726</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>1.851</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>1.5324</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>1.458</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>1.610</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>1.3517</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>1.243</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1.470</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>1.4165</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>1.239</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1.619</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>1.0595</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0.837</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>1.340</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>1.0824</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0.717</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>1.635</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>0.7693</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0.424</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>1.397</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3393,17 +3641,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2823</t>
+          <t>1.3158</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.276</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.322</t>
+          <t>1.357</t>
         </is>
       </c>
     </row>
@@ -3462,17 +3710,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2202</t>
+          <t>1.2986</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.235</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -3485,17 +3733,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4155</t>
+          <t>1.4239</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.322</t>
+          <t>1.330</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.515</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -3531,17 +3779,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.8479</t>
+          <t>2.0696</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.342</t>
+          <t>1.503</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.544</t>
+          <t>2.849</t>
         </is>
       </c>
     </row>
@@ -3554,17 +3802,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.6339</t>
+          <t>0.7346</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.446</t>
+          <t>0.516</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>1.045</t>
         </is>
       </c>
     </row>
@@ -3577,17 +3825,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.5545</t>
+          <t>0.6613</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.324</t>
+          <t>0.386</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>1.133</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3848,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>3.9484</t>
+          <t>4.2108</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3610,7 +3858,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>39.484</t>
+          <t>42.108</t>
         </is>
       </c>
     </row>
@@ -3641,17 +3889,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.4465</t>
+          <t>1.4395</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.362</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.528</t>
+          <t>1.521</t>
         </is>
       </c>
     </row>
@@ -3889,17 +4137,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.3020</t>
+          <t>1.2990</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.258</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.341</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4385,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.2474</t>
+          <t>1.2451</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.215</t>
+          <t>1.212</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.279</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
KCOR slope2 normalization works. need second region
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.5012</t>
+          <t>1.4167</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.459</t>
+          <t>1.377</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.458</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.1943</t>
+          <t>0.9581</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -540,17 +540,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2437</t>
+          <t>1.1192</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.076</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.8376</t>
+          <t>1.6699</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.773</t>
+          <t>1.611</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.905</t>
+          <t>1.731</t>
         </is>
       </c>
     </row>
@@ -586,17 +586,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5456</t>
+          <t>1.6071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.419</t>
+          <t>1.476</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.683</t>
+          <t>1.750</t>
         </is>
       </c>
     </row>
@@ -609,17 +609,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5894</t>
+          <t>1.9472</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.625</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.906</t>
+          <t>2.334</t>
         </is>
       </c>
     </row>
@@ -632,17 +632,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.5770</t>
+          <t>1.7622</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.311</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.120</t>
+          <t>2.368</t>
         </is>
       </c>
     </row>
@@ -655,17 +655,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6376</t>
+          <t>2.1262</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>1.141</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.062</t>
+          <t>3.964</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.7281</t>
+          <t>1.3165</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>17.281</t>
+          <t>13.165</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8.0955</t>
+          <t>7.9791</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>80.955</t>
+          <t>79.791</t>
         </is>
       </c>
     </row>
@@ -742,17 +742,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.6843</t>
+          <t>1.5611</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.629</t>
+          <t>1.510</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.741</t>
+          <t>1.614</t>
         </is>
       </c>
     </row>
@@ -765,17 +765,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.5732</t>
+          <t>1.2666</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.478</t>
+          <t>1.190</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.675</t>
+          <t>1.348</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.9558</t>
+          <t>1.7540</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.886</t>
+          <t>1.691</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2.029</t>
+          <t>1.819</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.8148</t>
+          <t>1.6937</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.717</t>
+          <t>1.602</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.919</t>
+          <t>1.791</t>
         </is>
       </c>
     </row>
@@ -834,17 +834,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3536</t>
+          <t>1.2352</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.113</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>1.371</t>
         </is>
       </c>
     </row>
@@ -857,17 +857,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.4626</t>
+          <t>1.8737</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.537</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.784</t>
+          <t>2.283</t>
         </is>
       </c>
     </row>
@@ -880,17 +880,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3922</t>
+          <t>1.6215</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.162</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.945</t>
+          <t>2.264</t>
         </is>
       </c>
     </row>
@@ -903,17 +903,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6550</t>
+          <t>0.5699</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.438</t>
+          <t>0.381</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.853</t>
         </is>
       </c>
     </row>
@@ -926,17 +926,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.0453</t>
+          <t>1.9358</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.798</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.959</t>
+          <t>4.694</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.2189</t>
+          <t>3.1726</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>32.189</t>
+          <t>31.726</t>
         </is>
       </c>
     </row>
@@ -990,17 +990,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1203</t>
+          <t>1.1001</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.168</t>
+          <t>1.147</t>
         </is>
       </c>
     </row>
@@ -1013,17 +1013,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3173</t>
+          <t>1.3220</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.210</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5726</t>
+          <t>1.5672</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>1.497</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.647</t>
+          <t>1.641</t>
         </is>
       </c>
     </row>
@@ -1059,17 +1059,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9876</t>
+          <t>1.0143</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.928</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -1082,17 +1082,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.8758</t>
+          <t>0.7686</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.767</t>
+          <t>0.673</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.877</t>
         </is>
       </c>
     </row>
@@ -1105,17 +1105,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9202</t>
+          <t>0.9623</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.738</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.254</t>
         </is>
       </c>
     </row>
@@ -1128,17 +1128,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8828</t>
+          <t>0.9202</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.567</t>
+          <t>0.592</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.4000</t>
+          <t>0.2680</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.192</t>
+          <t>0.129</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.558</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.0896</t>
+          <t>1.3512</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1184,7 +1184,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>10.896</t>
+          <t>13.512</t>
         </is>
       </c>
     </row>
@@ -1295,17 +1295,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1956</t>
+          <t>1.0522</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.083</t>
         </is>
       </c>
     </row>
@@ -1318,17 +1318,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9462</t>
+          <t>0.9005</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.814</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>0.996</t>
         </is>
       </c>
     </row>
@@ -1341,17 +1341,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0840</t>
+          <t>0.9685</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>0.916</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.024</t>
         </is>
       </c>
     </row>
@@ -1364,17 +1364,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2713</t>
+          <t>1.0998</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.152</t>
         </is>
       </c>
     </row>
@@ -1387,17 +1387,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.3714</t>
+          <t>1.2016</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>1.269</t>
         </is>
       </c>
     </row>
@@ -1410,17 +1410,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.3244</t>
+          <t>1.0766</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>0.991</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
@@ -1433,17 +1433,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2309</t>
+          <t>1.0475</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.388</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -1456,17 +1456,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8595</t>
+          <t>0.6147</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.491</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>0.770</t>
         </is>
       </c>
     </row>
@@ -1479,17 +1479,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.9998</t>
+          <t>2.5299</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.642</t>
+          <t>1.024</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>9.745</t>
+          <t>6.253</t>
         </is>
       </c>
     </row>
@@ -1502,17 +1502,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.0927</t>
+          <t>1.3448</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.443</t>
+          <t>0.548</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.696</t>
+          <t>3.299</t>
         </is>
       </c>
     </row>
@@ -1543,17 +1543,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3673</t>
+          <t>1.1878</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.336</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.216</t>
         </is>
       </c>
     </row>
@@ -1566,17 +1566,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0828</t>
+          <t>0.8712</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>0.820</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>0.926</t>
         </is>
       </c>
     </row>
@@ -1589,17 +1589,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.2331</t>
+          <t>1.0528</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.092</t>
         </is>
       </c>
     </row>
@@ -1612,17 +1612,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.4916</t>
+          <t>1.2651</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.312</t>
         </is>
       </c>
     </row>
@@ -1635,17 +1635,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.6234</t>
+          <t>1.5152</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.537</t>
+          <t>1.434</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.601</t>
         </is>
       </c>
     </row>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3924</t>
+          <t>1.4005</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.255</t>
+          <t>1.263</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.554</t>
         </is>
       </c>
     </row>
@@ -1681,17 +1681,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.4244</t>
+          <t>1.4143</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.204</t>
+          <t>1.196</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.685</t>
+          <t>1.673</t>
         </is>
       </c>
     </row>
@@ -1704,17 +1704,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2366</t>
+          <t>1.2226</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.898</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.683</t>
+          <t>1.664</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.0700</t>
+          <t>0.9631</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.672</t>
+          <t>0.605</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.704</t>
+          <t>1.534</t>
         </is>
       </c>
     </row>
@@ -1750,17 +1750,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1812</t>
+          <t>0.6418</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.479</t>
+          <t>0.255</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.914</t>
+          <t>1.614</t>
         </is>
       </c>
     </row>
@@ -1791,17 +1791,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1436</t>
+          <t>1.1289</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.165</t>
         </is>
       </c>
     </row>
@@ -1814,17 +1814,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.1443</t>
+          <t>0.9674</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>0.877</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.067</t>
         </is>
       </c>
     </row>
@@ -1837,17 +1837,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1375</t>
+          <t>1.0871</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.146</t>
         </is>
       </c>
     </row>
@@ -1860,17 +1860,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1733</t>
+          <t>1.1503</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.098</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.229</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -1883,17 +1883,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.1838</t>
+          <t>1.2610</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.182</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.263</t>
+          <t>1.345</t>
         </is>
       </c>
     </row>
@@ -1906,17 +1906,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0514</t>
+          <t>1.3009</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>1.156</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.183</t>
+          <t>1.464</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1929,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1572</t>
+          <t>1.3502</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>1.117</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.632</t>
         </is>
       </c>
     </row>
@@ -1952,17 +1952,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.4386</t>
+          <t>1.9889</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.392</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.052</t>
+          <t>2.841</t>
         </is>
       </c>
     </row>
@@ -1975,17 +1975,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.2675</t>
+          <t>0.3807</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.100</t>
+          <t>0.141</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>1.028</t>
         </is>
       </c>
     </row>
@@ -1998,17 +1998,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0810</t>
+          <t>0.4773</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.312</t>
+          <t>0.137</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.739</t>
+          <t>1.667</t>
         </is>
       </c>
     </row>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0673</t>
+          <t>1.0719</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.120</t>
         </is>
       </c>
     </row>
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2860</t>
+          <t>1.2719</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.044</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.568</t>
+          <t>1.549</t>
         </is>
       </c>
     </row>
@@ -2142,17 +2142,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1245</t>
+          <t>1.1881</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.090</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.294</t>
         </is>
       </c>
     </row>
@@ -2165,17 +2165,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9575</t>
+          <t>0.9180</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>0.988</t>
         </is>
       </c>
     </row>
@@ -2188,17 +2188,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1957</t>
+          <t>1.2070</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.098</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.315</t>
+          <t>1.327</t>
         </is>
       </c>
     </row>
@@ -2211,17 +2211,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9700</t>
+          <t>1.0105</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.852</t>
+          <t>0.888</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9634</t>
+          <t>0.8909</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.751</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.057</t>
         </is>
       </c>
     </row>
@@ -2257,17 +2257,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0706</t>
+          <t>1.1599</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.871</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.427</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -2280,17 +2280,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1050</t>
+          <t>1.5780</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.699</t>
+          <t>2.414</t>
         </is>
       </c>
     </row>
@@ -2303,17 +2303,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.7519</t>
+          <t>2.5085</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>1.035</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.345</t>
+          <t>6.080</t>
         </is>
       </c>
     </row>
@@ -2344,17 +2344,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0599</t>
+          <t>1.0079</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.031</t>
         </is>
       </c>
     </row>
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9535</t>
+          <t>0.8176</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.758</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.882</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2390,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0785</t>
+          <t>1.0363</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>0.994</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -2413,17 +2413,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0149</t>
+          <t>0.9664</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -2436,17 +2436,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1590</t>
+          <t>1.1169</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.061</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.176</t>
         </is>
       </c>
     </row>
@@ -2459,17 +2459,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0527</t>
+          <t>1.0236</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.108</t>
         </is>
       </c>
     </row>
@@ -2482,17 +2482,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1585</t>
+          <t>1.0936</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>0.978</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.295</t>
+          <t>1.222</t>
         </is>
       </c>
     </row>
@@ -2505,17 +2505,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.1282</t>
+          <t>1.0699</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.295</t>
         </is>
       </c>
     </row>
@@ -2528,17 +2528,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.3582</t>
+          <t>1.4223</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.832</t>
+          <t>1.917</t>
         </is>
       </c>
     </row>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4233</t>
+          <t>1.3813</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>0.939</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.093</t>
+          <t>2.031</t>
         </is>
       </c>
     </row>
@@ -2592,17 +2592,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9931</t>
+          <t>0.9403</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>0.983</t>
         </is>
       </c>
     </row>
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.7415</t>
+          <t>0.6428</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.526</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>0.785</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9591</t>
+          <t>0.8722</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.800</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>0.951</t>
         </is>
       </c>
     </row>
@@ -2661,17 +2661,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0599</t>
+          <t>1.0527</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.979</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.132</t>
         </is>
       </c>
     </row>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9693</t>
+          <t>0.9254</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.840</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.019</t>
         </is>
       </c>
     </row>
@@ -2707,17 +2707,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0853</t>
+          <t>1.0130</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>
@@ -2730,17 +2730,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.2025</t>
+          <t>1.2276</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.027</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.437</t>
+          <t>1.467</t>
         </is>
       </c>
     </row>
@@ -2753,17 +2753,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.0537</t>
+          <t>0.9224</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.774</t>
+          <t>0.678</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>1.254</t>
         </is>
       </c>
     </row>
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.2292</t>
+          <t>0.9013</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.773</t>
+          <t>0.570</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.954</t>
+          <t>1.426</t>
         </is>
       </c>
     </row>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8124</t>
+          <t>0.5506</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.320</t>
+          <t>0.222</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2.065</t>
+          <t>1.369</t>
         </is>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.6883</t>
+          <t>1.4920</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>1.463</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.722</t>
+          <t>1.522</t>
         </is>
       </c>
     </row>
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.4012</t>
+          <t>1.2063</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.134</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>1.283</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.6389</t>
+          <t>1.4690</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.582</t>
+          <t>1.418</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.697</t>
+          <t>1.521</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.8140</t>
+          <t>1.5937</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.751</t>
+          <t>1.539</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.879</t>
+          <t>1.651</t>
         </is>
       </c>
     </row>
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.7760</t>
+          <t>1.5824</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.696</t>
+          <t>1.511</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.860</t>
+          <t>1.657</t>
         </is>
       </c>
     </row>
@@ -2955,17 +2955,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4229</t>
+          <t>1.2821</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.186</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.386</t>
         </is>
       </c>
     </row>
@@ -2978,17 +2978,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.6409</t>
+          <t>1.3494</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.191</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.858</t>
+          <t>1.529</t>
         </is>
       </c>
     </row>
@@ -3001,17 +3001,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1953</t>
+          <t>0.9958</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.808</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.227</t>
         </is>
       </c>
     </row>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.4701</t>
+          <t>1.2055</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>0.826</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2.139</t>
+          <t>1.758</t>
         </is>
       </c>
     </row>
@@ -3047,17 +3047,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0949</t>
+          <t>0.8977</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.627</t>
+          <t>0.511</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.912</t>
+          <t>1.576</t>
         </is>
       </c>
     </row>
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5819</t>
+          <t>1.3919</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.515</t>
+          <t>1.333</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.652</t>
+          <t>1.453</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0896</t>
+          <t>0.9484</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.895</t>
+          <t>0.780</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.153</t>
         </is>
       </c>
     </row>
@@ -3134,17 +3134,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.4574</t>
+          <t>1.2364</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.137</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.585</t>
+          <t>1.344</t>
         </is>
       </c>
     </row>
@@ -3157,17 +3157,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.8944</t>
+          <t>1.7360</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.764</t>
+          <t>1.617</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2.034</t>
+          <t>1.864</t>
         </is>
       </c>
     </row>
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.4853</t>
+          <t>1.3110</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.351</t>
+          <t>1.193</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.633</t>
+          <t>1.441</t>
         </is>
       </c>
     </row>
@@ -3203,17 +3203,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.4670</t>
+          <t>1.2687</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.285</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.675</t>
+          <t>1.448</t>
         </is>
       </c>
     </row>
@@ -3226,17 +3226,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.7033</t>
+          <t>1.5147</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.413</t>
+          <t>1.257</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2.053</t>
+          <t>1.826</t>
         </is>
       </c>
     </row>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.1164</t>
+          <t>0.8585</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.624</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.536</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -3272,17 +3272,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.3305</t>
+          <t>0.7640</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.794</t>
+          <t>0.457</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2.228</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -3295,17 +3295,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.6250</t>
+          <t>0.3578</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.226</t>
+          <t>0.132</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.726</t>
+          <t>0.971</t>
         </is>
       </c>
     </row>
@@ -3336,17 +3336,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.5929</t>
+          <t>1.4803</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.560</t>
+          <t>1.450</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.626</t>
+          <t>1.511</t>
         </is>
       </c>
     </row>
@@ -3359,17 +3359,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.4695</t>
+          <t>1.4754</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.374</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.584</t>
         </is>
       </c>
     </row>
@@ -3382,17 +3382,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.5195</t>
+          <t>1.4175</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.366</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.577</t>
+          <t>1.471</t>
         </is>
       </c>
     </row>
@@ -3405,17 +3405,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.7873</t>
+          <t>1.6491</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.726</t>
+          <t>1.593</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.851</t>
+          <t>1.708</t>
         </is>
       </c>
     </row>
@@ -3428,17 +3428,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.5324</t>
+          <t>1.4167</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.348</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.610</t>
+          <t>1.489</t>
         </is>
       </c>
     </row>
@@ -3451,17 +3451,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.3517</t>
+          <t>1.2524</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.151</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.470</t>
+          <t>1.363</t>
         </is>
       </c>
     </row>
@@ -3474,17 +3474,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.4165</t>
+          <t>1.2339</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.619</t>
+          <t>1.411</t>
         </is>
       </c>
     </row>
@@ -3497,17 +3497,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.0595</t>
+          <t>0.9308</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.340</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -3520,17 +3520,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.0824</t>
+          <t>0.8476</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.560</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.283</t>
         </is>
       </c>
     </row>
@@ -3543,17 +3543,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.7693</t>
+          <t>0.6499</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.424</t>
+          <t>0.356</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.186</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3624,7 +3624,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4 vs 0</t>
+          <t>1 vs 0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3158</t>
+          <t>0.9141</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.276</t>
+          <t>0.867</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.357</t>
+          <t>0.964</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.4970</t>
+          <t>1.3249</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.368</t>
+          <t>1.030</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.638</t>
+          <t>1.704</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2118</t>
+          <t>0.8771</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.154</t>
+          <t>0.787</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>0.978</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2986</t>
+          <t>0.8181</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>0.746</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>0.897</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4239</t>
+          <t>0.9551</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>0.859</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.062</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5274</t>
+          <t>1.1174</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.778</t>
+          <t>1.301</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.0696</t>
+          <t>0.8647</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.503</t>
+          <t>0.724</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.849</t>
+          <t>1.033</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7346</t>
+          <t>1.6562</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.516</t>
+          <t>1.136</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>2.414</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.6613</t>
+          <t>0.7241</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.386</t>
+          <t>0.470</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.133</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.2108</t>
+          <t>1.1002</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>42.108</t>
+          <t>11.002</t>
         </is>
       </c>
     </row>
@@ -3872,7 +3872,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4 vs 1</t>
+          <t>2 vs 0</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.4395</t>
+          <t>1.0121</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.362</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.521</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1299</t>
+          <t>1.3874</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>1.243</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>1.549</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3817</t>
+          <t>0.9440</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>0.895</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>0.996</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.5873</t>
+          <t>0.9921</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>0.942</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.740</t>
+          <t>1.045</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.4909</t>
+          <t>1.0939</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.029</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.163</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3669</t>
+          <t>1.0146</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.668</t>
+          <t>1.108</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2.3933</t>
+          <t>0.9613</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.687</t>
+          <t>0.856</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3.395</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.4435</t>
+          <t>0.9469</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.272</t>
+          <t>0.786</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9133</t>
+          <t>0.7101</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.480</t>
+          <t>0.547</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.738</t>
+          <t>0.922</t>
         </is>
       </c>
     </row>
@@ -4096,17 +4096,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.8273</t>
+          <t>0.7319</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.507</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>38.273</t>
+          <t>1.057</t>
         </is>
       </c>
     </row>
@@ -4120,7 +4120,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4 vs 2</t>
+          <t>2 vs 1</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.2990</t>
+          <t>1.1081</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.258</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.341</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0790</t>
+          <t>1.0472</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>1.359</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.2837</t>
+          <t>1.0763</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.201</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.3089</t>
+          <t>1.2126</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.105</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.331</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3016</t>
+          <t>1.1454</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.028</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.5054</t>
+          <t>0.9080</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>0.777</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.760</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.1529</t>
+          <t>1.1117</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.973</t>
+          <t>1.335</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.7758</t>
+          <t>0.5717</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.539</t>
+          <t>0.388</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>0.842</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9312</t>
+          <t>0.9807</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.541</t>
+          <t>0.633</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>1.520</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>5.0326</t>
+          <t>0.7605</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>50.326</t>
+          <t>7.605</t>
         </is>
       </c>
     </row>
@@ -4368,7 +4368,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4 vs 3</t>
+          <t>3 vs 0</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -4385,17 +4385,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.2451</t>
+          <t>1.0565</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -4408,17 +4408,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.3400</t>
+          <t>1.1172</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.037</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.204</t>
         </is>
       </c>
     </row>
@@ -4431,17 +4431,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.1606</t>
+          <t>1.0441</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -4454,17 +4454,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2272</t>
+          <t>1.0582</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.102</t>
         </is>
       </c>
     </row>
@@ -4477,17 +4477,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.3146</t>
+          <t>1.0831</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -4500,17 +4500,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.4505</t>
+          <t>1.0530</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.684</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -4523,17 +4523,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.8937</t>
+          <t>1.0929</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>0.980</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>2.608</t>
+          <t>1.219</t>
         </is>
       </c>
     </row>
@@ -4546,17 +4546,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.8047</t>
+          <t>0.9128</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.560</t>
+          <t>0.760</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -4569,17 +4569,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8414</t>
+          <t>0.7859</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.485</t>
+          <t>0.596</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.036</t>
         </is>
       </c>
     </row>
@@ -4592,17 +4592,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>4.9744</t>
+          <t>0.9440</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.565</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>49.744</t>
+          <t>1.578</t>
         </is>
       </c>
     </row>
@@ -4613,6 +4613,1494 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>3 vs 1</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1.1561</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>1.099</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>1.217</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>0.8432</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>0.658</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>1.080</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1.1904</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>1.072</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>1.321</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1.2934</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1.185</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>1.411</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1.1341</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>1.024</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1.256</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>0.9423</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>0.812</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1.094</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>1.2638</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1.057</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>1.511</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.5512</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.375</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0.811</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>1.0855</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.693</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>1.699</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0.7694</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>7.694</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>3 vs 2</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>1.0439</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>1.019</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>1.069</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>0.8053</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>0.728</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>0.891</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>1.1061</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>1.058</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>1.157</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>1.0666</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>1.022</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>1.113</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>0.9901</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>0.939</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>1.044</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>1.0378</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0.955</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>1.128</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>1.1369</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>1.011</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.9640</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0.786</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>1.183</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>1.1068</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0.830</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>1.475</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>1.2897</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>0.776</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>2.144</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>4 vs 0</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>1.3158</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>1.276</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>1.357</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>1.4970</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>1.368</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1.638</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>1.2118</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>1.154</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1.272</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>1.2986</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>1.235</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>1.365</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>1.4239</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>1.330</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>1.524</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>1.5274</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>1.312</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>1.778</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2.0696</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>1.503</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>2.849</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>0.7346</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>0.516</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>1.045</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0.6613</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0.386</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>1.133</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>4.2108</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>42.108</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>4 vs 1</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>1.4395</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>1.362</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>1.521</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>1.1299</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0.878</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>1.455</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>1.3817</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>1.241</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>1.538</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>1.5873</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>1.448</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>1.740</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>1.4909</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>1.332</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>1.669</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>1.3669</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>1.120</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>1.668</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2.3933</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>1.687</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>3.395</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>0.4435</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0.272</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>0.724</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>0.9133</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0.480</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>1.738</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>3.8273</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>38.273</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>4 vs 2</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>1.2990</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>1.258</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>1.341</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>1.0790</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>0.964</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>1.208</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>1.2837</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>1.219</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>1.352</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>1.3089</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>1.243</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>1.378</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>1.3016</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>1.212</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>1.398</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>1.5054</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>1.288</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>1.760</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2.1529</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>1.559</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2.973</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0.7758</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0.539</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>1.116</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0.9312</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0.541</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>1.604</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>5.0326</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>50.326</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>4 vs 3</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>ASMR (pooled)</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>1.2451</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>1.212</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>1.279</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>1.3400</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>1.239</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>1.449</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>1.1606</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>1.117</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>1.206</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>1.2272</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>1.179</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>1.277</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>1.3146</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>1.237</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>1.397</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>1.4505</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>1.250</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>1.684</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr"/>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>1.8937</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>1.375</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2.608</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>0.8047</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>0.560</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>1.156</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>0.8414</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>0.485</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>1.461</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>4.9744</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>49.744</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new slopes work for all cohorts
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -3641,17 +3641,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9141</t>
+          <t>0.9159</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.867</t>
+          <t>0.869</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.966</t>
         </is>
       </c>
     </row>
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.3249</t>
+          <t>1.5083</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.174</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.704</t>
+          <t>1.938</t>
         </is>
       </c>
     </row>
@@ -3687,17 +3687,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8771</t>
+          <t>0.9797</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.787</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>1.092</t>
         </is>
       </c>
     </row>
@@ -3710,17 +3710,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8181</t>
+          <t>0.7719</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.704</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.847</t>
         </is>
       </c>
     </row>
@@ -3733,17 +3733,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.9551</t>
+          <t>0.9542</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.858</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -3756,17 +3756,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1174</t>
+          <t>1.0988</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.944</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.301</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -3779,17 +3779,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8647</t>
+          <t>0.7458</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>0.624</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>0.891</t>
         </is>
       </c>
     </row>
@@ -3802,17 +3802,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.6562</t>
+          <t>1.0785</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>0.737</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2.414</t>
+          <t>1.578</t>
         </is>
       </c>
     </row>
@@ -3825,17 +3825,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.7241</t>
+          <t>0.4034</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.470</t>
+          <t>0.260</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>0.626</t>
         </is>
       </c>
     </row>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.1002</t>
+          <t>0.4649</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>11.002</t>
+          <t>4.649</t>
         </is>
       </c>
     </row>
@@ -3889,17 +3889,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0121</t>
+          <t>0.9854</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.013</t>
         </is>
       </c>
     </row>
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3874</t>
+          <t>1.5024</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.346</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>1.677</t>
         </is>
       </c>
     </row>
@@ -3935,17 +3935,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.9440</t>
+          <t>0.8917</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.895</t>
+          <t>0.845</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>0.941</t>
         </is>
       </c>
     </row>
@@ -3958,17 +3958,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9921</t>
+          <t>0.9406</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>0.893</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -3981,17 +3981,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0939</t>
+          <t>1.1755</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>1.106</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.249</t>
         </is>
       </c>
     </row>
@@ -4004,17 +4004,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0146</t>
+          <t>0.9190</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.842</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.003</t>
         </is>
       </c>
     </row>
@@ -4027,17 +4027,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9613</t>
+          <t>0.8755</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>0.779</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>0.983</t>
         </is>
       </c>
     </row>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9469</t>
+          <t>0.8059</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.786</t>
+          <t>0.669</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>0.971</t>
         </is>
       </c>
     </row>
@@ -4073,17 +4073,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.7101</t>
+          <t>0.7425</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.547</t>
+          <t>0.572</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.922</t>
+          <t>0.963</t>
         </is>
       </c>
     </row>
@@ -4096,17 +4096,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.7319</t>
+          <t>0.7581</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.507</t>
+          <t>0.526</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.093</t>
         </is>
       </c>
     </row>
@@ -4137,17 +4137,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1081</t>
+          <t>1.0766</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.050</t>
+          <t>1.020</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -4160,17 +4160,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.0472</t>
+          <t>0.9961</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.807</t>
+          <t>0.768</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.359</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -4183,17 +4183,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0763</t>
+          <t>0.9102</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.816</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.201</t>
+          <t>1.016</t>
         </is>
       </c>
     </row>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2126</t>
+          <t>1.2185</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.105</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.331</t>
+          <t>1.338</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.1454</t>
+          <t>1.2319</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.105</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.373</t>
         </is>
       </c>
     </row>
@@ -4252,17 +4252,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9080</t>
+          <t>0.8364</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.716</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>0.977</t>
         </is>
       </c>
     </row>
@@ -4275,17 +4275,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1117</t>
+          <t>1.1739</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.335</t>
+          <t>1.410</t>
         </is>
       </c>
     </row>
@@ -4298,17 +4298,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.5717</t>
+          <t>0.7472</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.388</t>
+          <t>0.505</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>1.105</t>
         </is>
       </c>
     </row>
@@ -4321,17 +4321,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9807</t>
+          <t>1.8405</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.633</t>
+          <t>1.179</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.520</t>
+          <t>2.874</t>
         </is>
       </c>
     </row>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.7605</t>
+          <t>1.8713</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>7.605</t>
+          <t>18.713</t>
         </is>
       </c>
     </row>
@@ -4385,17 +4385,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.0565</t>
+          <t>1.0185</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -4408,17 +4408,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.1172</t>
+          <t>1.2002</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.114</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.204</t>
+          <t>1.293</t>
         </is>
       </c>
     </row>
@@ -4431,17 +4431,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.0441</t>
+          <t>1.0152</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>0.974</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>1.058</t>
         </is>
       </c>
     </row>
@@ -4454,17 +4454,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0582</t>
+          <t>1.0137</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>0.973</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -4477,17 +4477,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.0831</t>
+          <t>1.0096</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>0.962</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>
@@ -4500,17 +4500,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.0530</t>
+          <t>0.9513</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.025</t>
         </is>
       </c>
     </row>
@@ -4523,17 +4523,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0929</t>
+          <t>1.0699</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.193</t>
         </is>
       </c>
     </row>
@@ -4546,17 +4546,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.9128</t>
+          <t>0.8359</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.760</t>
+          <t>0.696</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>1.003</t>
         </is>
       </c>
     </row>
@@ -4569,17 +4569,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.7859</t>
+          <t>0.9823</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.596</t>
+          <t>0.746</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.294</t>
         </is>
       </c>
     </row>
@@ -4592,17 +4592,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9440</t>
+          <t>1.0159</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.565</t>
+          <t>0.610</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.578</t>
+          <t>1.692</t>
         </is>
       </c>
     </row>
@@ -4633,17 +4633,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1561</t>
+          <t>1.1121</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.099</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.170</t>
         </is>
       </c>
     </row>
@@ -4656,17 +4656,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.8432</t>
+          <t>0.7957</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.658</t>
+          <t>0.622</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.019</t>
         </is>
       </c>
     </row>
@@ -4679,17 +4679,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.1904</t>
+          <t>1.0363</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.321</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -4702,17 +4702,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.2934</t>
+          <t>1.3132</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.203</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.411</t>
+          <t>1.433</t>
         </is>
       </c>
     </row>
@@ -4725,17 +4725,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.1341</t>
+          <t>1.0580</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.256</t>
+          <t>1.171</t>
         </is>
       </c>
     </row>
@@ -4748,17 +4748,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.9423</t>
+          <t>0.8658</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.746</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.004</t>
         </is>
       </c>
     </row>
@@ -4771,17 +4771,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.2638</t>
+          <t>1.4346</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.200</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.511</t>
+          <t>1.715</t>
         </is>
       </c>
     </row>
@@ -4794,17 +4794,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.5512</t>
+          <t>0.7751</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.375</t>
+          <t>0.525</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>1.145</t>
         </is>
       </c>
     </row>
@@ -4817,17 +4817,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.0855</t>
+          <t>2.4348</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.693</t>
+          <t>1.545</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.699</t>
+          <t>3.836</t>
         </is>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7694</t>
+          <t>1.9813</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4850,7 +4850,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>7.694</t>
+          <t>19.813</t>
         </is>
       </c>
     </row>
@@ -4881,17 +4881,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0439</t>
+          <t>1.0336</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.059</t>
         </is>
       </c>
     </row>
@@ -4904,17 +4904,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.8053</t>
+          <t>0.7988</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.728</t>
+          <t>0.722</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.884</t>
         </is>
       </c>
     </row>
@@ -4927,17 +4927,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.1061</t>
+          <t>1.1385</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.088</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.191</t>
         </is>
       </c>
     </row>
@@ -4950,17 +4950,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.0666</t>
+          <t>1.0776</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -4973,17 +4973,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.9901</t>
+          <t>0.8588</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>0.906</t>
         </is>
       </c>
     </row>
@@ -4996,17 +4996,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.0378</t>
+          <t>1.0351</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -5019,17 +5019,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.1369</t>
+          <t>1.2221</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>1.087</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.374</t>
         </is>
       </c>
     </row>
@@ -5042,17 +5042,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.9640</t>
+          <t>1.0373</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.786</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.183</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -5065,17 +5065,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.1068</t>
+          <t>1.3229</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.830</t>
+          <t>0.994</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.475</t>
+          <t>1.761</t>
         </is>
       </c>
     </row>
@@ -5088,17 +5088,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.2897</t>
+          <t>1.3401</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.776</t>
+          <t>0.810</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2.144</t>
+          <t>2.218</t>
         </is>
       </c>
     </row>
@@ -5129,17 +5129,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.3158</t>
+          <t>1.2643</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.276</t>
+          <t>1.226</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.357</t>
+          <t>1.304</t>
         </is>
       </c>
     </row>
@@ -5152,17 +5152,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.4970</t>
+          <t>1.6351</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.368</t>
+          <t>1.494</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.638</t>
+          <t>1.789</t>
         </is>
       </c>
     </row>
@@ -5175,17 +5175,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1.2118</t>
+          <t>1.1722</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.154</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>1.231</t>
         </is>
       </c>
     </row>
@@ -5198,17 +5198,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1.2986</t>
+          <t>1.1913</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.253</t>
         </is>
       </c>
     </row>
@@ -5221,17 +5221,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.4239</t>
+          <t>1.3495</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.261</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.445</t>
         </is>
       </c>
     </row>
@@ -5244,17 +5244,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1.5274</t>
+          <t>1.2486</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.072</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1.778</t>
+          <t>1.454</t>
         </is>
       </c>
     </row>
@@ -5267,17 +5267,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2.0696</t>
+          <t>2.6410</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.503</t>
+          <t>1.924</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2.849</t>
+          <t>3.625</t>
         </is>
       </c>
     </row>
@@ -5290,17 +5290,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0.7346</t>
+          <t>1.0920</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.516</t>
+          <t>0.775</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>1.539</t>
         </is>
       </c>
     </row>
@@ -5313,17 +5313,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.6613</t>
+          <t>0.7350</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.386</t>
+          <t>0.429</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1.133</t>
+          <t>1.258</t>
         </is>
       </c>
     </row>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>4.2108</t>
+          <t>3.7414</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>42.108</t>
+          <t>37.414</t>
         </is>
       </c>
     </row>
@@ -5377,17 +5377,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.4395</t>
+          <t>1.3805</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.362</t>
+          <t>1.306</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.521</t>
+          <t>1.459</t>
         </is>
       </c>
     </row>
@@ -5400,17 +5400,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1.1299</t>
+          <t>1.0841</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>1.395</t>
         </is>
       </c>
     </row>
@@ -5423,17 +5423,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1.3817</t>
+          <t>1.1965</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.075</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -5446,17 +5446,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.5873</t>
+          <t>1.5432</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>1.407</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.740</t>
+          <t>1.692</t>
         </is>
       </c>
     </row>
@@ -5469,17 +5469,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>1.4909</t>
+          <t>1.4143</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.264</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.583</t>
         </is>
       </c>
     </row>
@@ -5492,17 +5492,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1.3669</t>
+          <t>1.1364</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>0.931</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1.668</t>
+          <t>1.387</t>
         </is>
       </c>
     </row>
@@ -5515,17 +5515,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2.3933</t>
+          <t>3.5410</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1.687</t>
+          <t>2.502</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3.395</t>
+          <t>5.011</t>
         </is>
       </c>
     </row>
@@ -5538,17 +5538,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0.4435</t>
+          <t>1.0126</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.272</t>
+          <t>0.623</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>1.646</t>
         </is>
       </c>
     </row>
@@ -5561,17 +5561,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>0.9133</t>
+          <t>1.8218</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.480</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1.738</t>
+          <t>3.482</t>
         </is>
       </c>
     </row>
@@ -5584,7 +5584,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>3.8273</t>
+          <t>8.0481</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -5594,7 +5594,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>38.273</t>
+          <t>80.481</t>
         </is>
       </c>
     </row>
@@ -5625,17 +5625,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.2990</t>
+          <t>1.2822</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1.258</t>
+          <t>1.242</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.341</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -5648,17 +5648,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1.0790</t>
+          <t>1.0884</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -5671,17 +5671,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1.2837</t>
+          <t>1.3146</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.248</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.384</t>
         </is>
       </c>
     </row>
@@ -5694,17 +5694,17 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1.3089</t>
+          <t>1.2665</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.203</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.333</t>
         </is>
       </c>
     </row>
@@ -5717,17 +5717,17 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1.3016</t>
+          <t>1.1480</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.069</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.233</t>
         </is>
       </c>
     </row>
@@ -5740,17 +5740,17 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>1.5054</t>
+          <t>1.3586</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.162</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1.760</t>
+          <t>1.589</t>
         </is>
       </c>
     </row>
@@ -5763,17 +5763,17 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>2.1529</t>
+          <t>3.0165</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>2.191</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2.973</t>
+          <t>4.154</t>
         </is>
       </c>
     </row>
@@ -5786,17 +5786,17 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>0.7758</t>
+          <t>1.3551</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>0.539</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.933</t>
         </is>
       </c>
     </row>
@@ -5809,17 +5809,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>0.9312</t>
+          <t>0.9898</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>0.541</t>
+          <t>0.575</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>1.703</t>
         </is>
       </c>
     </row>
@@ -5832,7 +5832,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>5.0326</t>
+          <t>4.3008</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -5842,7 +5842,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>50.326</t>
+          <t>43.008</t>
         </is>
       </c>
     </row>
@@ -5873,17 +5873,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.2451</t>
+          <t>1.2413</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.208</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.275</t>
         </is>
       </c>
     </row>
@@ -5896,17 +5896,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1.3400</t>
+          <t>1.3624</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.260</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.474</t>
         </is>
       </c>
     </row>
@@ -5919,17 +5919,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1.1606</t>
+          <t>1.1547</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>1.200</t>
         </is>
       </c>
     </row>
@@ -5942,17 +5942,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>1.2272</t>
+          <t>1.1752</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.129</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.223</t>
         </is>
       </c>
     </row>
@@ -5965,17 +5965,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>1.3146</t>
+          <t>1.3367</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.257</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -5988,17 +5988,17 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>1.4505</t>
+          <t>1.3125</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.130</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>1.684</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -6011,17 +6011,17 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>1.8937</t>
+          <t>2.4684</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>1.797</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2.608</t>
+          <t>3.390</t>
         </is>
       </c>
     </row>
@@ -6034,17 +6034,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>0.8047</t>
+          <t>1.3064</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>0.560</t>
+          <t>0.918</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.860</t>
         </is>
       </c>
     </row>
@@ -6057,17 +6057,17 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>0.8414</t>
+          <t>0.7482</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>0.485</t>
+          <t>0.432</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.297</t>
         </is>
       </c>
     </row>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>4.9744</t>
+          <t>4.0621</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -6090,7 +6090,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>49.744</t>
+          <t>40.621</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated CI computation and README. Created new example directory with full spreadsheet implementation.
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -499,12 +499,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.377</t>
+          <t>1.397</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.437</t>
         </is>
       </c>
     </row>
@@ -522,12 +522,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.004</t>
         </is>
       </c>
     </row>
@@ -545,12 +545,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>1.145</t>
         </is>
       </c>
     </row>
@@ -568,12 +568,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.611</t>
+          <t>1.639</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.731</t>
+          <t>1.701</t>
         </is>
       </c>
     </row>
@@ -591,12 +591,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.476</t>
+          <t>1.540</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.750</t>
+          <t>1.677</t>
         </is>
       </c>
     </row>
@@ -614,12 +614,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.625</t>
+          <t>1.785</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2.334</t>
+          <t>2.124</t>
         </is>
       </c>
     </row>
@@ -637,12 +637,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.311</t>
+          <t>1.537</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.368</t>
+          <t>2.020</t>
         </is>
       </c>
     </row>
@@ -660,12 +660,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.655</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.964</t>
+          <t>2.732</t>
         </is>
       </c>
     </row>
@@ -683,12 +683,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.907</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>13.165</t>
+          <t>1.910</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>4.387</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>79.791</t>
+          <t>14.513</t>
         </is>
       </c>
     </row>
@@ -747,12 +747,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.510</t>
+          <t>1.535</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.614</t>
+          <t>1.588</t>
         </is>
       </c>
     </row>
@@ -770,12 +770,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.225</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.348</t>
+          <t>1.310</t>
         </is>
       </c>
     </row>
@@ -793,12 +793,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.691</t>
+          <t>1.722</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.819</t>
+          <t>1.787</t>
         </is>
       </c>
     </row>
@@ -816,12 +816,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.602</t>
+          <t>1.647</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.791</t>
+          <t>1.742</t>
         </is>
       </c>
     </row>
@@ -839,12 +839,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.168</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.306</t>
         </is>
       </c>
     </row>
@@ -862,12 +862,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.537</t>
+          <t>1.697</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2.283</t>
+          <t>2.069</t>
         </is>
       </c>
     </row>
@@ -885,12 +885,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.376</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2.264</t>
+          <t>1.910</t>
         </is>
       </c>
     </row>
@@ -908,12 +908,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.381</t>
+          <t>0.435</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.746</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>1.374</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.694</t>
+          <t>2.728</t>
         </is>
       </c>
     </row>
@@ -954,12 +954,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.019</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>31.726</t>
+          <t>9.873</t>
         </is>
       </c>
     </row>
@@ -995,12 +995,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.147</t>
+          <t>1.123</t>
         </is>
       </c>
     </row>
@@ -1018,12 +1018,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.210</t>
+          <t>1.261</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.386</t>
         </is>
       </c>
     </row>
@@ -1041,12 +1041,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.497</t>
+          <t>1.531</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.641</t>
+          <t>1.604</t>
         </is>
       </c>
     </row>
@@ -1064,12 +1064,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.045</t>
         </is>
       </c>
     </row>
@@ -1087,12 +1087,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.673</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>0.823</t>
         </is>
       </c>
     </row>
@@ -1110,12 +1110,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.738</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.254</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -1133,12 +1133,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.592</t>
+          <t>0.746</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.129</t>
+          <t>0.186</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.558</t>
+          <t>0.385</t>
         </is>
       </c>
     </row>
@@ -1179,12 +1179,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>13.512</t>
+          <t>2.220</t>
         </is>
       </c>
     </row>
@@ -1202,12 +1202,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.111</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3.976</t>
+          <t>1.425</t>
         </is>
       </c>
     </row>
@@ -1300,12 +1300,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.036</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.068</t>
         </is>
       </c>
     </row>
@@ -1323,12 +1323,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>0.958</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.916</t>
+          <t>0.939</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>0.999</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1369,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.050</t>
+          <t>1.073</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.152</t>
+          <t>1.127</t>
         </is>
       </c>
     </row>
@@ -1392,12 +1392,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.169</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.235</t>
         </is>
       </c>
     </row>
@@ -1415,12 +1415,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -1438,12 +1438,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.983</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.117</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.491</t>
+          <t>0.539</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.770</t>
+          <t>0.701</t>
         </is>
       </c>
     </row>
@@ -1484,12 +1484,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>2.010</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6.253</t>
+          <t>3.184</t>
         </is>
       </c>
     </row>
@@ -1507,12 +1507,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.548</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.299</t>
+          <t>2.046</t>
         </is>
       </c>
     </row>
@@ -1548,12 +1548,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.174</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -1571,12 +1571,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.840</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>0.903</t>
         </is>
       </c>
     </row>
@@ -1594,12 +1594,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -1617,12 +1617,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.241</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.290</t>
         </is>
       </c>
     </row>
@@ -1640,12 +1640,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>1.476</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.601</t>
+          <t>1.556</t>
         </is>
       </c>
     </row>
@@ -1663,12 +1663,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.263</t>
+          <t>1.330</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.554</t>
+          <t>1.475</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1686,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.196</t>
+          <t>1.303</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.673</t>
+          <t>1.535</t>
         </is>
       </c>
     </row>
@@ -1709,12 +1709,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.898</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.664</t>
+          <t>1.414</t>
         </is>
       </c>
     </row>
@@ -1732,12 +1732,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.605</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.534</t>
+          <t>1.209</t>
         </is>
       </c>
     </row>
@@ -1755,12 +1755,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.255</t>
+          <t>0.403</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.614</t>
+          <t>1.022</t>
         </is>
       </c>
     </row>
@@ -1796,12 +1796,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.112</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.147</t>
         </is>
       </c>
     </row>
@@ -1819,12 +1819,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>0.912</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>1.027</t>
         </is>
       </c>
     </row>
@@ -1842,12 +1842,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.118</t>
         </is>
       </c>
     </row>
@@ -1865,12 +1865,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.098</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -1888,12 +1888,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.224</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.299</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.464</t>
+          <t>1.378</t>
         </is>
       </c>
     </row>
@@ -1934,12 +1934,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.632</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -1957,12 +1957,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.392</t>
+          <t>1.658</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2.841</t>
+          <t>2.386</t>
         </is>
       </c>
     </row>
@@ -1980,12 +1980,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.141</t>
+          <t>0.281</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.516</t>
         </is>
       </c>
     </row>
@@ -2003,12 +2003,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.137</t>
+          <t>0.259</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.667</t>
+          <t>0.878</t>
         </is>
       </c>
     </row>
@@ -2101,12 +2101,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.026</t>
+          <t>1.030</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.116</t>
         </is>
       </c>
     </row>
@@ -2124,12 +2124,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.080</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>1.498</t>
         </is>
       </c>
     </row>
@@ -2147,12 +2147,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.095</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.289</t>
         </is>
       </c>
     </row>
@@ -2170,12 +2170,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -2193,12 +2193,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.098</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.327</t>
+          <t>1.312</t>
         </is>
       </c>
     </row>
@@ -2216,12 +2216,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.134</t>
         </is>
       </c>
     </row>
@@ -2239,12 +2239,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.751</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -2262,12 +2262,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.922</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.459</t>
         </is>
       </c>
     </row>
@@ -2285,12 +2285,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2.414</t>
+          <t>2.198</t>
         </is>
       </c>
     </row>
@@ -2308,12 +2308,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.437</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6.080</t>
+          <t>4.379</t>
         </is>
       </c>
     </row>
@@ -2349,12 +2349,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>0.987</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -2372,12 +2372,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.758</t>
+          <t>0.757</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.883</t>
         </is>
       </c>
     </row>
@@ -2400,7 +2400,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.081</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -2441,12 +2441,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.176</t>
+          <t>1.171</t>
         </is>
       </c>
     </row>
@@ -2464,12 +2464,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.945</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -2487,12 +2487,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.222</t>
+          <t>1.199</t>
         </is>
       </c>
     </row>
@@ -2510,12 +2510,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.921</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.295</t>
+          <t>1.243</t>
         </is>
       </c>
     </row>
@@ -2533,12 +2533,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.146</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.917</t>
+          <t>1.765</t>
         </is>
       </c>
     </row>
@@ -2556,12 +2556,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>1.044</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.031</t>
+          <t>1.828</t>
         </is>
       </c>
     </row>
@@ -2597,12 +2597,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.900</t>
+          <t>0.903</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -2620,12 +2620,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.526</t>
+          <t>0.543</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.785</t>
+          <t>0.761</t>
         </is>
       </c>
     </row>
@@ -2643,12 +2643,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>0.804</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.951</t>
+          <t>0.947</t>
         </is>
       </c>
     </row>
@@ -2666,12 +2666,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.132</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -2689,12 +2689,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.840</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -2712,12 +2712,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.467</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -2758,12 +2758,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.678</t>
+          <t>0.724</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.254</t>
+          <t>1.175</t>
         </is>
       </c>
     </row>
@@ -2781,12 +2781,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.570</t>
+          <t>0.639</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.426</t>
+          <t>1.271</t>
         </is>
       </c>
     </row>
@@ -2804,12 +2804,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.222</t>
+          <t>0.313</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>0.968</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.467</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.522</t>
+          <t>1.518</t>
         </is>
       </c>
     </row>
@@ -2868,12 +2868,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.134</t>
+          <t>1.140</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.277</t>
         </is>
       </c>
     </row>
@@ -2891,12 +2891,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.418</t>
+          <t>1.421</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.521</t>
+          <t>1.518</t>
         </is>
       </c>
     </row>
@@ -2914,12 +2914,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.539</t>
+          <t>1.543</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.651</t>
+          <t>1.646</t>
         </is>
       </c>
     </row>
@@ -2937,12 +2937,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.511</t>
+          <t>1.521</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.657</t>
+          <t>1.646</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.206</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.386</t>
+          <t>1.363</t>
         </is>
       </c>
     </row>
@@ -2983,12 +2983,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.529</t>
+          <t>1.478</t>
         </is>
       </c>
     </row>
@@ -3006,12 +3006,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.808</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
@@ -3029,12 +3029,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.826</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.758</t>
+          <t>1.565</t>
         </is>
       </c>
     </row>
@@ -3052,12 +3052,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.511</t>
+          <t>0.577</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -3093,12 +3093,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.339</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.446</t>
         </is>
       </c>
     </row>
@@ -3116,12 +3116,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.780</t>
+          <t>0.808</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.153</t>
+          <t>1.113</t>
         </is>
       </c>
     </row>
@@ -3139,12 +3139,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.144</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.344</t>
+          <t>1.336</t>
         </is>
       </c>
     </row>
@@ -3162,12 +3162,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.617</t>
+          <t>1.615</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.864</t>
+          <t>1.866</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.210</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.420</t>
         </is>
       </c>
     </row>
@@ -3208,12 +3208,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>1.132</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.448</t>
+          <t>1.422</t>
         </is>
       </c>
     </row>
@@ -3231,12 +3231,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.257</t>
+          <t>1.297</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.826</t>
+          <t>1.769</t>
         </is>
       </c>
     </row>
@@ -3254,12 +3254,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.624</t>
+          <t>0.669</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.101</t>
         </is>
       </c>
     </row>
@@ -3277,12 +3277,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.457</t>
+          <t>0.526</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -3300,12 +3300,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.132</t>
+          <t>0.185</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.692</t>
         </is>
       </c>
     </row>
@@ -3341,12 +3341,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.450</t>
+          <t>1.455</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.511</t>
+          <t>1.506</t>
         </is>
       </c>
     </row>
@@ -3364,12 +3364,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.378</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.584</t>
+          <t>1.580</t>
         </is>
       </c>
     </row>
@@ -3387,12 +3387,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.366</t>
+          <t>1.370</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.466</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.593</t>
+          <t>1.598</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.708</t>
+          <t>1.702</t>
         </is>
       </c>
     </row>
@@ -3433,12 +3433,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.348</t>
+          <t>1.361</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1.489</t>
+          <t>1.475</t>
         </is>
       </c>
     </row>
@@ -3456,12 +3456,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.151</t>
+          <t>1.172</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.363</t>
+          <t>1.338</t>
         </is>
       </c>
     </row>
@@ -3479,12 +3479,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.121</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.411</t>
+          <t>1.358</t>
         </is>
       </c>
     </row>
@@ -3502,12 +3502,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.735</t>
+          <t>0.778</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.113</t>
         </is>
       </c>
     </row>
@@ -3525,12 +3525,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.560</t>
+          <t>0.643</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.116</t>
         </is>
       </c>
     </row>
@@ -3548,12 +3548,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.356</t>
+          <t>0.414</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -3646,12 +3646,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.869</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.956</t>
         </is>
       </c>
     </row>
@@ -3669,12 +3669,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.174</t>
+          <t>1.241</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.938</t>
+          <t>1.833</t>
         </is>
       </c>
     </row>
@@ -3692,12 +3692,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.892</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.076</t>
         </is>
       </c>
     </row>
@@ -3715,12 +3715,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.704</t>
+          <t>0.713</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.847</t>
+          <t>0.836</t>
         </is>
       </c>
     </row>
@@ -3738,12 +3738,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -3761,12 +3761,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>0.988</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.222</t>
         </is>
       </c>
     </row>
@@ -3784,12 +3784,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.624</t>
+          <t>0.647</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.860</t>
         </is>
       </c>
     </row>
@@ -3807,12 +3807,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.737</t>
+          <t>0.874</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.578</t>
+          <t>1.331</t>
         </is>
       </c>
     </row>
@@ -3830,12 +3830,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.260</t>
+          <t>0.264</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.626</t>
+          <t>0.616</t>
         </is>
       </c>
     </row>
@@ -3853,12 +3853,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.249</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4.649</t>
+          <t>0.867</t>
         </is>
       </c>
     </row>
@@ -3894,12 +3894,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.013</t>
+          <t>1.007</t>
         </is>
       </c>
     </row>
@@ -3917,12 +3917,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.346</t>
+          <t>1.367</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.677</t>
+          <t>1.652</t>
         </is>
       </c>
     </row>
@@ -3940,12 +3940,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.845</t>
+          <t>0.852</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>0.933</t>
         </is>
       </c>
     </row>
@@ -3963,12 +3963,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>0.903</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.980</t>
         </is>
       </c>
     </row>
@@ -3986,12 +3986,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.106</t>
+          <t>1.121</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.249</t>
+          <t>1.233</t>
         </is>
       </c>
     </row>
@@ -4009,12 +4009,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.861</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>0.981</t>
         </is>
       </c>
     </row>
@@ -4032,12 +4032,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.779</t>
+          <t>0.802</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>0.955</t>
         </is>
       </c>
     </row>
@@ -4055,12 +4055,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.669</t>
+          <t>0.705</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.921</t>
         </is>
       </c>
     </row>
@@ -4078,12 +4078,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.572</t>
+          <t>0.603</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.915</t>
         </is>
       </c>
     </row>
@@ -4101,12 +4101,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.526</t>
+          <t>0.574</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.001</t>
         </is>
       </c>
     </row>
@@ -4142,12 +4142,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -4165,12 +4165,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.768</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.292</t>
+          <t>1.217</t>
         </is>
       </c>
     </row>
@@ -4188,12 +4188,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>0.828</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.001</t>
         </is>
       </c>
     </row>
@@ -4211,12 +4211,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.338</t>
+          <t>1.321</t>
         </is>
       </c>
     </row>
@@ -4234,12 +4234,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.105</t>
+          <t>1.128</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.373</t>
+          <t>1.345</t>
         </is>
       </c>
     </row>
@@ -4257,12 +4257,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.716</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.933</t>
         </is>
       </c>
     </row>
@@ -4280,12 +4280,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>1.013</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.410</t>
+          <t>1.360</t>
         </is>
       </c>
     </row>
@@ -4303,12 +4303,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.505</t>
+          <t>0.598</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.105</t>
+          <t>0.933</t>
         </is>
       </c>
     </row>
@@ -4326,12 +4326,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.188</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.874</t>
+          <t>2.852</t>
         </is>
       </c>
     </row>
@@ -4349,12 +4349,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.995</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>18.713</t>
+          <t>3.519</t>
         </is>
       </c>
     </row>
@@ -4390,12 +4390,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.036</t>
         </is>
       </c>
     </row>
@@ -4413,12 +4413,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>1.286</t>
         </is>
       </c>
     </row>
@@ -4436,12 +4436,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.981</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.050</t>
         </is>
       </c>
     </row>
@@ -4459,12 +4459,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>0.982</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.046</t>
         </is>
       </c>
     </row>
@@ -4482,12 +4482,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.962</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.049</t>
         </is>
       </c>
     </row>
@@ -4505,12 +4505,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -4528,12 +4528,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>
@@ -4551,12 +4551,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.696</t>
+          <t>0.732</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>0.955</t>
         </is>
       </c>
     </row>
@@ -4574,12 +4574,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.793</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.216</t>
         </is>
       </c>
     </row>
@@ -4597,12 +4597,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.708</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.692</t>
+          <t>1.457</t>
         </is>
       </c>
     </row>
@@ -4638,12 +4638,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.159</t>
         </is>
       </c>
     </row>
@@ -4661,12 +4661,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.622</t>
+          <t>0.658</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>0.962</t>
         </is>
       </c>
     </row>
@@ -4684,12 +4684,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.134</t>
         </is>
       </c>
     </row>
@@ -4707,12 +4707,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.203</t>
+          <t>1.217</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.433</t>
+          <t>1.417</t>
         </is>
       </c>
     </row>
@@ -4730,12 +4730,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.974</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.171</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -4753,12 +4753,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.004</t>
+          <t>0.960</t>
         </is>
       </c>
     </row>
@@ -4776,12 +4776,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.245</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.653</t>
         </is>
       </c>
     </row>
@@ -4799,12 +4799,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.525</t>
+          <t>0.621</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.145</t>
+          <t>0.967</t>
         </is>
       </c>
     </row>
@@ -4822,12 +4822,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.567</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>3.836</t>
+          <t>3.783</t>
         </is>
       </c>
     </row>
@@ -4845,12 +4845,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.012</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>19.813</t>
+          <t>3.880</t>
         </is>
       </c>
     </row>
@@ -4886,12 +4886,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>1.053</t>
         </is>
       </c>
     </row>
@@ -4909,12 +4909,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.722</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.869</t>
         </is>
       </c>
     </row>
@@ -4932,12 +4932,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>1.096</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.183</t>
         </is>
       </c>
     </row>
@@ -4955,12 +4955,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -4978,12 +4978,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>0.906</t>
+          <t>0.894</t>
         </is>
       </c>
     </row>
@@ -5001,12 +5001,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.974</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>1.100</t>
         </is>
       </c>
     </row>
@@ -5024,12 +5024,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.121</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -5047,12 +5047,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.892</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -5070,12 +5070,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.994</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.761</t>
+          <t>1.684</t>
         </is>
       </c>
     </row>
@@ -5093,12 +5093,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.810</t>
+          <t>0.921</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>2.218</t>
+          <t>1.949</t>
         </is>
       </c>
     </row>
@@ -5134,12 +5134,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.226</t>
+          <t>1.238</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.304</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -5157,12 +5157,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.494</t>
+          <t>1.515</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.789</t>
+          <t>1.764</t>
         </is>
       </c>
     </row>
@@ -5180,12 +5180,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.128</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -5203,12 +5203,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.133</t>
+          <t>1.149</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1.253</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -5226,12 +5226,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.286</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1.445</t>
+          <t>1.416</t>
         </is>
       </c>
     </row>
@@ -5249,12 +5249,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1.454</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -5272,12 +5272,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.924</t>
+          <t>2.242</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>3.625</t>
+          <t>3.110</t>
         </is>
       </c>
     </row>
@@ -5295,12 +5295,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.775</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.539</t>
+          <t>1.469</t>
         </is>
       </c>
     </row>
@@ -5318,12 +5318,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.429</t>
+          <t>0.454</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1.258</t>
+          <t>1.188</t>
         </is>
       </c>
     </row>
@@ -5341,12 +5341,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.528</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>37.414</t>
+          <t>9.159</t>
         </is>
       </c>
     </row>
@@ -5382,12 +5382,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.306</t>
+          <t>1.322</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.459</t>
+          <t>1.441</t>
         </is>
       </c>
     </row>
@@ -5405,12 +5405,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.395</t>
+          <t>1.314</t>
         </is>
       </c>
     </row>
@@ -5428,12 +5428,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.311</t>
         </is>
       </c>
     </row>
@@ -5451,12 +5451,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.407</t>
+          <t>1.427</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.692</t>
+          <t>1.669</t>
         </is>
       </c>
     </row>
@@ -5474,12 +5474,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.264</t>
+          <t>1.295</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1.583</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -5497,12 +5497,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1.387</t>
+          <t>1.291</t>
         </is>
       </c>
     </row>
@@ -5520,12 +5520,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2.502</t>
+          <t>2.894</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>5.011</t>
+          <t>4.333</t>
         </is>
       </c>
     </row>
@@ -5543,12 +5543,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.623</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1.646</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -5566,12 +5566,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3.482</t>
+          <t>3.373</t>
         </is>
       </c>
     </row>
@@ -5589,12 +5589,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>2.789</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>80.481</t>
+          <t>23.223</t>
         </is>
       </c>
     </row>
@@ -5630,12 +5630,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1.242</t>
+          <t>1.254</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.312</t>
         </is>
       </c>
     </row>
@@ -5653,12 +5653,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.995</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1.218</t>
+          <t>1.190</t>
         </is>
       </c>
     </row>
@@ -5676,12 +5676,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.248</t>
+          <t>1.261</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1.384</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -5699,12 +5699,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1.203</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.315</t>
         </is>
       </c>
     </row>
@@ -5722,12 +5722,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1.233</t>
+          <t>1.207</t>
         </is>
       </c>
     </row>
@@ -5745,12 +5745,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.234</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1.589</t>
+          <t>1.496</t>
         </is>
       </c>
     </row>
@@ -5768,12 +5768,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2.191</t>
+          <t>2.551</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>4.154</t>
+          <t>3.567</t>
         </is>
       </c>
     </row>
@@ -5791,12 +5791,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.999</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1.933</t>
+          <t>1.838</t>
         </is>
       </c>
     </row>
@@ -5814,12 +5814,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>0.575</t>
+          <t>0.604</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.703</t>
+          <t>1.621</t>
         </is>
       </c>
     </row>
@@ -5837,12 +5837,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.747</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>43.008</t>
+          <t>10.589</t>
         </is>
       </c>
     </row>
@@ -5878,12 +5878,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1.275</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -5901,12 +5901,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1.260</t>
+          <t>1.281</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.474</t>
+          <t>1.449</t>
         </is>
       </c>
     </row>
@@ -5924,12 +5924,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>1.122</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.188</t>
         </is>
       </c>
     </row>
@@ -5947,12 +5947,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>1.129</t>
+          <t>1.143</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>1.223</t>
+          <t>1.208</t>
         </is>
       </c>
     </row>
@@ -5970,12 +5970,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>1.257</t>
+          <t>1.283</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.393</t>
         </is>
       </c>
     </row>
@@ -5993,12 +5993,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1.130</t>
+          <t>1.200</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>1.524</t>
+          <t>1.436</t>
         </is>
       </c>
     </row>
@@ -6016,12 +6016,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>1.797</t>
+          <t>2.097</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>3.390</t>
+          <t>2.906</t>
         </is>
       </c>
     </row>
@@ -6039,12 +6039,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>0.918</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>1.860</t>
+          <t>1.771</t>
         </is>
       </c>
     </row>
@@ -6062,12 +6062,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>0.432</t>
+          <t>0.456</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>1.297</t>
+          <t>1.228</t>
         </is>
       </c>
     </row>
@@ -6085,12 +6085,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.603</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>40.621</t>
+          <t>10.295</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
KCOR now updated with MFG
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.4167</t>
+          <t>1.4169</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9581</t>
+          <t>0.9580</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.004</t>
+          <t>1.003</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1192</t>
+          <t>1.1194</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -563,12 +563,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6699</t>
+          <t>1.6703</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.639</t>
+          <t>1.640</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6071</t>
+          <t>1.6072</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -701,17 +701,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.9791</t>
+          <t>7.9810</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>4.387</t>
+          <t>4.388</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>14.513</t>
+          <t>14.515</t>
         </is>
       </c>
     </row>
@@ -742,12 +742,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5611</t>
+          <t>1.5616</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.535</t>
+          <t>1.536</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -765,7 +765,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.2666</t>
+          <t>1.2670</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -788,17 +788,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.7540</t>
+          <t>1.7549</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.722</t>
+          <t>1.723</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.787</t>
+          <t>1.788</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6937</t>
+          <t>1.6942</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.647</t>
+          <t>1.648</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -834,7 +834,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2352</t>
+          <t>1.2353</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.6215</t>
+          <t>1.6216</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -949,12 +949,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>3.1726</t>
+          <t>3.1733</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.020</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.1001</t>
+          <t>1.1003</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1013,12 +1013,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.3220</t>
+          <t>1.3226</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5672</t>
+          <t>1.5677</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>1.605</t>
         </is>
       </c>
     </row>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9623</t>
+          <t>0.9622</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.425</t>
+          <t>1.424</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0522</t>
+          <t>1.0520</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9005</t>
+          <t>0.9001</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9685</t>
+          <t>0.9682</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0998</t>
+          <t>1.0997</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1878</t>
+          <t>1.1876</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8712</t>
+          <t>0.8705</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.902</t>
         </is>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0528</t>
+          <t>1.0526</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1612,7 +1612,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2651</t>
+          <t>1.2650</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1658,7 +1658,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.4005</t>
+          <t>1.4006</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9674</t>
+          <t>0.9672</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.026</t>
         </is>
       </c>
     </row>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.259</t>
+          <t>0.260</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0719</t>
+          <t>1.0722</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2119,17 +2119,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2719</t>
+          <t>1.2733</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.082</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.498</t>
+          <t>1.499</t>
         </is>
       </c>
     </row>
@@ -2142,12 +2142,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.1881</t>
+          <t>1.1887</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.096</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9180</t>
+          <t>0.9181</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2070</t>
+          <t>1.2071</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2367,17 +2367,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8176</t>
+          <t>0.8169</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.756</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.882</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0363</t>
+          <t>1.0364</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9664</t>
+          <t>0.9663</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1169</t>
+          <t>1.1170</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0236</t>
+          <t>1.0237</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9403</t>
+          <t>0.9400</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2615,17 +2615,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.6428</t>
+          <t>0.6415</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.543</t>
+          <t>0.542</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.761</t>
+          <t>0.759</t>
         </is>
       </c>
     </row>
@@ -2638,17 +2638,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.8722</t>
+          <t>0.8718</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.804</t>
+          <t>0.803</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.947</t>
+          <t>0.946</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0527</t>
+          <t>1.0526</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9254</t>
+          <t>0.9253</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.4920</t>
+          <t>1.4926</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2863,17 +2863,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.2063</t>
+          <t>1.2074</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.141</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.277</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2886,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.4690</t>
+          <t>1.4701</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.422</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1.518</t>
+          <t>1.519</t>
         </is>
       </c>
     </row>
@@ -2909,12 +2909,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.5937</t>
+          <t>1.5942</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.543</t>
+          <t>1.544</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.5824</t>
+          <t>1.5825</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3088,17 +3088,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.3919</t>
+          <t>1.3921</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.339</t>
+          <t>1.340</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.446</t>
+          <t>1.447</t>
         </is>
       </c>
     </row>
@@ -3111,17 +3111,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.9484</t>
+          <t>0.9482</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.808</t>
+          <t>0.809</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.112</t>
         </is>
       </c>
     </row>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.2364</t>
+          <t>1.2367</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3157,12 +3157,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.7360</t>
+          <t>1.7364</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.615</t>
+          <t>1.616</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.210</t>
+          <t>1.211</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -3336,17 +3336,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.4803</t>
+          <t>1.4810</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.455</t>
+          <t>1.456</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.506</t>
+          <t>1.507</t>
         </is>
       </c>
     </row>
@@ -3359,17 +3359,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.4754</t>
+          <t>1.4780</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.380</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.583</t>
         </is>
       </c>
     </row>
@@ -3382,17 +3382,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.4175</t>
+          <t>1.4185</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.370</t>
+          <t>1.371</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.466</t>
+          <t>1.467</t>
         </is>
       </c>
     </row>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.6491</t>
+          <t>1.6497</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1.702</t>
+          <t>1.703</t>
         </is>
       </c>
     </row>
@@ -3428,7 +3428,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.4167</t>
+          <t>1.4168</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.2524</t>
+          <t>1.2525</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9159</t>
+          <t>0.9160</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3664,17 +3664,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.5083</t>
+          <t>1.5109</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.833</t>
+          <t>1.835</t>
         </is>
       </c>
     </row>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9797</t>
+          <t>0.9798</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3912,17 +3912,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.5024</t>
+          <t>1.5048</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.367</t>
+          <t>1.369</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.652</t>
+          <t>1.654</t>
         </is>
       </c>
     </row>
@@ -3935,7 +3935,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8917</t>
+          <t>0.8914</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -4137,7 +4137,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0766</t>
+          <t>1.0765</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9961</t>
+          <t>0.9960</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.216</t>
         </is>
       </c>
     </row>
@@ -4183,7 +4183,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9102</t>
+          <t>0.9098</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2319</t>
+          <t>1.2320</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.0185</t>
+          <t>1.0186</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -4408,17 +4408,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.2002</t>
+          <t>1.2008</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.121</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1.286</t>
+          <t>1.287</t>
         </is>
       </c>
     </row>
@@ -4431,7 +4431,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.0152</t>
+          <t>1.0153</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1121</t>
+          <t>1.1120</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4656,7 +4656,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.7957</t>
+          <t>0.7947</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4666,7 +4666,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.962</t>
+          <t>0.960</t>
         </is>
       </c>
     </row>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.3132</t>
+          <t>1.3133</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4712,7 +4712,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.417</t>
+          <t>1.418</t>
         </is>
       </c>
     </row>
@@ -4881,7 +4881,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0336</t>
+          <t>1.0337</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -4904,17 +4904,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.7988</t>
+          <t>0.7980</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.735</t>
+          <t>0.734</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.869</t>
+          <t>0.867</t>
         </is>
       </c>
     </row>
@@ -4927,12 +4927,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.1385</t>
+          <t>1.1389</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.097</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.0776</t>
+          <t>1.0778</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5129,7 +5129,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.2643</t>
+          <t>1.2646</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -5152,17 +5152,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.6351</t>
+          <t>1.6377</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.515</t>
+          <t>1.518</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.764</t>
+          <t>1.767</t>
         </is>
       </c>
     </row>
@@ -5175,12 +5175,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1.1722</t>
+          <t>1.1725</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.129</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>1.1913</t>
+          <t>1.1914</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.3495</t>
+          <t>1.3496</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -5267,7 +5267,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2.6410</t>
+          <t>2.6411</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>3.110</t>
+          <t>3.111</t>
         </is>
       </c>
     </row>
@@ -5336,12 +5336,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>3.7414</t>
+          <t>3.7419</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>1.528</t>
+          <t>1.529</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.3805</t>
+          <t>1.3806</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -5400,17 +5400,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1.0841</t>
+          <t>1.0839</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>0.895</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1.314</t>
+          <t>1.313</t>
         </is>
       </c>
     </row>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1.1965</t>
+          <t>1.1968</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -5446,7 +5446,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.5432</t>
+          <t>1.5435</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.670</t>
         </is>
       </c>
     </row>
@@ -5515,7 +5515,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>3.5410</t>
+          <t>3.5411</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -5584,17 +5584,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>8.0481</t>
+          <t>8.0491</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2.789</t>
+          <t>2.790</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>23.223</t>
+          <t>23.224</t>
         </is>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.2822</t>
+          <t>1.2825</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -5648,12 +5648,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1.0884</t>
+          <t>1.0883</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.995</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -5671,17 +5671,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1.3146</t>
+          <t>1.3153</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1.370</t>
+          <t>1.371</t>
         </is>
       </c>
     </row>
@@ -5694,12 +5694,12 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1.2665</t>
+          <t>1.2667</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>3.0165</t>
+          <t>3.0166</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>4.3008</t>
+          <t>4.3013</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.2413</t>
+          <t>1.2415</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -5896,17 +5896,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1.3624</t>
+          <t>1.3638</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1.281</t>
+          <t>1.282</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.450</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1.1547</t>
+          <t>1.1549</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -5929,7 +5929,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.189</t>
         </is>
       </c>
     </row>
@@ -5942,7 +5942,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>1.1752</t>
+          <t>1.1753</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -5988,7 +5988,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>1.3125</t>
+          <t>1.3126</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>4.0621</t>
+          <t>4.0626</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">

</xml_diff>

<commit_message>
Update analysis files and fixed double subtract bug KCOR_CMR.py
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -519,17 +519,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8956</t>
+          <t>0.8952</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.854</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.938</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3550</t>
+          <t>1.3551</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.3358</t>
+          <t>1.3357</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.359</t>
+          <t>1.358</t>
         </is>
       </c>
     </row>
@@ -767,17 +767,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1200</t>
+          <t>1.1193</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.082</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.159</t>
+          <t>1.158</t>
         </is>
       </c>
     </row>
@@ -992,12 +992,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9559</t>
+          <t>0.9558</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.936</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>1.2506</t>
+          <t>1.2504</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.311</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.3512</t>
+          <t>1.3511</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1320,12 +1320,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9209</t>
+          <t>0.9204</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.159</t>
+          <t>1.158</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1568,17 +1568,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8903</t>
+          <t>0.8897</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.858</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>0.922</t>
         </is>
       </c>
     </row>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9668</t>
+          <t>0.9667</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1977,12 +1977,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.9134</t>
+          <t>1.9133</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>1.307</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0278</t>
+          <t>1.0277</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2121,17 +2121,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8045</t>
+          <t>0.8040</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.756</t>
+          <t>0.755</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.857</t>
+          <t>0.856</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8308</t>
+          <t>0.8303</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>0.861</t>
         </is>
       </c>
     </row>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7682</t>
+          <t>0.7680</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.836</t>
+          <t>0.835</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.7596</t>
+          <t>0.7592</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.736</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.9888</t>
+          <t>0.9886</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -3700,17 +3700,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1180</t>
+          <t>1.1152</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.073</t>
+          <t>1.071</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>1.161</t>
         </is>
       </c>
     </row>
@@ -3723,17 +3723,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2913</t>
+          <t>1.2958</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.097</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.526</t>
+          <t>1.530</t>
         </is>
       </c>
     </row>
@@ -3746,17 +3746,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.2948</t>
+          <t>1.2968</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.194</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.407</t>
+          <t>1.409</t>
         </is>
       </c>
     </row>
@@ -3769,12 +3769,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9987</t>
+          <t>0.9993</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.924</t>
+          <t>0.925</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0556</t>
+          <t>1.0558</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3802,7 +3802,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.151</t>
         </is>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.4020</t>
+          <t>3.4021</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3948,17 +3948,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0369</t>
+          <t>1.0382</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -3971,17 +3971,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8829</t>
+          <t>0.8876</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>0.820</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.961</t>
         </is>
       </c>
     </row>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0132</t>
+          <t>1.0135</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0492</t>
+          <t>1.0489</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1025</t>
+          <t>1.1023</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -4196,17 +4196,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.9275</t>
+          <t>0.9309</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -4219,17 +4219,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.6837</t>
+          <t>0.6850</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.576</t>
+          <t>0.577</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.813</t>
         </is>
       </c>
     </row>
@@ -4242,17 +4242,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.7825</t>
+          <t>0.7816</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.720</t>
+          <t>0.719</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.849</t>
         </is>
       </c>
     </row>
@@ -4265,17 +4265,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0505</t>
+          <t>1.0497</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.971</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.134</t>
         </is>
       </c>
     </row>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0444</t>
+          <t>1.0440</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.138</t>
         </is>
       </c>
     </row>
@@ -4444,17 +4444,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.4225</t>
+          <t>1.4256</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.401</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.447</t>
+          <t>1.451</t>
         </is>
       </c>
     </row>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.2112</t>
+          <t>1.2110</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -4692,17 +4692,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.2724</t>
+          <t>1.2783</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.230</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.323</t>
+          <t>1.329</t>
         </is>
       </c>
     </row>
@@ -4715,17 +4715,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.9380</t>
+          <t>0.9345</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.797</t>
+          <t>0.795</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>1.099</t>
         </is>
       </c>
     </row>
@@ -4738,17 +4738,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1.0762</t>
+          <t>1.0746</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.995</t>
+          <t>0.993</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.163</t>
         </is>
       </c>
     </row>
@@ -4761,17 +4761,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.5417</t>
+          <t>1.5408</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.432</t>
+          <t>1.431</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.660</t>
+          <t>1.658</t>
         </is>
       </c>
     </row>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.4046</t>
+          <t>1.4042</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4794,7 +4794,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.3429</t>
+          <t>1.3430</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4940,17 +4940,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.3719</t>
+          <t>1.3732</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1.348</t>
+          <t>1.349</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.396</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -4963,17 +4963,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1.3719</t>
+          <t>1.3643</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.272</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1.472</t>
+          <t>1.464</t>
         </is>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.3753</t>
+          <t>1.3749</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -4996,7 +4996,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.424</t>
+          <t>1.423</t>
         </is>
       </c>
     </row>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.4676</t>
+          <t>1.4679</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5032,12 +5032,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1.3448</t>
+          <t>1.3450</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1.290</t>
+          <t>1.291</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -5245,17 +5245,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9327</t>
+          <t>0.9260</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.967</t>
         </is>
       </c>
     </row>
@@ -5268,17 +5268,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.9755</t>
+          <t>1.9155</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.624</t>
+          <t>1.575</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2.403</t>
+          <t>2.329</t>
         </is>
       </c>
     </row>
@@ -5291,17 +5291,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0349</t>
+          <t>1.0366</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.940</t>
+          <t>0.942</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -5314,12 +5314,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.7428</t>
+          <t>0.7436</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>0.685</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -5337,12 +5337,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8701</t>
+          <t>0.8707</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.795</t>
+          <t>0.796</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.4943</t>
+          <t>1.4944</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -5493,17 +5493,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0020</t>
+          <t>1.0007</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.979</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>1.023</t>
         </is>
       </c>
     </row>
@@ -5516,17 +5516,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.7383</t>
+          <t>1.7629</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.578</t>
+          <t>1.600</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.915</t>
+          <t>1.943</t>
         </is>
       </c>
     </row>
@@ -5539,17 +5539,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8849</t>
+          <t>0.8865</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.845</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.927</t>
+          <t>0.929</t>
         </is>
       </c>
     </row>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9394</t>
+          <t>0.9395</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -5585,12 +5585,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1669</t>
+          <t>1.1667</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -5741,17 +5741,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1.0742</t>
+          <t>1.0807</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1.122</t>
+          <t>1.129</t>
         </is>
       </c>
     </row>
@@ -5764,17 +5764,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.8799</t>
+          <t>0.9203</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>0.753</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -5787,12 +5787,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.8551</t>
+          <t>0.8552</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.775</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -5810,17 +5810,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2646</t>
+          <t>1.2635</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>1.163</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.373</t>
         </is>
       </c>
     </row>
@@ -5833,17 +5833,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3411</t>
+          <t>1.3399</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.225</t>
+          <t>1.224</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.468</t>
+          <t>1.467</t>
         </is>
       </c>
     </row>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>0.931</t>
         </is>
       </c>
     </row>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1700</t>
+          <t>1.1699</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -5989,17 +5989,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.0572</t>
+          <t>1.0562</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.038</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.075</t>
         </is>
       </c>
     </row>
@@ -6012,7 +6012,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>1.1860</t>
+          <t>1.1858</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -6237,17 +6237,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.1335</t>
+          <t>1.1407</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.189</t>
         </is>
       </c>
     </row>
@@ -6260,17 +6260,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.6004</t>
+          <t>0.6191</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.496</t>
+          <t>0.512</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.726</t>
+          <t>0.749</t>
         </is>
       </c>
     </row>
@@ -6283,17 +6283,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>0.9965</t>
+          <t>0.9948</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.907</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.091</t>
         </is>
       </c>
     </row>
@@ -6306,17 +6306,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>1.4103</t>
+          <t>1.4089</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.303</t>
+          <t>1.302</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1.526</t>
+          <t>1.524</t>
         </is>
       </c>
     </row>
@@ -6329,17 +6329,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.2083</t>
+          <t>1.2074</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.109</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.316</t>
         </is>
       </c>
     </row>
@@ -6352,7 +6352,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8607</t>
+          <t>0.8606</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -6375,7 +6375,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.5417</t>
+          <t>1.5415</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -6398,7 +6398,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.8016</t>
+          <t>0.8015</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0551</t>
+          <t>1.0555</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -6508,17 +6508,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.6823</t>
+          <t>0.6727</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0.627</t>
+          <t>0.618</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>0.743</t>
+          <t>0.733</t>
         </is>
       </c>
     </row>
@@ -6531,17 +6531,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.1654</t>
+          <t>1.1633</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.119</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.210</t>
         </is>
       </c>
     </row>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1.1152</t>
+          <t>1.1150</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6577,12 +6577,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.9010</t>
+          <t>0.9011</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.864</t>
+          <t>0.865</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -6733,17 +6733,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.2678</t>
+          <t>1.2651</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.238</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.296</t>
+          <t>1.293</t>
         </is>
       </c>
     </row>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.5641</t>
+          <t>1.5638</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6940,7 +6940,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>3.9243</t>
+          <t>3.9244</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6981,17 +6981,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.3558</t>
+          <t>1.3632</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.298</t>
+          <t>1.305</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.416</t>
+          <t>1.424</t>
         </is>
       </c>
     </row>
@@ -7004,17 +7004,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>0.7917</t>
+          <t>0.8164</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>0.653</t>
+          <t>0.673</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.990</t>
         </is>
       </c>
     </row>
@@ -7027,17 +7027,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>1.1287</t>
+          <t>1.1268</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>1.238</t>
         </is>
       </c>
     </row>
@@ -7050,17 +7050,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.5553</t>
+          <t>1.5537</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>1.433</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1.687</t>
+          <t>1.685</t>
         </is>
       </c>
     </row>
@@ -7073,17 +7073,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>1.5544</t>
+          <t>1.5533</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.419</t>
+          <t>1.418</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1.702</t>
+          <t>1.701</t>
         </is>
       </c>
     </row>
@@ -7096,7 +7096,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>1.1551</t>
+          <t>1.1550</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -7119,12 +7119,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>3.3811</t>
+          <t>3.3807</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2.753</t>
+          <t>2.752</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -7165,7 +7165,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>2.2184</t>
+          <t>2.2185</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -7188,17 +7188,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>8.0491</t>
+          <t>6.6309</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2.760</t>
+          <t>2.274</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>23.474</t>
+          <t>19.338</t>
         </is>
       </c>
     </row>
@@ -7229,17 +7229,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.2635</t>
+          <t>1.2626</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.234</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.293</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -7252,17 +7252,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>0.8998</t>
+          <t>0.8871</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.822</t>
+          <t>0.810</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>0.972</t>
         </is>
       </c>
     </row>
@@ -7275,17 +7275,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>1.3200</t>
+          <t>1.3176</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.262</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1.378</t>
+          <t>1.375</t>
         </is>
       </c>
     </row>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1.2299</t>
+          <t>1.2297</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -7308,7 +7308,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.278</t>
         </is>
       </c>
     </row>
@@ -7321,12 +7321,12 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1.1590</t>
+          <t>1.1592</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.102</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -7436,17 +7436,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>4.5568</t>
+          <t>4.6310</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1.848</t>
+          <t>1.878</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>11.239</t>
+          <t>11.421</t>
         </is>
       </c>
     </row>
@@ -7477,17 +7477,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.1978</t>
+          <t>1.1965</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1.176</t>
+          <t>1.175</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added 20 week post booster enrollment showing flat lines
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -12,7 +12,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_24" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021_30" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_06" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_47" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_26" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022_47" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5593,6 +5594,1689 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dose_Combination</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>YearOfBirth</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>KCOR</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CI_Lower</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CI_Upper</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Reporting date: 2024-10-07</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1 vs 0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>0.9657</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.915</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.019</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.8722</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.828</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0.919</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.4515</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.358</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0.569</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1.2649</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.138</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1.406</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.2618</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1.139</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1.398</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0.5530</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.489</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.625</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1.0483</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.899</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1.223</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1.4149</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1.163</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1.722</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2.9145</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2.274</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>3.735</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0.3441</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.219</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0.540</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0.8313</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.427</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1.617</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2 vs 0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1.0184</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.003</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1.035</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1.0148</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.999</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1.031</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>0.9420</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.879</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1.009</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1.0452</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>1.011</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1.080</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1.0552</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>1.025</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1.087</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.9694</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.938</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1.002</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>0.8955</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.856</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.937</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1.1982</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1.128</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1.273</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1.1335</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>1.031</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1.246</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0.8963</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.780</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1.030</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1.0430</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.865</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1.257</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2 vs 1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>1.0545</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.999</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1.114</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>1.1635</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>1.104</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>1.227</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2.0865</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>1.651</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2.638</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0.8263</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.743</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0.919</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.8362</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.754</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0.927</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1.7530</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>1.549</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>1.984</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>0.8542</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.732</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0.997</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0.8468</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.695</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>1.032</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0.3889</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0.302</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>0.501</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2.6050</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>1.651</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>4.109</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0.7206</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0.370</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>1.405</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>3 vs 0</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0.9774</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0.966</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>0.989</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0.9785</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0.967</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0.990</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0.7326</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0.699</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0.768</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>0.9938</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0.971</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>1.017</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>1.0876</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>1.064</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>1.112</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0.8885</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0.866</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0.912</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0.9816</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0.944</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>1.021</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>1.0094</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0.954</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>1.068</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>1.0888</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0.989</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>1.198</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>0.8034</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>0.689</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>0.937</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>1.5111</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1.177</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>1.941</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>3 vs 1</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>1.0106</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0.958</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>1.066</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>1.1219</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>1.065</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>1.182</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>1.6227</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>1.291</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2.040</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0.7857</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0.708</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0.872</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>0.8619</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>0.779</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>0.954</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>1.6068</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>1.422</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>1.815</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0.9364</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0.803</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>1.091</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0.7134</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0.586</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0.868</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0.3736</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0.290</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0.481</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2.3350</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>1.473</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>3.701</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0.8349</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0.420</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>1.661</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>3 vs 2</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ASMR (direct)</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0.9597</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0.947</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0.973</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>All Ages</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>0.9642</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>0.952</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>0.977</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>1920</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>0.7777</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>0.732</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>0.826</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>1930</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0.9508</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0.925</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0.977</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>1940</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>1.0308</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>1.006</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>1.056</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>1950</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>0.9166</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>0.891</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>0.943</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>1.0962</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>1.050</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>1.144</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>1970</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.8424</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>0.793</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>0.895</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>0.9605</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>0.863</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>1.069</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>0.8964</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>0.759</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>1.059</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>1.4488</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>1.121</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>1.872</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E132"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
forced to be LINEAR fit only
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -497,17 +497,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1649</t>
+          <t>1.3933</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.368</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.419</t>
         </is>
       </c>
     </row>
@@ -520,17 +520,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.5829</t>
+          <t>1.5595</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.558</t>
+          <t>1.535</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.608</t>
+          <t>1.584</t>
         </is>
       </c>
     </row>
@@ -543,17 +543,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.7960</t>
+          <t>0.8778</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.823</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.936</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8271</t>
+          <t>1.1126</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.802</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>1.147</t>
         </is>
       </c>
     </row>
@@ -589,17 +589,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4488</t>
+          <t>1.7086</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.417</t>
+          <t>1.671</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.747</t>
         </is>
       </c>
     </row>
@@ -612,17 +612,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4716</t>
+          <t>1.6673</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.389</t>
+          <t>1.574</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.766</t>
         </is>
       </c>
     </row>
@@ -768,17 +768,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.2611</t>
+          <t>1.5062</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>1.481</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.532</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.8521</t>
+          <t>1.8247</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.829</t>
+          <t>1.802</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.875</t>
+          <t>1.847</t>
         </is>
       </c>
     </row>
@@ -814,17 +814,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.1341</t>
+          <t>1.2507</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.207</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.175</t>
+          <t>1.295</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2374</t>
+          <t>1.6646</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.632</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.697</t>
         </is>
       </c>
     </row>
@@ -860,17 +860,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.4619</t>
+          <t>1.7241</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.676</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.504</t>
+          <t>1.774</t>
         </is>
       </c>
     </row>
@@ -883,17 +883,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0628</t>
+          <t>1.2041</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.004</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.274</t>
         </is>
       </c>
     </row>
@@ -1367,17 +1367,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9028</t>
+          <t>1.1440</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.5300</t>
+          <t>1.4941</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.507</t>
+          <t>1.472</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.553</t>
+          <t>1.516</t>
         </is>
       </c>
     </row>
@@ -1413,17 +1413,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6374</t>
+          <t>0.6791</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.587</t>
+          <t>0.626</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.692</t>
+          <t>0.737</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.7403</t>
+          <t>1.0028</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.712</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.770</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
@@ -1459,17 +1459,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.9179</t>
+          <t>1.1946</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>1.163</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>1.227</t>
         </is>
       </c>
     </row>
@@ -1482,17 +1482,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2600</t>
+          <t>1.6221</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.580</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.666</t>
         </is>
       </c>
     </row>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2956</t>
+          <t>1.4516</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.237</t>
+          <t>1.386</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.357</t>
+          <t>1.520</t>
         </is>
       </c>
     </row>
@@ -1638,17 +1638,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9259</t>
+          <t>1.1724</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>1.157</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>1.188</t>
         </is>
       </c>
     </row>
@@ -1661,17 +1661,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.4400</t>
+          <t>1.4053</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.424</t>
+          <t>1.389</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.457</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -1684,17 +1684,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8404</t>
+          <t>0.9038</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.810</t>
+          <t>0.871</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>0.938</t>
         </is>
       </c>
     </row>
@@ -1707,17 +1707,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.7868</t>
+          <t>1.0657</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.771</t>
+          <t>1.044</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>1.088</t>
         </is>
       </c>
     </row>
@@ -1730,17 +1730,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0521</t>
+          <t>1.3693</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.341</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -1753,17 +1753,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.8887</t>
+          <t>1.1442</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>1.100</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.924</t>
+          <t>1.190</t>
         </is>
       </c>
     </row>
@@ -1776,17 +1776,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2729</t>
+          <t>1.4262</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.328</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.367</t>
+          <t>1.532</t>
         </is>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0267</t>
+          <t>1.0277</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
@@ -1932,17 +1932,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.9412</t>
+          <t>0.9406</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.927</t>
+          <t>0.926</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.955</t>
         </is>
       </c>
     </row>
@@ -1955,17 +1955,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3185</t>
+          <t>1.3309</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.429</t>
+          <t>1.442</t>
         </is>
       </c>
     </row>
@@ -2237,17 +2237,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.7427</t>
+          <t>0.9611</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.727</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.759</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2602</t>
+          <t>1.2303</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>1.209</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.252</t>
         </is>
       </c>
     </row>
@@ -2283,17 +2283,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.5136</t>
+          <t>0.5876</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.467</t>
+          <t>0.534</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.565</t>
+          <t>0.647</t>
         </is>
       </c>
     </row>
@@ -2306,17 +2306,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.6799</t>
+          <t>0.9032</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.650</t>
+          <t>0.863</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.711</t>
+          <t>0.945</t>
         </is>
       </c>
     </row>
@@ -2329,17 +2329,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.6884</t>
+          <t>0.9572</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.665</t>
+          <t>0.925</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.713</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -2352,17 +2352,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9287</t>
+          <t>1.2414</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.899</t>
+          <t>1.202</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>1.282</t>
         </is>
       </c>
     </row>
@@ -2375,17 +2375,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0338</t>
+          <t>1.1506</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>1.099</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8666</t>
+          <t>1.1216</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -2531,17 +2531,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3808</t>
+          <t>1.3480</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.333</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.363</t>
         </is>
       </c>
     </row>
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.7337</t>
+          <t>0.8394</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>0.808</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.762</t>
+          <t>0.872</t>
         </is>
       </c>
     </row>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.7588</t>
+          <t>1.0080</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.743</t>
+          <t>0.987</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.775</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -2600,17 +2600,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.8412</t>
+          <t>1.1697</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.824</t>
+          <t>1.146</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>1.194</t>
         </is>
       </c>
     </row>
@@ -2623,17 +2623,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0926</t>
+          <t>1.4605</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.063</t>
+          <t>1.420</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.502</t>
         </is>
       </c>
     </row>
@@ -2646,17 +2646,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0083</t>
+          <t>1.1222</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>1.062</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.185</t>
         </is>
       </c>
     </row>
@@ -3107,17 +3107,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.5044</t>
+          <t>0.5920</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.492</t>
+          <t>0.577</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.517</t>
+          <t>0.607</t>
         </is>
       </c>
     </row>
@@ -3130,17 +3130,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8870</t>
+          <t>0.8511</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.868</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.906</t>
+          <t>0.870</t>
         </is>
       </c>
     </row>
@@ -3153,17 +3153,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.2138</t>
+          <t>0.2325</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.189</t>
+          <t>0.205</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.242</t>
+          <t>0.263</t>
         </is>
       </c>
     </row>
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.5461</t>
+          <t>0.5703</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.517</t>
+          <t>0.540</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.577</t>
+          <t>0.603</t>
         </is>
       </c>
     </row>
@@ -3199,17 +3199,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.4641</t>
+          <t>0.6048</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.445</t>
+          <t>0.580</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.484</t>
+          <t>0.631</t>
         </is>
       </c>
     </row>
@@ -3222,17 +3222,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.5325</t>
+          <t>0.6974</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.510</t>
+          <t>0.668</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.556</t>
+          <t>0.729</t>
         </is>
       </c>
     </row>
@@ -3245,17 +3245,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8361</t>
+          <t>0.9134</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.860</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -3268,17 +3268,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0132</t>
+          <t>1.0337</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.9686</t>
+          <t>1.9685</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3378,17 +3378,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.7646</t>
+          <t>0.9579</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.758</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.771</t>
+          <t>0.966</t>
         </is>
       </c>
     </row>
@@ -3401,17 +3401,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.4680</t>
+          <t>1.3946</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.456</t>
+          <t>1.383</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.480</t>
+          <t>1.406</t>
         </is>
       </c>
     </row>
@@ -3424,17 +3424,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.6289</t>
+          <t>0.6841</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.609</t>
+          <t>0.662</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.650</t>
+          <t>0.707</t>
         </is>
       </c>
     </row>
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.6360</t>
+          <t>0.8251</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.626</t>
+          <t>0.812</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.646</t>
+          <t>0.839</t>
         </is>
       </c>
     </row>
@@ -3470,17 +3470,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.8149</t>
+          <t>1.0620</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.827</t>
+          <t>1.078</t>
         </is>
       </c>
     </row>
@@ -3493,17 +3493,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.8153</t>
+          <t>1.0679</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>1.048</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.830</t>
+          <t>1.088</t>
         </is>
       </c>
     </row>
@@ -3516,17 +3516,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2804</t>
+          <t>1.3986</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.360</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.438</t>
         </is>
       </c>
     </row>
@@ -3539,17 +3539,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.0441</t>
+          <t>1.0652</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -3649,17 +3649,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.5158</t>
+          <t>1.6179</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.479</t>
+          <t>1.579</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.554</t>
+          <t>1.658</t>
         </is>
       </c>
     </row>
@@ -3672,17 +3672,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.6550</t>
+          <t>1.6386</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.620</t>
+          <t>1.604</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.690</t>
+          <t>1.674</t>
         </is>
       </c>
     </row>
@@ -3718,17 +3718,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.1646</t>
+          <t>1.4469</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>1.371</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.229</t>
+          <t>1.527</t>
         </is>
       </c>
     </row>
@@ -3977,17 +3977,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9268</t>
+          <t>0.9413</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.867</t>
+          <t>0.881</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -4000,17 +4000,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9384</t>
+          <t>0.9405</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.007</t>
         </is>
       </c>
     </row>
@@ -4023,17 +4023,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8436</t>
+          <t>0.9059</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.621</t>
+          <t>0.667</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.231</t>
         </is>
       </c>
     </row>
@@ -4046,17 +4046,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1505</t>
+          <t>1.1784</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.301</t>
+          <t>1.334</t>
         </is>
       </c>
     </row>
@@ -4069,17 +4069,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8210</t>
+          <t>0.8521</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.721</t>
+          <t>0.747</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.973</t>
         </is>
       </c>
     </row>
@@ -4092,17 +4092,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9008</t>
+          <t>0.9074</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.773</t>
+          <t>0.777</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>
@@ -4115,17 +4115,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9398</t>
+          <t>0.8141</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.761</t>
+          <t>0.657</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.160</t>
+          <t>1.008</t>
         </is>
       </c>
     </row>
@@ -4138,17 +4138,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0740</t>
+          <t>1.0414</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.821</t>
+          <t>0.795</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.364</t>
         </is>
       </c>
     </row>
@@ -4161,17 +4161,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9242</t>
+          <t>0.9602</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.619</t>
+          <t>0.643</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.379</t>
+          <t>1.433</t>
         </is>
       </c>
     </row>
@@ -4248,17 +4248,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0598</t>
+          <t>1.0764</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.053</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.101</t>
         </is>
       </c>
     </row>
@@ -4271,17 +4271,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0955</t>
+          <t>1.0937</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.070</t>
+          <t>1.069</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.119</t>
         </is>
       </c>
     </row>
@@ -4294,17 +4294,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8910</t>
+          <t>0.8931</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.818</t>
+          <t>0.820</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.973</t>
         </is>
       </c>
     </row>
@@ -4317,17 +4317,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0816</t>
+          <t>1.0467</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.132</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -4340,17 +4340,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0588</t>
+          <t>1.0978</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.105</t>
+          <t>1.147</t>
         </is>
       </c>
     </row>
@@ -4363,17 +4363,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1225</t>
+          <t>1.1602</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.103</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.220</t>
         </is>
       </c>
     </row>
@@ -4386,17 +4386,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8739</t>
+          <t>0.9113</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -4409,17 +4409,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1931</t>
+          <t>1.2032</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -4432,17 +4432,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1020</t>
+          <t>1.1448</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.946</t>
+          <t>0.982</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.284</t>
+          <t>1.334</t>
         </is>
       </c>
     </row>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>1.068</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -4542,17 +4542,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1673</t>
+          <t>1.1629</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>1.085</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.251</t>
+          <t>1.246</t>
         </is>
       </c>
     </row>
@@ -4565,17 +4565,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.0561</t>
+          <t>0.9858</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.774</t>
+          <t>0.723</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.345</t>
         </is>
       </c>
     </row>
@@ -4588,17 +4588,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9401</t>
+          <t>0.8883</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.830</t>
+          <t>0.784</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.007</t>
         </is>
       </c>
     </row>
@@ -4611,17 +4611,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.2896</t>
+          <t>1.2882</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.132</t>
+          <t>1.128</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.469</t>
+          <t>1.471</t>
         </is>
       </c>
     </row>
@@ -4634,17 +4634,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.2461</t>
+          <t>1.2787</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.094</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.495</t>
         </is>
       </c>
     </row>
@@ -4657,17 +4657,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9299</t>
+          <t>1.1195</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.752</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.390</t>
         </is>
       </c>
     </row>
@@ -4680,17 +4680,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.1109</t>
+          <t>1.1554</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.456</t>
+          <t>1.517</t>
         </is>
       </c>
     </row>
@@ -4790,17 +4790,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.2467</t>
+          <t>1.4111</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.225</t>
+          <t>1.386</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.437</t>
         </is>
       </c>
     </row>
@@ -4813,17 +4813,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.5735</t>
+          <t>1.5542</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.526</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.603</t>
+          <t>1.583</t>
         </is>
       </c>
     </row>
@@ -4836,17 +4836,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.0789</t>
+          <t>1.1586</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.091</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.145</t>
+          <t>1.230</t>
         </is>
       </c>
     </row>
@@ -4859,17 +4859,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.2369</t>
+          <t>1.3822</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>1.335</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.280</t>
+          <t>1.431</t>
         </is>
       </c>
     </row>
@@ -4882,17 +4882,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.2941</t>
+          <t>1.5137</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.251</t>
+          <t>1.463</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.339</t>
+          <t>1.567</t>
         </is>
       </c>
     </row>
@@ -4905,17 +4905,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.3029</t>
+          <t>1.5111</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.449</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.358</t>
+          <t>1.576</t>
         </is>
       </c>
     </row>
@@ -4928,17 +4928,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0192</t>
+          <t>1.0628</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -4951,17 +4951,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.3025</t>
+          <t>1.3136</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.192</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.435</t>
+          <t>1.447</t>
         </is>
       </c>
     </row>
@@ -4974,17 +4974,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.1996</t>
+          <t>1.2463</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.013</t>
+          <t>1.052</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.420</t>
+          <t>1.476</t>
         </is>
       </c>
     </row>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.3451</t>
+          <t>1.4997</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.260</t>
+          <t>1.405</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.436</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.6767</t>
+          <t>1.6525</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.544</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.795</t>
+          <t>1.768</t>
         </is>
       </c>
     </row>
@@ -5130,17 +5130,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0751</t>
+          <t>1.1729</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.324</t>
         </is>
       </c>
     </row>
@@ -5153,17 +5153,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.5762</t>
+          <t>1.7763</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.387</t>
+          <t>1.560</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.791</t>
+          <t>2.023</t>
         </is>
       </c>
     </row>
@@ -5176,17 +5176,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.4463</t>
+          <t>1.6654</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.244</t>
+          <t>1.428</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.682</t>
+          <t>1.942</t>
         </is>
       </c>
     </row>
@@ -5199,17 +5199,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1.0844</t>
+          <t>1.3056</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>1.054</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1.339</t>
+          <t>1.617</t>
         </is>
       </c>
     </row>
@@ -5222,17 +5222,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.2128</t>
+          <t>1.2614</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.925</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.591</t>
+          <t>1.657</t>
         </is>
       </c>
     </row>
@@ -5332,17 +5332,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.1764</t>
+          <t>1.3110</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.154</t>
+          <t>1.286</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.200</t>
+          <t>1.337</t>
         </is>
       </c>
     </row>
@@ -5355,17 +5355,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.4364</t>
+          <t>1.4210</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.408</t>
+          <t>1.393</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.466</t>
+          <t>1.450</t>
         </is>
       </c>
     </row>
@@ -5378,17 +5378,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.2109</t>
+          <t>1.2973</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.199</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.310</t>
+          <t>1.404</t>
         </is>
       </c>
     </row>
@@ -5401,17 +5401,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.1436</t>
+          <t>1.3205</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>1.270</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.373</t>
         </is>
       </c>
     </row>
@@ -5424,17 +5424,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.2223</t>
+          <t>1.3788</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.329</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.268</t>
+          <t>1.430</t>
         </is>
       </c>
     </row>
@@ -5447,17 +5447,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.1607</t>
+          <t>1.3025</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.246</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.362</t>
         </is>
       </c>
     </row>
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0175</t>
+          <t>0.9655</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.019</t>
         </is>
       </c>
     </row>
@@ -5683,17 +5683,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8698</t>
+          <t>0.8757</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.923</t>
         </is>
       </c>
     </row>
@@ -5706,17 +5706,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.4332</t>
+          <t>0.4515</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.344</t>
+          <t>0.358</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.546</t>
+          <t>0.569</t>
         </is>
       </c>
     </row>
@@ -5729,17 +5729,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.3347</t>
+          <t>1.2649</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.203</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.406</t>
         </is>
       </c>
     </row>
@@ -5752,17 +5752,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1845</t>
+          <t>1.2618</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.139</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.313</t>
+          <t>1.399</t>
         </is>
       </c>
     </row>
@@ -5775,17 +5775,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.7216</t>
+          <t>0.5530</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.639</t>
+          <t>0.489</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.625</t>
         </is>
       </c>
     </row>
@@ -5798,17 +5798,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0531</t>
+          <t>1.0504</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.225</t>
         </is>
       </c>
     </row>
@@ -5821,17 +5821,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.4149</t>
+          <t>1.4044</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.154</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.722</t>
+          <t>1.709</t>
         </is>
       </c>
     </row>
@@ -5890,17 +5890,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.1273</t>
+          <t>1.0460</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.580</t>
+          <t>0.538</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.192</t>
+          <t>2.035</t>
         </is>
       </c>
     </row>
@@ -5931,17 +5931,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9985</t>
+          <t>1.0182</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.034</t>
         </is>
       </c>
     </row>
@@ -5954,17 +5954,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0596</t>
+          <t>1.0622</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.076</t>
+          <t>1.079</t>
         </is>
       </c>
     </row>
@@ -5977,17 +5977,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9040</t>
+          <t>0.9420</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>1.009</t>
         </is>
       </c>
     </row>
@@ -6000,17 +6000,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0521</t>
+          <t>1.0452</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.018</t>
+          <t>1.011</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.080</t>
         </is>
       </c>
     </row>
@@ -6023,17 +6023,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0457</t>
+          <t>1.0552</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.025</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.087</t>
         </is>
       </c>
     </row>
@@ -6046,17 +6046,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.8991</t>
+          <t>0.9694</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>1.002</t>
         </is>
       </c>
     </row>
@@ -6069,17 +6069,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8996</t>
+          <t>0.8972</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.860</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>0.939</t>
         </is>
       </c>
     </row>
@@ -6092,17 +6092,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1982</t>
+          <t>1.1893</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.119</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.273</t>
+          <t>1.264</t>
         </is>
       </c>
     </row>
@@ -6138,17 +6138,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9643</t>
+          <t>0.8963</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.840</t>
+          <t>0.780</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.030</t>
         </is>
       </c>
     </row>
@@ -6161,17 +6161,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.0061</t>
+          <t>1.0430</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.835</t>
+          <t>0.865</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.257</t>
         </is>
       </c>
     </row>
@@ -6202,17 +6202,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9812</t>
+          <t>1.0545</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.999</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.036</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -6225,17 +6225,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2182</t>
+          <t>1.2130</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.155</t>
+          <t>1.150</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.284</t>
+          <t>1.279</t>
         </is>
       </c>
     </row>
@@ -6271,17 +6271,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.7883</t>
+          <t>0.8263</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.710</t>
+          <t>0.743</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.919</t>
         </is>
       </c>
     </row>
@@ -6294,17 +6294,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8828</t>
+          <t>0.8362</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.796</t>
+          <t>0.754</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.927</t>
         </is>
       </c>
     </row>
@@ -6317,17 +6317,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.2460</t>
+          <t>1.7530</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.549</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.409</t>
+          <t>1.984</t>
         </is>
       </c>
     </row>
@@ -6409,17 +6409,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.8024</t>
+          <t>2.6050</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.777</t>
+          <t>1.651</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4.420</t>
+          <t>4.109</t>
         </is>
       </c>
     </row>
@@ -6473,17 +6473,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9424</t>
+          <t>0.9772</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.989</t>
         </is>
       </c>
     </row>
@@ -6496,17 +6496,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.1927</t>
+          <t>1.1755</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.162</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.207</t>
+          <t>1.189</t>
         </is>
       </c>
     </row>
@@ -6519,17 +6519,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.7030</t>
+          <t>0.7326</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.671</t>
+          <t>0.699</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.737</t>
+          <t>0.768</t>
         </is>
       </c>
     </row>
@@ -6542,17 +6542,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.9871</t>
+          <t>0.9938</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.971</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.010</t>
+          <t>1.017</t>
         </is>
       </c>
     </row>
@@ -6565,17 +6565,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0210</t>
+          <t>1.0876</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.064</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.112</t>
         </is>
       </c>
     </row>
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8421</t>
+          <t>0.8885</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.866</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.864</t>
+          <t>0.912</t>
         </is>
       </c>
     </row>
@@ -6611,17 +6611,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9861</t>
+          <t>0.9835</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.946</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.022</t>
         </is>
       </c>
     </row>
@@ -6634,17 +6634,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.0094</t>
+          <t>1.0019</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>
@@ -6703,17 +6703,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.4577</t>
+          <t>1.5112</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.177</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.871</t>
+          <t>1.941</t>
         </is>
       </c>
     </row>
@@ -6744,17 +6744,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9248</t>
+          <t>1.0106</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -6767,17 +6767,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3712</t>
+          <t>1.3423</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.302</t>
+          <t>1.274</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.444</t>
+          <t>1.414</t>
         </is>
       </c>
     </row>
@@ -6813,17 +6813,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.7396</t>
+          <t>0.7857</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.708</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.872</t>
         </is>
       </c>
     </row>
@@ -6859,17 +6859,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.1670</t>
+          <t>1.6068</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>1.422</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.815</t>
         </is>
       </c>
     </row>
@@ -7015,17 +7015,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.9439</t>
+          <t>0.9597</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.973</t>
         </is>
       </c>
     </row>
@@ -7038,17 +7038,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.1256</t>
+          <t>1.1066</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>1.092</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.121</t>
         </is>
       </c>
     </row>
@@ -7084,17 +7084,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>0.9382</t>
+          <t>0.9508</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>0.925</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.977</t>
         </is>
       </c>
     </row>
@@ -7107,17 +7107,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.9764</t>
+          <t>1.0308</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.953</t>
+          <t>1.006</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -7130,17 +7130,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.9365</t>
+          <t>0.9166</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.910</t>
+          <t>0.891</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.943</t>
         </is>
       </c>
     </row>
@@ -7222,17 +7222,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.8332</t>
+          <t>0.8964</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.705</t>
+          <t>0.759</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>1.059</t>
         </is>
       </c>
     </row>
@@ -7343,17 +7343,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1084</t>
+          <t>1.0732</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>1.156</t>
         </is>
       </c>
     </row>
@@ -7366,17 +7366,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9776</t>
+          <t>0.9465</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.906</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -7389,17 +7389,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.7925</t>
+          <t>2.2692</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.326</t>
+          <t>1.679</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.422</t>
+          <t>3.067</t>
         </is>
       </c>
     </row>
@@ -7412,17 +7412,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9651</t>
+          <t>0.9468</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.835</t>
+          <t>0.818</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -7435,17 +7435,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.9693</t>
+          <t>0.8850</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.837</t>
+          <t>0.764</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.123</t>
+          <t>1.026</t>
         </is>
       </c>
     </row>
@@ -7458,17 +7458,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2774</t>
+          <t>1.1913</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.522</t>
+          <t>1.419</t>
         </is>
       </c>
     </row>
@@ -7481,17 +7481,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.6459</t>
+          <t>1.7992</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.308</t>
+          <t>1.429</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.072</t>
+          <t>2.265</t>
         </is>
       </c>
     </row>
@@ -7504,17 +7504,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9478</t>
+          <t>0.8380</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.708</t>
+          <t>0.625</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.269</t>
+          <t>1.123</t>
         </is>
       </c>
     </row>
@@ -7573,17 +7573,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.4345</t>
+          <t>1.3982</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.586</t>
+          <t>0.571</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3.513</t>
+          <t>3.425</t>
         </is>
       </c>
     </row>
@@ -7614,17 +7614,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9221</t>
+          <t>1.0057</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.983</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -7637,17 +7637,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0814</t>
+          <t>1.0362</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.012</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -7660,17 +7660,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2660</t>
+          <t>1.6028</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.446</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.403</t>
+          <t>1.777</t>
         </is>
       </c>
     </row>
@@ -7683,17 +7683,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8688</t>
+          <t>0.9559</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.827</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -7706,17 +7706,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9096</t>
+          <t>0.9561</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.999</t>
         </is>
       </c>
     </row>
@@ -7729,17 +7729,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9783</t>
+          <t>1.0855</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.142</t>
         </is>
       </c>
     </row>
@@ -7752,17 +7752,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8235</t>
+          <t>0.9002</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.770</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.963</t>
         </is>
       </c>
     </row>
@@ -7775,17 +7775,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.7731</t>
+          <t>0.8513</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.707</t>
+          <t>0.778</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.932</t>
         </is>
       </c>
     </row>
@@ -7844,17 +7844,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.4351</t>
+          <t>0.4638</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.327</t>
+          <t>0.348</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.580</t>
+          <t>0.618</t>
         </is>
       </c>
     </row>
@@ -7885,17 +7885,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.8313</t>
+          <t>0.9376</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.770</t>
+          <t>0.870</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>1.011</t>
         </is>
       </c>
     </row>
@@ -7908,17 +7908,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1061</t>
+          <t>1.0948</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -7954,17 +7954,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9003</t>
+          <t>1.0096</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.871</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.170</t>
         </is>
       </c>
     </row>
@@ -7977,17 +7977,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.9384</t>
+          <t>1.0803</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.809</t>
+          <t>0.931</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>1.253</t>
         </is>
       </c>
     </row>
@@ -8000,17 +8000,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.7659</t>
+          <t>0.9112</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.642</t>
+          <t>0.764</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>1.086</t>
         </is>
       </c>
     </row>
@@ -8046,17 +8046,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8156</t>
+          <t>1.0158</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.608</t>
+          <t>0.756</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -8156,17 +8156,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0258</t>
+          <t>1.0504</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.069</t>
         </is>
       </c>
     </row>
@@ -8179,17 +8179,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.1042</t>
+          <t>1.0753</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.056</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>1.095</t>
         </is>
       </c>
     </row>
@@ -8202,17 +8202,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.9080</t>
+          <t>0.9916</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.921</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>1.067</t>
         </is>
       </c>
     </row>
@@ -8225,17 +8225,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0112</t>
+          <t>1.0005</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>0.965</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.037</t>
         </is>
       </c>
     </row>
@@ -8248,17 +8248,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0860</t>
+          <t>1.0706</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.035</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.123</t>
+          <t>1.107</t>
         </is>
       </c>
     </row>
@@ -8271,17 +8271,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.0077</t>
+          <t>1.0947</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -8294,17 +8294,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9383</t>
+          <t>1.0258</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.886</t>
+          <t>0.968</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.994</t>
+          <t>1.087</t>
         </is>
       </c>
     </row>
@@ -8317,17 +8317,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.8784</t>
+          <t>0.9672</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.809</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -8386,17 +8386,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.6381</t>
+          <t>0.6803</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.442</t>
+          <t>0.471</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -8427,17 +8427,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9215</t>
+          <t>0.9747</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.905</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.993</t>
+          <t>1.049</t>
         </is>
       </c>
     </row>
@@ -8450,17 +8450,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.1295</t>
+          <t>1.1360</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.054</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.217</t>
+          <t>1.224</t>
         </is>
       </c>
     </row>
@@ -8473,17 +8473,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.5066</t>
+          <t>0.4370</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.376</t>
+          <t>0.324</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.683</t>
+          <t>0.589</t>
         </is>
       </c>
     </row>
@@ -8496,17 +8496,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0478</t>
+          <t>1.0568</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.908</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.209</t>
+          <t>1.220</t>
         </is>
       </c>
     </row>
@@ -8519,17 +8519,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.1204</t>
+          <t>1.2097</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.969</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.295</t>
+          <t>1.399</t>
         </is>
       </c>
     </row>
@@ -8542,17 +8542,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.7889</t>
+          <t>0.9189</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.663</t>
+          <t>0.773</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>1.092</t>
         </is>
       </c>
     </row>
@@ -8588,17 +8588,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>0.9267</t>
+          <t>1.1542</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.692</t>
+          <t>0.861</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.547</t>
         </is>
       </c>
     </row>
@@ -8698,17 +8698,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.1125</t>
+          <t>1.0445</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.023</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -8721,17 +8721,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.0211</t>
+          <t>1.0377</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>1.060</t>
         </is>
       </c>
     </row>
@@ -8744,17 +8744,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.7172</t>
+          <t>0.6187</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.653</t>
+          <t>0.563</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.680</t>
         </is>
       </c>
     </row>
@@ -8767,17 +8767,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.1639</t>
+          <t>1.0467</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.094</t>
         </is>
       </c>
     </row>
@@ -8790,17 +8790,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.1940</t>
+          <t>1.1198</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>1.163</t>
         </is>
       </c>
     </row>
@@ -8813,17 +8813,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.0301</t>
+          <t>1.0084</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.054</t>
         </is>
       </c>
     </row>
@@ -8969,17 +8969,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0.9546</t>
+          <t>1.1338</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>1.161</t>
         </is>
       </c>
     </row>
@@ -8992,17 +8992,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.2877</t>
+          <t>1.2059</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.259</t>
+          <t>1.180</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.317</t>
+          <t>1.233</t>
         </is>
       </c>
     </row>
@@ -9015,17 +9015,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.8789</t>
+          <t>1.1126</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>1.027</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0.952</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -9038,17 +9038,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>0.8359</t>
+          <t>1.0357</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.995</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>1.078</t>
         </is>
       </c>
     </row>
@@ -9061,17 +9061,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>0.8953</t>
+          <t>1.0422</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>0.860</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>1.085</t>
         </is>
       </c>
     </row>
@@ -9084,17 +9084,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>0.9811</t>
+          <t>1.2076</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>1.145</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.274</t>
         </is>
       </c>
     </row>
@@ -9107,17 +9107,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.2386</t>
+          <t>1.3540</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.223</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.499</t>
         </is>
       </c>
     </row>
@@ -9130,17 +9130,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2.4023</t>
+          <t>2.6452</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.008</t>
+          <t>2.211</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2.874</t>
+          <t>3.165</t>
         </is>
       </c>
     </row>
@@ -9199,17 +9199,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>4.0410</t>
+          <t>3.9388</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.491</t>
+          <t>1.453</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>10.951</t>
+          <t>10.675</t>
         </is>
       </c>
     </row>
@@ -9240,17 +9240,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0.8582</t>
+          <t>1.0552</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.795</t>
+          <t>0.979</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>1.138</t>
         </is>
       </c>
     </row>
@@ -9263,17 +9263,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1.3171</t>
+          <t>1.2740</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1.221</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.374</t>
         </is>
       </c>
     </row>
@@ -9309,17 +9309,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0.8661</t>
+          <t>1.0940</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.946</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.265</t>
         </is>
       </c>
     </row>
@@ -9332,17 +9332,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0.9237</t>
+          <t>1.1776</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>1.016</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1.070</t>
+          <t>1.365</t>
         </is>
       </c>
     </row>
@@ -9355,17 +9355,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>0.7681</t>
+          <t>1.0137</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.850</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>1.209</t>
         </is>
       </c>
     </row>
@@ -9401,17 +9401,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2.5345</t>
+          <t>3.1565</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>1.818</t>
+          <t>2.261</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3.534</t>
+          <t>4.406</t>
         </is>
       </c>
     </row>
@@ -9511,17 +9511,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>1.0332</t>
+          <t>1.1251</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.096</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.155</t>
         </is>
       </c>
     </row>
@@ -9534,17 +9534,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1.1908</t>
+          <t>1.1637</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.136</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.193</t>
         </is>
       </c>
     </row>
@@ -9580,17 +9580,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>0.9620</t>
+          <t>1.0836</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>0.918</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -9603,17 +9603,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>0.9843</t>
+          <t>1.0901</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -9626,17 +9626,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1.0029</t>
+          <t>1.1125</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>0.948</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -9782,17 +9782,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>0.9294</t>
+          <t>1.0782</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>1.102</t>
         </is>
       </c>
     </row>
@@ -9805,17 +9805,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1.1662</t>
+          <t>1.1215</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>1.144</t>
+          <t>1.100</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.143</t>
         </is>
       </c>
     </row>
@@ -9828,17 +9828,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>0.9679</t>
+          <t>1.1220</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>1.047</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -9851,17 +9851,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>0.8266</t>
+          <t>1.0352</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.800</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>0.854</t>
+          <t>1.069</t>
         </is>
       </c>
     </row>
@@ -9874,17 +9874,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>0.8244</t>
+          <t>0.9735</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>0.797</t>
+          <t>0.942</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>0.852</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -9897,17 +9897,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>0.9736</t>
+          <t>1.1032</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>0.928</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.157</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
prior to slope7 changes
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -497,17 +497,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3933</t>
+          <t>1.1752</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.368</t>
+          <t>1.154</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.419</t>
+          <t>1.197</t>
         </is>
       </c>
     </row>
@@ -520,17 +520,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.5595</t>
+          <t>1.5842</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.535</t>
+          <t>1.559</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.584</t>
+          <t>1.609</t>
         </is>
       </c>
     </row>
@@ -543,17 +543,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8778</t>
+          <t>0.8202</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.823</t>
+          <t>0.769</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.875</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1126</t>
+          <t>0.8467</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>0.821</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.147</t>
+          <t>0.873</t>
         </is>
       </c>
     </row>
@@ -589,17 +589,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.7086</t>
+          <t>1.4416</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.671</t>
+          <t>1.410</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.747</t>
+          <t>1.474</t>
         </is>
       </c>
     </row>
@@ -612,17 +612,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.6673</t>
+          <t>1.4717</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.574</t>
+          <t>1.390</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.766</t>
+          <t>1.559</t>
         </is>
       </c>
     </row>
@@ -768,17 +768,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.5062</t>
+          <t>1.2721</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.251</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.532</t>
+          <t>1.294</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.8247</t>
+          <t>1.8536</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.802</t>
+          <t>1.831</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.847</t>
+          <t>1.877</t>
         </is>
       </c>
     </row>
@@ -814,17 +814,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2507</t>
+          <t>1.1686</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.207</t>
+          <t>1.128</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.295</t>
+          <t>1.210</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.6646</t>
+          <t>1.2667</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.632</t>
+          <t>1.242</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.697</t>
+          <t>1.292</t>
         </is>
       </c>
     </row>
@@ -860,17 +860,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.7241</t>
+          <t>1.4547</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.676</t>
+          <t>1.414</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.774</t>
+          <t>1.497</t>
         </is>
       </c>
     </row>
@@ -883,17 +883,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.2041</t>
+          <t>1.0628</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.004</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.274</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -1367,17 +1367,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1440</t>
+          <t>0.9016</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>0.886</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.164</t>
+          <t>0.918</t>
         </is>
       </c>
     </row>
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.4941</t>
+          <t>1.5311</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.472</t>
+          <t>1.508</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.516</t>
+          <t>1.554</t>
         </is>
       </c>
     </row>
@@ -1413,17 +1413,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6791</t>
+          <t>0.6361</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.626</t>
+          <t>0.586</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.737</t>
+          <t>0.690</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0028</t>
+          <t>0.7374</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.709</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>0.767</t>
         </is>
       </c>
     </row>
@@ -1459,17 +1459,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1946</t>
+          <t>0.9156</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>0.892</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>0.940</t>
         </is>
       </c>
     </row>
@@ -1482,17 +1482,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.6221</t>
+          <t>1.2711</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.238</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.666</t>
+          <t>1.305</t>
         </is>
       </c>
     </row>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.4516</t>
+          <t>1.2784</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.386</t>
+          <t>1.221</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.520</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -1638,17 +1638,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1724</t>
+          <t>0.9249</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>0.913</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>0.937</t>
         </is>
       </c>
     </row>
@@ -1661,17 +1661,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.4053</t>
+          <t>1.4402</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.389</t>
+          <t>1.424</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.457</t>
         </is>
       </c>
     </row>
@@ -1684,17 +1684,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9038</t>
+          <t>0.8403</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.810</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>0.872</t>
         </is>
       </c>
     </row>
@@ -1707,17 +1707,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0657</t>
+          <t>0.7837</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>0.768</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>0.800</t>
         </is>
       </c>
     </row>
@@ -1730,17 +1730,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3693</t>
+          <t>1.0495</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.341</t>
+          <t>1.028</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.398</t>
+          <t>1.072</t>
         </is>
       </c>
     </row>
@@ -1753,17 +1753,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1442</t>
+          <t>0.8966</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>0.932</t>
         </is>
       </c>
     </row>
@@ -1776,17 +1776,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.4262</t>
+          <t>1.2560</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.328</t>
+          <t>1.170</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.532</t>
+          <t>1.349</t>
         </is>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0277</t>
+          <t>1.0269</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1955,17 +1955,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3309</t>
+          <t>1.3210</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.442</t>
+          <t>1.431</t>
         </is>
       </c>
     </row>
@@ -2237,17 +2237,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9611</t>
+          <t>0.7470</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.941</t>
+          <t>0.731</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.763</t>
         </is>
       </c>
     </row>
@@ -2260,17 +2260,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.2303</t>
+          <t>1.2617</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.209</t>
+          <t>1.240</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>1.284</t>
         </is>
       </c>
     </row>
@@ -2283,17 +2283,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.5876</t>
+          <t>0.5352</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.534</t>
+          <t>0.486</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.647</t>
+          <t>0.589</t>
         </is>
       </c>
     </row>
@@ -2306,17 +2306,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9032</t>
+          <t>0.6739</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.863</t>
+          <t>0.644</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.945</t>
+          <t>0.705</t>
         </is>
       </c>
     </row>
@@ -2329,17 +2329,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.9572</t>
+          <t>0.6911</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.925</t>
+          <t>0.668</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.716</t>
         </is>
       </c>
     </row>
@@ -2352,17 +2352,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.2414</t>
+          <t>0.9492</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>0.919</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.282</t>
+          <t>0.981</t>
         </is>
       </c>
     </row>
@@ -2375,17 +2375,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1506</t>
+          <t>1.0356</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.099</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.085</t>
         </is>
       </c>
     </row>
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1216</t>
+          <t>0.8718</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>0.861</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>0.883</t>
         </is>
       </c>
     </row>
@@ -2531,17 +2531,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3480</t>
+          <t>1.3824</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.367</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.363</t>
+          <t>1.398</t>
         </is>
       </c>
     </row>
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8394</t>
+          <t>0.7645</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.808</t>
+          <t>0.736</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>0.794</t>
         </is>
       </c>
     </row>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0080</t>
+          <t>0.7520</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.736</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.768</t>
         </is>
       </c>
     </row>
@@ -2600,17 +2600,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1697</t>
+          <t>0.8445</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>0.827</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>0.862</t>
         </is>
       </c>
     </row>
@@ -2623,17 +2623,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.4605</t>
+          <t>1.1167</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.420</t>
+          <t>1.086</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.502</t>
+          <t>1.148</t>
         </is>
       </c>
     </row>
@@ -2646,17 +2646,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.1222</t>
+          <t>1.0100</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.062</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.067</t>
         </is>
       </c>
     </row>
@@ -3107,17 +3107,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.5920</t>
+          <t>0.5225</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.577</t>
+          <t>0.510</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.607</t>
+          <t>0.536</t>
         </is>
       </c>
     </row>
@@ -3130,17 +3130,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8511</t>
+          <t>0.8814</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.863</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>0.901</t>
         </is>
       </c>
     </row>
@@ -3153,17 +3153,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.2325</t>
+          <t>0.2130</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.205</t>
+          <t>0.188</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.263</t>
+          <t>0.241</t>
         </is>
       </c>
     </row>
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.5703</t>
+          <t>0.5989</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.540</t>
+          <t>0.567</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.603</t>
+          <t>0.633</t>
         </is>
       </c>
     </row>
@@ -3199,17 +3199,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.6048</t>
+          <t>0.4665</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.580</t>
+          <t>0.447</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.631</t>
+          <t>0.486</t>
         </is>
       </c>
     </row>
@@ -3222,17 +3222,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.6974</t>
+          <t>0.5552</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.668</t>
+          <t>0.531</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.729</t>
+          <t>0.580</t>
         </is>
       </c>
     </row>
@@ -3245,17 +3245,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9134</t>
+          <t>0.8126</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.860</t>
+          <t>0.765</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.863</t>
         </is>
       </c>
     </row>
@@ -3268,17 +3268,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0337</t>
+          <t>1.0200</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.100</t>
         </is>
       </c>
     </row>
@@ -3378,17 +3378,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9579</t>
+          <t>0.7878</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.795</t>
         </is>
       </c>
     </row>
@@ -3401,17 +3401,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.3946</t>
+          <t>1.4691</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.383</t>
+          <t>1.457</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -3424,17 +3424,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.6841</t>
+          <t>0.6268</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.662</t>
+          <t>0.607</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.707</t>
+          <t>0.648</t>
         </is>
       </c>
     </row>
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8251</t>
+          <t>0.6851</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.674</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.839</t>
+          <t>0.696</t>
         </is>
       </c>
     </row>
@@ -3470,17 +3470,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0620</t>
+          <t>0.8191</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>0.832</t>
         </is>
       </c>
     </row>
@@ -3493,17 +3493,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0679</t>
+          <t>0.8500</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>0.835</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.088</t>
+          <t>0.866</t>
         </is>
       </c>
     </row>
@@ -3516,17 +3516,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.3986</t>
+          <t>1.2443</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.360</t>
+          <t>1.210</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.438</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -3539,17 +3539,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.0652</t>
+          <t>1.0511</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -3649,17 +3649,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.6179</t>
+          <t>1.5076</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.579</t>
+          <t>1.471</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.658</t>
+          <t>1.545</t>
         </is>
       </c>
     </row>
@@ -3672,17 +3672,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.6386</t>
+          <t>1.6668</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.604</t>
+          <t>1.632</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.674</t>
+          <t>1.702</t>
         </is>
       </c>
     </row>
@@ -3718,17 +3718,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.4469</t>
+          <t>1.1438</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.084</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.527</t>
+          <t>1.207</t>
         </is>
       </c>
     </row>
@@ -3977,17 +3977,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9413</t>
+          <t>0.9108</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>0.973</t>
         </is>
       </c>
     </row>
@@ -4000,17 +4000,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9405</t>
+          <t>0.9428</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.010</t>
         </is>
       </c>
     </row>
@@ -4023,17 +4023,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9059</t>
+          <t>0.8563</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.667</t>
+          <t>0.630</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.231</t>
+          <t>1.163</t>
         </is>
       </c>
     </row>
@@ -4046,17 +4046,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1784</t>
+          <t>1.1129</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.259</t>
         </is>
       </c>
     </row>
@@ -4069,17 +4069,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8521</t>
+          <t>0.8167</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.747</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>0.930</t>
         </is>
       </c>
     </row>
@@ -4092,17 +4092,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9074</t>
+          <t>0.8806</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.756</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.027</t>
         </is>
       </c>
     </row>
@@ -4115,17 +4115,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8141</t>
+          <t>0.9055</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.657</t>
+          <t>0.733</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.118</t>
         </is>
       </c>
     </row>
@@ -4138,17 +4138,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0414</t>
+          <t>1.0357</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.795</t>
+          <t>0.791</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.364</t>
+          <t>1.356</t>
         </is>
       </c>
     </row>
@@ -4161,17 +4161,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9602</t>
+          <t>0.9501</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.637</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.433</t>
+          <t>1.418</t>
         </is>
       </c>
     </row>
@@ -4248,17 +4248,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0764</t>
+          <t>1.0566</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.053</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.081</t>
         </is>
       </c>
     </row>
@@ -4271,17 +4271,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0937</t>
+          <t>1.0946</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.070</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.120</t>
         </is>
       </c>
     </row>
@@ -4294,17 +4294,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8931</t>
+          <t>0.8835</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>0.962</t>
         </is>
       </c>
     </row>
@@ -4317,17 +4317,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0467</t>
+          <t>1.0811</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.033</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.132</t>
         </is>
       </c>
     </row>
@@ -4340,17 +4340,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0978</t>
+          <t>1.0467</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.003</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.147</t>
+          <t>1.092</t>
         </is>
       </c>
     </row>
@@ -4363,17 +4363,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1602</t>
+          <t>1.1374</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.103</t>
+          <t>1.082</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -4386,17 +4386,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9113</t>
+          <t>0.8748</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.939</t>
         </is>
       </c>
     </row>
@@ -4409,17 +4409,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.2032</t>
+          <t>1.1712</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.288</t>
         </is>
       </c>
     </row>
@@ -4432,17 +4432,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1448</t>
+          <t>1.1328</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -4519,17 +4519,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1407</t>
+          <t>1.1572</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.083</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.237</t>
         </is>
       </c>
     </row>
@@ -4542,17 +4542,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1629</t>
+          <t>1.1610</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.083</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.246</t>
+          <t>1.244</t>
         </is>
       </c>
     </row>
@@ -4565,17 +4565,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.9858</t>
+          <t>1.0318</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.723</t>
+          <t>0.756</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.407</t>
         </is>
       </c>
     </row>
@@ -4588,17 +4588,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.8883</t>
+          <t>0.9715</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.784</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.101</t>
         </is>
       </c>
     </row>
@@ -4611,17 +4611,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.2882</t>
+          <t>1.2816</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.125</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.460</t>
         </is>
       </c>
     </row>
@@ -4634,17 +4634,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.2787</t>
+          <t>1.2916</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.495</t>
+          <t>1.507</t>
         </is>
       </c>
     </row>
@@ -4657,17 +4657,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.1195</t>
+          <t>0.9661</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.902</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.390</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -4680,17 +4680,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.1554</t>
+          <t>1.1308</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.517</t>
+          <t>1.484</t>
         </is>
       </c>
     </row>
@@ -4790,17 +4790,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.4111</t>
+          <t>1.2482</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.386</t>
+          <t>1.226</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.437</t>
+          <t>1.271</t>
         </is>
       </c>
     </row>
@@ -4813,17 +4813,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.5542</t>
+          <t>1.5710</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.526</t>
+          <t>1.543</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.583</t>
+          <t>1.600</t>
         </is>
       </c>
     </row>
@@ -4836,17 +4836,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.1586</t>
+          <t>1.0951</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.230</t>
+          <t>1.162</t>
         </is>
       </c>
     </row>
@@ -4859,17 +4859,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.3822</t>
+          <t>1.2365</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.335</t>
+          <t>1.195</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.431</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -4882,17 +4882,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.5137</t>
+          <t>1.2864</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.331</t>
         </is>
       </c>
     </row>
@@ -4905,17 +4905,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.5111</t>
+          <t>1.3252</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.271</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.382</t>
         </is>
       </c>
     </row>
@@ -4928,17 +4928,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0628</t>
+          <t>1.0202</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -4951,17 +4951,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.3136</t>
+          <t>1.2786</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.160</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.447</t>
+          <t>1.409</t>
         </is>
       </c>
     </row>
@@ -4974,17 +4974,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.2463</t>
+          <t>1.2332</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.476</t>
+          <t>1.460</t>
         </is>
       </c>
     </row>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.4997</t>
+          <t>1.3704</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.405</t>
+          <t>1.284</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.463</t>
         </is>
       </c>
     </row>
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.6525</t>
+          <t>1.6664</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.544</t>
+          <t>1.557</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.768</t>
+          <t>1.783</t>
         </is>
       </c>
     </row>
@@ -5130,17 +5130,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.1729</t>
+          <t>1.1111</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.324</t>
+          <t>1.254</t>
         </is>
       </c>
     </row>
@@ -5153,17 +5153,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.7763</t>
+          <t>1.5752</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.560</t>
+          <t>1.386</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2.023</t>
+          <t>1.790</t>
         </is>
       </c>
     </row>
@@ -5176,17 +5176,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.6654</t>
+          <t>1.5048</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.428</t>
+          <t>1.293</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.942</t>
+          <t>1.751</t>
         </is>
       </c>
     </row>
@@ -5199,17 +5199,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1.3056</t>
+          <t>1.1267</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1.054</t>
+          <t>0.912</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1.617</t>
+          <t>1.391</t>
         </is>
       </c>
     </row>
@@ -5222,17 +5222,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.2614</t>
+          <t>1.2346</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>0.940</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.657</t>
+          <t>1.621</t>
         </is>
       </c>
     </row>
@@ -5332,17 +5332,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.3110</t>
+          <t>1.1814</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.286</t>
+          <t>1.158</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -5355,17 +5355,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.4210</t>
+          <t>1.4353</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.393</t>
+          <t>1.407</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.450</t>
+          <t>1.465</t>
         </is>
       </c>
     </row>
@@ -5378,17 +5378,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.2973</t>
+          <t>1.2394</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.146</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.404</t>
+          <t>1.341</t>
         </is>
       </c>
     </row>
@@ -5401,17 +5401,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.3205</t>
+          <t>1.1437</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.270</t>
+          <t>1.100</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.373</t>
+          <t>1.189</t>
         </is>
       </c>
     </row>
@@ -5424,17 +5424,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.3788</t>
+          <t>1.2291</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.329</t>
+          <t>1.185</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.430</t>
+          <t>1.275</t>
         </is>
       </c>
     </row>
@@ -5447,17 +5447,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.3025</t>
+          <t>1.1651</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.246</t>
+          <t>1.115</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.362</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9655</t>
+          <t>0.9929</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.019</t>
+          <t>1.048</t>
         </is>
       </c>
     </row>
@@ -5683,17 +5683,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.8757</t>
+          <t>0.8673</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.831</t>
+          <t>0.823</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>0.914</t>
         </is>
       </c>
     </row>
@@ -5706,17 +5706,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.4515</t>
+          <t>0.4401</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.358</t>
+          <t>0.349</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.569</t>
+          <t>0.555</t>
         </is>
       </c>
     </row>
@@ -5729,17 +5729,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2649</t>
+          <t>1.3744</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.238</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.406</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -5752,17 +5752,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2618</t>
+          <t>1.1963</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.326</t>
         </is>
       </c>
     </row>
@@ -5775,17 +5775,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.5530</t>
+          <t>0.6228</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.489</t>
+          <t>0.551</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>0.704</t>
         </is>
       </c>
     </row>
@@ -5798,17 +5798,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0504</t>
+          <t>1.0146</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.901</t>
+          <t>0.870</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.225</t>
+          <t>1.183</t>
         </is>
       </c>
     </row>
@@ -5890,17 +5890,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.0460</t>
+          <t>1.1312</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.538</t>
+          <t>0.582</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.035</t>
+          <t>2.200</t>
         </is>
       </c>
     </row>
@@ -5931,17 +5931,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0182</t>
+          <t>1.0048</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -5954,17 +5954,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0622</t>
+          <t>1.0672</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.079</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -5977,17 +5977,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9420</t>
+          <t>0.9182</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.857</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>0.984</t>
         </is>
       </c>
     </row>
@@ -6000,17 +6000,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0452</t>
+          <t>1.0488</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -6023,17 +6023,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0552</t>
+          <t>1.0438</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.014</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.075</t>
         </is>
       </c>
     </row>
@@ -6046,17 +6046,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9694</t>
+          <t>0.9376</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.938</t>
+          <t>0.907</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>0.969</t>
         </is>
       </c>
     </row>
@@ -6069,17 +6069,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8972</t>
+          <t>0.8667</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.857</t>
+          <t>0.828</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.907</t>
         </is>
       </c>
     </row>
@@ -6138,17 +6138,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.8963</t>
+          <t>0.9547</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.780</t>
+          <t>0.832</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -6161,17 +6161,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.0430</t>
+          <t>1.0061</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.865</t>
+          <t>0.835</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.257</t>
+          <t>1.212</t>
         </is>
       </c>
     </row>
@@ -6202,17 +6202,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0545</t>
+          <t>1.0119</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>1.068</t>
         </is>
       </c>
     </row>
@@ -6225,17 +6225,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2130</t>
+          <t>1.2306</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.167</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.298</t>
         </is>
       </c>
     </row>
@@ -6271,17 +6271,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.8263</t>
+          <t>0.7631</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.743</t>
+          <t>0.687</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.848</t>
         </is>
       </c>
     </row>
@@ -6294,17 +6294,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8362</t>
+          <t>0.8725</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.754</t>
+          <t>0.787</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.927</t>
+          <t>0.967</t>
         </is>
       </c>
     </row>
@@ -6317,17 +6317,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.7530</t>
+          <t>1.5053</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.549</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.984</t>
+          <t>1.701</t>
         </is>
       </c>
     </row>
@@ -6409,17 +6409,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.6050</t>
+          <t>2.7745</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.651</t>
+          <t>1.759</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4.109</t>
+          <t>4.376</t>
         </is>
       </c>
     </row>
@@ -6473,17 +6473,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9772</t>
+          <t>0.9461</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.935</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>0.957</t>
         </is>
       </c>
     </row>
@@ -6496,17 +6496,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.1755</t>
+          <t>1.1975</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.184</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.212</t>
         </is>
       </c>
     </row>
@@ -6519,17 +6519,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.7326</t>
+          <t>0.7141</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.699</t>
+          <t>0.681</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.768</t>
+          <t>0.748</t>
         </is>
       </c>
     </row>
@@ -6542,17 +6542,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.9938</t>
+          <t>0.9822</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.960</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -6565,17 +6565,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0876</t>
+          <t>1.0311</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.064</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.054</t>
         </is>
       </c>
     </row>
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8885</t>
+          <t>0.8562</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.866</t>
+          <t>0.834</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.912</t>
+          <t>0.879</t>
         </is>
       </c>
     </row>
@@ -6611,17 +6611,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9835</t>
+          <t>0.9500</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.946</t>
+          <t>0.914</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>0.988</t>
         </is>
       </c>
     </row>
@@ -6703,17 +6703,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.5112</t>
+          <t>1.4576</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.135</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.941</t>
+          <t>1.871</t>
         </is>
       </c>
     </row>
@@ -6744,17 +6744,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0106</t>
+          <t>0.9515</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.004</t>
         </is>
       </c>
     </row>
@@ -6767,17 +6767,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.3423</t>
+          <t>1.3808</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.274</t>
+          <t>1.311</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.414</t>
+          <t>1.455</t>
         </is>
       </c>
     </row>
@@ -6813,17 +6813,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.7857</t>
+          <t>0.7147</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.708</t>
+          <t>0.645</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.872</t>
+          <t>0.792</t>
         </is>
       </c>
     </row>
@@ -6859,17 +6859,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.6068</t>
+          <t>1.3747</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.422</t>
+          <t>1.218</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.815</t>
+          <t>1.551</t>
         </is>
       </c>
     </row>
@@ -7015,17 +7015,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.9597</t>
+          <t>0.9416</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.947</t>
+          <t>0.929</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>0.954</t>
         </is>
       </c>
     </row>
@@ -7038,17 +7038,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.1066</t>
+          <t>1.1221</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -7084,17 +7084,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>0.9508</t>
+          <t>0.9365</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.925</t>
+          <t>0.911</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.963</t>
         </is>
       </c>
     </row>
@@ -7107,17 +7107,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.0308</t>
+          <t>0.9879</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.012</t>
         </is>
       </c>
     </row>
@@ -7130,17 +7130,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.9166</t>
+          <t>0.9133</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.887</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.943</t>
+          <t>0.940</t>
         </is>
       </c>
     </row>
@@ -7222,17 +7222,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.8964</t>
+          <t>0.8416</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.759</t>
+          <t>0.713</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>0.994</t>
         </is>
       </c>
     </row>
@@ -7343,17 +7343,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0732</t>
+          <t>1.0932</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.014</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.156</t>
+          <t>1.179</t>
         </is>
       </c>
     </row>
@@ -7366,17 +7366,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9465</t>
+          <t>0.9643</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
@@ -7389,17 +7389,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2.2692</t>
+          <t>1.8095</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.679</t>
+          <t>1.339</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.067</t>
+          <t>2.445</t>
         </is>
       </c>
     </row>
@@ -7412,17 +7412,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9468</t>
+          <t>1.0115</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.818</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
@@ -7435,17 +7435,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8850</t>
+          <t>0.9044</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>0.781</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.026</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
@@ -7458,17 +7458,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1913</t>
+          <t>1.2546</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.054</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.419</t>
+          <t>1.494</t>
         </is>
       </c>
     </row>
@@ -7481,17 +7481,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.7992</t>
+          <t>1.6407</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.429</t>
+          <t>1.303</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.265</t>
+          <t>2.065</t>
         </is>
       </c>
     </row>
@@ -7504,17 +7504,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8380</t>
+          <t>0.9337</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.625</t>
+          <t>0.698</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.123</t>
+          <t>1.249</t>
         </is>
       </c>
     </row>
@@ -7573,17 +7573,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.3982</t>
+          <t>1.4395</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.571</t>
+          <t>0.588</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3.425</t>
+          <t>3.525</t>
         </is>
       </c>
     </row>
@@ -7614,17 +7614,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0057</t>
+          <t>0.9298</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>0.951</t>
         </is>
       </c>
     </row>
@@ -7637,17 +7637,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0362</t>
+          <t>1.0765</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.012</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.102</t>
         </is>
       </c>
     </row>
@@ -7660,17 +7660,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6028</t>
+          <t>1.2781</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.446</t>
+          <t>1.153</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.777</t>
+          <t>1.416</t>
         </is>
       </c>
     </row>
@@ -7683,17 +7683,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.9559</t>
+          <t>0.8784</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.836</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>0.923</t>
         </is>
       </c>
     </row>
@@ -7706,17 +7706,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9561</t>
+          <t>0.9162</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.877</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>0.957</t>
         </is>
       </c>
     </row>
@@ -7729,17 +7729,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0855</t>
+          <t>0.9902</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>0.942</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -7752,17 +7752,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.9002</t>
+          <t>0.8209</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>0.767</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.878</t>
         </is>
       </c>
     </row>
@@ -7775,17 +7775,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8513</t>
+          <t>0.7811</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.778</t>
+          <t>0.714</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>0.855</t>
         </is>
       </c>
     </row>
@@ -7844,17 +7844,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.4638</t>
+          <t>0.4281</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.348</t>
+          <t>0.321</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.618</t>
+          <t>0.570</t>
         </is>
       </c>
     </row>
@@ -7885,17 +7885,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9376</t>
+          <t>0.8501</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.870</t>
+          <t>0.788</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>0.917</t>
         </is>
       </c>
     </row>
@@ -7908,17 +7908,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0948</t>
+          <t>1.1163</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.205</t>
         </is>
       </c>
     </row>
@@ -7954,17 +7954,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0096</t>
+          <t>0.8684</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -7977,17 +7977,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0803</t>
+          <t>1.0131</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>0.874</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.253</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -8000,17 +8000,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.9112</t>
+          <t>0.7893</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>0.662</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>0.941</t>
         </is>
       </c>
     </row>
@@ -8046,17 +8046,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0158</t>
+          <t>0.8365</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.756</t>
+          <t>0.623</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.122</t>
         </is>
       </c>
     </row>
@@ -8156,17 +8156,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0504</t>
+          <t>1.0130</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>0.995</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.031</t>
         </is>
       </c>
     </row>
@@ -8179,17 +8179,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>1.0753</t>
+          <t>1.0993</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.056</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.120</t>
         </is>
       </c>
     </row>
@@ -8202,17 +8202,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.9916</t>
+          <t>0.9296</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.864</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -8225,17 +8225,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0005</t>
+          <t>0.9936</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.965</t>
+          <t>0.959</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -8248,17 +8248,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0706</t>
+          <t>1.0469</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.013</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -8271,17 +8271,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.0947</t>
+          <t>1.0240</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.984</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.066</t>
         </is>
       </c>
     </row>
@@ -8294,17 +8294,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1.0258</t>
+          <t>0.9354</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>0.991</t>
         </is>
       </c>
     </row>
@@ -8317,17 +8317,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.9672</t>
+          <t>0.8874</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.817</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.964</t>
         </is>
       </c>
     </row>
@@ -8386,17 +8386,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.6803</t>
+          <t>0.6279</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.471</t>
+          <t>0.435</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.906</t>
         </is>
       </c>
     </row>
@@ -8427,17 +8427,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9747</t>
+          <t>0.9224</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>0.856</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>0.994</t>
         </is>
       </c>
     </row>
@@ -8450,17 +8450,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1.1360</t>
+          <t>1.1399</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1.054</t>
+          <t>1.057</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.229</t>
         </is>
       </c>
     </row>
@@ -8473,17 +8473,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.4370</t>
+          <t>0.5137</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.324</t>
+          <t>0.381</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.589</t>
+          <t>0.692</t>
         </is>
       </c>
     </row>
@@ -8496,17 +8496,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0568</t>
+          <t>0.9823</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.851</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.220</t>
+          <t>1.133</t>
         </is>
       </c>
     </row>
@@ -8519,17 +8519,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.2097</t>
+          <t>1.1576</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.338</t>
         </is>
       </c>
     </row>
@@ -8542,17 +8542,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.9189</t>
+          <t>0.8162</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.773</t>
+          <t>0.687</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.092</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -8588,17 +8588,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.1542</t>
+          <t>0.9504</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.861</t>
+          <t>0.710</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -8698,17 +8698,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.0445</t>
+          <t>1.0895</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.112</t>
         </is>
       </c>
     </row>
@@ -8721,17 +8721,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.0377</t>
+          <t>1.0211</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.043</t>
         </is>
       </c>
     </row>
@@ -8744,17 +8744,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.6187</t>
+          <t>0.7273</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.563</t>
+          <t>0.662</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.680</t>
+          <t>0.799</t>
         </is>
       </c>
     </row>
@@ -8767,17 +8767,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.0467</t>
+          <t>1.1311</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>1.083</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -8790,17 +8790,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.1198</t>
+          <t>1.1426</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>1.100</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.186</t>
         </is>
       </c>
     </row>
@@ -8813,17 +8813,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.0084</t>
+          <t>1.0341</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.964</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.054</t>
+          <t>1.081</t>
         </is>
       </c>
     </row>
@@ -8969,17 +8969,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1.1338</t>
+          <t>0.9447</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>0.922</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>0.968</t>
         </is>
       </c>
     </row>
@@ -8992,17 +8992,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.2059</t>
+          <t>1.2812</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.253</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1.233</t>
+          <t>1.310</t>
         </is>
       </c>
     </row>
@@ -9015,17 +9015,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>1.1126</t>
+          <t>0.8872</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1.027</t>
+          <t>0.819</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1.206</t>
+          <t>0.961</t>
         </is>
       </c>
     </row>
@@ -9038,17 +9038,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.0357</t>
+          <t>0.8391</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>0.995</t>
+          <t>0.806</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1.078</t>
+          <t>0.873</t>
         </is>
       </c>
     </row>
@@ -9061,17 +9061,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1.0422</t>
+          <t>0.8630</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>0.829</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>0.898</t>
         </is>
       </c>
     </row>
@@ -9084,17 +9084,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1.2076</t>
+          <t>0.9812</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1.145</t>
+          <t>0.931</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1.274</t>
+          <t>1.035</t>
         </is>
       </c>
     </row>
@@ -9107,17 +9107,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.3540</t>
+          <t>1.2347</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.223</t>
+          <t>1.115</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.499</t>
+          <t>1.367</t>
         </is>
       </c>
     </row>
@@ -9130,17 +9130,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2.6452</t>
+          <t>2.4270</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.211</t>
+          <t>2.029</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>3.165</t>
+          <t>2.903</t>
         </is>
       </c>
     </row>
@@ -9199,17 +9199,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>3.9388</t>
+          <t>4.0551</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>1.453</t>
+          <t>1.496</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>10.675</t>
+          <t>10.989</t>
         </is>
       </c>
     </row>
@@ -9240,17 +9240,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>1.0552</t>
+          <t>0.8611</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.798</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>0.929</t>
         </is>
       </c>
     </row>
@@ -9263,17 +9263,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1.2740</t>
+          <t>1.3286</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>1.181</t>
+          <t>1.231</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1.374</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -9309,17 +9309,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1.0940</t>
+          <t>0.8295</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>0.946</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>0.958</t>
         </is>
       </c>
     </row>
@@ -9332,17 +9332,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>1.1776</t>
+          <t>0.9542</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>0.824</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1.365</t>
+          <t>1.105</t>
         </is>
       </c>
     </row>
@@ -9355,17 +9355,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.0137</t>
+          <t>0.7821</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.656</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.209</t>
+          <t>0.933</t>
         </is>
       </c>
     </row>
@@ -9401,17 +9401,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>3.1565</t>
+          <t>2.5993</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2.261</t>
+          <t>1.865</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4.406</t>
+          <t>3.624</t>
         </is>
       </c>
     </row>
@@ -9511,17 +9511,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>1.1251</t>
+          <t>1.0140</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>0.988</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.155</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -9534,17 +9534,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1.1637</t>
+          <t>1.1901</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.161</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>1.193</t>
+          <t>1.220</t>
         </is>
       </c>
     </row>
@@ -9580,17 +9580,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>1.0836</t>
+          <t>0.9552</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>1.033</t>
+          <t>0.911</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1.136</t>
+          <t>1.002</t>
         </is>
       </c>
     </row>
@@ -9603,17 +9603,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.0901</t>
+          <t>0.9419</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>1.043</t>
+          <t>0.901</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>0.984</t>
         </is>
       </c>
     </row>
@@ -9626,17 +9626,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>1.1125</t>
+          <t>0.9909</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.937</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.048</t>
         </is>
       </c>
     </row>
@@ -9782,17 +9782,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1.0782</t>
+          <t>0.9314</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>0.911</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>0.952</t>
         </is>
       </c>
     </row>
@@ -9805,17 +9805,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>1.1215</t>
+          <t>1.1655</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>1.100</t>
+          <t>1.143</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>1.143</t>
+          <t>1.188</t>
         </is>
       </c>
     </row>
@@ -9828,17 +9828,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>1.1220</t>
+          <t>0.9545</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>0.891</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>1.023</t>
         </is>
       </c>
     </row>
@@ -9851,17 +9851,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>1.0352</t>
+          <t>0.8444</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>0.818</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>0.872</t>
         </is>
       </c>
     </row>
@@ -9874,17 +9874,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>0.9735</t>
+          <t>0.8243</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>0.797</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>0.852</t>
         </is>
       </c>
     </row>
@@ -9897,17 +9897,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>1.1032</t>
+          <t>0.9582</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>0.913</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>1.157</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed logging bug and calculation bug
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.1083</t>
+          <t>0.1084</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3291,17 +3291,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.4279</t>
+          <t>1.4360</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.290</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.590</t>
+          <t>1.599</t>
         </is>
       </c>
     </row>
@@ -3337,17 +3337,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.5081</t>
+          <t>1.5102</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.250</t>
+          <t>1.252</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.820</t>
+          <t>1.822</t>
         </is>
       </c>
     </row>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.2585</t>
+          <t>0.2589</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4169</t>
+          <t>1.4168</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -3833,17 +3833,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.0992</t>
+          <t>1.0930</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.973</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.228</t>
         </is>
       </c>
     </row>
@@ -3977,17 +3977,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0262</t>
+          <t>1.0277</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.962</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.098</t>
         </is>
       </c>
     </row>
@@ -4000,17 +4000,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.1982</t>
+          <t>0.1986</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.184</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.214</t>
+          <t>0.215</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0762</t>
+          <t>1.0765</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -4092,12 +4092,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9243</t>
+          <t>0.9248</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.796</t>
+          <t>0.797</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4115,17 +4115,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9071</t>
+          <t>0.9213</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.735</t>
+          <t>0.747</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.136</t>
         </is>
       </c>
     </row>
@@ -4138,17 +4138,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1910</t>
+          <t>1.1992</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.924</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.557</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.2433</t>
+          <t>0.2431</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.984</t>
         </is>
       </c>
     </row>
@@ -4478,17 +4478,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.3247</t>
+          <t>1.3235</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.759</t>
+          <t>1.757</t>
         </is>
       </c>
     </row>
@@ -4519,17 +4519,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9924</t>
+          <t>0.9909</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.927</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.061</t>
+          <t>1.059</t>
         </is>
       </c>
     </row>
@@ -4542,17 +4542,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.6645</t>
+          <t>0.6630</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.615</t>
+          <t>0.613</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.718</t>
+          <t>0.717</t>
         </is>
       </c>
     </row>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9341</t>
+          <t>0.9340</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.056</t>
         </is>
       </c>
     </row>
@@ -4634,12 +4634,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.1273</t>
+          <t>1.1267</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.970</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4657,17 +4657,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9391</t>
+          <t>0.9246</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.760</t>
+          <t>0.748</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.142</t>
         </is>
       </c>
     </row>
@@ -4680,17 +4680,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.9462</t>
+          <t>0.9397</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.727</t>
+          <t>0.722</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>1.223</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0949</t>
+          <t>1.0939</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -5030,7 +5030,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.714</t>
+          <t>1.713</t>
         </is>
       </c>
     </row>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0989</t>
+          <t>1.0973</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.028</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.171</t>
         </is>
       </c>
     </row>
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.3532</t>
+          <t>0.3524</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.327</t>
+          <t>0.326</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.381</t>
+          <t>0.380</t>
         </is>
       </c>
     </row>
@@ -5130,7 +5130,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0068</t>
+          <t>1.0066</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -5176,17 +5176,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.2856</t>
+          <t>1.2849</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.109</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.490</t>
+          <t>1.489</t>
         </is>
       </c>
     </row>
@@ -5199,17 +5199,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1.0952</t>
+          <t>1.0783</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.874</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1.351</t>
+          <t>1.330</t>
         </is>
       </c>
     </row>
@@ -5222,17 +5222,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.0329</t>
+          <t>1.0259</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.793</t>
+          <t>0.788</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.346</t>
+          <t>1.336</t>
         </is>
       </c>
     </row>
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9305</t>
+          <t>0.9327</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.982</t>
+          <t>0.984</t>
         </is>
       </c>
     </row>
@@ -5729,17 +5729,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2105</t>
+          <t>1.2220</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>1.099</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.345</t>
+          <t>1.358</t>
         </is>
       </c>
     </row>
@@ -5752,17 +5752,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2004</t>
+          <t>1.2059</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.088</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.336</t>
         </is>
       </c>
     </row>
@@ -5775,17 +5775,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.5848</t>
+          <t>0.5801</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.518</t>
+          <t>0.514</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.655</t>
         </is>
       </c>
     </row>
@@ -5821,17 +5821,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8722</t>
+          <t>0.8779</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.719</t>
+          <t>0.724</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.065</t>
         </is>
       </c>
     </row>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0046</t>
+          <t>1.0048</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -6138,17 +6138,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.9355</t>
+          <t>0.9484</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.826</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.075</t>
+          <t>1.090</t>
         </is>
       </c>
     </row>
@@ -6161,17 +6161,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.1439</t>
+          <t>1.1376</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.377</t>
+          <t>1.370</t>
         </is>
       </c>
     </row>
@@ -6202,17 +6202,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0792</t>
+          <t>1.0768</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.020</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -6225,17 +6225,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.2022</t>
+          <t>4.1915</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3.796</t>
+          <t>3.787</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4.651</t>
+          <t>4.640</t>
         </is>
       </c>
     </row>
@@ -6271,17 +6271,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.8419</t>
+          <t>0.8340</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.750</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.928</t>
         </is>
       </c>
     </row>
@@ -6294,17 +6294,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.8844</t>
+          <t>0.8804</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.798</t>
+          <t>0.794</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.976</t>
         </is>
       </c>
     </row>
@@ -6317,17 +6317,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.6281</t>
+          <t>1.6411</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.441</t>
+          <t>1.452</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.840</t>
+          <t>1.855</t>
         </is>
       </c>
     </row>
@@ -6363,17 +6363,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.3007</t>
+          <t>1.2922</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.064</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.570</t>
         </is>
       </c>
     </row>
@@ -6409,17 +6409,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.7188</t>
+          <t>2.7563</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.724</t>
+          <t>1.747</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4.289</t>
+          <t>4.348</t>
         </is>
       </c>
     </row>
@@ -6703,17 +6703,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.6573</t>
+          <t>1.6482</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.291</t>
+          <t>1.284</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2.127</t>
+          <t>2.115</t>
         </is>
       </c>
     </row>
@@ -6744,17 +6744,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0162</t>
+          <t>1.0138</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.961</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.069</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.0180</t>
+          <t>0.0179</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -6813,17 +6813,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.7905</t>
+          <t>0.7831</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.712</t>
+          <t>0.706</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.877</t>
+          <t>0.869</t>
         </is>
       </c>
     </row>
@@ -6836,17 +6836,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.8804</t>
+          <t>0.8764</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.796</t>
+          <t>0.792</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.970</t>
         </is>
       </c>
     </row>
@@ -6859,17 +6859,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.4652</t>
+          <t>1.4769</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.309</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.653</t>
+          <t>1.666</t>
         </is>
       </c>
     </row>
@@ -6905,17 +6905,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.0958</t>
+          <t>1.0886</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.897</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.329</t>
+          <t>1.321</t>
         </is>
       </c>
     </row>
@@ -7015,7 +7015,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.9429</t>
+          <t>0.9428</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -7222,17 +7222,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.8588</t>
+          <t>0.8472</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.727</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.001</t>
         </is>
       </c>
     </row>
@@ -7343,17 +7343,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0947</t>
+          <t>1.0933</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.178</t>
         </is>
       </c>
     </row>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0649</t>
+          <t>0.0640</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -7376,7 +7376,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.072</t>
+          <t>0.071</t>
         </is>
       </c>
     </row>
@@ -7412,12 +7412,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0170</t>
+          <t>1.0174</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.882</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -7435,17 +7435,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0626</t>
+          <t>1.0643</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.920</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.229</t>
+          <t>1.231</t>
         </is>
       </c>
     </row>
@@ -7458,17 +7458,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0023</t>
+          <t>1.0046</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.845</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -7504,17 +7504,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.7089</t>
+          <t>0.6724</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.529</t>
+          <t>0.501</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.902</t>
         </is>
       </c>
     </row>
@@ -7844,17 +7844,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.5483</t>
+          <t>0.5492</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.411</t>
+          <t>0.412</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.731</t>
+          <t>0.732</t>
         </is>
       </c>
     </row>
@@ -7885,17 +7885,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9083</t>
+          <t>0.9094</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.981</t>
         </is>
       </c>
     </row>
@@ -7908,17 +7908,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.2729</t>
+          <t>2.3050</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.048</t>
+          <t>2.077</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.523</t>
+          <t>2.558</t>
         </is>
       </c>
     </row>
@@ -7954,7 +7954,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9648</t>
+          <t>0.9645</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -7964,7 +7964,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.115</t>
         </is>
       </c>
     </row>
@@ -7977,17 +7977,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.9190</t>
+          <t>0.9175</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.794</t>
+          <t>0.792</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.064</t>
+          <t>1.062</t>
         </is>
       </c>
     </row>
@@ -8000,17 +8000,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.0421</t>
+          <t>1.0397</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.875</t>
+          <t>0.873</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.241</t>
+          <t>1.238</t>
         </is>
       </c>
     </row>
@@ -8046,17 +8046,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.1533</t>
+          <t>1.2158</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.904</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.548</t>
+          <t>1.635</t>
         </is>
       </c>
     </row>
@@ -8386,17 +8386,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.8042</t>
+          <t>0.8054</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.557</t>
+          <t>0.558</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.163</t>
         </is>
       </c>
     </row>
@@ -8427,17 +8427,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9276</t>
+          <t>0.9287</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.861</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -8450,17 +8450,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.8961</t>
+          <t>0.9088</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.809</t>
+          <t>0.821</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.992</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -8496,12 +8496,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.9692</t>
+          <t>0.9688</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.842</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -8519,17 +8519,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.9822</t>
+          <t>0.9806</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.851</t>
+          <t>0.849</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.134</t>
+          <t>1.132</t>
         </is>
       </c>
     </row>
@@ -8542,17 +8542,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.0468</t>
+          <t>1.0444</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.879</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.243</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -8588,17 +8588,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.3104</t>
+          <t>1.3814</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>1.029</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.755</t>
+          <t>1.854</t>
         </is>
       </c>
     </row>
@@ -9240,17 +9240,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0.8857</t>
+          <t>0.8868</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.821</t>
+          <t>0.822</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.956</t>
         </is>
       </c>
     </row>
@@ -9263,17 +9263,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>0.1326</t>
+          <t>0.1344</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.120</t>
+          <t>0.121</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>0.147</t>
+          <t>0.149</t>
         </is>
       </c>
     </row>
@@ -9309,7 +9309,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0.8544</t>
+          <t>0.8541</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -9332,17 +9332,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0.8475</t>
+          <t>0.8461</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0.733</t>
+          <t>0.732</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -9355,17 +9355,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.0109</t>
+          <t>1.0086</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -9401,17 +9401,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>3.5838</t>
+          <t>3.7779</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2.569</t>
+          <t>2.704</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>4.999</t>
+          <t>5.278</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
for linear fit, we have a match in test harness vs. KCOR fit!
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -497,17 +497,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2386</t>
+          <t>1.2417</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.265</t>
         </is>
       </c>
     </row>
@@ -543,17 +543,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9289</t>
+          <t>0.9497</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.871</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>1.013</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0815</t>
+          <t>1.0842</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.049</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.118</t>
         </is>
       </c>
     </row>
@@ -589,17 +589,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.3198</t>
+          <t>1.3211</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.291</t>
+          <t>1.292</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.349</t>
+          <t>1.351</t>
         </is>
       </c>
     </row>
@@ -635,17 +635,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.4010</t>
+          <t>1.3880</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.255</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.564</t>
+          <t>1.549</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3.3948</t>
+          <t>3.3950</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3402</t>
+          <t>1.3405</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -814,17 +814,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3235</t>
+          <t>1.3291</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.278</t>
+          <t>1.283</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.371</t>
+          <t>1.376</t>
         </is>
       </c>
     </row>
@@ -837,17 +837,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.6181</t>
+          <t>1.6203</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.587</t>
+          <t>1.589</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.650</t>
+          <t>1.652</t>
         </is>
       </c>
     </row>
@@ -906,17 +906,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.4708</t>
+          <t>1.4566</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.318</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.626</t>
+          <t>1.610</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.410</t>
+          <t>1.409</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.2730</t>
+          <t>1.2729</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -998,7 +998,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>3.3055</t>
+          <t>3.3053</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>10.286</t>
+          <t>10.285</t>
         </is>
       </c>
     </row>
@@ -1039,17 +1039,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0825</t>
+          <t>1.0800</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.055</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.105</t>
         </is>
       </c>
     </row>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.1700</t>
+          <t>1.1697</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1085,17 +1085,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.4248</t>
+          <t>1.3995</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.336</t>
+          <t>1.312</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.520</t>
+          <t>1.493</t>
         </is>
       </c>
     </row>
@@ -1108,17 +1108,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.4961</t>
+          <t>1.4945</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.451</t>
+          <t>1.450</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.543</t>
+          <t>1.541</t>
         </is>
       </c>
     </row>
@@ -1131,17 +1131,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.0091</t>
+          <t>1.0081</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.042</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1.0498</t>
+          <t>1.0494</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1.712</t>
+          <t>1.711</t>
         </is>
       </c>
     </row>
@@ -1367,17 +1367,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1216</t>
+          <t>1.1278</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.108</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.148</t>
         </is>
       </c>
     </row>
@@ -1390,17 +1390,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0903</t>
+          <t>0.0392</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.089</t>
+          <t>0.038</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.092</t>
+          <t>0.040</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0397</t>
+          <t>1.0419</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.082</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -1482,17 +1482,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5120</t>
+          <t>1.5495</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.509</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.553</t>
+          <t>1.591</t>
         </is>
       </c>
     </row>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.3835</t>
+          <t>1.3737</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.321</t>
+          <t>1.312</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.449</t>
+          <t>1.439</t>
         </is>
       </c>
     </row>
@@ -1528,17 +1528,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1430</t>
+          <t>1.1697</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.072</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.276</t>
         </is>
       </c>
     </row>
@@ -1638,17 +1638,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1495</t>
+          <t>1.1560</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.141</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.165</t>
+          <t>1.171</t>
         </is>
       </c>
     </row>
@@ -1661,17 +1661,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.1084</t>
+          <t>0.0470</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.107</t>
+          <t>0.046</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.110</t>
+          <t>0.048</t>
         </is>
       </c>
     </row>
@@ -1684,17 +1684,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9627</t>
+          <t>0.9714</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.928</t>
+          <t>0.937</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.008</t>
         </is>
       </c>
     </row>
@@ -1707,17 +1707,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1049</t>
+          <t>1.1138</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.091</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.137</t>
         </is>
       </c>
     </row>
@@ -1730,17 +1730,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2862</t>
+          <t>1.2956</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.260</t>
+          <t>1.269</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.313</t>
+          <t>1.323</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0665</t>
+          <t>1.0666</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1799,17 +1799,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9836</t>
+          <t>0.9846</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.879</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.102</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.7931</t>
+          <t>2.7932</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1909,12 +1909,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0276</t>
+          <t>1.0278</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1932,7 +1932,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2004</t>
+          <t>1.2001</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1955,17 +1955,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.3664</t>
+          <t>1.3787</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.261</t>
+          <t>1.273</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.480</t>
+          <t>1.494</t>
         </is>
       </c>
     </row>
@@ -1978,17 +1978,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0627</t>
+          <t>1.0691</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.029</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.104</t>
+          <t>1.111</t>
         </is>
       </c>
     </row>
@@ -2001,17 +2001,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.1463</t>
+          <t>1.1547</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.124</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.186</t>
         </is>
       </c>
     </row>
@@ -2024,17 +2024,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.7053</t>
+          <t>0.6883</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.677</t>
+          <t>0.660</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.735</t>
+          <t>0.717</t>
         </is>
       </c>
     </row>
@@ -2047,17 +2047,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9327</t>
+          <t>0.9393</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>0.868</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.016</t>
         </is>
       </c>
     </row>
@@ -2070,17 +2070,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.8606</t>
+          <t>0.8418</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.751</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>0.964</t>
         </is>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.4486</t>
+          <t>1.4487</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.8231</t>
+          <t>0.8230</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2237,17 +2237,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9248</t>
+          <t>0.9279</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.944</t>
+          <t>0.948</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0807</t>
+          <t>0.0808</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2283,17 +2283,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6135</t>
+          <t>0.6169</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.557</t>
+          <t>0.561</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.675</t>
+          <t>0.679</t>
         </is>
       </c>
     </row>
@@ -2306,17 +2306,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9184</t>
+          <t>0.9356</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.878</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.979</t>
         </is>
       </c>
     </row>
@@ -2329,17 +2329,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.8826</t>
+          <t>0.8621</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.833</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>0.893</t>
         </is>
       </c>
     </row>
@@ -2352,17 +2352,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1207</t>
+          <t>1.1436</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.158</t>
+          <t>1.181</t>
         </is>
       </c>
     </row>
@@ -2375,17 +2375,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0581</t>
+          <t>1.0681</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.010</t>
+          <t>1.020</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.119</t>
         </is>
       </c>
     </row>
@@ -2398,17 +2398,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2433</t>
+          <t>1.2505</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.162</t>
+          <t>1.169</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.338</t>
         </is>
       </c>
     </row>
@@ -2421,17 +2421,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.8184</t>
+          <t>0.8212</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.718</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.940</t>
         </is>
       </c>
     </row>
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0791</t>
+          <t>1.0833</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.070</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0884</t>
+          <t>0.0885</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8763</t>
+          <t>0.8874</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.855</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.910</t>
+          <t>0.921</t>
         </is>
       </c>
     </row>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0249</t>
+          <t>1.0264</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>1.005</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.048</t>
         </is>
       </c>
     </row>
@@ -2600,17 +2600,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0785</t>
+          <t>1.0870</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.101</t>
+          <t>1.110</t>
         </is>
       </c>
     </row>
@@ -2623,17 +2623,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.3185</t>
+          <t>1.3204</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.282</t>
+          <t>1.284</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.356</t>
+          <t>1.358</t>
         </is>
       </c>
     </row>
@@ -2646,17 +2646,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.0319</t>
+          <t>1.0247</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.970</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.082</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1244</t>
+          <t>1.1253</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.228</t>
         </is>
       </c>
     </row>
@@ -2779,17 +2779,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.1669</t>
+          <t>1.1674</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.143</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.193</t>
         </is>
       </c>
     </row>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0956</t>
+          <t>1.0952</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2812,7 +2812,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.115</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -2825,17 +2825,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.4284</t>
+          <t>1.4385</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.300</t>
+          <t>1.309</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.570</t>
+          <t>1.581</t>
         </is>
       </c>
     </row>
@@ -2848,17 +2848,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.1160</t>
+          <t>1.0970</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.166</t>
+          <t>1.146</t>
         </is>
       </c>
     </row>
@@ -2871,17 +2871,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.2219</t>
+          <t>1.2609</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.219</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.264</t>
+          <t>1.304</t>
         </is>
       </c>
     </row>
@@ -2894,17 +2894,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.1765</t>
+          <t>1.1546</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.218</t>
+          <t>1.195</t>
         </is>
       </c>
     </row>
@@ -2917,17 +2917,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9753</t>
+          <t>0.9593</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.020</t>
         </is>
       </c>
     </row>
@@ -2940,17 +2940,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.9044</t>
+          <t>0.8999</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.820</t>
+          <t>0.816</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.998</t>
+          <t>0.993</t>
         </is>
       </c>
     </row>
@@ -2963,17 +2963,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.6674</t>
+          <t>1.6616</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1.379</t>
+          <t>1.374</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2.016</t>
+          <t>2.009</t>
         </is>
       </c>
     </row>
@@ -3014,12 +3014,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.683</t>
+          <t>0.682</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2.210</t>
+          <t>2.209</t>
         </is>
       </c>
     </row>
@@ -3107,17 +3107,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6279</t>
+          <t>0.6315</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.612</t>
+          <t>0.616</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.644</t>
+          <t>0.648</t>
         </is>
       </c>
     </row>
@@ -3130,17 +3130,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0037</t>
+          <t>0.0005</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.001</t>
         </is>
       </c>
     </row>
@@ -3268,17 +3268,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9680</t>
+          <t>1.2211</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.316</t>
         </is>
       </c>
     </row>
@@ -3291,17 +3291,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.4360</t>
+          <t>1.3106</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.290</t>
+          <t>1.177</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.599</t>
+          <t>1.459</t>
         </is>
       </c>
     </row>
@@ -3314,17 +3314,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.8513</t>
+          <t>0.7704</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.729</t>
+          <t>0.660</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.994</t>
+          <t>0.899</t>
         </is>
       </c>
     </row>
@@ -3378,17 +3378,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8896</t>
+          <t>0.9015</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.909</t>
         </is>
       </c>
     </row>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -3424,17 +3424,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.7623</t>
+          <t>0.7979</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.738</t>
+          <t>0.772</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.787</t>
+          <t>0.824</t>
         </is>
       </c>
     </row>
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8394</t>
+          <t>0.8552</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.826</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.869</t>
         </is>
       </c>
     </row>
@@ -3470,17 +3470,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.9049</t>
+          <t>0.9115</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.891</t>
+          <t>0.898</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.925</t>
         </is>
       </c>
     </row>
@@ -3493,17 +3493,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9086</t>
+          <t>0.9134</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.897</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.925</t>
+          <t>0.930</t>
         </is>
       </c>
     </row>
@@ -3539,17 +3539,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9975</t>
+          <t>1.0490</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>1.007</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.040</t>
+          <t>1.093</t>
         </is>
       </c>
     </row>
@@ -3562,17 +3562,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.5695</t>
+          <t>1.4325</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.458</t>
+          <t>1.331</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.689</t>
+          <t>1.542</t>
         </is>
       </c>
     </row>
@@ -3585,17 +3585,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.0556</t>
+          <t>0.9324</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>0.824</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.054</t>
         </is>
       </c>
     </row>
@@ -3649,17 +3649,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4168</t>
+          <t>1.4276</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.382</t>
+          <t>1.393</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.452</t>
+          <t>1.463</t>
         </is>
       </c>
     </row>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.0463</t>
+          <t>0.0461</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3695,17 +3695,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.9422</t>
+          <t>3.0799</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.603</t>
+          <t>2.725</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>3.325</t>
+          <t>3.481</t>
         </is>
       </c>
     </row>
@@ -3718,17 +3718,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0614</t>
+          <t>1.0815</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>1.025</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.141</t>
         </is>
       </c>
     </row>
@@ -3741,17 +3741,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1.7560</t>
+          <t>1.7687</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.686</t>
+          <t>1.698</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1.829</t>
+          <t>1.842</t>
         </is>
       </c>
     </row>
@@ -3764,17 +3764,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.2193</t>
+          <t>1.2257</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>1.175</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.272</t>
+          <t>1.279</t>
         </is>
       </c>
     </row>
@@ -3810,17 +3810,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.0305</t>
+          <t>0.8591</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.954</t>
+          <t>0.796</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.114</t>
+          <t>0.927</t>
         </is>
       </c>
     </row>
@@ -3856,17 +3856,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.2400</t>
+          <t>1.2102</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.015</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1.480</t>
+          <t>1.444</t>
         </is>
       </c>
     </row>
@@ -4000,17 +4000,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.1986</t>
+          <t>0.4015</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.184</t>
+          <t>0.371</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.215</t>
+          <t>0.434</t>
         </is>
       </c>
     </row>
@@ -4023,17 +4023,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8591</t>
+          <t>0.8569</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.632</t>
+          <t>0.631</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.167</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -4184,17 +4184,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.1913</t>
+          <t>1.1928</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.682</t>
+          <t>0.683</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2.081</t>
+          <t>2.084</t>
         </is>
       </c>
     </row>
@@ -4207,17 +4207,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.2431</t>
+          <t>0.2558</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.060</t>
+          <t>0.063</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>1.036</t>
         </is>
       </c>
     </row>
@@ -4248,17 +4248,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0211</t>
+          <t>1.0315</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.044</t>
+          <t>1.055</t>
         </is>
       </c>
     </row>
@@ -4271,17 +4271,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.1317</t>
+          <t>0.4044</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.128</t>
+          <t>0.393</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.135</t>
+          <t>0.416</t>
         </is>
       </c>
     </row>
@@ -4386,17 +4386,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8518</t>
+          <t>0.9819</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.793</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>1.053</t>
         </is>
       </c>
     </row>
@@ -4409,17 +4409,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1269</t>
+          <t>1.1449</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.025</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.259</t>
         </is>
       </c>
     </row>
@@ -4455,17 +4455,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2.0419</t>
+          <t>2.0402</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.634</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2.550</t>
+          <t>2.548</t>
         </is>
       </c>
     </row>
@@ -4478,17 +4478,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1.3235</t>
+          <t>1.3927</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1.757</t>
+          <t>1.855</t>
         </is>
       </c>
     </row>
@@ -4519,17 +4519,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9909</t>
+          <t>1.0011</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.927</t>
+          <t>0.937</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.059</t>
+          <t>1.070</t>
         </is>
       </c>
     </row>
@@ -4542,17 +4542,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.6630</t>
+          <t>1.0072</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.613</t>
+          <t>0.931</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -4565,17 +4565,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.2017</t>
+          <t>1.2047</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.639</t>
+          <t>1.643</t>
         </is>
       </c>
     </row>
@@ -4657,17 +4657,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9246</t>
+          <t>1.0658</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.748</t>
+          <t>0.863</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.317</t>
         </is>
       </c>
     </row>
@@ -4680,17 +4680,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>0.9397</t>
+          <t>0.9547</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.722</t>
+          <t>0.734</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.223</t>
+          <t>1.242</t>
         </is>
       </c>
     </row>
@@ -4790,17 +4790,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.1283</t>
+          <t>1.1341</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.114</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.149</t>
+          <t>1.155</t>
         </is>
       </c>
     </row>
@@ -4813,17 +4813,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.0700</t>
+          <t>0.1416</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.068</t>
+          <t>0.139</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.072</t>
+          <t>0.145</t>
         </is>
       </c>
     </row>
@@ -4836,17 +4836,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.0986</t>
+          <t>1.1034</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.039</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1.166</t>
+          <t>1.171</t>
         </is>
       </c>
     </row>
@@ -4859,17 +4859,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.0836</t>
+          <t>1.0876</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.121</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -4882,17 +4882,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.1466</t>
+          <t>1.1550</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.109</t>
+          <t>1.117</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.186</t>
+          <t>1.194</t>
         </is>
       </c>
     </row>
@@ -4905,17 +4905,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.1883</t>
+          <t>1.1897</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.142</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1.238</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -4928,17 +4928,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9934</t>
+          <t>1.0036</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -4951,17 +4951,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1.2303</t>
+          <t>1.2336</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.120</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.355</t>
+          <t>1.359</t>
         </is>
       </c>
     </row>
@@ -4997,17 +4997,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.2715</t>
+          <t>1.2704</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.967</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.672</t>
+          <t>1.670</t>
         </is>
       </c>
     </row>
@@ -5020,17 +5020,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1.0939</t>
+          <t>1.1511</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.699</t>
+          <t>0.734</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.713</t>
+          <t>1.806</t>
         </is>
       </c>
     </row>
@@ -5061,17 +5061,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0973</t>
+          <t>1.1031</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1.028</t>
+          <t>1.034</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.171</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.3524</t>
+          <t>0.3526</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.326</t>
+          <t>0.327</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0.380</t>
+          <t>0.381</t>
         </is>
       </c>
     </row>
@@ -5107,17 +5107,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.2789</t>
+          <t>1.2876</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.943</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1.734</t>
+          <t>1.746</t>
         </is>
       </c>
     </row>
@@ -5130,17 +5130,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>1.0066</t>
+          <t>1.0104</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.893</t>
+          <t>0.896</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -5153,17 +5153,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1.0514</t>
+          <t>1.0591</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.931</t>
+          <t>0.938</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1.187</t>
+          <t>1.196</t>
         </is>
       </c>
     </row>
@@ -5176,17 +5176,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.2849</t>
+          <t>1.2864</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.109</t>
+          <t>1.110</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.489</t>
+          <t>1.491</t>
         </is>
       </c>
     </row>
@@ -5199,17 +5199,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1.0783</t>
+          <t>1.0894</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.874</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1.330</t>
+          <t>1.343</t>
         </is>
       </c>
     </row>
@@ -5222,17 +5222,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.0259</t>
+          <t>1.0287</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.790</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.336</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.5708</t>
+          <t>0.5709</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5332,17 +5332,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.1050</t>
+          <t>1.0994</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.127</t>
+          <t>1.121</t>
         </is>
       </c>
     </row>
@@ -5355,17 +5355,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.5316</t>
+          <t>0.3501</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.521</t>
+          <t>0.342</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0.543</t>
+          <t>0.358</t>
         </is>
       </c>
     </row>
@@ -5378,17 +5378,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1.0643</t>
+          <t>1.0688</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.989</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1.150</t>
+          <t>1.155</t>
         </is>
       </c>
     </row>
@@ -5401,17 +5401,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.0778</t>
+          <t>1.0818</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.041</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.124</t>
         </is>
       </c>
     </row>
@@ -5424,17 +5424,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1.1114</t>
+          <t>1.1196</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.080</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.152</t>
+          <t>1.160</t>
         </is>
       </c>
     </row>
@@ -5447,17 +5447,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1.1404</t>
+          <t>1.1418</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.093</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.193</t>
         </is>
       </c>
     </row>
@@ -5470,17 +5470,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1.1663</t>
+          <t>1.0221</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>0.952</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1.253</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -5493,17 +5493,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.0917</t>
+          <t>1.0775</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.985</t>
+          <t>0.972</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.210</t>
+          <t>1.194</t>
         </is>
       </c>
     </row>
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9327</t>
+          <t>0.9318</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.983</t>
         </is>
       </c>
     </row>
@@ -5706,17 +5706,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.4597</t>
+          <t>0.4527</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.365</t>
+          <t>0.359</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.579</t>
+          <t>0.571</t>
         </is>
       </c>
     </row>
@@ -5798,7 +5798,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9975</t>
+          <t>0.9974</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -5844,7 +5844,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.9145</t>
+          <t>2.9141</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.735</t>
+          <t>3.734</t>
         </is>
       </c>
     </row>
@@ -5931,17 +5931,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0048</t>
+          <t>1.0058</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>0.990</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.022</t>
         </is>
       </c>
     </row>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0377</t>
+          <t>0.0376</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -6069,17 +6069,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8520</t>
+          <t>0.8787</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.814</t>
+          <t>0.840</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.919</t>
         </is>
       </c>
     </row>
@@ -6092,17 +6092,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1345</t>
+          <t>1.1435</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.076</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.205</t>
+          <t>1.215</t>
         </is>
       </c>
     </row>
@@ -6115,17 +6115,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1340</t>
+          <t>0.9999</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.100</t>
         </is>
       </c>
     </row>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -6202,17 +6202,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0768</t>
+          <t>1.0790</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.022</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.139</t>
         </is>
       </c>
     </row>
@@ -6225,17 +6225,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.1915</t>
+          <t>4.1800</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3.787</t>
+          <t>3.776</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4.640</t>
+          <t>4.627</t>
         </is>
       </c>
     </row>
@@ -6248,17 +6248,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.0421</t>
+          <t>2.0735</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.615</t>
+          <t>1.640</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2.581</t>
+          <t>2.622</t>
         </is>
       </c>
     </row>
@@ -6340,17 +6340,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.8542</t>
+          <t>0.8810</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.732</t>
+          <t>0.755</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.997</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -6363,17 +6363,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.2922</t>
+          <t>1.3025</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.064</t>
+          <t>1.072</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.570</t>
+          <t>1.582</t>
         </is>
       </c>
     </row>
@@ -6386,17 +6386,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0.3891</t>
+          <t>0.3431</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.302</t>
+          <t>0.266</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0.501</t>
+          <t>0.442</t>
         </is>
       </c>
     </row>
@@ -6473,17 +6473,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9473</t>
+          <t>0.9608</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.949</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>0.972</t>
         </is>
       </c>
     </row>
@@ -6519,17 +6519,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.7459</t>
+          <t>0.7510</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>0.712</t>
+          <t>0.717</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0.782</t>
+          <t>0.787</t>
         </is>
       </c>
     </row>
@@ -6542,17 +6542,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.9569</t>
+          <t>0.9771</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>1.000</t>
         </is>
       </c>
     </row>
@@ -6565,17 +6565,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.0568</t>
+          <t>1.0659</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.034</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1.080</t>
+          <t>1.090</t>
         </is>
       </c>
     </row>
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8568</t>
+          <t>0.8652</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0.835</t>
+          <t>0.843</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.888</t>
         </is>
       </c>
     </row>
@@ -6611,17 +6611,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9340</t>
+          <t>0.9383</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.898</t>
+          <t>0.903</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>0.975</t>
         </is>
       </c>
     </row>
@@ -6634,17 +6634,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.9557</t>
+          <t>0.9749</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.922</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.011</t>
+          <t>1.031</t>
         </is>
       </c>
     </row>
@@ -6657,17 +6657,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.0889</t>
+          <t>1.3356</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.989</t>
+          <t>1.214</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>1.469</t>
         </is>
       </c>
     </row>
@@ -6680,17 +6680,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>0.8035</t>
+          <t>0.8165</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>0.689</t>
+          <t>0.700</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.952</t>
         </is>
       </c>
     </row>
@@ -6744,17 +6744,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0138</t>
+          <t>1.0293</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.976</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.086</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.0179</t>
+          <t>0.0181</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -6790,17 +6790,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1.6227</t>
+          <t>1.6590</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1.291</t>
+          <t>1.319</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2.040</t>
+          <t>2.086</t>
         </is>
       </c>
     </row>
@@ -6813,17 +6813,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.7831</t>
+          <t>0.7996</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.706</t>
+          <t>0.720</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.869</t>
+          <t>0.888</t>
         </is>
       </c>
     </row>
@@ -6836,17 +6836,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.8764</t>
+          <t>0.8839</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0.792</t>
+          <t>0.799</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>0.970</t>
+          <t>0.978</t>
         </is>
       </c>
     </row>
@@ -6859,17 +6859,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.4769</t>
+          <t>1.4913</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.322</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1.666</t>
+          <t>1.682</t>
         </is>
       </c>
     </row>
@@ -6882,17 +6882,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>0.9363</t>
+          <t>0.9407</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.096</t>
         </is>
       </c>
     </row>
@@ -6905,17 +6905,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.0886</t>
+          <t>1.1104</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.897</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.321</t>
+          <t>1.347</t>
         </is>
       </c>
     </row>
@@ -6928,17 +6928,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0.3736</t>
+          <t>0.4583</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.290</t>
+          <t>0.356</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>0.481</t>
+          <t>0.590</t>
         </is>
       </c>
     </row>
@@ -6951,17 +6951,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2.3350</t>
+          <t>2.3730</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.473</t>
+          <t>1.497</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>3.701</t>
+          <t>3.761</t>
         </is>
       </c>
     </row>
@@ -7015,17 +7015,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.9428</t>
+          <t>0.9553</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>0.943</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.968</t>
         </is>
       </c>
     </row>
@@ -7061,17 +7061,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.7946</t>
+          <t>0.8001</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.748</t>
+          <t>0.753</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.844</t>
+          <t>0.850</t>
         </is>
       </c>
     </row>
@@ -7084,17 +7084,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>0.9390</t>
+          <t>0.9588</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>0.933</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>0.965</t>
+          <t>0.986</t>
         </is>
       </c>
     </row>
@@ -7107,17 +7107,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.9955</t>
+          <t>1.0041</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.980</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1.020</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -7130,17 +7130,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.9000</t>
+          <t>0.9087</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.874</t>
+          <t>0.883</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.926</t>
+          <t>0.935</t>
         </is>
       </c>
     </row>
@@ -7153,17 +7153,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1.0961</t>
+          <t>1.0677</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.050</t>
+          <t>1.023</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1.144</t>
+          <t>1.114</t>
         </is>
       </c>
     </row>
@@ -7176,17 +7176,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>0.8424</t>
+          <t>0.8525</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>0.793</t>
+          <t>0.802</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>0.895</t>
+          <t>0.906</t>
         </is>
       </c>
     </row>
@@ -7199,17 +7199,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0.9602</t>
+          <t>1.3357</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.863</t>
+          <t>1.200</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.069</t>
+          <t>1.486</t>
         </is>
       </c>
     </row>
@@ -7222,17 +7222,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>0.8472</t>
+          <t>0.8609</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.729</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.017</t>
         </is>
       </c>
     </row>
@@ -7343,12 +7343,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0933</t>
+          <t>1.0927</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.015</t>
+          <t>1.014</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -7366,17 +7366,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0640</t>
+          <t>0.0056</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.058</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.071</t>
+          <t>0.006</t>
         </is>
       </c>
     </row>
@@ -7389,17 +7389,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.8031</t>
+          <t>1.8057</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.336</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2.437</t>
+          <t>2.440</t>
         </is>
       </c>
     </row>
@@ -7481,7 +7481,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.5996</t>
+          <t>1.5994</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -7491,7 +7491,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.014</t>
+          <t>2.013</t>
         </is>
       </c>
     </row>
@@ -7527,17 +7527,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3671</t>
+          <t>1.3164</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.936</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.922</t>
+          <t>1.851</t>
         </is>
       </c>
     </row>
@@ -7550,17 +7550,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.9874</t>
+          <t>0.0000</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.524</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.860</t>
+          <t>0.000</t>
         </is>
       </c>
     </row>
@@ -7614,17 +7614,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9944</t>
+          <t>0.9993</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.018</t>
+          <t>1.023</t>
         </is>
       </c>
     </row>
@@ -7637,17 +7637,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.1475</t>
+          <t>0.0129</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.142</t>
+          <t>0.012</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.153</t>
+          <t>0.013</t>
         </is>
       </c>
     </row>
@@ -7752,17 +7752,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8004</t>
+          <t>0.8581</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.748</t>
+          <t>0.802</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.856</t>
+          <t>0.918</t>
         </is>
       </c>
     </row>
@@ -7775,17 +7775,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8176</t>
+          <t>0.8466</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.747</t>
+          <t>0.774</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.895</t>
+          <t>0.926</t>
         </is>
       </c>
     </row>
@@ -7798,17 +7798,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.2725</t>
+          <t>1.2254</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.462</t>
+          <t>1.407</t>
         </is>
       </c>
     </row>
@@ -7821,17 +7821,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.1284</t>
+          <t>1.0026</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.912</t>
+          <t>0.811</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.397</t>
+          <t>1.240</t>
         </is>
       </c>
     </row>
@@ -7885,17 +7885,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9094</t>
+          <t>0.9159</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.843</t>
+          <t>0.849</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.981</t>
+          <t>0.988</t>
         </is>
       </c>
     </row>
@@ -7908,17 +7908,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.3050</t>
+          <t>2.3164</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.077</t>
+          <t>2.087</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.558</t>
+          <t>2.571</t>
         </is>
       </c>
     </row>
@@ -7931,17 +7931,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.8023</t>
+          <t>0.8011</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.590</t>
+          <t>0.589</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1.090</t>
+          <t>1.089</t>
         </is>
       </c>
     </row>
@@ -8023,17 +8023,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.5003</t>
+          <t>0.5365</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.397</t>
+          <t>0.425</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.631</t>
+          <t>0.677</t>
         </is>
       </c>
     </row>
@@ -8046,17 +8046,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.2158</t>
+          <t>1.2590</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.904</t>
+          <t>0.936</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.693</t>
         </is>
       </c>
     </row>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0.9309</t>
+          <t>0.9308</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -8156,17 +8156,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0205</t>
+          <t>1.0196</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1.039</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -8179,17 +8179,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.0582</t>
+          <t>0.0151</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>0.057</t>
+          <t>0.015</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0.060</t>
+          <t>0.016</t>
         </is>
       </c>
     </row>
@@ -8294,17 +8294,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9120</t>
+          <t>0.9048</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.861</t>
+          <t>0.854</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.959</t>
         </is>
       </c>
     </row>
@@ -8317,17 +8317,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.9289</t>
+          <t>0.9352</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.861</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.016</t>
         </is>
       </c>
     </row>
@@ -8340,17 +8340,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.3625</t>
+          <t>1.4404</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.178</t>
+          <t>1.247</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.663</t>
         </is>
       </c>
     </row>
@@ -8363,17 +8363,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.5798</t>
+          <t>1.4037</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.259</t>
+          <t>1.119</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.982</t>
+          <t>1.760</t>
         </is>
       </c>
     </row>
@@ -8427,17 +8427,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.9287</t>
+          <t>0.9299</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.862</t>
+          <t>0.864</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.001</t>
         </is>
       </c>
     </row>
@@ -8450,17 +8450,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.9088</t>
+          <t>2.7143</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.821</t>
+          <t>2.451</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1.006</t>
+          <t>3.006</t>
         </is>
       </c>
     </row>
@@ -8473,17 +8473,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.5687</t>
+          <t>0.5679</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0.422</t>
+          <t>0.421</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0.767</t>
+          <t>0.765</t>
         </is>
       </c>
     </row>
@@ -8565,17 +8565,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>0.5701</t>
+          <t>0.5657</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>0.453</t>
+          <t>0.450</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>0.717</t>
+          <t>0.712</t>
         </is>
       </c>
     </row>
@@ -8588,17 +8588,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.3814</t>
+          <t>1.3908</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>1.036</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.854</t>
+          <t>1.867</t>
         </is>
       </c>
     </row>
@@ -8611,17 +8611,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>0.9967</t>
+          <t>1.0941</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.702</t>
+          <t>0.771</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1.415</t>
+          <t>1.553</t>
         </is>
       </c>
     </row>
@@ -8698,17 +8698,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.0263</t>
+          <t>1.0203</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.000</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -8721,17 +8721,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>0.3943</t>
+          <t>1.1718</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>0.383</t>
+          <t>1.137</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>0.406</t>
+          <t>1.208</t>
         </is>
       </c>
     </row>
@@ -8836,17 +8836,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1.1395</t>
+          <t>1.0544</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>0.988</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1.216</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -8859,17 +8859,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1.1362</t>
+          <t>1.1047</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.037</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.210</t>
         </is>
       </c>
     </row>
@@ -8882,17 +8882,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.0707</t>
+          <t>1.1754</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>0.911</t>
+          <t>1.001</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.259</t>
+          <t>1.380</t>
         </is>
       </c>
     </row>
@@ -8969,17 +8969,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0.9727</t>
+          <t>0.9813</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.958</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>0.996</t>
+          <t>1.005</t>
         </is>
       </c>
     </row>
@@ -8992,17 +8992,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>0.0086</t>
+          <t>0.0008</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>0.008</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>0.009</t>
+          <t>0.001</t>
         </is>
       </c>
     </row>
@@ -9015,17 +9015,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.8841</t>
+          <t>0.8937</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>0.816</t>
+          <t>0.825</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.968</t>
         </is>
       </c>
     </row>
@@ -9061,17 +9061,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>0.9005</t>
+          <t>0.9082</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>0.865</t>
+          <t>0.873</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.945</t>
         </is>
       </c>
     </row>
@@ -9084,17 +9084,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>1.0132</t>
+          <t>1.0507</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1.068</t>
+          <t>1.108</t>
         </is>
       </c>
     </row>
@@ -9107,17 +9107,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1.2038</t>
+          <t>1.2205</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.103</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.351</t>
         </is>
       </c>
     </row>
@@ -9130,7 +9130,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2.5404</t>
+          <t>2.5405</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -9153,17 +9153,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>0.6857</t>
+          <t>0.6603</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0.487</t>
+          <t>0.469</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>0.965</t>
+          <t>0.929</t>
         </is>
       </c>
     </row>
@@ -9176,17 +9176,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.2446</t>
+          <t>1.1059</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>0.653</t>
+          <t>0.580</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2.373</t>
+          <t>2.108</t>
         </is>
       </c>
     </row>
@@ -9240,17 +9240,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>0.8868</t>
+          <t>0.8967</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>0.822</t>
+          <t>0.831</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>0.956</t>
+          <t>0.967</t>
         </is>
       </c>
     </row>
@@ -9263,12 +9263,12 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>0.1344</t>
+          <t>0.1347</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>0.121</t>
+          <t>0.122</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -9286,17 +9286,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0.4903</t>
+          <t>0.4949</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>0.363</t>
+          <t>0.367</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>0.662</t>
+          <t>0.668</t>
         </is>
       </c>
     </row>
@@ -9332,17 +9332,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>0.8461</t>
+          <t>0.8533</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>0.732</t>
+          <t>0.738</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.987</t>
         </is>
       </c>
     </row>
@@ -9355,17 +9355,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.0086</t>
+          <t>1.0459</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>0.846</t>
+          <t>0.878</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>1.246</t>
         </is>
       </c>
     </row>
@@ -9378,17 +9378,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>0.7526</t>
+          <t>0.7631</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>0.589</t>
+          <t>0.598</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
@@ -9401,7 +9401,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>3.7779</t>
+          <t>3.7780</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -9511,17 +9511,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>0.9767</t>
+          <t>0.9805</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>0.951</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.003</t>
+          <t>1.007</t>
         </is>
       </c>
     </row>
@@ -9534,12 +9534,12 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>0.0583</t>
+          <t>0.0582</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>0.057</t>
+          <t>0.056</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -9557,17 +9557,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>0.6112</t>
+          <t>0.6179</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>0.553</t>
+          <t>0.560</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>0.675</t>
+          <t>0.682</t>
         </is>
       </c>
     </row>
@@ -9603,17 +9603,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>0.9222</t>
+          <t>0.9300</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>0.963</t>
+          <t>0.972</t>
         </is>
       </c>
     </row>
@@ -9626,17 +9626,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>0.9701</t>
+          <t>1.0060</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.951</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1.026</t>
+          <t>1.064</t>
         </is>
       </c>
     </row>
@@ -9649,17 +9649,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>1.5041</t>
+          <t>1.4223</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.353</t>
+          <t>1.279</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1.673</t>
+          <t>1.581</t>
         </is>
       </c>
     </row>
@@ -9672,17 +9672,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>3.1074</t>
+          <t>3.0008</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2.586</t>
+          <t>2.498</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3.733</t>
+          <t>3.605</t>
         </is>
       </c>
     </row>
@@ -9782,17 +9782,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>0.9525</t>
+          <t>0.9618</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>0.941</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>0.983</t>
         </is>
       </c>
     </row>
@@ -9805,17 +9805,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>0.1479</t>
+          <t>0.0496</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>0.145</t>
+          <t>0.049</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>0.151</t>
+          <t>0.051</t>
         </is>
       </c>
     </row>
@@ -9828,17 +9828,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>0.8621</t>
+          <t>0.8715</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>0.805</t>
+          <t>0.814</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>0.923</t>
+          <t>0.933</t>
         </is>
       </c>
     </row>
@@ -9874,17 +9874,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>0.8628</t>
+          <t>0.8702</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>0.835</t>
+          <t>0.842</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>0.892</t>
+          <t>0.900</t>
         </is>
       </c>
     </row>
@@ -9897,17 +9897,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>0.9657</t>
+          <t>1.0015</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>1.013</t>
+          <t>1.050</t>
         </is>
       </c>
     </row>
@@ -9920,17 +9920,17 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>1.3200</t>
+          <t>1.3489</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>1.194</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>1.459</t>
+          <t>1.491</t>
         </is>
       </c>
     </row>
@@ -9943,17 +9943,17 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>2.7348</t>
+          <t>2.7165</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2.284</t>
+          <t>2.269</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>3.274</t>
+          <t>3.252</t>
         </is>
       </c>
     </row>
@@ -9966,17 +9966,17 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>0.5033</t>
+          <t>0.4585</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>0.354</t>
+          <t>0.323</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.651</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated KCOR to reduce failure on number of iterations
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -497,17 +497,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2417</t>
+          <t>1.2615</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.238</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.265</t>
+          <t>1.285</t>
         </is>
       </c>
     </row>
@@ -520,17 +520,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.3020</t>
+          <t>0.3031</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.297</t>
+          <t>0.298</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.307</t>
+          <t>0.308</t>
         </is>
       </c>
     </row>
@@ -543,17 +543,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9497</t>
+          <t>1.1377</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>1.067</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.013</t>
+          <t>1.213</t>
         </is>
       </c>
     </row>
@@ -768,17 +768,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3405</t>
+          <t>1.3617</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.318</t>
+          <t>1.339</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.363</t>
+          <t>1.385</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.3533</t>
+          <t>0.3545</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.349</t>
+          <t>0.350</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.358</t>
+          <t>0.359</t>
         </is>
       </c>
     </row>
@@ -814,17 +814,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3291</t>
+          <t>1.5922</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.283</t>
+          <t>1.537</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.376</t>
+          <t>1.649</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3318</t>
+          <t>1.3317</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1367,17 +1367,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1278</t>
+          <t>1.2250</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.108</t>
+          <t>1.204</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.148</t>
+          <t>1.247</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1390,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0392</t>
+          <t>0.0397</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.038</t>
+          <t>0.039</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1413,17 +1413,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.7046</t>
+          <t>0.9869</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.649</t>
+          <t>0.910</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -1436,17 +1436,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0419</t>
+          <t>1.2028</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.002</t>
+          <t>1.156</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.084</t>
+          <t>1.251</t>
         </is>
       </c>
     </row>
@@ -1505,17 +1505,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.3737</t>
+          <t>1.4201</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.356</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.439</t>
+          <t>1.488</t>
         </is>
       </c>
     </row>
@@ -1528,17 +1528,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1697</t>
+          <t>1.2709</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.165</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.276</t>
+          <t>1.386</t>
         </is>
       </c>
     </row>
@@ -1638,17 +1638,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.1560</t>
+          <t>1.2365</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.141</t>
+          <t>1.220</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.171</t>
+          <t>1.253</t>
         </is>
       </c>
     </row>
@@ -1661,12 +1661,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0470</t>
+          <t>0.0476</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.046</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1684,17 +1684,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9714</t>
+          <t>1.3607</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>1.312</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.008</t>
+          <t>1.412</t>
         </is>
       </c>
     </row>
@@ -1707,17 +1707,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1138</t>
+          <t>1.2859</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.260</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.312</t>
         </is>
       </c>
     </row>
@@ -1776,17 +1776,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2904</t>
+          <t>1.0003</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.202</t>
+          <t>0.930</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.386</t>
+          <t>1.076</t>
         </is>
       </c>
     </row>
@@ -1799,17 +1799,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9846</t>
+          <t>1.0699</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.880</t>
+          <t>0.956</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.198</t>
         </is>
       </c>
     </row>
@@ -1909,17 +1909,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0278</t>
+          <t>1.0126</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>0.994</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.032</t>
         </is>
       </c>
     </row>
@@ -1932,17 +1932,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.2001</t>
+          <t>1.1990</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1.219</t>
+          <t>1.218</t>
         </is>
       </c>
     </row>
@@ -2047,17 +2047,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.9393</t>
+          <t>0.7044</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.868</t>
+          <t>0.650</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1.016</t>
+          <t>0.763</t>
         </is>
       </c>
     </row>
@@ -2237,17 +2237,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9279</t>
+          <t>1.0244</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>1.003</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.948</t>
+          <t>1.046</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0808</t>
+          <t>0.0811</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.082</t>
+          <t>0.083</t>
         </is>
       </c>
     </row>
@@ -2283,17 +2283,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6169</t>
+          <t>0.8714</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.561</t>
+          <t>0.792</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.679</t>
+          <t>0.959</t>
         </is>
       </c>
     </row>
@@ -2306,17 +2306,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9356</t>
+          <t>1.1562</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>1.105</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>1.210</t>
         </is>
       </c>
     </row>
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0833</t>
+          <t>1.1959</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.070</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.097</t>
+          <t>1.211</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0885</t>
+          <t>0.0888</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2554,17 +2554,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8874</t>
+          <t>1.2534</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>1.207</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>1.302</t>
         </is>
       </c>
     </row>
@@ -2577,17 +2577,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0264</t>
+          <t>1.2684</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.242</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.296</t>
         </is>
       </c>
     </row>
@@ -3107,17 +3107,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6315</t>
+          <t>0.7029</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.616</t>
+          <t>0.685</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.648</t>
+          <t>0.721</t>
         </is>
       </c>
     </row>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.0005</t>
+          <t>0.0006</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3153,17 +3153,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.2591</t>
+          <t>0.3491</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.229</t>
+          <t>0.308</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.293</t>
+          <t>0.395</t>
         </is>
       </c>
     </row>
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.7908</t>
+          <t>1.0040</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.748</t>
+          <t>0.950</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.835</t>
+          <t>1.061</t>
         </is>
       </c>
     </row>
@@ -3245,17 +3245,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.8037</t>
+          <t>0.9148</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.757</t>
+          <t>0.862</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.853</t>
+          <t>0.971</t>
         </is>
       </c>
     </row>
@@ -3291,17 +3291,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3106</t>
+          <t>1.2151</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.177</t>
+          <t>1.091</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.459</t>
+          <t>1.353</t>
         </is>
       </c>
     </row>
@@ -3337,17 +3337,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1.5102</t>
+          <t>1.8438</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>1.527</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.822</t>
+          <t>2.226</t>
         </is>
       </c>
     </row>
@@ -3378,17 +3378,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9015</t>
+          <t>1.0041</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>1.013</t>
         </is>
       </c>
     </row>
@@ -3424,17 +3424,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.7979</t>
+          <t>1.0752</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.772</t>
+          <t>1.040</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.824</t>
+          <t>1.111</t>
         </is>
       </c>
     </row>
@@ -3447,17 +3447,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.8552</t>
+          <t>1.0858</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>1.068</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.869</t>
+          <t>1.104</t>
         </is>
       </c>
     </row>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9134</t>
+          <t>0.9133</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -3516,17 +3516,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2307</t>
+          <t>1.4008</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.362</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.266</t>
+          <t>1.441</t>
         </is>
       </c>
     </row>
@@ -3608,17 +3608,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.2589</t>
+          <t>0.3161</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.202</t>
+          <t>0.247</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.331</t>
+          <t>0.405</t>
         </is>
       </c>
     </row>
@@ -3649,17 +3649,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.4276</t>
+          <t>1.4285</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.393</t>
+          <t>1.394</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.463</t>
+          <t>1.464</t>
         </is>
       </c>
     </row>
@@ -3672,7 +3672,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.0461</t>
+          <t>0.0462</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1.0815</t>
+          <t>1.0814</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -3833,17 +3833,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1.0930</t>
+          <t>1.1789</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.973</t>
+          <t>1.049</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.325</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0277</t>
+          <t>1.0279</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -4161,17 +4161,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.9593</t>
+          <t>0.9836</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.659</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.432</t>
+          <t>1.468</t>
         </is>
       </c>
     </row>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0315</t>
+          <t>1.0317</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.4044</t>
+          <t>0.4045</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.051</t>
         </is>
       </c>
     </row>
@@ -4432,17 +4432,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.1438</t>
+          <t>1.1727</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.981</t>
+          <t>1.006</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.333</t>
+          <t>1.368</t>
         </is>
       </c>
     </row>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.9340</t>
+          <t>0.9339</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.1341</t>
+          <t>1.1343</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1.1034</t>
+          <t>1.1033</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4974,17 +4974,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.2451</t>
+          <t>1.2767</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.051</t>
+          <t>1.078</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.474</t>
+          <t>1.512</t>
         </is>
       </c>
     </row>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1.2864</t>
+          <t>1.2865</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9318</t>
+          <t>0.9126</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.864</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.983</t>
+          <t>0.963</t>
         </is>
       </c>
     </row>
@@ -5729,17 +5729,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.2220</t>
+          <t>1.1229</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.099</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.358</t>
+          <t>1.251</t>
         </is>
       </c>
     </row>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.2059</t>
+          <t>1.2058</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5798,17 +5798,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.9974</t>
+          <t>1.0361</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.855</t>
+          <t>0.888</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.208</t>
         </is>
       </c>
     </row>
@@ -5821,17 +5821,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.8779</t>
+          <t>0.8538</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.724</t>
+          <t>0.703</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.065</t>
+          <t>1.037</t>
         </is>
       </c>
     </row>
@@ -5931,17 +5931,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0058</t>
+          <t>1.0130</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>0.997</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.029</t>
         </is>
       </c>
     </row>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.0376</t>
+          <t>0.0377</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -5977,17 +5977,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9387</t>
+          <t>0.8749</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.817</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>0.937</t>
         </is>
       </c>
     </row>
@@ -6000,17 +6000,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0191</t>
+          <t>1.0936</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>1.058</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.053</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -6046,17 +6046,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.9521</t>
+          <t>0.9143</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.921</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>0.945</t>
         </is>
       </c>
     </row>
@@ -6069,17 +6069,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.8787</t>
+          <t>0.9128</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.840</t>
+          <t>0.872</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.919</t>
+          <t>0.955</t>
         </is>
       </c>
     </row>
@@ -6202,17 +6202,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0790</t>
+          <t>1.1096</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.051</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1.139</t>
+          <t>1.172</t>
         </is>
       </c>
     </row>
@@ -6225,17 +6225,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.1800</t>
+          <t>4.1745</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3.776</t>
+          <t>3.771</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4.627</t>
+          <t>4.621</t>
         </is>
       </c>
     </row>
@@ -6248,17 +6248,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.0735</t>
+          <t>1.9326</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.640</t>
+          <t>1.528</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2.622</t>
+          <t>2.444</t>
         </is>
       </c>
     </row>
@@ -6271,17 +6271,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.8340</t>
+          <t>0.9739</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.750</t>
+          <t>0.873</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.928</t>
+          <t>1.086</t>
         </is>
       </c>
     </row>
@@ -6317,17 +6317,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.6411</t>
+          <t>1.5759</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.452</t>
+          <t>1.394</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1.855</t>
+          <t>1.781</t>
         </is>
       </c>
     </row>
@@ -6363,17 +6363,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.3025</t>
+          <t>1.3393</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.072</t>
+          <t>1.101</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1.582</t>
+          <t>1.628</t>
         </is>
       </c>
     </row>
@@ -6473,17 +6473,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.9608</t>
+          <t>0.9810</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.969</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.993</t>
         </is>
       </c>
     </row>
@@ -6542,17 +6542,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.9771</t>
+          <t>1.0486</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>1.024</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.074</t>
         </is>
       </c>
     </row>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.8652</t>
+          <t>0.8651</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -6611,17 +6611,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.9383</t>
+          <t>0.9746</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0.903</t>
+          <t>0.937</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>0.975</t>
+          <t>1.013</t>
         </is>
       </c>
     </row>
@@ -6744,17 +6744,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1.0293</t>
+          <t>1.0732</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>1.017</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1.086</t>
+          <t>1.132</t>
         </is>
       </c>
     </row>
@@ -6813,17 +6813,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.7996</t>
+          <t>0.9338</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.720</t>
+          <t>0.840</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>1.039</t>
         </is>
       </c>
     </row>
@@ -6905,17 +6905,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1.1104</t>
+          <t>1.1418</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.940</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1.347</t>
+          <t>1.386</t>
         </is>
       </c>
     </row>
@@ -7015,17 +7015,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.9553</t>
+          <t>0.9684</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>0.943</t>
+          <t>0.955</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>0.968</t>
+          <t>0.982</t>
         </is>
       </c>
     </row>
@@ -7061,17 +7061,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.8001</t>
+          <t>0.8584</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>0.753</t>
+          <t>0.808</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.912</t>
         </is>
       </c>
     </row>
@@ -7130,17 +7130,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.9087</t>
+          <t>0.9463</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>0.883</t>
+          <t>0.919</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.974</t>
         </is>
       </c>
     </row>
@@ -7343,17 +7343,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0927</t>
+          <t>1.0920</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.014</t>
+          <t>1.013</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.178</t>
+          <t>1.177</t>
         </is>
       </c>
     </row>
@@ -7527,17 +7527,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3164</t>
+          <t>1.2721</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.905</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.851</t>
+          <t>1.788</t>
         </is>
       </c>
     </row>
@@ -7614,17 +7614,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9993</t>
+          <t>0.9975</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.021</t>
         </is>
       </c>
     </row>
@@ -7798,17 +7798,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.2254</t>
+          <t>1.0447</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.067</t>
+          <t>0.908</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.407</t>
+          <t>1.202</t>
         </is>
       </c>
     </row>
@@ -7821,17 +7821,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.0026</t>
+          <t>1.0683</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.811</t>
+          <t>0.863</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1.240</t>
+          <t>1.322</t>
         </is>
       </c>
     </row>
@@ -7844,17 +7844,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.5492</t>
+          <t>0.5913</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.412</t>
+          <t>0.442</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.732</t>
+          <t>0.790</t>
         </is>
       </c>
     </row>
@@ -7885,17 +7885,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.9159</t>
+          <t>0.9139</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.847</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.986</t>
         </is>
       </c>
     </row>
@@ -7908,17 +7908,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2.3164</t>
+          <t>2.3079</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.087</t>
+          <t>2.080</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2.571</t>
+          <t>2.561</t>
         </is>
       </c>
     </row>
@@ -8069,17 +8069,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>0.9308</t>
+          <t>0.8212</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>0.657</t>
+          <t>0.579</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1.318</t>
+          <t>1.164</t>
         </is>
       </c>
     </row>
@@ -8156,7 +8156,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>1.0196</t>
+          <t>1.0201</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -8340,17 +8340,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1.4404</t>
+          <t>1.3919</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1.247</t>
+          <t>1.206</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1.663</t>
+          <t>1.607</t>
         </is>
       </c>
     </row>
@@ -8363,17 +8363,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1.4037</t>
+          <t>1.4956</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.119</t>
+          <t>1.192</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1.760</t>
+          <t>1.876</t>
         </is>
       </c>
     </row>
@@ -8386,17 +8386,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.8054</t>
+          <t>0.8672</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0.558</t>
+          <t>0.599</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.255</t>
         </is>
       </c>
     </row>
@@ -8519,7 +8519,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.9806</t>
+          <t>0.9805</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0941</t>
+          <t>1.0942</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -8698,17 +8698,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1.0203</t>
+          <t>1.0226</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>1.002</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1.041</t>
+          <t>1.044</t>
         </is>
       </c>
     </row>
@@ -8721,17 +8721,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1.1718</t>
+          <t>1.1761</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1.137</t>
+          <t>1.141</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1.208</t>
+          <t>1.212</t>
         </is>
       </c>
     </row>
@@ -8882,17 +8882,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1.1754</t>
+          <t>1.3324</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1.001</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1.380</t>
+          <t>1.567</t>
         </is>
       </c>
     </row>
@@ -8969,7 +8969,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>0.9813</t>
+          <t>0.9815</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -8979,7 +8979,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1.005</t>
+          <t>1.006</t>
         </is>
       </c>
     </row>
@@ -9130,7 +9130,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2.5405</t>
+          <t>2.5404</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -9153,17 +9153,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>0.6603</t>
+          <t>0.6381</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0.469</t>
+          <t>0.453</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>0.929</t>
+          <t>0.898</t>
         </is>
       </c>
     </row>
@@ -9176,17 +9176,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.1059</t>
+          <t>1.1782</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>0.580</t>
+          <t>0.618</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>2.108</t>
+          <t>2.247</t>
         </is>
       </c>
     </row>
@@ -9511,17 +9511,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>0.9805</t>
+          <t>0.9827</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.957</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1.007</t>
+          <t>1.009</t>
         </is>
       </c>
     </row>
@@ -9534,12 +9534,12 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>0.0582</t>
+          <t>0.0584</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>0.056</t>
+          <t>0.057</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -9557,7 +9557,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>0.6179</t>
+          <t>0.6178</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -9695,17 +9695,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>0.5389</t>
+          <t>0.6108</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>0.380</t>
+          <t>0.431</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>0.867</t>
         </is>
       </c>
     </row>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>0.4585</t>
+          <t>0.4584</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">

</xml_diff>

<commit_message>
this is awesome. We are done.
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -704,17 +704,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.2699</t>
+          <t>2.7164</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.181</t>
+          <t>1.823</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.402</t>
+          <t>4.048</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.1163</t>
+          <t>17.0855</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.064</t>
+          <t>9.376</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.212</t>
+          <t>31.133</t>
         </is>
       </c>
     </row>
@@ -998,17 +998,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.0319</t>
+          <t>8.0417</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.010</t>
+          <t>2.583</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.099</t>
+          <t>25.039</t>
         </is>
       </c>
     </row>
@@ -1246,17 +1246,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.4400</t>
+          <t>1.0213</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>0.859</t>
+          <t>0.609</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.413</t>
+          <t>1.711</t>
         </is>
       </c>
     </row>
@@ -1269,17 +1269,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.2746</t>
+          <t>0.4707</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.077</t>
+          <t>0.131</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0.984</t>
+          <t>1.686</t>
         </is>
       </c>
     </row>
@@ -1574,17 +1574,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.4817</t>
+          <t>1.9442</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.351</t>
+          <t>1.418</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>2.666</t>
         </is>
       </c>
     </row>
@@ -1597,17 +1597,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.2433</t>
+          <t>10.4248</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.155</t>
+          <t>6.649</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.381</t>
+          <t>16.344</t>
         </is>
       </c>
     </row>
@@ -1868,17 +1868,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.1621</t>
+          <t>8.5882</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.095</t>
+          <t>5.036</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.276</t>
+          <t>14.645</t>
         </is>
       </c>
     </row>
@@ -2116,17 +2116,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.6192</t>
+          <t>1.4483</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.093</t>
+          <t>0.978</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2.399</t>
+          <t>2.146</t>
         </is>
       </c>
     </row>
@@ -2139,17 +2139,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.6665</t>
+          <t>0.8238</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.337</t>
+          <t>0.416</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.319</t>
+          <t>1.630</t>
         </is>
       </c>
     </row>
@@ -4184,17 +4184,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.3073</t>
+          <t>1.5388</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.176</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.537</t>
+          <t>2.690</t>
         </is>
       </c>
     </row>
@@ -4726,17 +4726,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2.9090</t>
+          <t>0.2939</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.649</t>
+          <t>0.167</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>5.132</t>
+          <t>0.519</t>
         </is>
       </c>
     </row>
@@ -5268,17 +5268,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2.8259</t>
+          <t>0.5775</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.572</t>
+          <t>0.321</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5.079</t>
+          <t>1.038</t>
         </is>
       </c>
     </row>
@@ -5890,17 +5890,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.0777</t>
+          <t>0.7206</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.040</t>
+          <t>0.369</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.152</t>
+          <t>1.405</t>
         </is>
       </c>
     </row>
@@ -6432,17 +6432,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>11.5875</t>
+          <t>0.8083</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5.927</t>
+          <t>0.413</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>22.655</t>
+          <t>1.580</t>
         </is>
       </c>
     </row>
@@ -6974,17 +6974,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>9.5929</t>
+          <t>0.9365</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4.807</t>
+          <t>0.469</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>19.142</t>
+          <t>1.869</t>
         </is>
       </c>
     </row>
@@ -7550,17 +7550,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.1623</t>
+          <t>0.8948</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.086</t>
+          <t>0.475</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.306</t>
+          <t>1.685</t>
         </is>
       </c>
     </row>
@@ -7573,17 +7573,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>1.4727</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.601</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>3.609</t>
         </is>
       </c>
     </row>
@@ -8092,17 +8092,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>5.8898</t>
+          <t>0.6503</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3.098</t>
+          <t>0.342</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>11.199</t>
+          <t>1.236</t>
         </is>
       </c>
     </row>
@@ -8115,17 +8115,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>124178.0726</t>
+          <t>0.6018</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>50304.818</t>
+          <t>0.244</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>306535.127</t>
+          <t>1.486</t>
         </is>
       </c>
     </row>
@@ -8634,17 +8634,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>4.7811</t>
+          <t>0.5430</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2.498</t>
+          <t>0.284</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>9.152</t>
+          <t>1.040</t>
         </is>
       </c>
     </row>
@@ -8657,17 +8657,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>109276.7000</t>
+          <t>0.6597</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>43027.672</t>
+          <t>0.260</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>277528.311</t>
+          <t>1.675</t>
         </is>
       </c>
     </row>
@@ -9199,17 +9199,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>4.1487</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.530</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>11.251</t>
         </is>
       </c>
     </row>
@@ -9447,17 +9447,17 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>1.3000</t>
+          <t>1.7815</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>0.536</t>
+          <t>0.735</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3.152</t>
+          <t>4.319</t>
         </is>
       </c>
     </row>
@@ -9741,17 +9741,17 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>4.6807</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.715</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>12.776</t>
         </is>
       </c>
     </row>
@@ -10012,17 +10012,17 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>0.0000</t>
+          <t>4.2705</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.525</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>11.959</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Makefile fixed to depend on yaml for KCOR. so if change yaml params, it only will run KCOR which will be much faster. in this latest run I set the COVID correction factor to 1.7
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -498,17 +498,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2730</t>
+          <t>1.3458</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.316</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.302</t>
+          <t>1.376</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.9372</t>
+          <t>1.0312</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.860</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.125</t>
         </is>
       </c>
     </row>
@@ -544,17 +544,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0132</t>
+          <t>1.0921</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.971</t>
+          <t>1.046</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.140</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.5400</t>
+          <t>1.6362</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.492</t>
+          <t>1.585</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.589</t>
+          <t>1.689</t>
         </is>
       </c>
     </row>
@@ -590,17 +590,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6034</t>
+          <t>1.6638</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.482</t>
+          <t>1.538</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.734</t>
+          <t>1.800</t>
         </is>
       </c>
     </row>
@@ -613,17 +613,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4221</t>
+          <t>1.4938</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.232</t>
+          <t>1.294</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.641</t>
+          <t>1.724</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.9826</t>
+          <t>3.1706</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.341</t>
+          <t>2.488</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3.800</t>
+          <t>4.041</t>
         </is>
       </c>
     </row>
@@ -659,17 +659,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0472</t>
+          <t>1.1314</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.691</t>
+          <t>0.746</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.586</t>
+          <t>1.715</t>
         </is>
       </c>
     </row>
@@ -682,17 +682,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.5682</t>
+          <t>2.7688</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.632</t>
+          <t>1.756</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.041</t>
+          <t>4.366</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12.4845</t>
+          <t>12.7611</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5.875</t>
+          <t>6.001</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>26.530</t>
+          <t>27.134</t>
         </is>
       </c>
     </row>
@@ -746,17 +746,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5337</t>
+          <t>1.6214</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.508</t>
+          <t>1.594</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.559</t>
+          <t>1.649</t>
         </is>
       </c>
     </row>
@@ -769,17 +769,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.2853</t>
+          <t>1.4143</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.230</t>
+          <t>1.351</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.343</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -792,17 +792,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.5126</t>
+          <t>1.6304</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.474</t>
+          <t>1.588</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.552</t>
+          <t>1.674</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6057</t>
+          <t>1.7061</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.545</t>
+          <t>1.640</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.669</t>
+          <t>1.774</t>
         </is>
       </c>
     </row>
@@ -838,17 +838,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2380</t>
+          <t>1.2846</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.149</t>
+          <t>1.192</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.334</t>
+          <t>1.385</t>
         </is>
       </c>
     </row>
@@ -861,17 +861,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2537</t>
+          <t>1.3170</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.083</t>
+          <t>1.138</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.451</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -884,17 +884,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1030</t>
+          <t>1.1725</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.868</t>
+          <t>0.922</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.402</t>
+          <t>1.491</t>
         </is>
       </c>
     </row>
@@ -907,17 +907,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.5983</t>
+          <t>0.6465</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.388</t>
+          <t>0.418</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.924</t>
+          <t>0.999</t>
         </is>
       </c>
     </row>
@@ -930,17 +930,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1881</t>
+          <t>1.2809</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.709</t>
+          <t>0.763</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.991</t>
+          <t>2.150</t>
         </is>
       </c>
     </row>
@@ -953,17 +953,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.2478</t>
+          <t>2.2976</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.315</t>
+          <t>0.322</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>16.031</t>
+          <t>16.390</t>
         </is>
       </c>
     </row>
@@ -1299,17 +1299,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.1573</t>
+          <t>1.2374</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.214</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.180</t>
+          <t>1.262</t>
         </is>
       </c>
     </row>
@@ -1322,17 +1322,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.6681</t>
+          <t>0.7333</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.604</t>
+          <t>0.662</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.739</t>
+          <t>0.812</t>
         </is>
       </c>
     </row>
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9813</t>
+          <t>1.0742</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.933</t>
+          <t>1.021</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.032</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1368,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.0733</t>
+          <t>1.1453</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.038</t>
+          <t>1.107</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.185</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.4924</t>
+          <t>1.5805</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.442</t>
+          <t>1.527</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.544</t>
+          <t>1.636</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1414,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4221</t>
+          <t>1.5105</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.338</t>
+          <t>1.420</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.511</t>
+          <t>1.607</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1437,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2246</t>
+          <t>1.2898</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>1.146</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.377</t>
+          <t>1.451</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2424</t>
+          <t>1.3457</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>1.071</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.558</t>
+          <t>1.690</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0686</t>
+          <t>1.1705</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.661</t>
+          <t>0.722</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.728</t>
+          <t>1.897</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>11.9909</t>
+          <t>12.1927</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8.184</t>
+          <t>8.314</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>17.569</t>
+          <t>17.880</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1039</t>
+          <t>1.1803</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.089</t>
+          <t>1.163</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.197</t>
         </is>
       </c>
     </row>
@@ -1570,17 +1570,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9198</t>
+          <t>1.0096</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.882</t>
+          <t>0.966</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.959</t>
+          <t>1.055</t>
         </is>
       </c>
     </row>
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0100</t>
+          <t>1.1056</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>1.077</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.135</t>
         </is>
       </c>
     </row>
@@ -1616,17 +1616,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.2556</t>
+          <t>1.3398</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.224</t>
+          <t>1.305</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.288</t>
+          <t>1.375</t>
         </is>
       </c>
     </row>
@@ -1639,17 +1639,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.0692</t>
+          <t>1.1323</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.017</t>
+          <t>1.077</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.124</t>
+          <t>1.191</t>
         </is>
       </c>
     </row>
@@ -1662,17 +1662,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2528</t>
+          <t>1.3306</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.142</t>
+          <t>1.212</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>1.461</t>
         </is>
       </c>
     </row>
@@ -1685,17 +1685,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0301</t>
+          <t>1.0849</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.934</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.195</t>
+          <t>1.260</t>
         </is>
       </c>
     </row>
@@ -1708,17 +1708,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2.7059</t>
+          <t>2.9310</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2.116</t>
+          <t>2.289</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3.460</t>
+          <t>3.754</t>
         </is>
       </c>
     </row>
@@ -1731,17 +1731,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.8828</t>
+          <t>0.9670</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.635</t>
+          <t>0.693</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.227</t>
+          <t>1.349</t>
         </is>
       </c>
     </row>
@@ -1754,17 +1754,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.0935</t>
+          <t>7.2128</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3.762</t>
+          <t>3.823</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>13.377</t>
+          <t>13.609</t>
         </is>
       </c>
     </row>
@@ -2100,17 +2100,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9292</t>
+          <t>1.0013</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.979</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.950</t>
+          <t>1.024</t>
         </is>
       </c>
     </row>
@@ -2123,17 +2123,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.6358</t>
+          <t>0.6993</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.565</t>
+          <t>0.621</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.787</t>
         </is>
       </c>
     </row>
@@ -2146,17 +2146,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.8751</t>
+          <t>0.9678</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.828</t>
+          <t>0.915</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.924</t>
+          <t>1.023</t>
         </is>
       </c>
     </row>
@@ -2169,17 +2169,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8511</t>
+          <t>0.9154</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.815</t>
+          <t>0.876</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.889</t>
+          <t>0.957</t>
         </is>
       </c>
     </row>
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.0902</t>
+          <t>1.1634</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.047</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.213</t>
         </is>
       </c>
     </row>
@@ -2215,17 +2215,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1077</t>
+          <t>1.1809</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>1.112</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.175</t>
+          <t>1.254</t>
         </is>
       </c>
     </row>
@@ -2238,17 +2238,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2436</t>
+          <t>1.3103</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.197</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.359</t>
+          <t>1.434</t>
         </is>
       </c>
     </row>
@@ -2261,17 +2261,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9481</t>
+          <t>1.0123</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.797</t>
+          <t>0.849</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.207</t>
         </is>
       </c>
     </row>
@@ -2284,17 +2284,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.1828</t>
+          <t>3.5341</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.274</t>
+          <t>2.513</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.455</t>
+          <t>4.970</t>
         </is>
       </c>
     </row>
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.5841</t>
+          <t>0.6005</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.300</t>
+          <t>0.309</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.168</t>
         </is>
       </c>
     </row>
@@ -2348,17 +2348,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0172</t>
+          <t>1.0962</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.004</t>
+          <t>1.081</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.031</t>
+          <t>1.111</t>
         </is>
       </c>
     </row>
@@ -2371,17 +2371,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8401</t>
+          <t>0.9238</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.805</t>
+          <t>0.884</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.966</t>
         </is>
       </c>
     </row>
@@ -2394,17 +2394,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.9366</t>
+          <t>1.0358</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.914</t>
+          <t>1.009</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.960</t>
+          <t>1.063</t>
         </is>
       </c>
     </row>
@@ -2417,17 +2417,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.0464</t>
+          <t>1.1255</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.098</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.154</t>
         </is>
       </c>
     </row>
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2922</t>
+          <t>1.3789</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.249</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.337</t>
+          <t>1.428</t>
         </is>
       </c>
     </row>
@@ -2463,17 +2463,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.0562</t>
+          <t>1.1260</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.986</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.131</t>
+          <t>1.207</t>
         </is>
       </c>
     </row>
@@ -2486,17 +2486,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1184</t>
+          <t>1.1784</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.052</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.252</t>
+          <t>1.320</t>
         </is>
       </c>
     </row>
@@ -2509,17 +2509,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.2819</t>
+          <t>1.3687</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.117</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.568</t>
+          <t>1.678</t>
         </is>
       </c>
     </row>
@@ -2532,17 +2532,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.1448</t>
+          <t>2.3815</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.600</t>
+          <t>1.767</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.875</t>
+          <t>3.209</t>
         </is>
       </c>
     </row>
@@ -2555,17 +2555,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.3659</t>
+          <t>1.4043</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.955</t>
+          <t>0.980</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.954</t>
+          <t>2.012</t>
         </is>
       </c>
     </row>
@@ -2901,17 +2901,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6229</t>
+          <t>0.6761</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.601</t>
+          <t>0.652</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.646</t>
+          <t>0.701</t>
         </is>
       </c>
     </row>
@@ -2924,17 +2924,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.4255</t>
+          <t>0.4698</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.354</t>
+          <t>0.391</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.511</t>
+          <t>0.564</t>
         </is>
       </c>
     </row>
@@ -2947,17 +2947,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.5884</t>
+          <t>0.6539</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.542</t>
+          <t>0.602</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.638</t>
+          <t>0.710</t>
         </is>
       </c>
     </row>
@@ -2970,17 +2970,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.5786</t>
+          <t>0.6278</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.540</t>
+          <t>0.585</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.620</t>
+          <t>0.673</t>
         </is>
       </c>
     </row>
@@ -2993,17 +2993,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.6146</t>
+          <t>0.6577</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.570</t>
+          <t>0.610</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.662</t>
+          <t>0.709</t>
         </is>
       </c>
     </row>
@@ -3016,17 +3016,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9494</t>
+          <t>1.0153</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.850</t>
+          <t>0.909</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.060</t>
+          <t>1.134</t>
         </is>
       </c>
     </row>
@@ -3039,17 +3039,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.0622</t>
+          <t>1.1324</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.230</t>
+          <t>1.313</t>
         </is>
       </c>
     </row>
@@ -3062,17 +3062,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2058</t>
+          <t>1.2971</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.990</t>
+          <t>1.063</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.468</t>
+          <t>1.583</t>
         </is>
       </c>
     </row>
@@ -3085,17 +3085,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0090</t>
+          <t>1.1033</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.738</t>
+          <t>0.803</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.379</t>
+          <t>1.516</t>
         </is>
       </c>
     </row>
@@ -3108,17 +3108,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.1597</t>
+          <t>1.2412</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.789</t>
+          <t>0.841</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.704</t>
+          <t>1.831</t>
         </is>
       </c>
     </row>
@@ -3149,17 +3149,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.8737</t>
+          <t>0.9484</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.863</t>
+          <t>0.936</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.885</t>
+          <t>0.961</t>
         </is>
       </c>
     </row>
@@ -3172,17 +3172,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.7453</t>
+          <t>0.8229</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.715</t>
+          <t>0.788</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.777</t>
+          <t>0.860</t>
         </is>
       </c>
     </row>
@@ -3195,17 +3195,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.7838</t>
+          <t>0.8709</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.765</t>
+          <t>0.849</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.894</t>
         </is>
       </c>
     </row>
@@ -3218,17 +3218,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.8780</t>
+          <t>0.9526</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.930</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.898</t>
+          <t>0.976</t>
         </is>
       </c>
     </row>
@@ -3241,17 +3241,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.9147</t>
+          <t>0.9788</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.888</t>
+          <t>0.949</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.942</t>
+          <t>1.009</t>
         </is>
       </c>
     </row>
@@ -3264,17 +3264,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2633</t>
+          <t>1.3510</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.203</t>
+          <t>1.284</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.327</t>
+          <t>1.421</t>
         </is>
       </c>
     </row>
@@ -3287,17 +3287,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1025</t>
+          <t>1.1753</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.087</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.271</t>
         </is>
       </c>
     </row>
@@ -3310,17 +3310,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.6227</t>
+          <t>1.7456</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.410</t>
+          <t>1.511</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>2.016</t>
         </is>
       </c>
     </row>
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1200</t>
+          <t>1.2247</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.881</t>
+          <t>0.957</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.424</t>
+          <t>1.567</t>
         </is>
       </c>
     </row>
@@ -3356,17 +3356,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.2840</t>
+          <t>0.3039</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.182</t>
+          <t>0.194</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.444</t>
+          <t>0.477</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
completed KCOR with a 2X covid correction. Vaccine had a benefit period even with the 2x correction but it was pretty mild..
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -498,17 +498,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3458</t>
+          <t>1.3624</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.316</t>
+          <t>1.332</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.376</t>
+          <t>1.393</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0312</t>
+          <t>1.0536</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.945</t>
+          <t>0.965</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.125</t>
+          <t>1.150</t>
         </is>
       </c>
     </row>
@@ -544,17 +544,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0921</t>
+          <t>1.1105</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.046</t>
+          <t>1.063</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.160</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6362</t>
+          <t>1.6583</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.585</t>
+          <t>1.606</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.689</t>
+          <t>1.712</t>
         </is>
       </c>
     </row>
@@ -590,17 +590,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6638</t>
+          <t>1.6773</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.538</t>
+          <t>1.550</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.800</t>
+          <t>1.814</t>
         </is>
       </c>
     </row>
@@ -613,17 +613,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4938</t>
+          <t>1.5101</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.308</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.724</t>
+          <t>1.743</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.1706</t>
+          <t>3.2140</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.488</t>
+          <t>2.522</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4.041</t>
+          <t>4.097</t>
         </is>
       </c>
     </row>
@@ -659,17 +659,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1314</t>
+          <t>1.1513</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.759</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.715</t>
+          <t>1.746</t>
         </is>
       </c>
     </row>
@@ -682,17 +682,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.7688</t>
+          <t>2.8159</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.756</t>
+          <t>1.785</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.366</t>
+          <t>4.443</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12.7611</t>
+          <t>12.8220</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.001</t>
+          <t>6.029</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>27.134</t>
+          <t>27.268</t>
         </is>
       </c>
     </row>
@@ -746,17 +746,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.6214</t>
+          <t>1.6414</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.594</t>
+          <t>1.614</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.649</t>
+          <t>1.669</t>
         </is>
       </c>
     </row>
@@ -769,17 +769,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.4143</t>
+          <t>1.4450</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.351</t>
+          <t>1.379</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.481</t>
+          <t>1.514</t>
         </is>
       </c>
     </row>
@@ -792,17 +792,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.6304</t>
+          <t>1.6579</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.588</t>
+          <t>1.614</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.674</t>
+          <t>1.703</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.7061</t>
+          <t>1.7291</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.640</t>
+          <t>1.662</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.774</t>
+          <t>1.798</t>
         </is>
       </c>
     </row>
@@ -838,17 +838,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2846</t>
+          <t>1.2950</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.192</t>
+          <t>1.201</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.385</t>
+          <t>1.396</t>
         </is>
       </c>
     </row>
@@ -861,17 +861,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3170</t>
+          <t>1.3314</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.138</t>
+          <t>1.150</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.525</t>
+          <t>1.541</t>
         </is>
       </c>
     </row>
@@ -884,17 +884,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1725</t>
+          <t>1.1886</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.922</t>
+          <t>0.935</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.491</t>
+          <t>1.511</t>
         </is>
       </c>
     </row>
@@ -907,17 +907,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6465</t>
+          <t>0.6578</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.418</t>
+          <t>0.426</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.999</t>
+          <t>1.016</t>
         </is>
       </c>
     </row>
@@ -930,17 +930,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.2809</t>
+          <t>1.3027</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.763</t>
+          <t>0.776</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.150</t>
+          <t>2.188</t>
         </is>
       </c>
     </row>
@@ -953,17 +953,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.2976</t>
+          <t>2.3086</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.322</t>
+          <t>0.324</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>16.390</t>
+          <t>16.470</t>
         </is>
       </c>
     </row>
@@ -1299,17 +1299,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2374</t>
+          <t>1.2558</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.214</t>
+          <t>1.232</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.262</t>
+          <t>1.280</t>
         </is>
       </c>
     </row>
@@ -1322,17 +1322,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7333</t>
+          <t>0.7488</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.662</t>
+          <t>0.676</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.812</t>
+          <t>0.829</t>
         </is>
       </c>
     </row>
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0742</t>
+          <t>1.0962</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.021</t>
+          <t>1.042</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.130</t>
+          <t>1.154</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1368,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1453</t>
+          <t>1.1618</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.107</t>
+          <t>1.122</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.185</t>
+          <t>1.203</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5805</t>
+          <t>1.6006</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.527</t>
+          <t>1.546</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.636</t>
+          <t>1.657</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1414,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.5105</t>
+          <t>1.5308</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.420</t>
+          <t>1.439</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.607</t>
+          <t>1.629</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1437,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2898</t>
+          <t>1.3047</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.146</t>
+          <t>1.159</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.451</t>
+          <t>1.468</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.3457</t>
+          <t>1.3702</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.071</t>
+          <t>1.090</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.690</t>
+          <t>1.722</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1705</t>
+          <t>1.1949</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.722</t>
+          <t>0.737</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.897</t>
+          <t>1.938</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12.1927</t>
+          <t>12.2368</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8.314</t>
+          <t>8.343</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>17.880</t>
+          <t>17.949</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1803</t>
+          <t>1.1978</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.163</t>
+          <t>1.181</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.215</t>
         </is>
       </c>
     </row>
@@ -1570,17 +1570,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0096</t>
+          <t>1.0309</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.055</t>
+          <t>1.078</t>
         </is>
       </c>
     </row>
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.1056</t>
+          <t>1.1283</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.099</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.135</t>
+          <t>1.158</t>
         </is>
       </c>
     </row>
@@ -1616,17 +1616,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3398</t>
+          <t>1.3592</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.305</t>
+          <t>1.324</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.375</t>
+          <t>1.396</t>
         </is>
       </c>
     </row>
@@ -1639,17 +1639,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1323</t>
+          <t>1.1468</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.077</t>
+          <t>1.090</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.191</t>
+          <t>1.206</t>
         </is>
       </c>
     </row>
@@ -1662,17 +1662,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3306</t>
+          <t>1.3485</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.212</t>
+          <t>1.228</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.461</t>
+          <t>1.481</t>
         </is>
       </c>
     </row>
@@ -1685,17 +1685,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0849</t>
+          <t>1.0974</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.934</t>
+          <t>0.945</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.260</t>
+          <t>1.274</t>
         </is>
       </c>
     </row>
@@ -1708,17 +1708,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2.9310</t>
+          <t>2.9842</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2.289</t>
+          <t>2.329</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3.754</t>
+          <t>3.823</t>
         </is>
       </c>
     </row>
@@ -1731,17 +1731,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9670</t>
+          <t>0.9872</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.693</t>
+          <t>0.707</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.349</t>
+          <t>1.379</t>
         </is>
       </c>
     </row>
@@ -1754,17 +1754,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.2128</t>
+          <t>7.2390</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3.823</t>
+          <t>3.836</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>13.609</t>
+          <t>13.660</t>
         </is>
       </c>
     </row>
@@ -2100,17 +2100,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.0013</t>
+          <t>1.0180</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.979</t>
+          <t>0.996</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>1.041</t>
         </is>
       </c>
     </row>
@@ -2123,17 +2123,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.6993</t>
+          <t>0.7143</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.621</t>
+          <t>0.634</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.787</t>
+          <t>0.804</t>
         </is>
       </c>
     </row>
@@ -2146,17 +2146,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9678</t>
+          <t>0.9900</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.915</t>
+          <t>0.936</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.023</t>
+          <t>1.047</t>
         </is>
       </c>
     </row>
@@ -2169,17 +2169,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.9154</t>
+          <t>0.9303</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.876</t>
+          <t>0.890</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.972</t>
         </is>
       </c>
     </row>
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1634</t>
+          <t>1.1803</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.116</t>
+          <t>1.132</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.213</t>
+          <t>1.230</t>
         </is>
       </c>
     </row>
@@ -2215,17 +2215,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1809</t>
+          <t>1.1977</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.112</t>
+          <t>1.128</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.254</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -2238,17 +2238,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.3103</t>
+          <t>1.3255</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.197</t>
+          <t>1.211</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.434</t>
+          <t>1.451</t>
         </is>
       </c>
     </row>
@@ -2261,17 +2261,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.0123</t>
+          <t>1.0272</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.861</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.207</t>
+          <t>1.226</t>
         </is>
       </c>
     </row>
@@ -2284,17 +2284,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.5341</t>
+          <t>3.6197</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.513</t>
+          <t>2.571</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.970</t>
+          <t>5.096</t>
         </is>
       </c>
     </row>
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.6005</t>
+          <t>0.6042</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.309</t>
+          <t>0.310</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.168</t>
+          <t>1.176</t>
         </is>
       </c>
     </row>
@@ -2348,17 +2348,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0962</t>
+          <t>1.1145</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.081</t>
+          <t>1.099</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.111</t>
+          <t>1.130</t>
         </is>
       </c>
     </row>
@@ -2371,17 +2371,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9238</t>
+          <t>0.9437</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.884</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.966</t>
+          <t>0.987</t>
         </is>
       </c>
     </row>
@@ -2394,17 +2394,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0358</t>
+          <t>1.0595</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.032</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.063</t>
+          <t>1.088</t>
         </is>
       </c>
     </row>
@@ -2417,17 +2417,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.1255</t>
+          <t>1.1438</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.098</t>
+          <t>1.116</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.154</t>
+          <t>1.173</t>
         </is>
       </c>
     </row>
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3789</t>
+          <t>1.3989</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.332</t>
+          <t>1.351</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.428</t>
+          <t>1.448</t>
         </is>
       </c>
     </row>
@@ -2463,17 +2463,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1260</t>
+          <t>1.1421</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.050</t>
+          <t>1.065</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.207</t>
+          <t>1.225</t>
         </is>
       </c>
     </row>
@@ -2486,17 +2486,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1784</t>
+          <t>1.1921</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.052</t>
+          <t>1.064</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.320</t>
+          <t>1.336</t>
         </is>
       </c>
     </row>
@@ -2509,17 +2509,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.3687</t>
+          <t>1.3888</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.117</t>
+          <t>1.133</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.678</t>
+          <t>1.703</t>
         </is>
       </c>
     </row>
@@ -2532,17 +2532,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.3815</t>
+          <t>2.4392</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.767</t>
+          <t>1.808</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3.209</t>
+          <t>3.291</t>
         </is>
       </c>
     </row>
@@ -2555,17 +2555,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.4043</t>
+          <t>1.4128</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.980</t>
+          <t>0.986</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2.012</t>
+          <t>2.025</t>
         </is>
       </c>
     </row>
@@ -2901,17 +2901,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6761</t>
+          <t>0.6885</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.652</t>
+          <t>0.664</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.701</t>
+          <t>0.714</t>
         </is>
       </c>
     </row>
@@ -2924,17 +2924,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.4698</t>
+          <t>0.4804</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.391</t>
+          <t>0.400</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.564</t>
+          <t>0.577</t>
         </is>
       </c>
     </row>
@@ -2947,17 +2947,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6539</t>
+          <t>0.6696</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.602</t>
+          <t>0.617</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.710</t>
+          <t>0.727</t>
         </is>
       </c>
     </row>
@@ -2970,17 +2970,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.6278</t>
+          <t>0.6393</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.585</t>
+          <t>0.596</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.673</t>
+          <t>0.686</t>
         </is>
       </c>
     </row>
@@ -2993,17 +2993,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.6577</t>
+          <t>0.6676</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.610</t>
+          <t>0.619</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.709</t>
+          <t>0.720</t>
         </is>
       </c>
     </row>
@@ -3016,17 +3016,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.0153</t>
+          <t>1.0305</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.909</t>
+          <t>0.922</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.134</t>
+          <t>1.151</t>
         </is>
       </c>
     </row>
@@ -3039,17 +3039,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1324</t>
+          <t>1.1486</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.977</t>
+          <t>0.991</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.313</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -3062,17 +3062,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2971</t>
+          <t>1.3185</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.063</t>
+          <t>1.080</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.583</t>
+          <t>1.610</t>
         </is>
       </c>
     </row>
@@ -3085,17 +3085,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1033</t>
+          <t>1.1258</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.803</t>
+          <t>0.818</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.516</t>
+          <t>1.549</t>
         </is>
       </c>
     </row>
@@ -3108,17 +3108,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.2412</t>
+          <t>1.2602</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.841</t>
+          <t>0.853</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.831</t>
+          <t>1.861</t>
         </is>
       </c>
     </row>
@@ -3149,17 +3149,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.9484</t>
+          <t>0.9658</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.953</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.961</t>
+          <t>0.978</t>
         </is>
       </c>
     </row>
@@ -3172,17 +3172,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8229</t>
+          <t>0.8414</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.805</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.860</t>
+          <t>0.880</t>
         </is>
       </c>
     </row>
@@ -3195,17 +3195,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8709</t>
+          <t>0.8919</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.849</t>
+          <t>0.869</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.894</t>
+          <t>0.915</t>
         </is>
       </c>
     </row>
@@ -3218,17 +3218,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9526</t>
+          <t>0.9701</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.976</t>
+          <t>0.994</t>
         </is>
       </c>
     </row>
@@ -3241,17 +3241,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.9788</t>
+          <t>0.9935</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.949</t>
+          <t>0.964</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.009</t>
+          <t>1.024</t>
         </is>
       </c>
     </row>
@@ -3264,17 +3264,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3510</t>
+          <t>1.3713</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.284</t>
+          <t>1.303</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.421</t>
+          <t>1.443</t>
         </is>
       </c>
     </row>
@@ -3287,17 +3287,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1753</t>
+          <t>1.1921</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.087</t>
+          <t>1.102</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.271</t>
+          <t>1.289</t>
         </is>
       </c>
     </row>
@@ -3310,17 +3310,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.7456</t>
+          <t>1.7743</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.511</t>
+          <t>1.535</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2.016</t>
+          <t>2.051</t>
         </is>
       </c>
     </row>
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.2247</t>
+          <t>1.2497</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.602</t>
         </is>
       </c>
     </row>
@@ -3356,17 +3356,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.3039</t>
+          <t>0.3086</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.194</t>
+          <t>0.197</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.477</t>
+          <t>0.484</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1/27 correction for COVID
</commit_message>
<xml_diff>
--- a/data/Czech/KCOR_summary.xlsx
+++ b/data/Czech/KCOR_summary.xlsx
@@ -498,17 +498,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.3227</t>
+          <t>1.3097</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.294</t>
+          <t>1.281</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.352</t>
+          <t>1.339</t>
         </is>
       </c>
     </row>
@@ -521,17 +521,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1.0006</t>
+          <t>0.9837</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.917</t>
+          <t>0.902</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.073</t>
         </is>
       </c>
     </row>
@@ -544,17 +544,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0667</t>
+          <t>1.0525</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.022</t>
+          <t>1.008</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.113</t>
+          <t>1.099</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.6055</t>
+          <t>1.5883</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.555</t>
+          <t>1.539</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.657</t>
+          <t>1.639</t>
         </is>
       </c>
     </row>
@@ -590,17 +590,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.6449</t>
+          <t>1.6341</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.521</t>
+          <t>1.511</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.779</t>
+          <t>1.768</t>
         </is>
       </c>
     </row>
@@ -613,17 +613,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4711</t>
+          <t>1.4582</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.275</t>
+          <t>1.264</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.698</t>
+          <t>1.683</t>
         </is>
       </c>
     </row>
@@ -636,17 +636,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>3.1106</t>
+          <t>3.0768</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.441</t>
+          <t>2.415</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3.964</t>
+          <t>3.920</t>
         </is>
       </c>
     </row>
@@ -659,17 +659,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.1042</t>
+          <t>1.0891</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.729</t>
+          <t>0.719</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.673</t>
+          <t>1.650</t>
         </is>
       </c>
     </row>
@@ -682,17 +682,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2.7042</t>
+          <t>2.6680</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.716</t>
+          <t>1.694</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.261</t>
+          <t>4.203</t>
         </is>
       </c>
     </row>
@@ -705,17 +705,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12.6752</t>
+          <t>12.6258</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5.962</t>
+          <t>5.940</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>26.946</t>
+          <t>26.839</t>
         </is>
       </c>
     </row>
@@ -746,17 +746,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.5935</t>
+          <t>1.5778</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.567</t>
+          <t>1.552</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.621</t>
+          <t>1.604</t>
         </is>
       </c>
     </row>
@@ -769,17 +769,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.3723</t>
+          <t>1.3491</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.312</t>
+          <t>1.290</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.436</t>
+          <t>1.411</t>
         </is>
       </c>
     </row>
@@ -792,17 +792,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.5926</t>
+          <t>1.5714</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.551</t>
+          <t>1.531</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.635</t>
+          <t>1.613</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.6741</t>
+          <t>1.6561</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.610</t>
+          <t>1.593</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.741</t>
+          <t>1.722</t>
         </is>
       </c>
     </row>
@@ -838,17 +838,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2699</t>
+          <t>1.2616</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.178</t>
+          <t>1.171</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.369</t>
+          <t>1.360</t>
         </is>
       </c>
     </row>
@@ -861,17 +861,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.2970</t>
+          <t>1.2856</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.120</t>
+          <t>1.111</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.501</t>
+          <t>1.488</t>
         </is>
       </c>
     </row>
@@ -884,17 +884,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1503</t>
+          <t>1.1379</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.905</t>
+          <t>0.895</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.462</t>
+          <t>1.446</t>
         </is>
       </c>
     </row>
@@ -907,17 +907,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.6309</t>
+          <t>0.6223</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.409</t>
+          <t>0.403</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.974</t>
+          <t>0.961</t>
         </is>
       </c>
     </row>
@@ -930,17 +930,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.2510</t>
+          <t>1.2343</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.746</t>
+          <t>0.736</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2.099</t>
+          <t>2.070</t>
         </is>
       </c>
     </row>
@@ -953,17 +953,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2.2822</t>
+          <t>2.2733</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.320</t>
+          <t>0.319</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>16.279</t>
+          <t>16.215</t>
         </is>
       </c>
     </row>
@@ -1299,17 +1299,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1.2119</t>
+          <t>1.1975</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.189</t>
+          <t>1.175</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.235</t>
+          <t>1.221</t>
         </is>
       </c>
     </row>
@@ -1322,17 +1322,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.7122</t>
+          <t>0.7004</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.643</t>
+          <t>0.633</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.788</t>
+          <t>0.775</t>
         </is>
       </c>
     </row>
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1.0441</t>
+          <t>1.0274</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.993</t>
+          <t>0.977</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.098</t>
+          <t>1.081</t>
         </is>
       </c>
     </row>
@@ -1368,17 +1368,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.1224</t>
+          <t>1.1094</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.072</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.161</t>
+          <t>1.148</t>
         </is>
       </c>
     </row>
@@ -1391,17 +1391,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.5525</t>
+          <t>1.5367</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.500</t>
+          <t>1.485</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.607</t>
+          <t>1.590</t>
         </is>
       </c>
     </row>
@@ -1414,17 +1414,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.4824</t>
+          <t>1.4665</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.394</t>
+          <t>1.379</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.576</t>
+          <t>1.559</t>
         </is>
       </c>
     </row>
@@ -1437,17 +1437,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2691</t>
+          <t>1.2574</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.128</t>
+          <t>1.118</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.428</t>
+          <t>1.414</t>
         </is>
       </c>
     </row>
@@ -1460,17 +1460,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.3123</t>
+          <t>1.2937</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.045</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.647</t>
+          <t>1.624</t>
         </is>
       </c>
     </row>
@@ -1483,17 +1483,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.1373</t>
+          <t>1.1189</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.702</t>
+          <t>0.691</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.842</t>
+          <t>1.811</t>
         </is>
       </c>
     </row>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12.1302</t>
+          <t>12.0943</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8.274</t>
+          <t>8.251</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>17.784</t>
+          <t>17.728</t>
         </is>
       </c>
     </row>
@@ -1547,17 +1547,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.1559</t>
+          <t>1.1422</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.140</t>
+          <t>1.126</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.173</t>
+          <t>1.159</t>
         </is>
       </c>
     </row>
@@ -1570,17 +1570,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.9805</t>
+          <t>0.9643</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.939</t>
+          <t>0.923</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.024</t>
+          <t>1.007</t>
         </is>
       </c>
     </row>
@@ -1593,17 +1593,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0747</t>
+          <t>1.0574</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.048</t>
+          <t>1.031</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.102</t>
+          <t>1.084</t>
         </is>
       </c>
     </row>
@@ -1616,17 +1616,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.3130</t>
+          <t>1.2979</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.279</t>
+          <t>1.265</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.348</t>
+          <t>1.332</t>
         </is>
       </c>
     </row>
@@ -1639,17 +1639,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.1123</t>
+          <t>1.1010</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.058</t>
+          <t>1.047</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.170</t>
+          <t>1.158</t>
         </is>
       </c>
     </row>
@@ -1662,17 +1662,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3058</t>
+          <t>1.2918</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.190</t>
+          <t>1.177</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.433</t>
+          <t>1.418</t>
         </is>
       </c>
     </row>
@@ -1685,17 +1685,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.0675</t>
+          <t>1.0577</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.920</t>
+          <t>0.911</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.239</t>
+          <t>1.228</t>
         </is>
       </c>
     </row>
@@ -1708,17 +1708,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2.8582</t>
+          <t>2.8176</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2.233</t>
+          <t>2.202</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3.658</t>
+          <t>3.605</t>
         </is>
       </c>
     </row>
@@ -1731,17 +1731,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.9396</t>
+          <t>0.9244</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.674</t>
+          <t>0.664</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.309</t>
+          <t>1.287</t>
         </is>
       </c>
     </row>
@@ -1754,17 +1754,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>7.1759</t>
+          <t>7.1546</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3.804</t>
+          <t>3.793</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>13.537</t>
+          <t>13.495</t>
         </is>
       </c>
     </row>
@@ -2100,17 +2100,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.9783</t>
+          <t>0.9653</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.957</t>
+          <t>0.944</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.000</t>
+          <t>0.987</t>
         </is>
       </c>
     </row>
@@ -2123,17 +2123,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.6787</t>
+          <t>0.6673</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.603</t>
+          <t>0.593</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>0.751</t>
         </is>
       </c>
     </row>
@@ -2146,17 +2146,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.9376</t>
+          <t>0.9209</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.887</t>
+          <t>0.871</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.991</t>
+          <t>0.973</t>
         </is>
       </c>
     </row>
@@ -2169,17 +2169,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.8948</t>
+          <t>0.8833</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.857</t>
+          <t>0.846</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.935</t>
+          <t>0.923</t>
         </is>
       </c>
     </row>
@@ -2192,17 +2192,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1.1401</t>
+          <t>1.1270</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1.094</t>
+          <t>1.082</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.188</t>
+          <t>1.174</t>
         </is>
       </c>
     </row>
@@ -2215,17 +2215,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1.1575</t>
+          <t>1.1444</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.091</t>
+          <t>1.079</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.228</t>
+          <t>1.214</t>
         </is>
       </c>
     </row>
@@ -2238,17 +2238,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.2892</t>
+          <t>1.2772</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.179</t>
+          <t>1.168</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.410</t>
+          <t>1.397</t>
         </is>
       </c>
     </row>
@@ -2261,17 +2261,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.9918</t>
+          <t>0.9802</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.832</t>
+          <t>0.823</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.182</t>
+          <t>1.168</t>
         </is>
       </c>
     </row>
@@ -2284,17 +2284,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.4186</t>
+          <t>3.3550</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2.435</t>
+          <t>2.392</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.800</t>
+          <t>4.707</t>
         </is>
       </c>
     </row>
@@ -2307,17 +2307,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.5954</t>
+          <t>0.5925</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.306</t>
+          <t>0.305</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.158</t>
+          <t>1.152</t>
         </is>
       </c>
     </row>
@@ -2348,17 +2348,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1.0709</t>
+          <t>1.0567</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.057</t>
+          <t>1.043</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.085</t>
+          <t>1.071</t>
         </is>
       </c>
     </row>
@@ -2371,17 +2371,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.8967</t>
+          <t>0.8816</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.858</t>
+          <t>0.844</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.937</t>
+          <t>0.921</t>
         </is>
       </c>
     </row>
@@ -2394,17 +2394,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.0035</t>
+          <t>0.9856</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.978</t>
+          <t>0.961</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.029</t>
+          <t>1.011</t>
         </is>
       </c>
     </row>
@@ -2417,17 +2417,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.1002</t>
+          <t>1.0860</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.074</t>
+          <t>1.060</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.127</t>
+          <t>1.113</t>
         </is>
       </c>
     </row>
@@ -2440,17 +2440,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.3513</t>
+          <t>1.3357</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.306</t>
+          <t>1.291</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.399</t>
+          <t>1.382</t>
         </is>
       </c>
     </row>
@@ -2463,17 +2463,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1037</t>
+          <t>1.0912</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.030</t>
+          <t>1.018</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.183</t>
+          <t>1.169</t>
         </is>
       </c>
     </row>
@@ -2486,17 +2486,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1594</t>
+          <t>1.1486</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.035</t>
+          <t>1.026</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.299</t>
+          <t>1.286</t>
         </is>
       </c>
     </row>
@@ -2509,17 +2509,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.3409</t>
+          <t>1.3253</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.095</t>
+          <t>1.082</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.643</t>
+          <t>1.623</t>
         </is>
       </c>
     </row>
@@ -2532,17 +2532,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2.3036</t>
+          <t>2.2608</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1.713</t>
+          <t>1.683</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3.098</t>
+          <t>3.038</t>
         </is>
       </c>
     </row>
@@ -2555,17 +2555,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1.3923</t>
+          <t>1.3854</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.972</t>
+          <t>0.968</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1.994</t>
+          <t>1.984</t>
         </is>
       </c>
     </row>
@@ -2901,17 +2901,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.6590</t>
+          <t>0.6494</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.635</t>
+          <t>0.626</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.684</t>
+          <t>0.674</t>
         </is>
       </c>
     </row>
@@ -2924,17 +2924,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.4555</t>
+          <t>0.4475</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.379</t>
+          <t>0.373</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.547</t>
+          <t>0.537</t>
         </is>
       </c>
     </row>
@@ -2947,17 +2947,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.6325</t>
+          <t>0.6207</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.583</t>
+          <t>0.572</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.687</t>
+          <t>0.674</t>
         </is>
       </c>
     </row>
@@ -2970,17 +2970,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.6120</t>
+          <t>0.6032</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.571</t>
+          <t>0.562</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.656</t>
+          <t>0.647</t>
         </is>
       </c>
     </row>
@@ -2993,17 +2993,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.6440</t>
+          <t>0.6362</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.597</t>
+          <t>0.590</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.694</t>
+          <t>0.686</t>
         </is>
       </c>
     </row>
@@ -3016,17 +3016,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.9943</t>
+          <t>0.9824</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.890</t>
+          <t>0.880</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1.110</t>
+          <t>1.097</t>
         </is>
       </c>
     </row>
@@ -3039,17 +3039,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1.1100</t>
+          <t>1.0974</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.958</t>
+          <t>0.947</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1.286</t>
+          <t>1.272</t>
         </is>
       </c>
     </row>
@@ -3062,17 +3062,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1.2678</t>
+          <t>1.2513</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.040</t>
+          <t>1.027</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.546</t>
+          <t>1.525</t>
         </is>
       </c>
     </row>
@@ -3085,17 +3085,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.0726</t>
+          <t>1.0556</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.782</t>
+          <t>0.770</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1.471</t>
+          <t>1.446</t>
         </is>
       </c>
     </row>
@@ -3108,17 +3108,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.2151</t>
+          <t>1.2004</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.825</t>
+          <t>0.815</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1.790</t>
+          <t>1.767</t>
         </is>
       </c>
     </row>
@@ -3149,17 +3149,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.9245</t>
+          <t>0.9110</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.913</t>
+          <t>0.900</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.936</t>
+          <t>0.923</t>
         </is>
       </c>
     </row>
@@ -3172,17 +3172,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.7977</t>
+          <t>0.7837</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.764</t>
+          <t>0.751</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.833</t>
+          <t>0.818</t>
         </is>
       </c>
     </row>
@@ -3195,17 +3195,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.8425</t>
+          <t>0.8268</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.822</t>
+          <t>0.807</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.864</t>
+          <t>0.848</t>
         </is>
       </c>
     </row>
@@ -3218,17 +3218,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.9287</t>
+          <t>0.9152</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.907</t>
+          <t>0.894</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.951</t>
+          <t>0.937</t>
         </is>
       </c>
     </row>
@@ -3241,17 +3241,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.9584</t>
+          <t>0.9469</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.930</t>
+          <t>0.919</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.988</t>
+          <t>0.976</t>
         </is>
       </c>
     </row>
@@ -3264,17 +3264,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.3230</t>
+          <t>1.3073</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.258</t>
+          <t>1.244</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1.391</t>
+          <t>1.374</t>
         </is>
       </c>
     </row>
@@ -3287,17 +3287,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.1521</t>
+          <t>1.1390</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.066</t>
+          <t>1.054</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1.245</t>
+          <t>1.230</t>
         </is>
       </c>
     </row>
@@ -3310,17 +3310,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1.7061</t>
+          <t>1.6839</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1.479</t>
+          <t>1.460</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1.968</t>
+          <t>1.942</t>
         </is>
       </c>
     </row>
@@ -3333,17 +3333,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1.1906</t>
+          <t>1.1717</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.932</t>
+          <t>0.919</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.520</t>
+          <t>1.495</t>
         </is>
       </c>
     </row>
@@ -3356,17 +3356,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.2975</t>
+          <t>0.2940</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.190</t>
+          <t>0.188</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.466</t>
+          <t>0.460</t>
         </is>
       </c>
     </row>

</xml_diff>